<commit_message>
rev excel db file
</commit_message>
<xml_diff>
--- a/db/excel/api-function-granted-users-cdld.xlsx
+++ b/db/excel/api-function-granted-users-cdld.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10613"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E298DE-9DC0-F54B-815E-4436FD306413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8233836-81E7-1041-A6D8-9F1BEED0725C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" tabRatio="800" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" tabRatio="800" firstSheet="1" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_types" sheetId="27" r:id="rId1"/>
@@ -275,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1270" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="516">
   <si>
     <t>status</t>
   </si>
@@ -4741,10 +4741,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4757,13 +4757,12 @@
     <col min="6" max="6" width="28.33203125" style="89" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="62.5" style="85" customWidth="1"/>
     <col min="8" max="8" width="55" style="85" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.1640625" style="85" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" style="85" customWidth="1"/>
-    <col min="11" max="11" width="65" style="85" customWidth="1"/>
-    <col min="12" max="16384" width="11.5" style="85"/>
+    <col min="9" max="9" width="10.83203125" style="85" customWidth="1"/>
+    <col min="10" max="10" width="65" style="85" customWidth="1"/>
+    <col min="11" max="16384" width="11.5" style="85"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="84" t="s">
         <v>18</v>
       </c>
@@ -4789,19 +4788,25 @@
         <v>4</v>
       </c>
       <c r="I1" s="84" t="s">
+        <v>153</v>
+      </c>
+      <c r="J1" s="84" t="s">
+        <v>160</v>
+      </c>
+      <c r="K1" s="84" t="s">
+        <v>154</v>
+      </c>
+      <c r="L1" s="84" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="84" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="K1" s="84" t="s">
-        <v>160</v>
-      </c>
-      <c r="L1" s="84" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="90">
         <v>1</v>
       </c>
@@ -4822,14 +4827,16 @@
       <c r="H2" s="90" t="s">
         <v>500</v>
       </c>
-      <c r="I2" s="90">
-        <v>1</v>
-      </c>
+      <c r="I2" s="90"/>
       <c r="J2" s="90"/>
       <c r="K2" s="90"/>
       <c r="L2" s="90"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" s="90"/>
+      <c r="N2" s="90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="86">
         <v>11</v>
       </c>
@@ -4850,14 +4857,16 @@
       <c r="H3" s="86" t="s">
         <v>396</v>
       </c>
-      <c r="I3" s="86">
-        <v>1</v>
-      </c>
+      <c r="I3" s="86"/>
       <c r="J3" s="86"/>
       <c r="K3" s="86"/>
       <c r="L3" s="86"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3" s="86"/>
+      <c r="N3" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="86">
         <v>12</v>
       </c>
@@ -4878,14 +4887,16 @@
       <c r="H4" s="86" t="s">
         <v>397</v>
       </c>
-      <c r="I4" s="86">
-        <v>1</v>
-      </c>
+      <c r="I4" s="86"/>
       <c r="J4" s="86"/>
       <c r="K4" s="86"/>
       <c r="L4" s="86"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4" s="86"/>
+      <c r="N4" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="86">
         <v>13</v>
       </c>
@@ -4906,14 +4917,16 @@
       <c r="H5" s="86" t="s">
         <v>398</v>
       </c>
-      <c r="I5" s="86">
-        <v>1</v>
-      </c>
+      <c r="I5" s="86"/>
       <c r="J5" s="86"/>
       <c r="K5" s="86"/>
       <c r="L5" s="86"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M5" s="86"/>
+      <c r="N5" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="86">
         <v>14</v>
       </c>
@@ -4934,14 +4947,16 @@
       <c r="H6" s="86" t="s">
         <v>400</v>
       </c>
-      <c r="I6" s="86">
-        <v>1</v>
-      </c>
+      <c r="I6" s="86"/>
       <c r="J6" s="86"/>
       <c r="K6" s="86"/>
       <c r="L6" s="86"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M6" s="86"/>
+      <c r="N6" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="86">
         <v>15</v>
       </c>
@@ -4962,14 +4977,16 @@
       <c r="H7" s="86" t="s">
         <v>402</v>
       </c>
-      <c r="I7" s="86">
-        <v>1</v>
-      </c>
+      <c r="I7" s="86"/>
       <c r="J7" s="86"/>
       <c r="K7" s="86"/>
       <c r="L7" s="86"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M7" s="86"/>
+      <c r="N7" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="86">
         <v>16</v>
       </c>
@@ -4990,14 +5007,16 @@
       <c r="H8" s="86" t="s">
         <v>407</v>
       </c>
-      <c r="I8" s="86">
-        <v>1</v>
-      </c>
+      <c r="I8" s="86"/>
       <c r="J8" s="86"/>
       <c r="K8" s="86"/>
       <c r="L8" s="86"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M8" s="86"/>
+      <c r="N8" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="90">
         <v>2</v>
       </c>
@@ -5016,14 +5035,16 @@
         <v>492</v>
       </c>
       <c r="H9" s="90"/>
-      <c r="I9" s="90">
-        <v>1</v>
-      </c>
+      <c r="I9" s="90"/>
       <c r="J9" s="90"/>
       <c r="K9" s="90"/>
       <c r="L9" s="90"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M9" s="90"/>
+      <c r="N9" s="90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="86">
         <v>21</v>
       </c>
@@ -5044,14 +5065,16 @@
       <c r="H10" s="86" t="s">
         <v>474</v>
       </c>
-      <c r="I10" s="86">
-        <v>1</v>
-      </c>
-      <c r="J10" s="86"/>
-      <c r="K10" s="88"/>
+      <c r="I10" s="86"/>
+      <c r="J10" s="88"/>
+      <c r="K10" s="86"/>
       <c r="L10" s="86"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M10" s="86"/>
+      <c r="N10" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="86">
         <v>22</v>
       </c>
@@ -5072,14 +5095,16 @@
       <c r="H11" s="86" t="s">
         <v>475</v>
       </c>
-      <c r="I11" s="86">
-        <v>1</v>
-      </c>
+      <c r="I11" s="86"/>
       <c r="J11" s="86"/>
       <c r="K11" s="86"/>
       <c r="L11" s="86"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M11" s="86"/>
+      <c r="N11" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="86">
         <v>23</v>
       </c>
@@ -5100,14 +5125,16 @@
       <c r="H12" s="86" t="s">
         <v>476</v>
       </c>
-      <c r="I12" s="86">
-        <v>1</v>
-      </c>
+      <c r="I12" s="86"/>
       <c r="J12" s="86"/>
       <c r="K12" s="86"/>
       <c r="L12" s="86"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M12" s="86"/>
+      <c r="N12" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="86">
         <v>24</v>
       </c>
@@ -5128,14 +5155,16 @@
       <c r="H13" s="86" t="s">
         <v>477</v>
       </c>
-      <c r="I13" s="86">
-        <v>1</v>
-      </c>
+      <c r="I13" s="86"/>
       <c r="J13" s="86"/>
       <c r="K13" s="86"/>
       <c r="L13" s="86"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M13" s="86"/>
+      <c r="N13" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="90">
         <v>3</v>
       </c>
@@ -5154,14 +5183,16 @@
         <v>499</v>
       </c>
       <c r="H14" s="90"/>
-      <c r="I14" s="90">
-        <v>1</v>
-      </c>
+      <c r="I14" s="90"/>
       <c r="J14" s="90"/>
       <c r="K14" s="90"/>
       <c r="L14" s="90"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M14" s="90"/>
+      <c r="N14" s="90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="86">
         <v>31</v>
       </c>
@@ -5182,14 +5213,16 @@
       <c r="H15" s="86" t="s">
         <v>482</v>
       </c>
-      <c r="I15" s="86">
-        <v>1</v>
-      </c>
-      <c r="J15" s="86"/>
-      <c r="K15" s="88"/>
+      <c r="I15" s="86"/>
+      <c r="J15" s="88"/>
+      <c r="K15" s="86"/>
       <c r="L15" s="86"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M15" s="86"/>
+      <c r="N15" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="90">
         <v>4</v>
       </c>
@@ -5210,12 +5243,14 @@
       <c r="H16" s="90" t="s">
         <v>484</v>
       </c>
-      <c r="I16" s="90">
-        <v>1</v>
-      </c>
+      <c r="I16" s="90"/>
       <c r="J16" s="90"/>
       <c r="K16" s="90"/>
       <c r="L16" s="90"/>
+      <c r="M16" s="90"/>
+      <c r="N16" s="90">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5232,7 +5267,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -5404,19 +5439,18 @@
   </sheetPr>
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="3" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -5432,16 +5466,16 @@
         <v>245</v>
       </c>
       <c r="D1" s="40" t="s">
+        <v>181</v>
+      </c>
+      <c r="E1" s="40" t="s">
         <v>140</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="F1" s="40" t="s">
         <v>206</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="G1" s="40" t="s">
         <v>19</v>
-      </c>
-      <c r="G1" s="40" t="s">
-        <v>181</v>
       </c>
       <c r="H1" s="40" t="s">
         <v>45</v>
@@ -5477,7 +5511,7 @@
       <c r="C3" t="s">
         <v>357</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0</v>
       </c>
       <c r="H3" t="s">
@@ -5497,7 +5531,7 @@
       <c r="C4" t="s">
         <v>358</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>0</v>
       </c>
       <c r="H4" t="s">
@@ -5517,7 +5551,7 @@
       <c r="C5" t="s">
         <v>356</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>0</v>
       </c>
       <c r="H5" t="s">
@@ -5537,7 +5571,7 @@
       <c r="C6" t="s">
         <v>356</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>0</v>
       </c>
       <c r="H6" t="s">
@@ -5557,7 +5591,7 @@
       <c r="C7" t="s">
         <v>359</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>0</v>
       </c>
       <c r="H7" t="s">
@@ -5577,7 +5611,7 @@
       <c r="C8" t="s">
         <v>360</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>0</v>
       </c>
       <c r="H8" t="s">
@@ -5597,7 +5631,7 @@
       <c r="C9" t="s">
         <v>361</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>0</v>
       </c>
       <c r="H9" t="s">
@@ -5617,7 +5651,7 @@
       <c r="C10" t="s">
         <v>362</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>0</v>
       </c>
       <c r="H10" t="s">
@@ -5637,7 +5671,7 @@
       <c r="C11" t="s">
         <v>364</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>0</v>
       </c>
       <c r="H11" t="s">
@@ -5657,7 +5691,7 @@
       <c r="C12" t="s">
         <v>363</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>0</v>
       </c>
       <c r="H12" t="s">
@@ -5677,7 +5711,7 @@
       <c r="C13" t="s">
         <v>365</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>0</v>
       </c>
       <c r="H13" t="s">
@@ -5697,7 +5731,7 @@
       <c r="C14" t="s">
         <v>366</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>0</v>
       </c>
       <c r="H14" t="s">
@@ -5717,7 +5751,7 @@
       <c r="C15" t="s">
         <v>367</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>0</v>
       </c>
       <c r="H15" t="s">
@@ -5737,7 +5771,7 @@
       <c r="C16" t="s">
         <v>368</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>0</v>
       </c>
       <c r="H16" t="s">
@@ -5757,7 +5791,7 @@
       <c r="C17" t="s">
         <v>369</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>0</v>
       </c>
       <c r="H17" t="s">
@@ -5777,7 +5811,7 @@
       <c r="C18" t="s">
         <v>370</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>0</v>
       </c>
       <c r="H18" t="s">
@@ -9223,10 +9257,10 @@
   <dimension ref="A1:Q62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="H6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="B49" sqref="B49:B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add transfer to user
</commit_message>
<xml_diff>
--- a/db/excel/api-function-granted-users-cdld.xlsx
+++ b/db/excel/api-function-granted-users-cdld.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10613"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11526D7-5662-0144-8C6D-4DB2F25AD704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF90A751-E1F6-5A40-9D1E-D725533530B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19460" tabRatio="800" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19460" tabRatio="800" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_types" sheetId="27" r:id="rId1"/>
@@ -275,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1278" uniqueCount="518">
   <si>
     <t>status</t>
   </si>
@@ -1878,12 +1878,18 @@
   <si>
     <t>ion-timer-outline</t>
   </si>
+  <si>
+    <t>Nhóm quản lý chỉ đạo lãnh đạo (chính)</t>
+  </si>
+  <si>
+    <t>Nhóm chức năng báo cáo</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2014,8 +2020,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2115,6 +2128,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3264,10 +3283,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4655,7 +4674,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4743,8 +4762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4755,11 +4774,13 @@
     <col min="4" max="4" width="19.33203125" style="85" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.1640625" style="89" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.33203125" style="89" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="62.5" style="85" customWidth="1"/>
-    <col min="8" max="8" width="55" style="85" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21" style="85" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="78.83203125" style="85" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.83203125" style="85" customWidth="1"/>
-    <col min="10" max="10" width="65" style="85" customWidth="1"/>
-    <col min="11" max="16384" width="11.5" style="85"/>
+    <col min="10" max="10" width="12.5" style="85" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" style="85"/>
+    <col min="12" max="12" width="14.1640625" style="85" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="11.5" style="85"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
@@ -5034,7 +5055,9 @@
       <c r="G9" s="91" t="s">
         <v>492</v>
       </c>
-      <c r="H9" s="90"/>
+      <c r="H9" s="90" t="s">
+        <v>516</v>
+      </c>
       <c r="I9" s="90"/>
       <c r="J9" s="90"/>
       <c r="K9" s="90"/>
@@ -5182,7 +5205,9 @@
       <c r="G14" s="91" t="s">
         <v>499</v>
       </c>
-      <c r="H14" s="90"/>
+      <c r="H14" s="90" t="s">
+        <v>517</v>
+      </c>
       <c r="I14" s="90"/>
       <c r="J14" s="90"/>
       <c r="K14" s="90"/>
@@ -5268,7 +5293,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5277,7 +5302,7 @@
     <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="22.83203125" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="29.83203125" customWidth="1"/>
@@ -5828,12 +5853,32 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58BC6DBE-9909-F047-9350-C064ACCA54DE}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="4" width="19.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="67" t="s">
+        <v>378</v>
+      </c>
+      <c r="B1" s="67" t="s">
+        <v>379</v>
+      </c>
+      <c r="C1" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="67" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -9257,10 +9302,10 @@
   <dimension ref="A1:Q62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B49" sqref="B49:B57"/>
+      <selection pane="bottomRight" activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11178,8 +11223,8 @@
   </sheetPr>
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="K42" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="7" ySplit="1" topLeftCell="K24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="E55" sqref="E55"/>

</xml_diff>

<commit_message>
add code add user and rev user right handler
</commit_message>
<xml_diff>
--- a/db/excel/api-function-granted-users-cdld.xlsx
+++ b/db/excel/api-function-granted-users-cdld.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10613"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFBDE97-7AC6-954A-AAD9-033DA598BB22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="38400" windowHeight="20055" tabRatio="800" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20060" tabRatio="800" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_types" sheetId="27" r:id="rId1"/>
@@ -238,12 +239,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
       <text>
         <r>
           <rPr>
@@ -265,12 +266,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
       <text>
         <r>
           <rPr>
@@ -2118,7 +2119,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4383,9 +4384,9 @@
     <cellStyle name="Hyperlink" xfId="756" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="758" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 4" xfId="738"/>
-    <cellStyle name="Normal 5" xfId="739"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00003A030000}"/>
+    <cellStyle name="Normal 4" xfId="738" xr:uid="{00000000-0005-0000-0000-00003B030000}"/>
+    <cellStyle name="Normal 5" xfId="739" xr:uid="{00000000-0005-0000-0000-00003C030000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -4482,6 +4483,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -4517,6 +4535,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4691,43 +4726,27 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="E1" dT="2021-06-29T02:35:14.09" personId="{00000000-0000-0000-0000-000000000000}" id="{152BA087-38CF-9641-BBDF-2A7034154D08}">
-    <text>Khi đơn vị cập nhập thực hiện thì nhập thông tin vào đây</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
-<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="E1" dT="2021-06-29T02:35:58.31" personId="{00000000-0000-0000-0000-000000000000}" id="{A523B58E-E469-E744-B82E-2CE5FD4DC608}">
-    <text>Khi đơn vị thay đổi trạng thái thì cập nhập mô tả cho thay đổi đó ở đây</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="9" customWidth="1"/>
     <col min="5" max="5" width="14" style="9" customWidth="1"/>
-    <col min="6" max="6" width="55.42578125" style="9" customWidth="1"/>
-    <col min="7" max="64" width="11.42578125" style="9" customWidth="1"/>
-    <col min="65" max="16384" width="9.140625" style="9"/>
+    <col min="6" max="6" width="55.5" style="9" customWidth="1"/>
+    <col min="7" max="64" width="11.5" style="9" customWidth="1"/>
+    <col min="65" max="16384" width="9.1640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>83</v>
       </c>
@@ -4747,7 +4766,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>15</v>
       </c>
@@ -4767,7 +4786,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>16</v>
       </c>
@@ -4787,7 +4806,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>98</v>
       </c>
@@ -4807,7 +4826,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>17</v>
       </c>
@@ -4827,7 +4846,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>104</v>
       </c>
@@ -4847,7 +4866,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>50</v>
       </c>
@@ -4867,7 +4886,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>107</v>
       </c>
@@ -4899,7 +4918,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor theme="2" tint="-0.249977111117893"/>
   </sheetPr>
@@ -4909,17 +4928,17 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.28515625" customWidth="1"/>
-    <col min="3" max="3" width="40.140625" customWidth="1"/>
+    <col min="2" max="2" width="48.33203125" customWidth="1"/>
+    <col min="3" max="3" width="40.1640625" customWidth="1"/>
     <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="103" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>18</v>
       </c>
@@ -4939,7 +4958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A2" s="96">
         <v>99</v>
       </c>
@@ -4959,7 +4978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="94">
         <v>21</v>
       </c>
@@ -4991,31 +5010,31 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" style="85" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="85" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" style="85" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" style="85" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" style="89" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" style="85" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" style="85" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" style="85" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" style="89" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" style="89" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21" style="85" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="78.85546875" style="85" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" style="85" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" style="85" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" style="85"/>
-    <col min="12" max="12" width="14.140625" style="85" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="85"/>
+    <col min="8" max="8" width="78.83203125" style="85" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="85" customWidth="1"/>
+    <col min="10" max="10" width="12.5" style="85" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" style="85"/>
+    <col min="12" max="12" width="14.1640625" style="85" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="11.5" style="85"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="84" t="s">
         <v>18</v>
       </c>
@@ -5521,29 +5540,29 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.85546875" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.83203125" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
         <v>1</v>
       </c>
@@ -5578,7 +5597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
         <v>166</v>
       </c>
@@ -5603,7 +5622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
         <v>221</v>
       </c>
@@ -5628,7 +5647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="28" t="s">
         <v>167</v>
       </c>
@@ -5653,7 +5672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="28" t="s">
         <v>168</v>
       </c>
@@ -5690,7 +5709,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
@@ -5700,19 +5719,19 @@
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="40" t="s">
         <v>18</v>
       </c>
@@ -5741,7 +5760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5758,7 +5777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5778,7 +5797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5798,7 +5817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5818,7 +5837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5838,7 +5857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5858,7 +5877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5878,7 +5897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -5898,7 +5917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5918,7 +5937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5938,7 +5957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -5958,7 +5977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -5978,7 +5997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5998,7 +6017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -6018,7 +6037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -6038,7 +6057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -6058,7 +6077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -6084,20 +6103,20 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="4" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="4" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="67" t="s">
         <v>359</v>
       </c>
@@ -6111,7 +6130,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>206</v>
       </c>
@@ -6122,7 +6141,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -6133,7 +6152,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>232</v>
       </c>
@@ -6144,7 +6163,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -6155,7 +6174,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -6166,7 +6185,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -6177,7 +6196,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -6188,7 +6207,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>299</v>
       </c>
@@ -6199,37 +6218,37 @@
         <v>189</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D10" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D11" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D12" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D15" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
         <v>189</v>
       </c>
@@ -6240,7 +6259,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q85"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -6250,26 +6269,26 @@
       <selection pane="bottomRight" activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.85546875" customWidth="1"/>
+    <col min="11" max="11" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.83203125" customWidth="1"/>
     <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="19" customWidth="1"/>
-    <col min="16" max="16" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="54" t="s">
         <v>2</v>
       </c>
@@ -6320,7 +6339,7 @@
       </c>
       <c r="Q1" s="41"/>
     </row>
-    <row r="2" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="50" t="s">
         <v>258</v>
       </c>
@@ -6359,7 +6378,7 @@
       </c>
       <c r="Q2" s="57"/>
     </row>
-    <row r="3" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="50" t="s">
         <v>258</v>
       </c>
@@ -6392,7 +6411,7 @@
       </c>
       <c r="Q3" s="57"/>
     </row>
-    <row r="4" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="50" t="s">
         <v>258</v>
       </c>
@@ -6425,7 +6444,7 @@
       </c>
       <c r="Q4" s="57"/>
     </row>
-    <row r="5" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="50" t="s">
         <v>258</v>
       </c>
@@ -6458,7 +6477,7 @@
       </c>
       <c r="Q5" s="57"/>
     </row>
-    <row r="6" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="50" t="s">
         <v>258</v>
       </c>
@@ -6491,7 +6510,7 @@
       </c>
       <c r="Q6" s="57"/>
     </row>
-    <row r="7" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="50" t="s">
         <v>258</v>
       </c>
@@ -6524,7 +6543,7 @@
       </c>
       <c r="Q7" s="57"/>
     </row>
-    <row r="8" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="50" t="s">
         <v>258</v>
       </c>
@@ -6557,7 +6576,7 @@
       </c>
       <c r="Q8" s="57"/>
     </row>
-    <row r="9" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="50" t="s">
         <v>258</v>
       </c>
@@ -6588,7 +6607,7 @@
       </c>
       <c r="Q9" s="57"/>
     </row>
-    <row r="10" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="50" t="s">
         <v>258</v>
       </c>
@@ -6623,7 +6642,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="50" t="s">
         <v>258</v>
       </c>
@@ -6654,7 +6673,7 @@
       </c>
       <c r="Q11" s="57"/>
     </row>
-    <row r="12" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="50" t="s">
         <v>258</v>
       </c>
@@ -6687,7 +6706,7 @@
       </c>
       <c r="Q12" s="57"/>
     </row>
-    <row r="13" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="50" t="s">
         <v>258</v>
       </c>
@@ -6720,7 +6739,7 @@
       </c>
       <c r="Q13" s="57"/>
     </row>
-    <row r="14" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="51" t="s">
         <v>222</v>
       </c>
@@ -6759,7 +6778,7 @@
       </c>
       <c r="Q14" s="57"/>
     </row>
-    <row r="15" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="51" t="s">
         <v>222</v>
       </c>
@@ -6792,7 +6811,7 @@
       </c>
       <c r="Q15" s="57"/>
     </row>
-    <row r="16" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="51" t="s">
         <v>222</v>
       </c>
@@ -6825,7 +6844,7 @@
       </c>
       <c r="Q16" s="57"/>
     </row>
-    <row r="17" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="51" t="s">
         <v>222</v>
       </c>
@@ -6856,7 +6875,7 @@
       <c r="P17" s="56"/>
       <c r="Q17" s="57"/>
     </row>
-    <row r="18" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="51" t="s">
         <v>222</v>
       </c>
@@ -6889,7 +6908,7 @@
       </c>
       <c r="Q18" s="57"/>
     </row>
-    <row r="19" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="51" t="s">
         <v>222</v>
       </c>
@@ -6922,7 +6941,7 @@
       </c>
       <c r="Q19" s="57"/>
     </row>
-    <row r="20" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="51" t="s">
         <v>222</v>
       </c>
@@ -6955,7 +6974,7 @@
       </c>
       <c r="Q20" s="57"/>
     </row>
-    <row r="21" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="51" t="s">
         <v>222</v>
       </c>
@@ -6988,7 +7007,7 @@
       </c>
       <c r="Q21" s="57"/>
     </row>
-    <row r="22" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="51" t="s">
         <v>222</v>
       </c>
@@ -7017,7 +7036,7 @@
       <c r="P22" s="56"/>
       <c r="Q22" s="57"/>
     </row>
-    <row r="23" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="51" t="s">
         <v>222</v>
       </c>
@@ -7048,7 +7067,7 @@
       </c>
       <c r="Q23" s="57"/>
     </row>
-    <row r="24" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="51" t="s">
         <v>222</v>
       </c>
@@ -7081,7 +7100,7 @@
       </c>
       <c r="Q24" s="57"/>
     </row>
-    <row r="25" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="51" t="s">
         <v>222</v>
       </c>
@@ -7112,7 +7131,7 @@
       </c>
       <c r="Q25" s="57"/>
     </row>
-    <row r="26" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="51" t="s">
         <v>222</v>
       </c>
@@ -7145,7 +7164,7 @@
       </c>
       <c r="Q26" s="57"/>
     </row>
-    <row r="27" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="51" t="s">
         <v>222</v>
       </c>
@@ -7180,7 +7199,7 @@
       </c>
       <c r="Q27" s="57"/>
     </row>
-    <row r="28" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="51" t="s">
         <v>222</v>
       </c>
@@ -7211,7 +7230,7 @@
       <c r="P28" s="56"/>
       <c r="Q28" s="57"/>
     </row>
-    <row r="29" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="51" t="s">
         <v>222</v>
       </c>
@@ -7242,7 +7261,7 @@
       <c r="P29" s="56"/>
       <c r="Q29" s="57"/>
     </row>
-    <row r="30" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="51" t="s">
         <v>222</v>
       </c>
@@ -7273,7 +7292,7 @@
       <c r="P30" s="56"/>
       <c r="Q30" s="57"/>
     </row>
-    <row r="31" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="100" t="s">
         <v>565</v>
       </c>
@@ -7302,7 +7321,7 @@
       <c r="P31" s="56"/>
       <c r="Q31" s="57"/>
     </row>
-    <row r="32" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="100" t="s">
         <v>565</v>
       </c>
@@ -7331,7 +7350,7 @@
       <c r="P32" s="56"/>
       <c r="Q32" s="57"/>
     </row>
-    <row r="33" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="100" t="s">
         <v>565</v>
       </c>
@@ -7362,7 +7381,7 @@
       <c r="P33" s="56"/>
       <c r="Q33" s="57"/>
     </row>
-    <row r="34" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="100" t="s">
         <v>565</v>
       </c>
@@ -7393,7 +7412,7 @@
       <c r="P34" s="56"/>
       <c r="Q34" s="57"/>
     </row>
-    <row r="35" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="100" t="s">
         <v>565</v>
       </c>
@@ -7424,7 +7443,7 @@
       <c r="P35" s="56"/>
       <c r="Q35" s="57"/>
     </row>
-    <row r="36" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="100" t="s">
         <v>565</v>
       </c>
@@ -7453,7 +7472,7 @@
       <c r="P36" s="56"/>
       <c r="Q36" s="57"/>
     </row>
-    <row r="37" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="100" t="s">
         <v>565</v>
       </c>
@@ -7482,7 +7501,7 @@
       <c r="P37" s="56"/>
       <c r="Q37" s="57"/>
     </row>
-    <row r="38" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="100" t="s">
         <v>565</v>
       </c>
@@ -7511,7 +7530,7 @@
       <c r="P38" s="56"/>
       <c r="Q38" s="57"/>
     </row>
-    <row r="39" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="100" t="s">
         <v>565</v>
       </c>
@@ -7542,7 +7561,7 @@
       <c r="P39" s="56"/>
       <c r="Q39" s="57"/>
     </row>
-    <row r="40" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="100" t="s">
         <v>565</v>
       </c>
@@ -7571,7 +7590,7 @@
       <c r="P40" s="56"/>
       <c r="Q40" s="57"/>
     </row>
-    <row r="41" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="100" t="s">
         <v>565</v>
       </c>
@@ -7600,7 +7619,7 @@
       <c r="P41" s="56"/>
       <c r="Q41" s="57"/>
     </row>
-    <row r="42" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="50" t="s">
         <v>281</v>
       </c>
@@ -7631,7 +7650,7 @@
       </c>
       <c r="Q42" s="59"/>
     </row>
-    <row r="43" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="50" t="s">
         <v>281</v>
       </c>
@@ -7662,7 +7681,7 @@
       </c>
       <c r="Q43" s="59"/>
     </row>
-    <row r="44" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="50" t="s">
         <v>281</v>
       </c>
@@ -7697,7 +7716,7 @@
       </c>
       <c r="Q44" s="59"/>
     </row>
-    <row r="45" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="50" t="s">
         <v>281</v>
       </c>
@@ -7726,7 +7745,7 @@
       </c>
       <c r="Q45" s="59"/>
     </row>
-    <row r="46" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="50" t="s">
         <v>281</v>
       </c>
@@ -7759,7 +7778,7 @@
       </c>
       <c r="Q46" s="59"/>
     </row>
-    <row r="47" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="50" t="s">
         <v>281</v>
       </c>
@@ -7792,7 +7811,7 @@
       </c>
       <c r="Q47" s="59"/>
     </row>
-    <row r="48" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="50" t="s">
         <v>281</v>
       </c>
@@ -7823,7 +7842,7 @@
       </c>
       <c r="Q48" s="59"/>
     </row>
-    <row r="49" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="50" t="s">
         <v>281</v>
       </c>
@@ -7856,7 +7875,7 @@
       </c>
       <c r="Q49" s="59"/>
     </row>
-    <row r="50" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="50" t="s">
         <v>281</v>
       </c>
@@ -7887,7 +7906,7 @@
       </c>
       <c r="Q50" s="59"/>
     </row>
-    <row r="51" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="50" t="s">
         <v>281</v>
       </c>
@@ -7920,7 +7939,7 @@
       </c>
       <c r="Q51" s="59"/>
     </row>
-    <row r="52" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="52" t="s">
         <v>280</v>
       </c>
@@ -7959,7 +7978,7 @@
       </c>
       <c r="Q52" s="57"/>
     </row>
-    <row r="53" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="52" t="s">
         <v>280</v>
       </c>
@@ -7994,7 +8013,7 @@
       </c>
       <c r="Q53" s="57"/>
     </row>
-    <row r="54" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="52" t="s">
         <v>280</v>
       </c>
@@ -8027,7 +8046,7 @@
       </c>
       <c r="Q54" s="57"/>
     </row>
-    <row r="55" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="52" t="s">
         <v>280</v>
       </c>
@@ -8060,7 +8079,7 @@
       </c>
       <c r="Q55" s="57"/>
     </row>
-    <row r="56" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="52" t="s">
         <v>280</v>
       </c>
@@ -8093,7 +8112,7 @@
       </c>
       <c r="Q56" s="57"/>
     </row>
-    <row r="57" spans="1:17" s="82" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" s="82" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="52" t="s">
         <v>280</v>
       </c>
@@ -8128,7 +8147,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="58" spans="1:17" s="82" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" s="82" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="52" t="s">
         <v>280</v>
       </c>
@@ -8161,7 +8180,7 @@
       </c>
       <c r="Q58" s="57"/>
     </row>
-    <row r="59" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="52" t="s">
         <v>280</v>
       </c>
@@ -8192,7 +8211,7 @@
       </c>
       <c r="Q59" s="57"/>
     </row>
-    <row r="60" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="52" t="s">
         <v>280</v>
       </c>
@@ -8223,7 +8242,7 @@
       </c>
       <c r="Q60" s="57"/>
     </row>
-    <row r="61" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="52" t="s">
         <v>280</v>
       </c>
@@ -8256,7 +8275,7 @@
       </c>
       <c r="Q61" s="57"/>
     </row>
-    <row r="62" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="52" t="s">
         <v>280</v>
       </c>
@@ -8287,7 +8306,7 @@
       </c>
       <c r="Q62" s="57"/>
     </row>
-    <row r="63" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="65" t="s">
         <v>280</v>
       </c>
@@ -8320,7 +8339,7 @@
       </c>
       <c r="Q63" s="57"/>
     </row>
-    <row r="64" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="53" t="s">
         <v>218</v>
       </c>
@@ -8359,7 +8378,7 @@
       </c>
       <c r="Q64" s="59"/>
     </row>
-    <row r="65" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="53" t="s">
         <v>218</v>
       </c>
@@ -8392,7 +8411,7 @@
       </c>
       <c r="Q65" s="59"/>
     </row>
-    <row r="66" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="53" t="s">
         <v>218</v>
       </c>
@@ -8427,7 +8446,7 @@
       </c>
       <c r="Q66" s="59"/>
     </row>
-    <row r="67" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="53" t="s">
         <v>218</v>
       </c>
@@ -8460,7 +8479,7 @@
       </c>
       <c r="Q67" s="59"/>
     </row>
-    <row r="68" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="53" t="s">
         <v>218</v>
       </c>
@@ -8493,7 +8512,7 @@
       </c>
       <c r="Q68" s="59"/>
     </row>
-    <row r="69" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="53" t="s">
         <v>218</v>
       </c>
@@ -8526,7 +8545,7 @@
       </c>
       <c r="Q69" s="59"/>
     </row>
-    <row r="70" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="53" t="s">
         <v>218</v>
       </c>
@@ -8559,7 +8578,7 @@
       </c>
       <c r="Q70" s="59"/>
     </row>
-    <row r="71" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="53" t="s">
         <v>218</v>
       </c>
@@ -8590,7 +8609,7 @@
       </c>
       <c r="Q71" s="59"/>
     </row>
-    <row r="72" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="53" t="s">
         <v>218</v>
       </c>
@@ -8623,7 +8642,7 @@
       </c>
       <c r="Q72" s="59"/>
     </row>
-    <row r="73" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="53" t="s">
         <v>218</v>
       </c>
@@ -8654,7 +8673,7 @@
       </c>
       <c r="Q73" s="59"/>
     </row>
-    <row r="74" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="53" t="s">
         <v>218</v>
       </c>
@@ -8687,7 +8706,7 @@
       </c>
       <c r="Q74" s="59"/>
     </row>
-    <row r="75" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="53" t="s">
         <v>218</v>
       </c>
@@ -8720,7 +8739,7 @@
       </c>
       <c r="Q75" s="59"/>
     </row>
-    <row r="76" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="44" t="s">
         <v>170</v>
       </c>
@@ -8759,7 +8778,7 @@
       </c>
       <c r="Q76" s="57"/>
     </row>
-    <row r="77" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="44" t="s">
         <v>170</v>
       </c>
@@ -8792,7 +8811,7 @@
       </c>
       <c r="Q77" s="57"/>
     </row>
-    <row r="78" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="44" t="s">
         <v>170</v>
       </c>
@@ -8827,7 +8846,7 @@
       </c>
       <c r="Q78" s="57"/>
     </row>
-    <row r="79" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="44" t="s">
         <v>170</v>
       </c>
@@ -8860,7 +8879,7 @@
       </c>
       <c r="Q79" s="57"/>
     </row>
-    <row r="80" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="44" t="s">
         <v>170</v>
       </c>
@@ -8893,7 +8912,7 @@
       </c>
       <c r="Q80" s="57"/>
     </row>
-    <row r="81" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="44" t="s">
         <v>170</v>
       </c>
@@ -8924,7 +8943,7 @@
       </c>
       <c r="Q81" s="57"/>
     </row>
-    <row r="82" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="44" t="s">
         <v>170</v>
       </c>
@@ -8957,7 +8976,7 @@
       </c>
       <c r="Q82" s="57"/>
     </row>
-    <row r="83" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="44" t="s">
         <v>170</v>
       </c>
@@ -8988,7 +9007,7 @@
       </c>
       <c r="Q83" s="57"/>
     </row>
-    <row r="84" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="44" t="s">
         <v>170</v>
       </c>
@@ -9021,7 +9040,7 @@
       </c>
       <c r="Q84" s="57"/>
     </row>
-    <row r="85" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="44" t="s">
         <v>170</v>
       </c>
@@ -9061,7 +9080,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
@@ -9071,19 +9090,19 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="52.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="39" t="s">
         <v>18</v>
       </c>
@@ -9112,7 +9131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="92">
         <v>1</v>
       </c>
@@ -9135,7 +9154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>11</v>
       </c>
@@ -9158,7 +9177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>12</v>
       </c>
@@ -9181,7 +9200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>13</v>
       </c>
@@ -9204,7 +9223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>14</v>
       </c>
@@ -9227,7 +9246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>15</v>
       </c>
@@ -9250,7 +9269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>16</v>
       </c>
@@ -9273,7 +9292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="92">
         <v>2</v>
       </c>
@@ -9296,7 +9315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>21</v>
       </c>
@@ -9319,7 +9338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>22</v>
       </c>
@@ -9342,7 +9361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="92">
         <v>3</v>
       </c>
@@ -9365,7 +9384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>31</v>
       </c>
@@ -9388,7 +9407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>32</v>
       </c>
@@ -9411,7 +9430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>33</v>
       </c>
@@ -9434,7 +9453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>34</v>
       </c>
@@ -9457,7 +9476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>35</v>
       </c>
@@ -9480,7 +9499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>36</v>
       </c>
@@ -9503,7 +9522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="92">
         <v>4</v>
       </c>
@@ -9526,7 +9545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>41</v>
       </c>
@@ -9549,7 +9568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>42</v>
       </c>
@@ -9572,7 +9591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>43</v>
       </c>
@@ -9595,7 +9614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>44</v>
       </c>
@@ -9618,7 +9637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="92">
         <v>5</v>
       </c>
@@ -9641,7 +9660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>51</v>
       </c>
@@ -9664,7 +9683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>52</v>
       </c>
@@ -9687,7 +9706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>53</v>
       </c>
@@ -9710,7 +9729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>54</v>
       </c>
@@ -9733,7 +9752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>55</v>
       </c>
@@ -9756,7 +9775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>56</v>
       </c>
@@ -9779,7 +9798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>57</v>
       </c>
@@ -9802,7 +9821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>58</v>
       </c>
@@ -9825,7 +9844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>59</v>
       </c>
@@ -9848,7 +9867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>510</v>
       </c>
@@ -9871,7 +9890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>511</v>
       </c>
@@ -9894,7 +9913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>512</v>
       </c>
@@ -9917,7 +9936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>513</v>
       </c>
@@ -9940,7 +9959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>514</v>
       </c>
@@ -9970,7 +9989,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
@@ -9980,16 +9999,16 @@
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
-    <col min="5" max="12" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" customWidth="1"/>
+    <col min="5" max="12" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="38" t="s">
         <v>18</v>
       </c>
@@ -10027,7 +10046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -10056,7 +10075,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
@@ -10066,22 +10085,22 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="61" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="66" t="s">
         <v>18</v>
       </c>
@@ -10119,7 +10138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="41">
         <v>1</v>
       </c>
@@ -10147,7 +10166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="41">
         <v>2</v>
       </c>
@@ -10175,7 +10194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="41">
         <v>3</v>
       </c>
@@ -10203,7 +10222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="41"/>
       <c r="B5" s="41"/>
       <c r="C5" s="41"/>
@@ -10217,7 +10236,7 @@
       <c r="K5" s="41"/>
       <c r="L5" s="41"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="41"/>
       <c r="B6" s="41"/>
       <c r="C6" s="41"/>
@@ -10237,7 +10256,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
@@ -10247,18 +10266,18 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" customWidth="1"/>
+    <col min="6" max="6" width="21.5" customWidth="1"/>
+    <col min="7" max="7" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="66" t="s">
         <v>18</v>
       </c>
@@ -10293,7 +10312,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -10307,7 +10326,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -10321,7 +10340,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -10335,7 +10354,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -10349,7 +10368,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -10363,7 +10382,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -10384,7 +10403,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
@@ -10394,22 +10413,22 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.140625" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.1640625" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="18.5" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="26.42578125" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" customWidth="1"/>
-    <col min="11" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.5" customWidth="1"/>
+    <col min="10" max="10" width="22.83203125" customWidth="1"/>
+    <col min="11" max="12" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="67" t="s">
         <v>18</v>
       </c>
@@ -10447,7 +10466,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -10471,37 +10490,37 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Q62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B31" sqref="B31"/>
+      <selection pane="bottomRight" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="85.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.42578125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="85.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.1640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.83203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.5" style="17" customWidth="1"/>
     <col min="16" max="16" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -10551,7 +10570,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
@@ -10587,7 +10606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>39</v>
       </c>
@@ -10615,7 +10634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>39</v>
       </c>
@@ -10645,7 +10664,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>39</v>
       </c>
@@ -10675,7 +10694,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>39</v>
       </c>
@@ -10709,7 +10728,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>39</v>
       </c>
@@ -10737,7 +10756,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>39</v>
       </c>
@@ -10765,7 +10784,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>39</v>
       </c>
@@ -10793,7 +10812,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>39</v>
       </c>
@@ -10821,7 +10840,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>39</v>
       </c>
@@ -10851,7 +10870,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>39</v>
       </c>
@@ -10879,7 +10898,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>39</v>
       </c>
@@ -10909,7 +10928,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>39</v>
       </c>
@@ -10937,7 +10956,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>39</v>
       </c>
@@ -10965,7 +10984,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="79" t="s">
         <v>38</v>
       </c>
@@ -10999,7 +11018,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="79" t="s">
         <v>38</v>
       </c>
@@ -11029,7 +11048,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="79" t="s">
         <v>38</v>
       </c>
@@ -11057,7 +11076,7 @@
       <c r="O18" s="80"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="79" t="s">
         <v>38</v>
       </c>
@@ -11087,7 +11106,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="79" t="s">
         <v>38</v>
       </c>
@@ -11115,7 +11134,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="79" t="s">
         <v>38</v>
       </c>
@@ -11143,7 +11162,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="79" t="s">
         <v>38</v>
       </c>
@@ -11173,7 +11192,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="79" t="s">
         <v>38</v>
       </c>
@@ -11203,7 +11222,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>46</v>
       </c>
@@ -11239,7 +11258,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>46</v>
       </c>
@@ -11251,11 +11270,9 @@
         <v>366</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" s="16">
-        <v>200</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="F25" s="16"/>
       <c r="G25" s="16"/>
       <c r="H25" s="16"/>
       <c r="I25" s="16"/>
@@ -11269,7 +11286,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>46</v>
       </c>
@@ -11299,7 +11316,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>46</v>
       </c>
@@ -11329,7 +11346,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>46</v>
       </c>
@@ -11359,7 +11376,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>46</v>
       </c>
@@ -11389,7 +11406,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>46</v>
       </c>
@@ -11419,7 +11436,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>46</v>
       </c>
@@ -11449,7 +11466,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>46</v>
       </c>
@@ -11477,7 +11494,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>46</v>
       </c>
@@ -11507,7 +11524,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>46</v>
       </c>
@@ -11537,7 +11554,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="79" t="s">
         <v>145</v>
       </c>
@@ -11573,7 +11590,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="79" t="s">
         <v>145</v>
       </c>
@@ -11601,7 +11618,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="79" t="s">
         <v>145</v>
       </c>
@@ -11631,7 +11648,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="79" t="s">
         <v>145</v>
       </c>
@@ -11661,7 +11678,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="79" t="s">
         <v>145</v>
       </c>
@@ -11691,7 +11708,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="79" t="s">
         <v>145</v>
       </c>
@@ -11721,7 +11738,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="79" t="s">
         <v>145</v>
       </c>
@@ -11751,7 +11768,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="79" t="s">
         <v>145</v>
       </c>
@@ -11781,7 +11798,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="79" t="s">
         <v>145</v>
       </c>
@@ -11811,7 +11828,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="79" t="s">
         <v>145</v>
       </c>
@@ -11841,7 +11858,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="79" t="s">
         <v>145</v>
       </c>
@@ -11869,7 +11886,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="79" t="s">
         <v>145</v>
       </c>
@@ -11897,7 +11914,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="79" t="s">
         <v>145</v>
       </c>
@@ -11927,7 +11944,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="79" t="s">
         <v>145</v>
       </c>
@@ -11957,7 +11974,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="42" t="s">
         <v>182</v>
       </c>
@@ -11994,7 +12011,7 @@
       </c>
       <c r="Q49" s="57"/>
     </row>
-    <row r="50" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="42" t="s">
         <v>182</v>
       </c>
@@ -12025,7 +12042,7 @@
       </c>
       <c r="Q50" s="57"/>
     </row>
-    <row r="51" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="42" t="s">
         <v>182</v>
       </c>
@@ -12056,7 +12073,7 @@
       </c>
       <c r="Q51" s="57"/>
     </row>
-    <row r="52" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="42" t="s">
         <v>182</v>
       </c>
@@ -12087,7 +12104,7 @@
       </c>
       <c r="Q52" s="57"/>
     </row>
-    <row r="53" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="42" t="s">
         <v>182</v>
       </c>
@@ -12116,7 +12133,7 @@
       </c>
       <c r="Q53" s="57"/>
     </row>
-    <row r="54" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="42" t="s">
         <v>182</v>
       </c>
@@ -12145,7 +12162,7 @@
       </c>
       <c r="Q54" s="57"/>
     </row>
-    <row r="55" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="42" t="s">
         <v>182</v>
       </c>
@@ -12174,7 +12191,7 @@
       </c>
       <c r="Q55" s="57"/>
     </row>
-    <row r="56" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="42" t="s">
         <v>182</v>
       </c>
@@ -12205,7 +12222,7 @@
       </c>
       <c r="Q56" s="57"/>
     </row>
-    <row r="57" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="42" t="s">
         <v>182</v>
       </c>
@@ -12236,7 +12253,7 @@
       </c>
       <c r="Q57" s="57"/>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" s="68" t="s">
         <v>358</v>
       </c>
@@ -12272,7 +12289,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" s="68" t="s">
         <v>358</v>
       </c>
@@ -12302,7 +12319,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" s="68" t="s">
         <v>358</v>
       </c>
@@ -12330,7 +12347,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" s="68" t="s">
         <v>358</v>
       </c>
@@ -12360,7 +12377,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" s="68"/>
       <c r="B62" s="68"/>
       <c r="C62" s="68"/>
@@ -12390,38 +12407,38 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor theme="2" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="7" ySplit="1" topLeftCell="K23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" customWidth="1"/>
     <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" customWidth="1"/>
+    <col min="7" max="7" width="13.5" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" customWidth="1"/>
+    <col min="9" max="9" width="12.5" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="57" customWidth="1"/>
-    <col min="11" max="11" width="54.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="35.7109375" style="5" customWidth="1"/>
-    <col min="14" max="14" width="51.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="54.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.6640625" style="5" customWidth="1"/>
+    <col min="14" max="14" width="51.1640625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
         <v>18</v>
       </c>
@@ -12465,7 +12482,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="25">
         <v>1</v>
       </c>
@@ -12503,7 +12520,7 @@
       <c r="M2" s="25"/>
       <c r="N2" s="26"/>
     </row>
-    <row r="3" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="25">
         <v>2</v>
       </c>
@@ -12541,7 +12558,7 @@
       <c r="M3" s="25"/>
       <c r="N3" s="26"/>
     </row>
-    <row r="4" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="25">
         <v>3</v>
       </c>
@@ -12579,7 +12596,7 @@
       <c r="M4" s="25"/>
       <c r="N4" s="26"/>
     </row>
-    <row r="5" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="25">
         <v>4</v>
       </c>
@@ -12617,7 +12634,7 @@
       <c r="M5" s="25"/>
       <c r="N5" s="26"/>
     </row>
-    <row r="6" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="25">
         <v>5</v>
       </c>
@@ -12655,7 +12672,7 @@
       <c r="M6" s="25"/>
       <c r="N6" s="26"/>
     </row>
-    <row r="7" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="25">
         <v>6</v>
       </c>
@@ -12693,7 +12710,7 @@
       <c r="M7" s="25"/>
       <c r="N7" s="26"/>
     </row>
-    <row r="8" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="25">
         <v>7</v>
       </c>
@@ -12731,7 +12748,7 @@
       <c r="M8" s="25"/>
       <c r="N8" s="26"/>
     </row>
-    <row r="9" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="25">
         <v>8</v>
       </c>
@@ -12769,7 +12786,7 @@
       <c r="M9" s="25"/>
       <c r="N9" s="26"/>
     </row>
-    <row r="10" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="25">
         <v>9</v>
       </c>
@@ -12807,7 +12824,7 @@
       <c r="M10" s="25"/>
       <c r="N10" s="26"/>
     </row>
-    <row r="11" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="25">
         <v>10</v>
       </c>
@@ -12845,7 +12862,7 @@
       <c r="M11" s="25"/>
       <c r="N11" s="26"/>
     </row>
-    <row r="12" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="25">
         <v>11</v>
       </c>
@@ -12883,7 +12900,7 @@
       <c r="M12" s="25"/>
       <c r="N12" s="26"/>
     </row>
-    <row r="13" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="25">
         <v>12</v>
       </c>
@@ -12921,7 +12938,7 @@
       <c r="M13" s="25"/>
       <c r="N13" s="26"/>
     </row>
-    <row r="14" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="25">
         <v>13</v>
       </c>
@@ -12959,7 +12976,7 @@
       <c r="M14" s="25"/>
       <c r="N14" s="26"/>
     </row>
-    <row r="15" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="25">
         <v>14</v>
       </c>
@@ -12997,7 +13014,7 @@
       <c r="M15" s="25"/>
       <c r="N15" s="26"/>
     </row>
-    <row r="16" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="25">
         <v>15</v>
       </c>
@@ -13035,7 +13052,7 @@
       <c r="M16" s="25"/>
       <c r="N16" s="26"/>
     </row>
-    <row r="17" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="25">
         <v>16</v>
       </c>
@@ -13073,7 +13090,7 @@
       <c r="M17" s="25"/>
       <c r="N17" s="26"/>
     </row>
-    <row r="18" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="25">
         <v>50</v>
       </c>
@@ -13111,7 +13128,7 @@
       <c r="M18" s="25"/>
       <c r="N18" s="26"/>
     </row>
-    <row r="19" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="68">
         <v>51</v>
       </c>
@@ -13145,7 +13162,7 @@
       <c r="M19" s="71"/>
       <c r="N19" s="73"/>
     </row>
-    <row r="20" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="25">
         <v>52</v>
       </c>
@@ -13179,7 +13196,7 @@
       <c r="M20" s="71"/>
       <c r="N20" s="73"/>
     </row>
-    <row r="21" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="68">
         <v>53</v>
       </c>
@@ -13213,7 +13230,7 @@
       <c r="M21" s="71"/>
       <c r="N21" s="73"/>
     </row>
-    <row r="22" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="25">
         <v>54</v>
       </c>
@@ -13247,7 +13264,7 @@
       <c r="M22" s="71"/>
       <c r="N22" s="73"/>
     </row>
-    <row r="23" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="68">
         <v>55</v>
       </c>
@@ -13281,7 +13298,7 @@
       <c r="M23" s="71"/>
       <c r="N23" s="73"/>
     </row>
-    <row r="24" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="25">
         <v>56</v>
       </c>
@@ -13315,7 +13332,7 @@
       <c r="M24" s="71"/>
       <c r="N24" s="73"/>
     </row>
-    <row r="25" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="68">
         <v>57</v>
       </c>
@@ -13349,7 +13366,7 @@
       <c r="M25" s="71"/>
       <c r="N25" s="73"/>
     </row>
-    <row r="26" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="25">
         <v>58</v>
       </c>
@@ -13383,7 +13400,7 @@
       <c r="M26" s="71"/>
       <c r="N26" s="73"/>
     </row>
-    <row r="27" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="68">
         <v>59</v>
       </c>
@@ -13417,7 +13434,7 @@
       <c r="M27" s="71"/>
       <c r="N27" s="73"/>
     </row>
-    <row r="28" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="25">
         <v>60</v>
       </c>
@@ -13451,7 +13468,7 @@
       <c r="M28" s="71"/>
       <c r="N28" s="73"/>
     </row>
-    <row r="29" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="68">
         <v>61</v>
       </c>
@@ -13485,7 +13502,7 @@
       <c r="M29" s="71"/>
       <c r="N29" s="73"/>
     </row>
-    <row r="30" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="25">
         <v>62</v>
       </c>
@@ -13519,7 +13536,7 @@
       <c r="M30" s="71"/>
       <c r="N30" s="73"/>
     </row>
-    <row r="31" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="68">
         <v>63</v>
       </c>
@@ -13553,7 +13570,7 @@
       <c r="M31" s="71"/>
       <c r="N31" s="73"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="34">
         <v>101</v>
       </c>
@@ -13586,7 +13603,7 @@
       </c>
       <c r="M32" s="36"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="34">
         <v>102</v>
       </c>
@@ -13619,7 +13636,7 @@
       </c>
       <c r="M33" s="36"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="34">
         <v>103</v>
       </c>
@@ -13652,7 +13669,7 @@
       </c>
       <c r="M34" s="36"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="34">
         <v>104</v>
       </c>
@@ -13685,7 +13702,7 @@
       </c>
       <c r="M35" s="36"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="34">
         <v>105</v>
       </c>
@@ -13720,7 +13737,7 @@
       </c>
       <c r="M36" s="36"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="34">
         <v>106</v>
       </c>
@@ -13753,7 +13770,7 @@
       </c>
       <c r="M37" s="36"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="34">
         <v>107</v>
       </c>
@@ -13786,7 +13803,7 @@
       </c>
       <c r="M38" s="36"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="34">
         <v>108</v>
       </c>
@@ -13819,7 +13836,7 @@
       </c>
       <c r="M39" s="36"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="34">
         <v>109</v>
       </c>
@@ -13854,7 +13871,7 @@
       </c>
       <c r="M40" s="36"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="34">
         <v>110</v>
       </c>
@@ -13887,7 +13904,7 @@
       </c>
       <c r="M41" s="36"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="34">
         <v>111</v>
       </c>
@@ -13920,7 +13937,7 @@
       </c>
       <c r="M42" s="36"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="34">
         <v>112</v>
       </c>
@@ -13953,7 +13970,7 @@
       </c>
       <c r="M43" s="36"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="34">
         <v>113</v>
       </c>
@@ -13986,7 +14003,7 @@
       </c>
       <c r="M44" s="36"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="34">
         <v>114</v>
       </c>
@@ -14019,7 +14036,7 @@
       </c>
       <c r="M45" s="3"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="34">
         <v>115</v>
       </c>
@@ -14052,7 +14069,7 @@
       </c>
       <c r="M46" s="3"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="34">
         <v>116</v>
       </c>
@@ -14085,7 +14102,7 @@
       </c>
       <c r="M47" s="3"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="34">
         <v>117</v>
       </c>
@@ -14118,7 +14135,7 @@
       </c>
       <c r="M48" s="3"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="34">
         <v>118</v>
       </c>
@@ -14151,7 +14168,7 @@
       </c>
       <c r="M49" s="3"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="102">
         <v>119</v>
       </c>
@@ -14184,7 +14201,7 @@
       </c>
       <c r="M50" s="104"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="102">
         <v>120</v>
       </c>
@@ -14217,7 +14234,7 @@
       </c>
       <c r="M51" s="104"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="102">
         <v>121</v>
       </c>
@@ -14251,7 +14268,7 @@
       <c r="M52" s="104"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M16"/>
+  <autoFilter ref="A1:M16" xr:uid="{00000000-0009-0000-0000-000008000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>

</xml_diff>

<commit_message>
add add meeting with multi files and add category
</commit_message>
<xml_diff>
--- a/db/excel/api-function-granted-users-cdld.xlsx
+++ b/db/excel/api-function-granted-users-cdld.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10613"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903592B1-D7B0-4941-896B-1DC370194514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C668C528-9F07-4745-B02F-8AC0B608E5B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20060" tabRatio="800" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="38400" windowHeight="20060" tabRatio="800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_types" sheetId="27" r:id="rId1"/>
@@ -293,7 +293,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1445" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1465" uniqueCount="599">
   <si>
     <t>status</t>
   </si>
@@ -1693,9 +1693,6 @@
     <t>Trang quản lý chỉ đạo theo từng đơn vị (lọc ra từng chỉ đạo theo từng đơn vị)</t>
   </si>
   <si>
-    <t>[21,22,23,24,25]</t>
-  </si>
-  <si>
     <t>report</t>
   </si>
   <si>
@@ -1792,9 +1789,6 @@
     <t>ion-document-text</t>
   </si>
   <si>
-    <t>ion-timer-outline</t>
-  </si>
-  <si>
     <t>Nhóm quản lý chỉ đạo lãnh đạo (chính)</t>
   </si>
   <si>
@@ -2120,6 +2114,36 @@
   </si>
   <si>
     <t>[1,11,12,13,14,15,16]</t>
+  </si>
+  <si>
+    <t>leader-direct-history</t>
+  </si>
+  <si>
+    <t>leader-direct-organization</t>
+  </si>
+  <si>
+    <t>ion-clock</t>
+  </si>
+  <si>
+    <t>[21,22,23,24]</t>
+  </si>
+  <si>
+    <t>leader-direct-mng</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>Menu Con</t>
+  </si>
+  <si>
+    <t>children</t>
+  </si>
+  <si>
+    <t>Cat con</t>
+  </si>
+  <si>
+    <t>Mảng chứa các Id con của thư mục này</t>
   </si>
 </sst>
 </file>
@@ -3303,7 +3327,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -3561,6 +3585,12 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="829">
@@ -4931,7 +4961,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4952,7 +4982,7 @@
         <v>39</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>25</v>
@@ -4969,16 +4999,16 @@
         <v>99</v>
       </c>
       <c r="B2" s="97" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C2" s="97" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D2" s="96" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="E2" s="96" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F2" s="96">
         <v>1</v>
@@ -4989,16 +5019,16 @@
         <v>21</v>
       </c>
       <c r="B3" s="95" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C3" s="95" t="s">
+        <v>473</v>
+      </c>
+      <c r="D3" s="94" t="s">
         <v>474</v>
       </c>
-      <c r="D3" s="94" t="s">
+      <c r="E3" s="94" t="s">
         <v>475</v>
-      </c>
-      <c r="E3" s="94" t="s">
-        <v>476</v>
       </c>
       <c r="F3" s="94">
         <v>1</v>
@@ -5020,7 +5050,7 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5037,7 +5067,9 @@
     <col min="10" max="10" width="12.5" style="85" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5" style="85"/>
     <col min="12" max="12" width="14.1640625" style="85" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="11.5" style="85"/>
+    <col min="13" max="13" width="14.33203125" style="85" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.1640625" style="85" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="11.5" style="85"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
@@ -5093,9 +5125,11 @@
         <v>370</v>
       </c>
       <c r="D2" s="90" t="s">
-        <v>461</v>
-      </c>
-      <c r="E2" s="91"/>
+        <v>460</v>
+      </c>
+      <c r="E2" s="91" t="s">
+        <v>370</v>
+      </c>
       <c r="F2" s="91" t="s">
         <v>375</v>
       </c>
@@ -5103,13 +5137,15 @@
         <v>371</v>
       </c>
       <c r="H2" s="90" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I2" s="90"/>
       <c r="J2" s="90"/>
       <c r="K2" s="90"/>
       <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
+      <c r="M2" s="106" t="s">
+        <v>188</v>
+      </c>
       <c r="N2" s="90">
         <v>1</v>
       </c>
@@ -5130,7 +5166,7 @@
       </c>
       <c r="F3" s="87"/>
       <c r="G3" s="87" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="H3" s="86" t="s">
         <v>376</v>
@@ -5139,7 +5175,9 @@
       <c r="J3" s="86"/>
       <c r="K3" s="86"/>
       <c r="L3" s="86"/>
-      <c r="M3" s="86"/>
+      <c r="M3" s="107" t="s">
+        <v>188</v>
+      </c>
       <c r="N3" s="86">
         <v>1</v>
       </c>
@@ -5160,7 +5198,7 @@
       </c>
       <c r="F4" s="87"/>
       <c r="G4" s="87" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H4" s="86" t="s">
         <v>377</v>
@@ -5169,7 +5207,9 @@
       <c r="J4" s="86"/>
       <c r="K4" s="86"/>
       <c r="L4" s="86"/>
-      <c r="M4" s="86"/>
+      <c r="M4" s="107" t="s">
+        <v>188</v>
+      </c>
       <c r="N4" s="86">
         <v>1</v>
       </c>
@@ -5190,7 +5230,7 @@
       </c>
       <c r="F5" s="87"/>
       <c r="G5" s="87" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="H5" s="86" t="s">
         <v>378</v>
@@ -5199,7 +5239,9 @@
       <c r="J5" s="86"/>
       <c r="K5" s="86"/>
       <c r="L5" s="86"/>
-      <c r="M5" s="86"/>
+      <c r="M5" s="107" t="s">
+        <v>188</v>
+      </c>
       <c r="N5" s="86">
         <v>1</v>
       </c>
@@ -5220,7 +5262,7 @@
       </c>
       <c r="F6" s="87"/>
       <c r="G6" s="87" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="H6" s="86" t="s">
         <v>380</v>
@@ -5229,7 +5271,9 @@
       <c r="J6" s="86"/>
       <c r="K6" s="86"/>
       <c r="L6" s="86"/>
-      <c r="M6" s="86"/>
+      <c r="M6" s="107" t="s">
+        <v>188</v>
+      </c>
       <c r="N6" s="86">
         <v>1</v>
       </c>
@@ -5250,7 +5294,7 @@
       </c>
       <c r="F7" s="87"/>
       <c r="G7" s="87" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="H7" s="86" t="s">
         <v>382</v>
@@ -5259,7 +5303,9 @@
       <c r="J7" s="86"/>
       <c r="K7" s="86"/>
       <c r="L7" s="86"/>
-      <c r="M7" s="86"/>
+      <c r="M7" s="107" t="s">
+        <v>188</v>
+      </c>
       <c r="N7" s="86">
         <v>1</v>
       </c>
@@ -5280,7 +5326,7 @@
       </c>
       <c r="F8" s="87"/>
       <c r="G8" s="87" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H8" s="86" t="s">
         <v>387</v>
@@ -5289,7 +5335,9 @@
       <c r="J8" s="86"/>
       <c r="K8" s="86"/>
       <c r="L8" s="86"/>
-      <c r="M8" s="86"/>
+      <c r="M8" s="107" t="s">
+        <v>188</v>
+      </c>
       <c r="N8" s="86">
         <v>1</v>
       </c>
@@ -5303,23 +5351,27 @@
         <v>383</v>
       </c>
       <c r="D9" s="90" t="s">
-        <v>448</v>
-      </c>
-      <c r="E9" s="91"/>
+        <v>592</v>
+      </c>
+      <c r="E9" s="91" t="s">
+        <v>383</v>
+      </c>
       <c r="F9" s="91" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G9" s="91" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="H9" s="90" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="I9" s="90"/>
       <c r="J9" s="90"/>
       <c r="K9" s="90"/>
       <c r="L9" s="90"/>
-      <c r="M9" s="90"/>
+      <c r="M9" s="106" t="s">
+        <v>188</v>
+      </c>
       <c r="N9" s="90">
         <v>1</v>
       </c>
@@ -5340,7 +5392,7 @@
       </c>
       <c r="F10" s="87"/>
       <c r="G10" s="87" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="H10" s="86" t="s">
         <v>444</v>
@@ -5349,7 +5401,9 @@
       <c r="J10" s="88"/>
       <c r="K10" s="86"/>
       <c r="L10" s="86"/>
-      <c r="M10" s="86"/>
+      <c r="M10" s="107" t="s">
+        <v>188</v>
+      </c>
       <c r="N10" s="86">
         <v>1</v>
       </c>
@@ -5366,11 +5420,11 @@
       </c>
       <c r="D11" s="86"/>
       <c r="E11" s="87" t="s">
-        <v>383</v>
+        <v>593</v>
       </c>
       <c r="F11" s="87"/>
       <c r="G11" s="87" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="H11" s="86" t="s">
         <v>445</v>
@@ -5379,7 +5433,9 @@
       <c r="J11" s="86"/>
       <c r="K11" s="86"/>
       <c r="L11" s="86"/>
-      <c r="M11" s="86"/>
+      <c r="M11" s="107" t="s">
+        <v>188</v>
+      </c>
       <c r="N11" s="86">
         <v>1</v>
       </c>
@@ -5396,11 +5452,11 @@
       </c>
       <c r="D12" s="86"/>
       <c r="E12" s="87" t="s">
-        <v>385</v>
+        <v>589</v>
       </c>
       <c r="F12" s="87"/>
       <c r="G12" s="87" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="H12" s="86" t="s">
         <v>446</v>
@@ -5409,7 +5465,9 @@
       <c r="J12" s="86"/>
       <c r="K12" s="86"/>
       <c r="L12" s="86"/>
-      <c r="M12" s="86"/>
+      <c r="M12" s="107" t="s">
+        <v>188</v>
+      </c>
       <c r="N12" s="86">
         <v>1</v>
       </c>
@@ -5426,11 +5484,11 @@
       </c>
       <c r="D13" s="86"/>
       <c r="E13" s="87" t="s">
-        <v>443</v>
+        <v>590</v>
       </c>
       <c r="F13" s="87"/>
       <c r="G13" s="87" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H13" s="86" t="s">
         <v>447</v>
@@ -5439,7 +5497,9 @@
       <c r="J13" s="86"/>
       <c r="K13" s="86"/>
       <c r="L13" s="86"/>
-      <c r="M13" s="86"/>
+      <c r="M13" s="107" t="s">
+        <v>188</v>
+      </c>
       <c r="N13" s="86">
         <v>1</v>
       </c>
@@ -5450,26 +5510,30 @@
       </c>
       <c r="B14" s="90"/>
       <c r="C14" s="90" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D14" s="90" t="s">
-        <v>451</v>
-      </c>
-      <c r="E14" s="91"/>
+        <v>450</v>
+      </c>
+      <c r="E14" s="91" t="s">
+        <v>448</v>
+      </c>
       <c r="F14" s="91" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="G14" s="91" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="H14" s="90" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="I14" s="90"/>
       <c r="J14" s="90"/>
       <c r="K14" s="90"/>
       <c r="L14" s="90"/>
-      <c r="M14" s="90"/>
+      <c r="M14" s="106" t="s">
+        <v>188</v>
+      </c>
       <c r="N14" s="90">
         <v>1</v>
       </c>
@@ -5482,24 +5546,26 @@
         <v>3</v>
       </c>
       <c r="C15" s="86" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D15" s="86"/>
       <c r="E15" s="87" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F15" s="87"/>
       <c r="G15" s="87" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="H15" s="86" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="I15" s="86"/>
       <c r="J15" s="88"/>
       <c r="K15" s="86"/>
       <c r="L15" s="86"/>
-      <c r="M15" s="86"/>
+      <c r="M15" s="107" t="s">
+        <v>188</v>
+      </c>
       <c r="N15" s="86">
         <v>1</v>
       </c>
@@ -5510,26 +5576,28 @@
       </c>
       <c r="B16" s="90"/>
       <c r="C16" s="90" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D16" s="90"/>
       <c r="E16" s="91" t="s">
+        <v>452</v>
+      </c>
+      <c r="F16" s="91" t="s">
+        <v>591</v>
+      </c>
+      <c r="G16" s="91" t="s">
+        <v>467</v>
+      </c>
+      <c r="H16" s="90" t="s">
         <v>453</v>
-      </c>
-      <c r="F16" s="91" t="s">
-        <v>481</v>
-      </c>
-      <c r="G16" s="91" t="s">
-        <v>468</v>
-      </c>
-      <c r="H16" s="90" t="s">
-        <v>454</v>
       </c>
       <c r="I16" s="90"/>
       <c r="J16" s="90"/>
       <c r="K16" s="90"/>
       <c r="L16" s="90"/>
-      <c r="M16" s="90"/>
+      <c r="M16" s="106" t="s">
+        <v>188</v>
+      </c>
       <c r="N16" s="90">
         <v>1</v>
       </c>
@@ -5549,8 +5617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5581,7 +5649,7 @@
         <v>39</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F1" s="22" t="s">
         <v>140</v>
@@ -5607,7 +5675,7 @@
         <v>165</v>
       </c>
       <c r="B2" s="31">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" s="28" t="s">
         <v>109</v>
@@ -5616,7 +5684,7 @@
         <v>138</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="F2" s="30"/>
       <c r="G2" s="30"/>
@@ -5634,7 +5702,7 @@
         <v>220</v>
       </c>
       <c r="B3" s="31">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C3" s="28" t="s">
         <v>109</v>
@@ -5643,7 +5711,7 @@
         <v>138</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="F3" s="30"/>
       <c r="G3" s="30"/>
@@ -5670,7 +5738,7 @@
         <v>138</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="F4" s="28"/>
       <c r="G4" s="28"/>
@@ -5688,7 +5756,7 @@
         <v>167</v>
       </c>
       <c r="B5" s="28">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5" s="32" t="s">
         <v>109</v>
@@ -5697,7 +5765,7 @@
         <v>138</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="F5" s="28"/>
       <c r="G5" s="28"/>
@@ -5729,7 +5797,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5795,10 +5863,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C3" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -5815,10 +5883,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -6117,10 +6185,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6183,7 +6251,7 @@
         <v>231</v>
       </c>
       <c r="C4" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="E4" t="s">
         <v>188</v>
@@ -6197,7 +6265,7 @@
         <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="E5" t="s">
         <v>188</v>
@@ -6225,7 +6293,7 @@
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="E7" t="s">
         <v>188</v>
@@ -6239,7 +6307,7 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="E8" t="s">
         <v>188</v>
@@ -6266,6 +6334,9 @@
       <c r="B10" t="s">
         <v>155</v>
       </c>
+      <c r="C10" t="s">
+        <v>594</v>
+      </c>
       <c r="E10" t="s">
         <v>188</v>
       </c>
@@ -6277,47 +6348,10 @@
       <c r="B11" t="s">
         <v>156</v>
       </c>
+      <c r="C11" t="s">
+        <v>595</v>
+      </c>
       <c r="E11" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="E12" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="E13" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="E14" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="E15" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="E16" t="s">
         <v>188</v>
       </c>
     </row>
@@ -6328,13 +6362,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Q85"/>
+  <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C57" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D46" sqref="D46"/>
+      <selection pane="bottomRight" activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6917,13 +6951,13 @@
         <v>221</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C17" s="51" t="s">
+        <v>482</v>
+      </c>
+      <c r="D17" s="51" t="s">
         <v>484</v>
-      </c>
-      <c r="D17" s="51" t="s">
-        <v>486</v>
       </c>
       <c r="E17" s="51" t="s">
         <v>15</v>
@@ -7080,13 +7114,13 @@
         <v>221</v>
       </c>
       <c r="B22" s="51" t="s">
+        <v>485</v>
+      </c>
+      <c r="C22" s="51" t="s">
+        <v>486</v>
+      </c>
+      <c r="D22" s="51" t="s">
         <v>487</v>
-      </c>
-      <c r="C22" s="51" t="s">
-        <v>488</v>
-      </c>
-      <c r="D22" s="51" t="s">
-        <v>489</v>
       </c>
       <c r="E22" s="51" t="s">
         <v>50</v>
@@ -7243,7 +7277,7 @@
         <v>278</v>
       </c>
       <c r="D27" s="51" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="E27" s="51" t="s">
         <v>15</v>
@@ -7272,13 +7306,13 @@
         <v>221</v>
       </c>
       <c r="B28" s="51" t="s">
+        <v>488</v>
+      </c>
+      <c r="C28" s="51" t="s">
+        <v>489</v>
+      </c>
+      <c r="D28" s="51" t="s">
         <v>490</v>
-      </c>
-      <c r="C28" s="51" t="s">
-        <v>491</v>
-      </c>
-      <c r="D28" s="51" t="s">
-        <v>492</v>
       </c>
       <c r="E28" s="51" t="s">
         <v>15</v>
@@ -7303,13 +7337,13 @@
         <v>221</v>
       </c>
       <c r="B29" s="51" t="s">
+        <v>527</v>
+      </c>
+      <c r="C29" s="51" t="s">
+        <v>528</v>
+      </c>
+      <c r="D29" s="51" t="s">
         <v>529</v>
-      </c>
-      <c r="C29" s="51" t="s">
-        <v>530</v>
-      </c>
-      <c r="D29" s="51" t="s">
-        <v>531</v>
       </c>
       <c r="E29" s="51" t="s">
         <v>15</v>
@@ -7334,13 +7368,13 @@
         <v>221</v>
       </c>
       <c r="B30" s="51" t="s">
+        <v>530</v>
+      </c>
+      <c r="C30" s="51" t="s">
+        <v>531</v>
+      </c>
+      <c r="D30" s="51" t="s">
         <v>532</v>
-      </c>
-      <c r="C30" s="51" t="s">
-        <v>533</v>
-      </c>
-      <c r="D30" s="51" t="s">
-        <v>534</v>
       </c>
       <c r="E30" s="51" t="s">
         <v>15</v>
@@ -7362,7 +7396,7 @@
     </row>
     <row r="31" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="100" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B31" s="100" t="s">
         <v>18</v>
@@ -7371,7 +7405,7 @@
         <v>243</v>
       </c>
       <c r="D31" s="100" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="E31" s="100" t="s">
         <v>97</v>
@@ -7391,16 +7425,16 @@
     </row>
     <row r="32" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="100" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B32" s="100" t="s">
         <v>222</v>
       </c>
       <c r="C32" s="100" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="D32" s="100" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="E32" s="100" t="s">
         <v>97</v>
@@ -7420,7 +7454,7 @@
     </row>
     <row r="33" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="100" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B33" s="100" t="s">
         <v>227</v>
@@ -7451,7 +7485,7 @@
     </row>
     <row r="34" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="100" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B34" s="100" t="s">
         <v>228</v>
@@ -7482,16 +7516,16 @@
     </row>
     <row r="35" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="100" t="s">
+        <v>561</v>
+      </c>
+      <c r="B35" s="100" t="s">
+        <v>562</v>
+      </c>
+      <c r="C35" s="100" t="s">
         <v>563</v>
       </c>
-      <c r="B35" s="100" t="s">
+      <c r="D35" s="100" t="s">
         <v>564</v>
-      </c>
-      <c r="C35" s="100" t="s">
-        <v>565</v>
-      </c>
-      <c r="D35" s="100" t="s">
-        <v>566</v>
       </c>
       <c r="E35" s="100" t="s">
         <v>15</v>
@@ -7513,16 +7547,16 @@
     </row>
     <row r="36" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="100" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B36" s="100" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C36" s="100" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="D36" s="100" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="E36" s="100" t="s">
         <v>97</v>
@@ -7542,7 +7576,7 @@
     </row>
     <row r="37" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="100" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B37" s="100" t="s">
         <v>205</v>
@@ -7571,7 +7605,7 @@
     </row>
     <row r="38" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="100" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B38" s="100" t="s">
         <v>231</v>
@@ -7600,7 +7634,7 @@
     </row>
     <row r="39" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="100" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B39" s="100" t="s">
         <v>19</v>
@@ -7631,7 +7665,7 @@
     </row>
     <row r="40" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="100" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B40" s="100" t="s">
         <v>45</v>
@@ -7660,7 +7694,7 @@
     </row>
     <row r="41" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="100" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B41" s="100" t="s">
         <v>0</v>
@@ -7669,7 +7703,7 @@
         <v>236</v>
       </c>
       <c r="D41" s="100" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="E41" s="100" t="s">
         <v>97</v>
@@ -8191,7 +8225,7 @@
         <v>299</v>
       </c>
       <c r="D57" s="98" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="E57" s="52" t="s">
         <v>15</v>
@@ -8256,10 +8290,10 @@
         <v>0</v>
       </c>
       <c r="C59" s="52" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="D59" s="52" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="E59" s="52" t="s">
         <v>97</v>
@@ -8354,7 +8388,7 @@
         <v>238</v>
       </c>
       <c r="D62" s="52" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="E62" s="52" t="s">
         <v>50</v>
@@ -8454,10 +8488,10 @@
         <v>327</v>
       </c>
       <c r="C65" s="53" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="D65" s="53" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="E65" s="53" t="s">
         <v>15</v>
@@ -8830,9 +8864,7 @@
       <c r="H76" s="45">
         <v>1</v>
       </c>
-      <c r="I76" s="45">
-        <v>1</v>
-      </c>
+      <c r="I76" s="45"/>
       <c r="J76" s="45">
         <v>1</v>
       </c>
@@ -8884,23 +8916,21 @@
         <v>169</v>
       </c>
       <c r="B78" s="44" t="s">
-        <v>242</v>
+        <v>596</v>
       </c>
       <c r="C78" s="44" t="s">
-        <v>244</v>
+        <v>597</v>
       </c>
       <c r="D78" s="63" t="s">
-        <v>303</v>
+        <v>598</v>
       </c>
       <c r="E78" s="63" t="s">
         <v>15</v>
       </c>
       <c r="F78" s="45">
-        <v>50</v>
-      </c>
-      <c r="G78" s="45">
-        <v>1</v>
-      </c>
+        <v>2000</v>
+      </c>
+      <c r="G78" s="45"/>
       <c r="H78" s="45"/>
       <c r="I78" s="45"/>
       <c r="J78" s="45"/>
@@ -8909,9 +8939,7 @@
       <c r="M78" s="45"/>
       <c r="N78" s="45"/>
       <c r="O78" s="45"/>
-      <c r="P78" s="56">
-        <v>73</v>
-      </c>
+      <c r="P78" s="56"/>
       <c r="Q78" s="57"/>
     </row>
     <row r="79" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
@@ -8919,13 +8947,13 @@
         <v>169</v>
       </c>
       <c r="B79" s="44" t="s">
-        <v>25</v>
+        <v>242</v>
       </c>
       <c r="C79" s="44" t="s">
-        <v>207</v>
+        <v>244</v>
       </c>
       <c r="D79" s="63" t="s">
-        <v>273</v>
+        <v>303</v>
       </c>
       <c r="E79" s="63" t="s">
         <v>15</v>
@@ -8933,7 +8961,9 @@
       <c r="F79" s="45">
         <v>50</v>
       </c>
-      <c r="G79" s="45"/>
+      <c r="G79" s="45">
+        <v>1</v>
+      </c>
       <c r="H79" s="45"/>
       <c r="I79" s="45"/>
       <c r="J79" s="45"/>
@@ -8943,7 +8973,7 @@
       <c r="N79" s="45"/>
       <c r="O79" s="45"/>
       <c r="P79" s="56">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q79" s="57"/>
     </row>
@@ -8952,19 +8982,19 @@
         <v>169</v>
       </c>
       <c r="B80" s="44" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="C80" s="44" t="s">
-        <v>245</v>
+        <v>207</v>
       </c>
       <c r="D80" s="63" t="s">
-        <v>234</v>
+        <v>273</v>
       </c>
       <c r="E80" s="63" t="s">
         <v>15</v>
       </c>
       <c r="F80" s="45">
-        <v>255</v>
+        <v>50</v>
       </c>
       <c r="G80" s="45"/>
       <c r="H80" s="45"/>
@@ -8976,7 +9006,7 @@
       <c r="N80" s="45"/>
       <c r="O80" s="45"/>
       <c r="P80" s="56">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Q80" s="57"/>
     </row>
@@ -8985,18 +9015,20 @@
         <v>169</v>
       </c>
       <c r="B81" s="44" t="s">
-        <v>205</v>
+        <v>4</v>
       </c>
       <c r="C81" s="44" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="D81" s="63" t="s">
-        <v>132</v>
-      </c>
-      <c r="E81" s="64" t="s">
-        <v>50</v>
-      </c>
-      <c r="F81" s="45"/>
+        <v>234</v>
+      </c>
+      <c r="E81" s="63" t="s">
+        <v>15</v>
+      </c>
+      <c r="F81" s="45">
+        <v>255</v>
+      </c>
       <c r="G81" s="45"/>
       <c r="H81" s="45"/>
       <c r="I81" s="45"/>
@@ -9007,7 +9039,7 @@
       <c r="N81" s="45"/>
       <c r="O81" s="45"/>
       <c r="P81" s="56">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q81" s="57"/>
     </row>
@@ -9016,20 +9048,18 @@
         <v>169</v>
       </c>
       <c r="B82" s="44" t="s">
-        <v>231</v>
+        <v>205</v>
       </c>
       <c r="C82" s="44" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="D82" s="63" t="s">
-        <v>241</v>
+        <v>132</v>
       </c>
       <c r="E82" s="64" t="s">
-        <v>15</v>
-      </c>
-      <c r="F82" s="45">
-        <v>255</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="F82" s="45"/>
       <c r="G82" s="45"/>
       <c r="H82" s="45"/>
       <c r="I82" s="45"/>
@@ -9040,7 +9070,7 @@
       <c r="N82" s="45"/>
       <c r="O82" s="45"/>
       <c r="P82" s="56">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q82" s="57"/>
     </row>
@@ -9049,18 +9079,20 @@
         <v>169</v>
       </c>
       <c r="B83" s="44" t="s">
-        <v>19</v>
+        <v>231</v>
       </c>
       <c r="C83" s="44" t="s">
-        <v>238</v>
+        <v>249</v>
       </c>
       <c r="D83" s="63" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="E83" s="64" t="s">
-        <v>50</v>
-      </c>
-      <c r="F83" s="45"/>
+        <v>15</v>
+      </c>
+      <c r="F83" s="45">
+        <v>255</v>
+      </c>
       <c r="G83" s="45"/>
       <c r="H83" s="45"/>
       <c r="I83" s="45"/>
@@ -9071,7 +9103,7 @@
       <c r="N83" s="45"/>
       <c r="O83" s="45"/>
       <c r="P83" s="56">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q83" s="57"/>
     </row>
@@ -9080,20 +9112,18 @@
         <v>169</v>
       </c>
       <c r="B84" s="44" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="C84" s="44" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="D84" s="63" t="s">
-        <v>171</v>
+        <v>247</v>
       </c>
       <c r="E84" s="64" t="s">
-        <v>15</v>
-      </c>
-      <c r="F84" s="45">
         <v>50</v>
       </c>
+      <c r="F84" s="45"/>
       <c r="G84" s="45"/>
       <c r="H84" s="45"/>
       <c r="I84" s="45"/>
@@ -9104,7 +9134,7 @@
       <c r="N84" s="45"/>
       <c r="O84" s="45"/>
       <c r="P84" s="56">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q84" s="57"/>
     </row>
@@ -9113,33 +9143,66 @@
         <v>169</v>
       </c>
       <c r="B85" s="44" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="C85" s="44" t="s">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="D85" s="63" t="s">
-        <v>172</v>
-      </c>
-      <c r="E85" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="F85" s="45"/>
+        <v>171</v>
+      </c>
+      <c r="E85" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="F85" s="45">
+        <v>50</v>
+      </c>
       <c r="G85" s="45"/>
       <c r="H85" s="45"/>
       <c r="I85" s="45"/>
       <c r="J85" s="45"/>
       <c r="K85" s="45"/>
       <c r="L85" s="45"/>
-      <c r="M85" s="45">
-        <v>1</v>
-      </c>
+      <c r="M85" s="45"/>
       <c r="N85" s="45"/>
       <c r="O85" s="45"/>
       <c r="P85" s="56">
+        <v>79</v>
+      </c>
+      <c r="Q85" s="57"/>
+    </row>
+    <row r="86" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="B86" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="C86" s="44" t="s">
+        <v>236</v>
+      </c>
+      <c r="D86" s="63" t="s">
+        <v>172</v>
+      </c>
+      <c r="E86" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="F86" s="45"/>
+      <c r="G86" s="45"/>
+      <c r="H86" s="45"/>
+      <c r="I86" s="45"/>
+      <c r="J86" s="45"/>
+      <c r="K86" s="45"/>
+      <c r="L86" s="45"/>
+      <c r="M86" s="45">
+        <v>1</v>
+      </c>
+      <c r="N86" s="45"/>
+      <c r="O86" s="45"/>
+      <c r="P86" s="56">
         <v>80</v>
       </c>
-      <c r="Q85" s="57"/>
+      <c r="Q86" s="57"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9299,13 +9362,13 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="D6" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="E6" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="H6" t="s">
         <v>188</v>
@@ -9322,7 +9385,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="D7" t="s">
         <v>395</v>
@@ -9345,7 +9408,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="D8" t="s">
         <v>396</v>
@@ -9435,7 +9498,7 @@
       </c>
       <c r="B12" s="92"/>
       <c r="C12" s="92" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="D12" s="92" t="s">
         <v>415</v>
@@ -9460,7 +9523,7 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="D13" t="s">
         <v>417</v>
@@ -9483,7 +9546,7 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="D14" t="s">
         <v>418</v>
@@ -9506,7 +9569,7 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="D15" t="s">
         <v>419</v>
@@ -9529,7 +9592,7 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="D16" t="s">
         <v>423</v>
@@ -9552,7 +9615,7 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="D17" t="s">
         <v>424</v>
@@ -9575,7 +9638,7 @@
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D18" t="s">
         <v>425</v>
@@ -9596,7 +9659,7 @@
       </c>
       <c r="B19" s="92"/>
       <c r="C19" s="92" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D19" s="92" t="s">
         <v>426</v>
@@ -9711,10 +9774,10 @@
       </c>
       <c r="B24" s="92"/>
       <c r="C24" s="92" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D24" s="92" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E24" s="92" t="s">
         <v>427</v>
@@ -9736,13 +9799,13 @@
         <v>5</v>
       </c>
       <c r="C25" t="s">
+        <v>558</v>
+      </c>
+      <c r="D25" t="s">
+        <v>559</v>
+      </c>
+      <c r="E25" t="s">
         <v>560</v>
-      </c>
-      <c r="D25" t="s">
-        <v>561</v>
-      </c>
-      <c r="E25" t="s">
-        <v>562</v>
       </c>
       <c r="H25" t="s">
         <v>188</v>
@@ -9759,13 +9822,13 @@
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D26" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="E26" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="H26" t="s">
         <v>188</v>
@@ -9782,13 +9845,13 @@
         <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D27" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E27" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="H27" t="s">
         <v>188</v>
@@ -9805,13 +9868,13 @@
         <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D28" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="E28" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H28" t="s">
         <v>188</v>
@@ -9828,13 +9891,13 @@
         <v>5</v>
       </c>
       <c r="C29" t="s">
+        <v>506</v>
+      </c>
+      <c r="D29" t="s">
+        <v>507</v>
+      </c>
+      <c r="E29" t="s">
         <v>508</v>
-      </c>
-      <c r="D29" t="s">
-        <v>509</v>
-      </c>
-      <c r="E29" t="s">
-        <v>510</v>
       </c>
       <c r="H29" t="s">
         <v>188</v>
@@ -9851,13 +9914,13 @@
         <v>5</v>
       </c>
       <c r="C30" t="s">
+        <v>509</v>
+      </c>
+      <c r="D30" t="s">
+        <v>510</v>
+      </c>
+      <c r="E30" t="s">
         <v>511</v>
-      </c>
-      <c r="D30" t="s">
-        <v>512</v>
-      </c>
-      <c r="E30" t="s">
-        <v>513</v>
       </c>
       <c r="H30" t="s">
         <v>188</v>
@@ -9874,13 +9937,13 @@
         <v>5</v>
       </c>
       <c r="C31" t="s">
+        <v>512</v>
+      </c>
+      <c r="D31" t="s">
+        <v>513</v>
+      </c>
+      <c r="E31" t="s">
         <v>514</v>
-      </c>
-      <c r="D31" t="s">
-        <v>515</v>
-      </c>
-      <c r="E31" t="s">
-        <v>516</v>
       </c>
       <c r="H31" t="s">
         <v>188</v>
@@ -9897,13 +9960,13 @@
         <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="D32" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="E32" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="H32" s="99" t="s">
         <v>188</v>
@@ -9920,13 +9983,13 @@
         <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D33" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="E33" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="H33" s="99" t="s">
         <v>188</v>
@@ -9943,13 +10006,13 @@
         <v>5</v>
       </c>
       <c r="C34" t="s">
+        <v>547</v>
+      </c>
+      <c r="D34" t="s">
+        <v>548</v>
+      </c>
+      <c r="E34" t="s">
         <v>549</v>
-      </c>
-      <c r="D34" t="s">
-        <v>550</v>
-      </c>
-      <c r="E34" t="s">
-        <v>551</v>
       </c>
       <c r="H34" s="99" t="s">
         <v>188</v>
@@ -9966,13 +10029,13 @@
         <v>5</v>
       </c>
       <c r="C35" t="s">
+        <v>533</v>
+      </c>
+      <c r="D35" t="s">
+        <v>534</v>
+      </c>
+      <c r="E35" t="s">
         <v>535</v>
-      </c>
-      <c r="D35" t="s">
-        <v>536</v>
-      </c>
-      <c r="E35" t="s">
-        <v>537</v>
       </c>
       <c r="H35" s="99" t="s">
         <v>188</v>
@@ -9989,13 +10052,13 @@
         <v>5</v>
       </c>
       <c r="C36" t="s">
+        <v>520</v>
+      </c>
+      <c r="D36" t="s">
         <v>522</v>
       </c>
-      <c r="D36" t="s">
-        <v>524</v>
-      </c>
       <c r="E36" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="H36" s="99" t="s">
         <v>188</v>
@@ -10012,13 +10075,13 @@
         <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="D37" t="s">
         <v>402</v>
       </c>
       <c r="E37" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="H37" s="99" t="s">
         <v>188</v>
@@ -10035,13 +10098,13 @@
         <v>5</v>
       </c>
       <c r="C38" t="s">
+        <v>536</v>
+      </c>
+      <c r="D38" t="s">
+        <v>537</v>
+      </c>
+      <c r="E38" t="s">
         <v>538</v>
-      </c>
-      <c r="D38" t="s">
-        <v>539</v>
-      </c>
-      <c r="E38" t="s">
-        <v>540</v>
       </c>
       <c r="H38" s="99" t="s">
         <v>188</v>
@@ -10562,7 +10625,7 @@
   <dimension ref="A1:Q63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
@@ -11123,11 +11186,11 @@
         <v>38</v>
       </c>
       <c r="B18" s="79" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C18" s="79"/>
       <c r="D18" s="79" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="E18" s="81" t="s">
         <v>15</v>
@@ -11421,11 +11484,11 @@
         <v>46</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>15</v>
@@ -12021,7 +12084,7 @@
       </c>
       <c r="C48" s="79"/>
       <c r="D48" s="79" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E48" s="79" t="s">
         <v>17</v>
@@ -12330,7 +12393,7 @@
       </c>
       <c r="C58" s="68"/>
       <c r="D58" s="72" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E58" s="68" t="s">
         <v>16</v>
@@ -12518,10 +12581,10 @@
   <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="K23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E30" sqref="E30"/>
+      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13484,7 +13547,7 @@
         <v>53</v>
       </c>
       <c r="E26" s="70" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="F26" s="68">
         <v>1</v>
@@ -13518,7 +13581,7 @@
         <v>53</v>
       </c>
       <c r="E27" s="70" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="F27" s="68">
         <v>1</v>
@@ -13552,7 +13615,7 @@
         <v>53</v>
       </c>
       <c r="E28" s="70" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="F28" s="68">
         <v>1</v>
@@ -13586,7 +13649,7 @@
         <v>53</v>
       </c>
       <c r="E29" s="70" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F29" s="68">
         <v>1</v>
@@ -13620,7 +13683,7 @@
         <v>53</v>
       </c>
       <c r="E30" s="70" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="F30" s="68">
         <v>1</v>
@@ -13654,7 +13717,7 @@
         <v>53</v>
       </c>
       <c r="E31" s="70" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="F31" s="68">
         <v>1</v>
@@ -14286,7 +14349,7 @@
         <v>168</v>
       </c>
       <c r="E50" s="103" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="F50" s="102">
         <v>1</v>
@@ -14319,7 +14382,7 @@
         <v>168</v>
       </c>
       <c r="E51" s="103" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="F51" s="102">
         <v>1</v>
@@ -14352,7 +14415,7 @@
         <v>168</v>
       </c>
       <c r="E52" s="103" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="F52" s="102">
         <v>1</v>

</xml_diff>

<commit_message>
rev grid list layout
</commit_message>
<xml_diff>
--- a/db/excel/api-function-granted-users-cdld.xlsx
+++ b/db/excel/api-function-granted-users-cdld.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10613"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C802BE7D-565C-9D4E-9D33-77140543047D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0FBA5D4-DC62-5A40-A5C7-03D901824460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="500" windowWidth="38400" windowHeight="20080" tabRatio="800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" tabRatio="800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_types" sheetId="27" r:id="rId1"/>
@@ -293,7 +293,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1567" uniqueCount="627">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1593" uniqueCount="640">
   <si>
     <t>status</t>
   </si>
@@ -1354,57 +1354,12 @@
     <t>User cập nhập người dùng này</t>
   </si>
   <si>
-    <t>P.TH</t>
-  </si>
-  <si>
-    <t>P.DVKT</t>
-  </si>
-  <si>
     <t>BGĐ</t>
   </si>
   <si>
-    <t>P.CSKH</t>
-  </si>
-  <si>
-    <t>P.KHCN</t>
-  </si>
-  <si>
-    <t>P.KHDN</t>
-  </si>
-  <si>
-    <t>P.KT</t>
-  </si>
-  <si>
-    <t>MBF.DNA2</t>
-  </si>
-  <si>
-    <t>MBF.DNA1</t>
-  </si>
-  <si>
-    <t>MBF.QNG</t>
-  </si>
-  <si>
-    <t>MBF.QNA</t>
-  </si>
-  <si>
-    <t>MBF.TTH</t>
-  </si>
-  <si>
-    <t>MBF.BDI</t>
-  </si>
-  <si>
-    <t>MBF.QTR</t>
-  </si>
-  <si>
-    <t>MBF.PYE</t>
-  </si>
-  <si>
     <t>Công ty 3</t>
   </si>
   <si>
-    <t>CTy3</t>
-  </si>
-  <si>
     <t>Mã của tổ chức (dùng khi select</t>
   </si>
   <si>
@@ -1663,18 +1618,6 @@
     <t>Cập nhập hoàn thành cho chỉ đạo này</t>
   </si>
   <si>
-    <t>MT_INST</t>
-  </si>
-  <si>
-    <t>MT_WEEK</t>
-  </si>
-  <si>
-    <t>MT_MONTH</t>
-  </si>
-  <si>
-    <t>MT_YEAR</t>
-  </si>
-  <si>
     <t>direct-organization</t>
   </si>
   <si>
@@ -1960,24 +1903,6 @@
     <t>P.TH nhập ý kiến của lãnh đạo</t>
   </si>
   <si>
-    <t>DT_WEEK</t>
-  </si>
-  <si>
-    <t>DT_MONTH</t>
-  </si>
-  <si>
-    <t>DT_YEAR</t>
-  </si>
-  <si>
-    <t>DT_1WEEK</t>
-  </si>
-  <si>
-    <t>DT_1MONTH</t>
-  </si>
-  <si>
-    <t>DT_1YEAR</t>
-  </si>
-  <si>
     <t>CMPLT_PERCENT</t>
   </si>
   <si>
@@ -2228,6 +2153,120 @@
   </si>
   <si>
     <t>/get-direct-by-ids</t>
+  </si>
+  <si>
+    <t>HDX</t>
+  </si>
+  <si>
+    <t>GBT</t>
+  </si>
+  <si>
+    <t>HTH</t>
+  </si>
+  <si>
+    <t>TKN</t>
+  </si>
+  <si>
+    <t>TUA</t>
+  </si>
+  <si>
+    <t>THA</t>
+  </si>
+  <si>
+    <t>NAM</t>
+  </si>
+  <si>
+    <t>TA1</t>
+  </si>
+  <si>
+    <t>TH1</t>
+  </si>
+  <si>
+    <t>NA1</t>
+  </si>
+  <si>
+    <t>CT3</t>
+  </si>
+  <si>
+    <t>DVK</t>
+  </si>
+  <si>
+    <t>TTH</t>
+  </si>
+  <si>
+    <t>PTH</t>
+  </si>
+  <si>
+    <t>CSH</t>
+  </si>
+  <si>
+    <t>KHC</t>
+  </si>
+  <si>
+    <t>KHD</t>
+  </si>
+  <si>
+    <t>KTO</t>
+  </si>
+  <si>
+    <t>DN1</t>
+  </si>
+  <si>
+    <t>DN2</t>
+  </si>
+  <si>
+    <t>QNG</t>
+  </si>
+  <si>
+    <t>QNA</t>
+  </si>
+  <si>
+    <t>BDI</t>
+  </si>
+  <si>
+    <t>QTR</t>
+  </si>
+  <si>
+    <t>PYE</t>
+  </si>
+  <si>
+    <t>BGD</t>
+  </si>
+  <si>
+    <t>Ban Giám Đốc</t>
+  </si>
+  <si>
+    <t>Danh mục thành viên BGĐ</t>
+  </si>
+  <si>
+    <t>GD</t>
+  </si>
+  <si>
+    <t>Trần Vinh</t>
+  </si>
+  <si>
+    <t>PG1</t>
+  </si>
+  <si>
+    <t>PG2</t>
+  </si>
+  <si>
+    <t>Nguyễn Thanh Tuyền</t>
+  </si>
+  <si>
+    <t>Võ Đình Mẫn</t>
+  </si>
+  <si>
+    <t>Giám Đốc Công Ty</t>
+  </si>
+  <si>
+    <t>Phó Giám Đốc thứ 1 của Công Ty</t>
+  </si>
+  <si>
+    <t>Phó Giám Đốc thứ 2 của Công Ty</t>
+  </si>
+  <si>
+    <t>Chỉ đạo chung của cả Ban Giám Đốc</t>
   </si>
 </sst>
 </file>
@@ -5084,7 +5123,7 @@
         <v>39</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>469</v>
+        <v>450</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>25</v>
@@ -5101,16 +5140,16 @@
         <v>99</v>
       </c>
       <c r="B2" s="97" t="s">
-        <v>573</v>
+        <v>548</v>
       </c>
       <c r="C2" s="97" t="s">
-        <v>471</v>
+        <v>452</v>
       </c>
       <c r="D2" s="96" t="s">
-        <v>583</v>
+        <v>558</v>
       </c>
       <c r="E2" s="96" t="s">
-        <v>470</v>
+        <v>451</v>
       </c>
       <c r="F2" s="96">
         <v>1</v>
@@ -5121,16 +5160,16 @@
         <v>21</v>
       </c>
       <c r="B3" s="95" t="s">
-        <v>574</v>
+        <v>549</v>
       </c>
       <c r="C3" s="95" t="s">
-        <v>472</v>
+        <v>453</v>
       </c>
       <c r="D3" s="94" t="s">
-        <v>473</v>
+        <v>454</v>
       </c>
       <c r="E3" s="94" t="s">
-        <v>474</v>
+        <v>455</v>
       </c>
       <c r="F3" s="94">
         <v>1</v>
@@ -5224,22 +5263,22 @@
       </c>
       <c r="B2" s="90"/>
       <c r="C2" s="90" t="s">
-        <v>369</v>
+        <v>354</v>
       </c>
       <c r="D2" s="90" t="s">
-        <v>459</v>
+        <v>440</v>
       </c>
       <c r="E2" s="91" t="s">
-        <v>369</v>
+        <v>354</v>
       </c>
       <c r="F2" s="91" t="s">
-        <v>374</v>
+        <v>359</v>
       </c>
       <c r="G2" s="91" t="s">
-        <v>370</v>
+        <v>355</v>
       </c>
       <c r="H2" s="90" t="s">
-        <v>468</v>
+        <v>449</v>
       </c>
       <c r="I2" s="90"/>
       <c r="J2" s="90"/>
@@ -5260,18 +5299,18 @@
         <v>1</v>
       </c>
       <c r="C3" s="86" t="s">
-        <v>371</v>
+        <v>356</v>
       </c>
       <c r="D3" s="86"/>
       <c r="E3" s="87" t="s">
-        <v>371</v>
+        <v>356</v>
       </c>
       <c r="F3" s="87"/>
       <c r="G3" s="87" t="s">
-        <v>453</v>
+        <v>434</v>
       </c>
       <c r="H3" s="86" t="s">
-        <v>375</v>
+        <v>360</v>
       </c>
       <c r="I3" s="86"/>
       <c r="J3" s="86"/>
@@ -5292,18 +5331,18 @@
         <v>1</v>
       </c>
       <c r="C4" s="86" t="s">
-        <v>372</v>
+        <v>357</v>
       </c>
       <c r="D4" s="86"/>
       <c r="E4" s="87" t="s">
-        <v>372</v>
+        <v>357</v>
       </c>
       <c r="F4" s="87"/>
       <c r="G4" s="87" t="s">
-        <v>454</v>
+        <v>435</v>
       </c>
       <c r="H4" s="86" t="s">
-        <v>376</v>
+        <v>361</v>
       </c>
       <c r="I4" s="86"/>
       <c r="J4" s="86"/>
@@ -5324,18 +5363,18 @@
         <v>1</v>
       </c>
       <c r="C5" s="86" t="s">
-        <v>373</v>
+        <v>358</v>
       </c>
       <c r="D5" s="86"/>
       <c r="E5" s="87" t="s">
-        <v>373</v>
+        <v>358</v>
       </c>
       <c r="F5" s="87"/>
       <c r="G5" s="87" t="s">
-        <v>455</v>
+        <v>436</v>
       </c>
       <c r="H5" s="86" t="s">
-        <v>377</v>
+        <v>362</v>
       </c>
       <c r="I5" s="86"/>
       <c r="J5" s="86"/>
@@ -5356,18 +5395,18 @@
         <v>1</v>
       </c>
       <c r="C6" s="86" t="s">
-        <v>378</v>
+        <v>363</v>
       </c>
       <c r="D6" s="86"/>
       <c r="E6" s="87" t="s">
-        <v>378</v>
+        <v>363</v>
       </c>
       <c r="F6" s="87"/>
       <c r="G6" s="87" t="s">
-        <v>456</v>
+        <v>437</v>
       </c>
       <c r="H6" s="86" t="s">
-        <v>379</v>
+        <v>364</v>
       </c>
       <c r="I6" s="86"/>
       <c r="J6" s="86"/>
@@ -5388,18 +5427,18 @@
         <v>1</v>
       </c>
       <c r="C7" s="86" t="s">
-        <v>380</v>
+        <v>365</v>
       </c>
       <c r="D7" s="86"/>
       <c r="E7" s="87" t="s">
-        <v>380</v>
+        <v>365</v>
       </c>
       <c r="F7" s="87"/>
       <c r="G7" s="87" t="s">
-        <v>457</v>
+        <v>438</v>
       </c>
       <c r="H7" s="86" t="s">
-        <v>381</v>
+        <v>366</v>
       </c>
       <c r="I7" s="86"/>
       <c r="J7" s="86"/>
@@ -5420,18 +5459,18 @@
         <v>1</v>
       </c>
       <c r="C8" s="86" t="s">
-        <v>385</v>
+        <v>370</v>
       </c>
       <c r="D8" s="86"/>
       <c r="E8" s="87" t="s">
-        <v>385</v>
+        <v>370</v>
       </c>
       <c r="F8" s="87"/>
       <c r="G8" s="87" t="s">
-        <v>458</v>
+        <v>439</v>
       </c>
       <c r="H8" s="86" t="s">
-        <v>386</v>
+        <v>371</v>
       </c>
       <c r="I8" s="86"/>
       <c r="J8" s="86"/>
@@ -5450,22 +5489,22 @@
       </c>
       <c r="B9" s="90"/>
       <c r="C9" s="90" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="D9" s="90" t="s">
-        <v>588</v>
+        <v>563</v>
       </c>
       <c r="E9" s="91" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F9" s="91" t="s">
-        <v>595</v>
+        <v>570</v>
       </c>
       <c r="G9" s="91" t="s">
-        <v>460</v>
+        <v>441</v>
       </c>
       <c r="H9" s="90" t="s">
-        <v>478</v>
+        <v>459</v>
       </c>
       <c r="I9" s="90"/>
       <c r="J9" s="90"/>
@@ -5486,18 +5525,18 @@
         <v>2</v>
       </c>
       <c r="C10" s="86" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="D10" s="86"/>
       <c r="E10" s="87" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F10" s="87"/>
       <c r="G10" s="87" t="s">
-        <v>461</v>
+        <v>442</v>
       </c>
       <c r="H10" s="86" t="s">
-        <v>443</v>
+        <v>424</v>
       </c>
       <c r="I10" s="86"/>
       <c r="J10" s="88"/>
@@ -5518,18 +5557,18 @@
         <v>2</v>
       </c>
       <c r="C11" s="86" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="D11" s="86"/>
       <c r="E11" s="87" t="s">
-        <v>589</v>
+        <v>564</v>
       </c>
       <c r="F11" s="87"/>
       <c r="G11" s="87" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="H11" s="86" t="s">
-        <v>444</v>
+        <v>425</v>
       </c>
       <c r="I11" s="86"/>
       <c r="J11" s="86"/>
@@ -5550,18 +5589,18 @@
         <v>2</v>
       </c>
       <c r="C12" s="86" t="s">
-        <v>384</v>
+        <v>369</v>
       </c>
       <c r="D12" s="86"/>
       <c r="E12" s="87" t="s">
-        <v>585</v>
+        <v>560</v>
       </c>
       <c r="F12" s="87"/>
       <c r="G12" s="87" t="s">
-        <v>463</v>
+        <v>444</v>
       </c>
       <c r="H12" s="86" t="s">
-        <v>445</v>
+        <v>426</v>
       </c>
       <c r="I12" s="86"/>
       <c r="J12" s="86"/>
@@ -5582,18 +5621,18 @@
         <v>2</v>
       </c>
       <c r="C13" s="86" t="s">
-        <v>442</v>
+        <v>423</v>
       </c>
       <c r="D13" s="86"/>
       <c r="E13" s="87" t="s">
-        <v>586</v>
+        <v>561</v>
       </c>
       <c r="F13" s="87"/>
       <c r="G13" s="87" t="s">
-        <v>464</v>
+        <v>445</v>
       </c>
       <c r="H13" s="86" t="s">
-        <v>446</v>
+        <v>427</v>
       </c>
       <c r="I13" s="86"/>
       <c r="J13" s="86"/>
@@ -5612,22 +5651,22 @@
       </c>
       <c r="B14" s="90"/>
       <c r="C14" s="90" t="s">
-        <v>447</v>
+        <v>428</v>
       </c>
       <c r="D14" s="90" t="s">
-        <v>449</v>
+        <v>430</v>
       </c>
       <c r="E14" s="91" t="s">
-        <v>447</v>
+        <v>428</v>
       </c>
       <c r="F14" s="91" t="s">
-        <v>477</v>
+        <v>458</v>
       </c>
       <c r="G14" s="91" t="s">
-        <v>467</v>
+        <v>448</v>
       </c>
       <c r="H14" s="90" t="s">
-        <v>479</v>
+        <v>460</v>
       </c>
       <c r="I14" s="90"/>
       <c r="J14" s="90"/>
@@ -5648,18 +5687,18 @@
         <v>3</v>
       </c>
       <c r="C15" s="86" t="s">
-        <v>448</v>
+        <v>429</v>
       </c>
       <c r="D15" s="86"/>
       <c r="E15" s="87" t="s">
-        <v>448</v>
+        <v>429</v>
       </c>
       <c r="F15" s="87"/>
       <c r="G15" s="87" t="s">
-        <v>465</v>
+        <v>446</v>
       </c>
       <c r="H15" s="86" t="s">
-        <v>450</v>
+        <v>431</v>
       </c>
       <c r="I15" s="86"/>
       <c r="J15" s="88"/>
@@ -5678,20 +5717,20 @@
       </c>
       <c r="B16" s="90"/>
       <c r="C16" s="90" t="s">
-        <v>451</v>
+        <v>432</v>
       </c>
       <c r="D16" s="90"/>
       <c r="E16" s="91" t="s">
-        <v>451</v>
+        <v>432</v>
       </c>
       <c r="F16" s="91" t="s">
-        <v>587</v>
+        <v>562</v>
       </c>
       <c r="G16" s="91" t="s">
-        <v>466</v>
+        <v>447</v>
       </c>
       <c r="H16" s="90" t="s">
-        <v>452</v>
+        <v>433</v>
       </c>
       <c r="I16" s="90"/>
       <c r="J16" s="90"/>
@@ -5742,7 +5781,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>363</v>
+        <v>348</v>
       </c>
       <c r="C1" s="22" t="s">
         <v>38</v>
@@ -5751,7 +5790,7 @@
         <v>39</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>469</v>
+        <v>450</v>
       </c>
       <c r="F1" s="22" t="s">
         <v>140</v>
@@ -5786,7 +5825,7 @@
         <v>138</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>584</v>
+        <v>559</v>
       </c>
       <c r="F2" s="30"/>
       <c r="G2" s="30"/>
@@ -5813,7 +5852,7 @@
         <v>138</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>584</v>
+        <v>559</v>
       </c>
       <c r="F3" s="30"/>
       <c r="G3" s="30"/>
@@ -5840,7 +5879,7 @@
         <v>138</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>584</v>
+        <v>559</v>
       </c>
       <c r="F4" s="28"/>
       <c r="G4" s="28"/>
@@ -5867,7 +5906,7 @@
         <v>138</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>584</v>
+        <v>559</v>
       </c>
       <c r="F5" s="28"/>
       <c r="G5" s="28"/>
@@ -5899,14 +5938,16 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:D11"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
     <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
@@ -5925,7 +5966,7 @@
         <v>242</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>596</v>
+        <v>571</v>
       </c>
       <c r="E1" s="40" t="s">
         <v>180</v>
@@ -5951,13 +5992,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>350</v>
+        <v>336</v>
       </c>
       <c r="C2" t="s">
-        <v>351</v>
+        <v>612</v>
       </c>
       <c r="D2" t="s">
-        <v>597</v>
+        <v>572</v>
       </c>
       <c r="I2" t="s">
         <v>188</v>
@@ -5974,10 +6015,10 @@
         <v>191</v>
       </c>
       <c r="C3" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D3" t="s">
-        <v>598</v>
+        <v>573</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -5997,10 +6038,10 @@
         <v>190</v>
       </c>
       <c r="C4" t="s">
-        <v>336</v>
+        <v>613</v>
       </c>
       <c r="D4" t="s">
-        <v>599</v>
+        <v>574</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -6020,10 +6061,10 @@
         <v>189</v>
       </c>
       <c r="C5" t="s">
-        <v>335</v>
+        <v>614</v>
       </c>
       <c r="D5" t="s">
-        <v>600</v>
+        <v>575</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -6043,10 +6084,10 @@
         <v>192</v>
       </c>
       <c r="C6" t="s">
-        <v>335</v>
+        <v>615</v>
       </c>
       <c r="D6" t="s">
-        <v>601</v>
+        <v>576</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -6066,10 +6107,10 @@
         <v>194</v>
       </c>
       <c r="C7" t="s">
-        <v>338</v>
+        <v>616</v>
       </c>
       <c r="D7" t="s">
-        <v>602</v>
+        <v>577</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -6089,10 +6130,10 @@
         <v>196</v>
       </c>
       <c r="C8" t="s">
-        <v>339</v>
+        <v>617</v>
       </c>
       <c r="D8" t="s">
-        <v>603</v>
+        <v>578</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -6112,10 +6153,10 @@
         <v>197</v>
       </c>
       <c r="C9" t="s">
-        <v>340</v>
+        <v>618</v>
       </c>
       <c r="D9" t="s">
-        <v>604</v>
+        <v>579</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -6135,10 +6176,10 @@
         <v>198</v>
       </c>
       <c r="C10" t="s">
-        <v>341</v>
+        <v>619</v>
       </c>
       <c r="D10" t="s">
-        <v>605</v>
+        <v>580</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -6158,10 +6199,10 @@
         <v>195</v>
       </c>
       <c r="C11" t="s">
-        <v>343</v>
+        <v>620</v>
       </c>
       <c r="D11" t="s">
-        <v>606</v>
+        <v>581</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -6181,10 +6222,10 @@
         <v>193</v>
       </c>
       <c r="C12" t="s">
-        <v>342</v>
+        <v>621</v>
       </c>
       <c r="D12" t="s">
-        <v>606</v>
+        <v>581</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -6204,10 +6245,10 @@
         <v>199</v>
       </c>
       <c r="C13" t="s">
-        <v>344</v>
+        <v>622</v>
       </c>
       <c r="D13" t="s">
-        <v>606</v>
+        <v>581</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -6227,10 +6268,10 @@
         <v>200</v>
       </c>
       <c r="C14" t="s">
-        <v>345</v>
+        <v>623</v>
       </c>
       <c r="D14" t="s">
-        <v>606</v>
+        <v>581</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -6250,10 +6291,10 @@
         <v>201</v>
       </c>
       <c r="C15" t="s">
-        <v>346</v>
+        <v>614</v>
       </c>
       <c r="D15" t="s">
-        <v>606</v>
+        <v>581</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -6273,10 +6314,10 @@
         <v>202</v>
       </c>
       <c r="C16" t="s">
-        <v>347</v>
+        <v>624</v>
       </c>
       <c r="D16" t="s">
-        <v>606</v>
+        <v>581</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -6296,10 +6337,10 @@
         <v>203</v>
       </c>
       <c r="C17" t="s">
-        <v>348</v>
+        <v>625</v>
       </c>
       <c r="D17" t="s">
-        <v>606</v>
+        <v>581</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -6319,10 +6360,10 @@
         <v>204</v>
       </c>
       <c r="C18" t="s">
-        <v>349</v>
+        <v>626</v>
       </c>
       <c r="D18" t="s">
-        <v>606</v>
+        <v>581</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -6359,10 +6400,10 @@
         <v>18</v>
       </c>
       <c r="B1" s="67" t="s">
-        <v>357</v>
+        <v>342</v>
       </c>
       <c r="C1" s="67" t="s">
-        <v>358</v>
+        <v>343</v>
       </c>
       <c r="D1" s="67" t="s">
         <v>19</v>
@@ -6407,7 +6448,7 @@
         <v>231</v>
       </c>
       <c r="C4" t="s">
-        <v>552</v>
+        <v>527</v>
       </c>
       <c r="E4" t="s">
         <v>188</v>
@@ -6421,7 +6462,7 @@
         <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>553</v>
+        <v>528</v>
       </c>
       <c r="E5" t="s">
         <v>188</v>
@@ -6449,7 +6490,7 @@
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>554</v>
+        <v>529</v>
       </c>
       <c r="E7" t="s">
         <v>188</v>
@@ -6463,7 +6504,7 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>555</v>
+        <v>530</v>
       </c>
       <c r="E8" t="s">
         <v>188</v>
@@ -6491,7 +6532,7 @@
         <v>155</v>
       </c>
       <c r="C10" t="s">
-        <v>590</v>
+        <v>565</v>
       </c>
       <c r="E10" t="s">
         <v>188</v>
@@ -6505,7 +6546,7 @@
         <v>156</v>
       </c>
       <c r="C11" t="s">
-        <v>591</v>
+        <v>566</v>
       </c>
       <c r="E11" t="s">
         <v>188</v>
@@ -6520,11 +6561,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C59" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C51" sqref="C51"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6587,10 +6628,10 @@
         <v>13</v>
       </c>
       <c r="N1" s="54" t="s">
-        <v>368</v>
+        <v>353</v>
       </c>
       <c r="O1" s="54" t="s">
-        <v>367</v>
+        <v>352</v>
       </c>
       <c r="P1" s="54" t="s">
         <v>14</v>
@@ -7044,10 +7085,10 @@
         <v>326</v>
       </c>
       <c r="C15" s="51" t="s">
-        <v>550</v>
+        <v>525</v>
       </c>
       <c r="D15" s="51" t="s">
-        <v>551</v>
+        <v>526</v>
       </c>
       <c r="E15" s="51" t="s">
         <v>15</v>
@@ -7144,13 +7185,13 @@
         <v>221</v>
       </c>
       <c r="B18" s="51" t="s">
-        <v>481</v>
+        <v>462</v>
       </c>
       <c r="C18" s="51" t="s">
-        <v>480</v>
+        <v>461</v>
       </c>
       <c r="D18" s="51" t="s">
-        <v>482</v>
+        <v>463</v>
       </c>
       <c r="E18" s="51" t="s">
         <v>15</v>
@@ -7309,13 +7350,13 @@
         <v>221</v>
       </c>
       <c r="B23" s="51" t="s">
-        <v>483</v>
+        <v>464</v>
       </c>
       <c r="C23" s="51" t="s">
-        <v>484</v>
+        <v>465</v>
       </c>
       <c r="D23" s="51" t="s">
-        <v>485</v>
+        <v>466</v>
       </c>
       <c r="E23" s="51" t="s">
         <v>50</v>
@@ -7474,7 +7515,7 @@
         <v>278</v>
       </c>
       <c r="D28" s="51" t="s">
-        <v>492</v>
+        <v>473</v>
       </c>
       <c r="E28" s="51" t="s">
         <v>15</v>
@@ -7503,13 +7544,13 @@
         <v>221</v>
       </c>
       <c r="B29" s="51" t="s">
-        <v>486</v>
+        <v>467</v>
       </c>
       <c r="C29" s="51" t="s">
-        <v>487</v>
+        <v>468</v>
       </c>
       <c r="D29" s="51" t="s">
-        <v>488</v>
+        <v>469</v>
       </c>
       <c r="E29" s="51" t="s">
         <v>15</v>
@@ -7536,13 +7577,13 @@
         <v>221</v>
       </c>
       <c r="B30" s="51" t="s">
-        <v>525</v>
+        <v>506</v>
       </c>
       <c r="C30" s="51" t="s">
-        <v>526</v>
+        <v>507</v>
       </c>
       <c r="D30" s="51" t="s">
-        <v>527</v>
+        <v>508</v>
       </c>
       <c r="E30" s="51" t="s">
         <v>15</v>
@@ -7569,13 +7610,13 @@
         <v>221</v>
       </c>
       <c r="B31" s="51" t="s">
-        <v>528</v>
+        <v>509</v>
       </c>
       <c r="C31" s="51" t="s">
-        <v>529</v>
+        <v>510</v>
       </c>
       <c r="D31" s="51" t="s">
-        <v>530</v>
+        <v>511</v>
       </c>
       <c r="E31" s="51" t="s">
         <v>15</v>
@@ -7599,7 +7640,7 @@
     </row>
     <row r="32" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="100" t="s">
-        <v>559</v>
+        <v>534</v>
       </c>
       <c r="B32" s="100" t="s">
         <v>18</v>
@@ -7608,7 +7649,7 @@
         <v>243</v>
       </c>
       <c r="D32" s="100" t="s">
-        <v>569</v>
+        <v>544</v>
       </c>
       <c r="E32" s="100" t="s">
         <v>97</v>
@@ -7630,16 +7671,16 @@
     </row>
     <row r="33" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="100" t="s">
-        <v>559</v>
+        <v>534</v>
       </c>
       <c r="B33" s="100" t="s">
         <v>222</v>
       </c>
       <c r="C33" s="100" t="s">
-        <v>570</v>
+        <v>545</v>
       </c>
       <c r="D33" s="100" t="s">
-        <v>571</v>
+        <v>546</v>
       </c>
       <c r="E33" s="100" t="s">
         <v>97</v>
@@ -7661,16 +7702,16 @@
     </row>
     <row r="34" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="100" t="s">
-        <v>559</v>
+        <v>534</v>
       </c>
       <c r="B34" s="100" t="s">
-        <v>613</v>
+        <v>588</v>
       </c>
       <c r="C34" s="100" t="s">
-        <v>614</v>
+        <v>589</v>
       </c>
       <c r="D34" s="100" t="s">
-        <v>615</v>
+        <v>590</v>
       </c>
       <c r="E34" s="100" t="s">
         <v>15</v>
@@ -7694,7 +7735,7 @@
     </row>
     <row r="35" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="100" t="s">
-        <v>559</v>
+        <v>534</v>
       </c>
       <c r="B35" s="100" t="s">
         <v>227</v>
@@ -7727,7 +7768,7 @@
     </row>
     <row r="36" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="100" t="s">
-        <v>559</v>
+        <v>534</v>
       </c>
       <c r="B36" s="100" t="s">
         <v>228</v>
@@ -7760,16 +7801,16 @@
     </row>
     <row r="37" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="100" t="s">
-        <v>559</v>
+        <v>534</v>
       </c>
       <c r="B37" s="100" t="s">
-        <v>560</v>
+        <v>535</v>
       </c>
       <c r="C37" s="100" t="s">
-        <v>561</v>
+        <v>536</v>
       </c>
       <c r="D37" s="100" t="s">
-        <v>562</v>
+        <v>537</v>
       </c>
       <c r="E37" s="100" t="s">
         <v>15</v>
@@ -7793,16 +7834,16 @@
     </row>
     <row r="38" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="100" t="s">
-        <v>559</v>
+        <v>534</v>
       </c>
       <c r="B38" s="100" t="s">
-        <v>565</v>
+        <v>540</v>
       </c>
       <c r="C38" s="100" t="s">
-        <v>563</v>
+        <v>538</v>
       </c>
       <c r="D38" s="100" t="s">
-        <v>564</v>
+        <v>539</v>
       </c>
       <c r="E38" s="100" t="s">
         <v>97</v>
@@ -7824,7 +7865,7 @@
     </row>
     <row r="39" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="100" t="s">
-        <v>559</v>
+        <v>534</v>
       </c>
       <c r="B39" s="100" t="s">
         <v>205</v>
@@ -7855,7 +7896,7 @@
     </row>
     <row r="40" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="100" t="s">
-        <v>559</v>
+        <v>534</v>
       </c>
       <c r="B40" s="100" t="s">
         <v>231</v>
@@ -7886,7 +7927,7 @@
     </row>
     <row r="41" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="100" t="s">
-        <v>559</v>
+        <v>534</v>
       </c>
       <c r="B41" s="100" t="s">
         <v>19</v>
@@ -7919,7 +7960,7 @@
     </row>
     <row r="42" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="100" t="s">
-        <v>559</v>
+        <v>534</v>
       </c>
       <c r="B42" s="100" t="s">
         <v>45</v>
@@ -7950,7 +7991,7 @@
     </row>
     <row r="43" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="100" t="s">
-        <v>559</v>
+        <v>534</v>
       </c>
       <c r="B43" s="100" t="s">
         <v>0</v>
@@ -7959,7 +8000,7 @@
         <v>236</v>
       </c>
       <c r="D43" s="100" t="s">
-        <v>566</v>
+        <v>541</v>
       </c>
       <c r="E43" s="100" t="s">
         <v>97</v>
@@ -8021,7 +8062,7 @@
         <v>282</v>
       </c>
       <c r="D45" s="50" t="s">
-        <v>366</v>
+        <v>351</v>
       </c>
       <c r="E45" s="50" t="s">
         <v>16</v>
@@ -8046,13 +8087,13 @@
         <v>280</v>
       </c>
       <c r="B46" s="50" t="s">
-        <v>613</v>
+        <v>588</v>
       </c>
       <c r="C46" s="50" t="s">
-        <v>616</v>
+        <v>591</v>
       </c>
       <c r="D46" s="50" t="s">
-        <v>617</v>
+        <v>592</v>
       </c>
       <c r="E46" s="50" t="s">
         <v>15</v>
@@ -8118,7 +8159,7 @@
         <v>286</v>
       </c>
       <c r="D48" s="50" t="s">
-        <v>618</v>
+        <v>593</v>
       </c>
       <c r="E48" s="50" t="s">
         <v>16</v>
@@ -8209,13 +8250,13 @@
         <v>280</v>
       </c>
       <c r="B51" s="50" t="s">
-        <v>486</v>
+        <v>467</v>
       </c>
       <c r="C51" s="50" t="s">
-        <v>487</v>
+        <v>468</v>
       </c>
       <c r="D51" s="50" t="s">
-        <v>488</v>
+        <v>469</v>
       </c>
       <c r="E51" s="50" t="s">
         <v>15</v>
@@ -8442,13 +8483,13 @@
         <v>279</v>
       </c>
       <c r="B58" s="52" t="s">
-        <v>613</v>
+        <v>588</v>
       </c>
       <c r="C58" s="52" t="s">
-        <v>616</v>
+        <v>591</v>
       </c>
       <c r="D58" s="52" t="s">
-        <v>619</v>
+        <v>594</v>
       </c>
       <c r="E58" s="52" t="s">
         <v>15</v>
@@ -8580,7 +8621,7 @@
         <v>298</v>
       </c>
       <c r="D62" s="98" t="s">
-        <v>489</v>
+        <v>470</v>
       </c>
       <c r="E62" s="52" t="s">
         <v>15</v>
@@ -8645,10 +8686,10 @@
         <v>0</v>
       </c>
       <c r="C64" s="52" t="s">
-        <v>490</v>
+        <v>471</v>
       </c>
       <c r="D64" s="52" t="s">
-        <v>523</v>
+        <v>504</v>
       </c>
       <c r="E64" s="52" t="s">
         <v>97</v>
@@ -8743,7 +8784,7 @@
         <v>238</v>
       </c>
       <c r="D67" s="52" t="s">
-        <v>491</v>
+        <v>472</v>
       </c>
       <c r="E67" s="52" t="s">
         <v>50</v>
@@ -8843,10 +8884,10 @@
         <v>326</v>
       </c>
       <c r="C70" s="53" t="s">
-        <v>550</v>
+        <v>525</v>
       </c>
       <c r="D70" s="53" t="s">
-        <v>551</v>
+        <v>526</v>
       </c>
       <c r="E70" s="53" t="s">
         <v>15</v>
@@ -9241,10 +9282,10 @@
         <v>139</v>
       </c>
       <c r="C82" s="44" t="s">
-        <v>412</v>
+        <v>397</v>
       </c>
       <c r="D82" s="63" t="s">
-        <v>413</v>
+        <v>398</v>
       </c>
       <c r="E82" s="63" t="s">
         <v>16</v>
@@ -9271,13 +9312,13 @@
         <v>169</v>
       </c>
       <c r="B83" s="44" t="s">
-        <v>592</v>
+        <v>567</v>
       </c>
       <c r="C83" s="44" t="s">
-        <v>593</v>
+        <v>568</v>
       </c>
       <c r="D83" s="63" t="s">
-        <v>594</v>
+        <v>569</v>
       </c>
       <c r="E83" s="63" t="s">
         <v>15</v>
@@ -9572,10 +9613,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9608,7 +9649,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="39" t="s">
-        <v>597</v>
+        <v>572</v>
       </c>
       <c r="G1" s="39" t="s">
         <v>205</v>
@@ -9629,16 +9670,16 @@
       </c>
       <c r="B2" s="92"/>
       <c r="C2" s="92" t="s">
-        <v>387</v>
+        <v>372</v>
       </c>
       <c r="D2" s="92" t="s">
-        <v>388</v>
+        <v>373</v>
       </c>
       <c r="E2" s="92" t="s">
-        <v>393</v>
+        <v>378</v>
       </c>
       <c r="F2" s="92" t="s">
-        <v>598</v>
+        <v>573</v>
       </c>
       <c r="G2" s="92"/>
       <c r="H2" s="92"/>
@@ -9657,16 +9698,16 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>390</v>
+        <v>375</v>
       </c>
       <c r="D3" t="s">
-        <v>389</v>
+        <v>374</v>
       </c>
       <c r="E3" t="s">
-        <v>396</v>
+        <v>381</v>
       </c>
       <c r="F3" t="s">
-        <v>599</v>
+        <v>574</v>
       </c>
       <c r="I3" t="s">
         <v>188</v>
@@ -9683,16 +9724,16 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>391</v>
+        <v>376</v>
       </c>
       <c r="D4" t="s">
-        <v>392</v>
+        <v>377</v>
       </c>
       <c r="E4" t="s">
-        <v>397</v>
+        <v>382</v>
       </c>
       <c r="F4" t="s">
-        <v>600</v>
+        <v>575</v>
       </c>
       <c r="I4" t="s">
         <v>188</v>
@@ -9709,16 +9750,16 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>400</v>
+        <v>385</v>
       </c>
       <c r="D5" t="s">
-        <v>401</v>
+        <v>386</v>
       </c>
       <c r="E5" t="s">
-        <v>402</v>
+        <v>387</v>
       </c>
       <c r="F5" t="s">
-        <v>601</v>
+        <v>576</v>
       </c>
       <c r="I5" t="s">
         <v>188</v>
@@ -9735,16 +9776,16 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>543</v>
+        <v>518</v>
       </c>
       <c r="D6" t="s">
-        <v>520</v>
+        <v>501</v>
       </c>
       <c r="E6" t="s">
-        <v>544</v>
+        <v>519</v>
       </c>
       <c r="F6" t="s">
-        <v>602</v>
+        <v>577</v>
       </c>
       <c r="I6" t="s">
         <v>188</v>
@@ -9761,16 +9802,16 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>567</v>
+        <v>542</v>
       </c>
       <c r="D7" t="s">
-        <v>394</v>
+        <v>379</v>
       </c>
       <c r="E7" t="s">
-        <v>398</v>
+        <v>383</v>
       </c>
       <c r="F7" t="s">
-        <v>603</v>
+        <v>578</v>
       </c>
       <c r="I7" t="s">
         <v>188</v>
@@ -9787,16 +9828,16 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>568</v>
+        <v>543</v>
       </c>
       <c r="D8" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
       <c r="E8" t="s">
-        <v>399</v>
+        <v>384</v>
       </c>
       <c r="F8" t="s">
-        <v>604</v>
+        <v>579</v>
       </c>
       <c r="I8" t="s">
         <v>188</v>
@@ -9811,16 +9852,16 @@
       </c>
       <c r="B9" s="92"/>
       <c r="C9" s="92" t="s">
-        <v>403</v>
+        <v>388</v>
       </c>
       <c r="D9" s="92" t="s">
-        <v>404</v>
+        <v>389</v>
       </c>
       <c r="E9" s="92" t="s">
-        <v>411</v>
+        <v>396</v>
       </c>
       <c r="F9" s="92" t="s">
-        <v>605</v>
+        <v>580</v>
       </c>
       <c r="G9" s="92"/>
       <c r="H9" s="92"/>
@@ -9839,16 +9880,16 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>405</v>
+        <v>390</v>
       </c>
       <c r="D10" t="s">
-        <v>408</v>
+        <v>393</v>
       </c>
       <c r="E10" t="s">
-        <v>409</v>
+        <v>394</v>
       </c>
       <c r="F10" t="s">
-        <v>603</v>
+        <v>578</v>
       </c>
       <c r="I10" t="s">
         <v>188</v>
@@ -9865,16 +9906,16 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>406</v>
+        <v>391</v>
       </c>
       <c r="D11" t="s">
-        <v>407</v>
+        <v>392</v>
       </c>
       <c r="E11" t="s">
-        <v>410</v>
+        <v>395</v>
       </c>
       <c r="F11" t="s">
-        <v>599</v>
+        <v>574</v>
       </c>
       <c r="I11" t="s">
         <v>188</v>
@@ -9889,16 +9930,16 @@
       </c>
       <c r="B12" s="92"/>
       <c r="C12" s="92" t="s">
-        <v>516</v>
+        <v>497</v>
       </c>
       <c r="D12" s="92" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
       <c r="E12" s="92" t="s">
-        <v>415</v>
+        <v>400</v>
       </c>
       <c r="F12" s="92" t="s">
-        <v>598</v>
+        <v>573</v>
       </c>
       <c r="G12" s="92"/>
       <c r="H12" s="92"/>
@@ -9917,16 +9958,16 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>537</v>
+        <v>606</v>
       </c>
       <c r="D13" t="s">
-        <v>416</v>
+        <v>401</v>
       </c>
       <c r="E13" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="F13" t="s">
-        <v>599</v>
+        <v>574</v>
       </c>
       <c r="I13" t="s">
         <v>188</v>
@@ -9943,16 +9984,16 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>538</v>
+        <v>607</v>
       </c>
       <c r="D14" t="s">
-        <v>417</v>
+        <v>402</v>
       </c>
       <c r="E14" t="s">
-        <v>420</v>
+        <v>405</v>
       </c>
       <c r="F14" t="s">
-        <v>600</v>
+        <v>575</v>
       </c>
       <c r="I14" t="s">
         <v>188</v>
@@ -9969,16 +10010,16 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>539</v>
+        <v>608</v>
       </c>
       <c r="D15" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="E15" t="s">
-        <v>421</v>
+        <v>406</v>
       </c>
       <c r="F15" t="s">
-        <v>601</v>
+        <v>576</v>
       </c>
       <c r="I15" t="s">
         <v>188</v>
@@ -9995,16 +10036,16 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>540</v>
+        <v>609</v>
       </c>
       <c r="D16" t="s">
-        <v>422</v>
+        <v>407</v>
       </c>
       <c r="E16" t="s">
-        <v>422</v>
+        <v>407</v>
       </c>
       <c r="F16" t="s">
-        <v>602</v>
+        <v>577</v>
       </c>
       <c r="I16" t="s">
         <v>188</v>
@@ -10021,16 +10062,16 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>541</v>
+        <v>610</v>
       </c>
       <c r="D17" t="s">
-        <v>423</v>
+        <v>408</v>
       </c>
       <c r="E17" t="s">
-        <v>423</v>
+        <v>408</v>
       </c>
       <c r="F17" t="s">
-        <v>603</v>
+        <v>578</v>
       </c>
       <c r="I17" t="s">
         <v>188</v>
@@ -10047,16 +10088,16 @@
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>542</v>
+        <v>611</v>
       </c>
       <c r="D18" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
       <c r="E18" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
       <c r="F18" t="s">
-        <v>604</v>
+        <v>579</v>
       </c>
       <c r="I18" t="s">
         <v>188</v>
@@ -10071,16 +10112,16 @@
       </c>
       <c r="B19" s="92"/>
       <c r="C19" s="92" t="s">
-        <v>517</v>
+        <v>498</v>
       </c>
       <c r="D19" s="92" t="s">
-        <v>425</v>
+        <v>410</v>
       </c>
       <c r="E19" s="92" t="s">
-        <v>426</v>
+        <v>411</v>
       </c>
       <c r="F19" s="92" t="s">
-        <v>605</v>
+        <v>580</v>
       </c>
       <c r="G19" s="92"/>
       <c r="H19" s="92"/>
@@ -10099,16 +10140,16 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>438</v>
+        <v>602</v>
       </c>
       <c r="D20" t="s">
-        <v>427</v>
+        <v>412</v>
       </c>
       <c r="E20" t="s">
-        <v>427</v>
+        <v>412</v>
       </c>
       <c r="F20" t="s">
-        <v>603</v>
+        <v>578</v>
       </c>
       <c r="I20" t="s">
         <v>188</v>
@@ -10125,16 +10166,16 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>439</v>
+        <v>603</v>
       </c>
       <c r="D21" t="s">
-        <v>428</v>
+        <v>413</v>
       </c>
       <c r="E21" t="s">
-        <v>428</v>
+        <v>413</v>
       </c>
       <c r="F21" t="s">
-        <v>599</v>
+        <v>574</v>
       </c>
       <c r="I21" t="s">
         <v>188</v>
@@ -10151,16 +10192,16 @@
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>440</v>
+        <v>604</v>
       </c>
       <c r="D22" t="s">
-        <v>429</v>
+        <v>414</v>
       </c>
       <c r="E22" t="s">
-        <v>429</v>
+        <v>414</v>
       </c>
       <c r="F22" t="s">
-        <v>598</v>
+        <v>573</v>
       </c>
       <c r="I22" t="s">
         <v>188</v>
@@ -10177,16 +10218,16 @@
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>441</v>
+        <v>605</v>
       </c>
       <c r="D23" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="E23" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="F23" t="s">
-        <v>599</v>
+        <v>574</v>
       </c>
       <c r="I23" t="s">
         <v>188</v>
@@ -10201,16 +10242,16 @@
       </c>
       <c r="B24" s="92"/>
       <c r="C24" s="92" t="s">
-        <v>493</v>
+        <v>474</v>
       </c>
       <c r="D24" s="92" t="s">
-        <v>494</v>
+        <v>475</v>
       </c>
       <c r="E24" s="92" t="s">
-        <v>426</v>
+        <v>411</v>
       </c>
       <c r="F24" s="92" t="s">
-        <v>600</v>
+        <v>575</v>
       </c>
       <c r="G24" s="92"/>
       <c r="H24" s="92"/>
@@ -10229,16 +10270,16 @@
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>556</v>
+        <v>531</v>
       </c>
       <c r="D25" t="s">
-        <v>557</v>
+        <v>532</v>
       </c>
       <c r="E25" t="s">
-        <v>558</v>
+        <v>533</v>
       </c>
       <c r="F25" t="s">
-        <v>601</v>
+        <v>576</v>
       </c>
       <c r="I25" t="s">
         <v>188</v>
@@ -10255,16 +10296,16 @@
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>495</v>
+        <v>476</v>
       </c>
       <c r="D26" t="s">
-        <v>501</v>
+        <v>482</v>
       </c>
       <c r="E26" t="s">
-        <v>496</v>
+        <v>477</v>
       </c>
       <c r="F26" t="s">
-        <v>602</v>
+        <v>577</v>
       </c>
       <c r="I26" t="s">
         <v>188</v>
@@ -10281,16 +10322,16 @@
         <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>497</v>
+        <v>478</v>
       </c>
       <c r="D27" t="s">
-        <v>502</v>
+        <v>483</v>
       </c>
       <c r="E27" t="s">
-        <v>498</v>
+        <v>479</v>
       </c>
       <c r="F27" t="s">
-        <v>603</v>
+        <v>578</v>
       </c>
       <c r="I27" t="s">
         <v>188</v>
@@ -10307,16 +10348,16 @@
         <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>499</v>
+        <v>480</v>
       </c>
       <c r="D28" t="s">
-        <v>503</v>
+        <v>484</v>
       </c>
       <c r="E28" t="s">
-        <v>500</v>
+        <v>481</v>
       </c>
       <c r="F28" t="s">
-        <v>604</v>
+        <v>579</v>
       </c>
       <c r="I28" t="s">
         <v>188</v>
@@ -10333,16 +10374,16 @@
         <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>504</v>
+        <v>485</v>
       </c>
       <c r="D29" t="s">
-        <v>505</v>
+        <v>486</v>
       </c>
       <c r="E29" t="s">
-        <v>506</v>
+        <v>487</v>
       </c>
       <c r="F29" t="s">
-        <v>605</v>
+        <v>580</v>
       </c>
       <c r="I29" t="s">
         <v>188</v>
@@ -10359,16 +10400,16 @@
         <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>507</v>
+        <v>488</v>
       </c>
       <c r="D30" t="s">
-        <v>508</v>
+        <v>489</v>
       </c>
       <c r="E30" t="s">
-        <v>509</v>
+        <v>490</v>
       </c>
       <c r="F30" t="s">
-        <v>603</v>
+        <v>578</v>
       </c>
       <c r="I30" t="s">
         <v>188</v>
@@ -10385,16 +10426,16 @@
         <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>510</v>
+        <v>491</v>
       </c>
       <c r="D31" t="s">
-        <v>511</v>
+        <v>492</v>
       </c>
       <c r="E31" t="s">
-        <v>512</v>
+        <v>493</v>
       </c>
       <c r="F31" t="s">
-        <v>599</v>
+        <v>574</v>
       </c>
       <c r="I31" t="s">
         <v>188</v>
@@ -10411,16 +10452,16 @@
         <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>515</v>
+        <v>496</v>
       </c>
       <c r="D32" t="s">
-        <v>514</v>
+        <v>495</v>
       </c>
       <c r="E32" t="s">
-        <v>513</v>
+        <v>494</v>
       </c>
       <c r="F32" t="s">
-        <v>606</v>
+        <v>581</v>
       </c>
       <c r="I32" s="99" t="s">
         <v>188</v>
@@ -10437,16 +10478,16 @@
         <v>5</v>
       </c>
       <c r="C33" t="s">
+        <v>505</v>
+      </c>
+      <c r="D33" t="s">
+        <v>523</v>
+      </c>
+      <c r="E33" t="s">
         <v>524</v>
       </c>
-      <c r="D33" t="s">
-        <v>548</v>
-      </c>
-      <c r="E33" t="s">
-        <v>549</v>
-      </c>
       <c r="F33" t="s">
-        <v>607</v>
+        <v>582</v>
       </c>
       <c r="I33" s="99" t="s">
         <v>188</v>
@@ -10463,16 +10504,16 @@
         <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>545</v>
+        <v>520</v>
       </c>
       <c r="D34" t="s">
-        <v>546</v>
+        <v>521</v>
       </c>
       <c r="E34" t="s">
-        <v>547</v>
+        <v>522</v>
       </c>
       <c r="F34" t="s">
-        <v>608</v>
+        <v>583</v>
       </c>
       <c r="I34" s="99" t="s">
         <v>188</v>
@@ -10489,16 +10530,16 @@
         <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>531</v>
+        <v>512</v>
       </c>
       <c r="D35" t="s">
-        <v>532</v>
+        <v>513</v>
       </c>
       <c r="E35" t="s">
-        <v>533</v>
+        <v>514</v>
       </c>
       <c r="F35" t="s">
-        <v>609</v>
+        <v>584</v>
       </c>
       <c r="I35" s="99" t="s">
         <v>188</v>
@@ -10515,16 +10556,16 @@
         <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>518</v>
+        <v>499</v>
       </c>
       <c r="D36" t="s">
-        <v>520</v>
+        <v>501</v>
       </c>
       <c r="E36" t="s">
-        <v>521</v>
+        <v>502</v>
       </c>
       <c r="F36" t="s">
-        <v>610</v>
+        <v>585</v>
       </c>
       <c r="I36" s="99" t="s">
         <v>188</v>
@@ -10541,16 +10582,16 @@
         <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>519</v>
+        <v>500</v>
       </c>
       <c r="D37" t="s">
-        <v>401</v>
+        <v>386</v>
       </c>
       <c r="E37" t="s">
-        <v>522</v>
+        <v>503</v>
       </c>
       <c r="F37" t="s">
-        <v>611</v>
+        <v>586</v>
       </c>
       <c r="I37" s="99" t="s">
         <v>188</v>
@@ -10567,21 +10608,151 @@
         <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>534</v>
+        <v>515</v>
       </c>
       <c r="D38" t="s">
-        <v>535</v>
+        <v>516</v>
       </c>
       <c r="E38" t="s">
-        <v>536</v>
+        <v>517</v>
       </c>
       <c r="F38" t="s">
-        <v>612</v>
+        <v>587</v>
       </c>
       <c r="I38" s="99" t="s">
         <v>188</v>
       </c>
       <c r="J38" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="92">
+        <v>6</v>
+      </c>
+      <c r="B39" s="92"/>
+      <c r="C39" s="92" t="s">
+        <v>627</v>
+      </c>
+      <c r="D39" s="92" t="s">
+        <v>628</v>
+      </c>
+      <c r="E39" s="92" t="s">
+        <v>629</v>
+      </c>
+      <c r="F39" s="92" t="s">
+        <v>575</v>
+      </c>
+      <c r="G39" s="92"/>
+      <c r="H39" s="92"/>
+      <c r="I39" s="92" t="s">
+        <v>188</v>
+      </c>
+      <c r="J39" s="92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>61</v>
+      </c>
+      <c r="B40">
+        <v>6</v>
+      </c>
+      <c r="C40" t="s">
+        <v>630</v>
+      </c>
+      <c r="D40" t="s">
+        <v>631</v>
+      </c>
+      <c r="E40" t="s">
+        <v>636</v>
+      </c>
+      <c r="F40" t="s">
+        <v>585</v>
+      </c>
+      <c r="I40" s="99" t="s">
+        <v>188</v>
+      </c>
+      <c r="J40" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>62</v>
+      </c>
+      <c r="B41">
+        <v>6</v>
+      </c>
+      <c r="C41" t="s">
+        <v>632</v>
+      </c>
+      <c r="D41" t="s">
+        <v>634</v>
+      </c>
+      <c r="E41" t="s">
+        <v>637</v>
+      </c>
+      <c r="F41" t="s">
+        <v>586</v>
+      </c>
+      <c r="I41" s="99" t="s">
+        <v>188</v>
+      </c>
+      <c r="J41" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>63</v>
+      </c>
+      <c r="B42">
+        <v>6</v>
+      </c>
+      <c r="C42" t="s">
+        <v>633</v>
+      </c>
+      <c r="D42" t="s">
+        <v>635</v>
+      </c>
+      <c r="E42" t="s">
+        <v>638</v>
+      </c>
+      <c r="F42" t="s">
+        <v>587</v>
+      </c>
+      <c r="I42" s="99" t="s">
+        <v>188</v>
+      </c>
+      <c r="J42" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>64</v>
+      </c>
+      <c r="B43">
+        <v>6</v>
+      </c>
+      <c r="C43" t="s">
+        <v>627</v>
+      </c>
+      <c r="D43" t="s">
+        <v>628</v>
+      </c>
+      <c r="E43" t="s">
+        <v>639</v>
+      </c>
+      <c r="F43" t="s">
+        <v>584</v>
+      </c>
+      <c r="I43" s="99" t="s">
+        <v>188</v>
+      </c>
+      <c r="J43" s="99">
         <v>1</v>
       </c>
     </row>
@@ -10599,7 +10770,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10682,10 +10853,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10693,17 +10864,18 @@
     <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="61" customWidth="1"/>
     <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="66" t="s">
         <v>18</v>
       </c>
@@ -10714,118 +10886,130 @@
         <v>169</v>
       </c>
       <c r="D1" s="66" t="s">
+        <v>462</v>
+      </c>
+      <c r="E1" s="66" t="s">
         <v>227</v>
       </c>
-      <c r="E1" s="66" t="s">
+      <c r="F1" s="66" t="s">
         <v>228</v>
       </c>
-      <c r="F1" s="66" t="s">
+      <c r="G1" s="66" t="s">
         <v>186</v>
       </c>
-      <c r="G1" s="66" t="s">
+      <c r="H1" s="66" t="s">
         <v>217</v>
       </c>
-      <c r="H1" s="66" t="s">
+      <c r="I1" s="66" t="s">
         <v>205</v>
       </c>
-      <c r="I1" s="66" t="s">
+      <c r="J1" s="66" t="s">
         <v>231</v>
       </c>
-      <c r="J1" s="66" t="s">
+      <c r="K1" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="66" t="s">
+      <c r="L1" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="66" t="s">
+      <c r="M1" s="66" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="41">
         <v>1</v>
       </c>
       <c r="B2" s="93" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="C2" s="41">
         <v>31</v>
       </c>
-      <c r="D2" s="41" t="s">
-        <v>433</v>
+      <c r="D2" s="41">
+        <v>61</v>
       </c>
       <c r="E2" s="41" t="s">
-        <v>433</v>
-      </c>
-      <c r="F2" s="41"/>
+        <v>418</v>
+      </c>
+      <c r="F2" s="41" t="s">
+        <v>418</v>
+      </c>
       <c r="G2" s="41"/>
       <c r="H2" s="41"/>
-      <c r="I2" s="41" t="s">
+      <c r="I2" s="41"/>
+      <c r="J2" s="41" t="s">
         <v>188</v>
       </c>
-      <c r="J2" s="41"/>
       <c r="K2" s="41"/>
-      <c r="L2" s="41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="L2" s="41"/>
+      <c r="M2" s="41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="41">
         <v>2</v>
       </c>
       <c r="B3" s="93" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="C3" s="41">
         <v>31</v>
       </c>
-      <c r="D3" s="41" t="s">
-        <v>436</v>
+      <c r="D3" s="41">
+        <v>61</v>
       </c>
       <c r="E3" s="41" t="s">
-        <v>436</v>
-      </c>
-      <c r="F3" s="41"/>
+        <v>421</v>
+      </c>
+      <c r="F3" s="41" t="s">
+        <v>421</v>
+      </c>
       <c r="G3" s="41"/>
       <c r="H3" s="41"/>
-      <c r="I3" s="41" t="s">
+      <c r="I3" s="41"/>
+      <c r="J3" s="41" t="s">
         <v>188</v>
       </c>
-      <c r="J3" s="41"/>
       <c r="K3" s="41"/>
-      <c r="L3" s="41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="L3" s="41"/>
+      <c r="M3" s="41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="41">
         <v>3</v>
       </c>
       <c r="B4" s="93" t="s">
-        <v>434</v>
+        <v>419</v>
       </c>
       <c r="C4" s="41">
         <v>31</v>
       </c>
-      <c r="D4" s="41" t="s">
-        <v>435</v>
+      <c r="D4" s="41">
+        <v>61</v>
       </c>
       <c r="E4" s="41" t="s">
-        <v>435</v>
-      </c>
-      <c r="F4" s="41"/>
+        <v>420</v>
+      </c>
+      <c r="F4" s="41" t="s">
+        <v>420</v>
+      </c>
       <c r="G4" s="41"/>
       <c r="H4" s="41"/>
-      <c r="I4" s="41" t="s">
+      <c r="I4" s="41"/>
+      <c r="J4" s="41" t="s">
         <v>188</v>
       </c>
-      <c r="J4" s="41"/>
       <c r="K4" s="41"/>
-      <c r="L4" s="41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L4" s="41"/>
+      <c r="M4" s="41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="41"/>
       <c r="B5" s="41"/>
       <c r="C5" s="41"/>
@@ -10838,8 +11022,9 @@
       <c r="J5" s="41"/>
       <c r="K5" s="41"/>
       <c r="L5" s="41"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M5" s="41"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="41"/>
       <c r="B6" s="41"/>
       <c r="C6" s="41"/>
@@ -10852,6 +11037,7 @@
       <c r="J6" s="41"/>
       <c r="K6" s="41"/>
       <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11083,7 +11269,7 @@
         <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>437</v>
+        <v>422</v>
       </c>
     </row>
   </sheetData>
@@ -11164,10 +11350,10 @@
         <v>13</v>
       </c>
       <c r="N1" s="75" t="s">
-        <v>368</v>
+        <v>353</v>
       </c>
       <c r="O1" s="75" t="s">
-        <v>367</v>
+        <v>352</v>
       </c>
       <c r="P1" s="20" t="s">
         <v>14</v>
@@ -11658,11 +11844,11 @@
         <v>38</v>
       </c>
       <c r="B18" s="79" t="s">
-        <v>469</v>
+        <v>450</v>
       </c>
       <c r="C18" s="79"/>
       <c r="D18" s="79" t="s">
-        <v>475</v>
+        <v>456</v>
       </c>
       <c r="E18" s="81" t="s">
         <v>15</v>
@@ -11776,7 +11962,7 @@
       </c>
       <c r="C22" s="79"/>
       <c r="D22" s="79" t="s">
-        <v>362</v>
+        <v>347</v>
       </c>
       <c r="E22" s="81" t="s">
         <v>15</v>
@@ -11868,11 +12054,11 @@
         <v>46</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>363</v>
+        <v>348</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4" t="s">
-        <v>364</v>
+        <v>349</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>16</v>
@@ -11956,11 +12142,11 @@
         <v>46</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>469</v>
+        <v>450</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4" t="s">
-        <v>582</v>
+        <v>557</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>15</v>
@@ -12320,7 +12506,7 @@
       </c>
       <c r="C40" s="79"/>
       <c r="D40" s="79" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="E40" s="79" t="s">
         <v>15</v>
@@ -12498,7 +12684,7 @@
       </c>
       <c r="C46" s="79"/>
       <c r="D46" s="79" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
       <c r="E46" s="79" t="s">
         <v>50</v>
@@ -12526,7 +12712,7 @@
       </c>
       <c r="C47" s="79"/>
       <c r="D47" s="79" t="s">
-        <v>355</v>
+        <v>340</v>
       </c>
       <c r="E47" s="79" t="s">
         <v>15</v>
@@ -12556,7 +12742,7 @@
       </c>
       <c r="C48" s="79"/>
       <c r="D48" s="79" t="s">
-        <v>476</v>
+        <v>457</v>
       </c>
       <c r="E48" s="79" t="s">
         <v>17</v>
@@ -12654,7 +12840,7 @@
       </c>
       <c r="C51" s="42"/>
       <c r="D51" s="43" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="E51" s="42" t="s">
         <v>15</v>
@@ -12685,7 +12871,7 @@
       </c>
       <c r="C52" s="42"/>
       <c r="D52" s="43" t="s">
-        <v>353</v>
+        <v>338</v>
       </c>
       <c r="E52" s="42" t="s">
         <v>15</v>
@@ -12858,14 +13044,14 @@
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" s="68" t="s">
-        <v>356</v>
+        <v>341</v>
       </c>
       <c r="B58" s="68" t="s">
         <v>18</v>
       </c>
       <c r="C58" s="68"/>
       <c r="D58" s="72" t="s">
-        <v>581</v>
+        <v>556</v>
       </c>
       <c r="E58" s="68" t="s">
         <v>16</v>
@@ -12894,14 +13080,14 @@
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" s="68" t="s">
-        <v>356</v>
+        <v>341</v>
       </c>
       <c r="B59" s="68" t="s">
-        <v>357</v>
+        <v>342</v>
       </c>
       <c r="C59" s="68"/>
       <c r="D59" s="72" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="E59" s="68" t="s">
         <v>15</v>
@@ -12930,14 +13116,14 @@
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" s="68" t="s">
-        <v>356</v>
+        <v>341</v>
       </c>
       <c r="B60" s="68" t="s">
-        <v>358</v>
+        <v>343</v>
       </c>
       <c r="C60" s="68"/>
       <c r="D60" s="72" t="s">
-        <v>360</v>
+        <v>345</v>
       </c>
       <c r="E60" s="68" t="s">
         <v>15</v>
@@ -12960,14 +13146,14 @@
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" s="68" t="s">
-        <v>356</v>
+        <v>341</v>
       </c>
       <c r="B61" s="68" t="s">
         <v>19</v>
       </c>
       <c r="C61" s="68"/>
       <c r="D61" s="72" t="s">
-        <v>361</v>
+        <v>346</v>
       </c>
       <c r="E61" s="72" t="s">
         <v>50</v>
@@ -12988,14 +13174,14 @@
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" s="68" t="s">
-        <v>356</v>
+        <v>341</v>
       </c>
       <c r="B62" s="68" t="s">
         <v>45</v>
       </c>
       <c r="C62" s="68"/>
       <c r="D62" s="72" t="s">
-        <v>362</v>
+        <v>347</v>
       </c>
       <c r="E62" s="72" t="s">
         <v>15</v>
@@ -14019,7 +14205,7 @@
         <v>53</v>
       </c>
       <c r="E26" s="70" t="s">
-        <v>575</v>
+        <v>550</v>
       </c>
       <c r="F26" s="68">
         <v>1</v>
@@ -14053,7 +14239,7 @@
         <v>53</v>
       </c>
       <c r="E27" s="70" t="s">
-        <v>576</v>
+        <v>551</v>
       </c>
       <c r="F27" s="68">
         <v>1</v>
@@ -14087,7 +14273,7 @@
         <v>53</v>
       </c>
       <c r="E28" s="70" t="s">
-        <v>577</v>
+        <v>552</v>
       </c>
       <c r="F28" s="68">
         <v>1</v>
@@ -14121,7 +14307,7 @@
         <v>53</v>
       </c>
       <c r="E29" s="70" t="s">
-        <v>578</v>
+        <v>553</v>
       </c>
       <c r="F29" s="68">
         <v>1</v>
@@ -14155,7 +14341,7 @@
         <v>53</v>
       </c>
       <c r="E30" s="70" t="s">
-        <v>579</v>
+        <v>554</v>
       </c>
       <c r="F30" s="68">
         <v>1</v>
@@ -14189,7 +14375,7 @@
         <v>53</v>
       </c>
       <c r="E31" s="70" t="s">
-        <v>580</v>
+        <v>555</v>
       </c>
       <c r="F31" s="68">
         <v>1</v>
@@ -14821,7 +15007,7 @@
         <v>168</v>
       </c>
       <c r="E50" s="109" t="s">
-        <v>572</v>
+        <v>547</v>
       </c>
       <c r="F50" s="108">
         <v>1</v>
@@ -14854,7 +15040,7 @@
         <v>168</v>
       </c>
       <c r="E51" s="103" t="s">
-        <v>622</v>
+        <v>597</v>
       </c>
       <c r="F51" s="102">
         <v>1</v>
@@ -14887,7 +15073,7 @@
         <v>168</v>
       </c>
       <c r="E52" s="103" t="s">
-        <v>623</v>
+        <v>598</v>
       </c>
       <c r="F52" s="102">
         <v>1</v>
@@ -14920,7 +15106,7 @@
         <v>168</v>
       </c>
       <c r="E53" s="103" t="s">
-        <v>621</v>
+        <v>596</v>
       </c>
       <c r="F53" s="102">
         <v>1</v>
@@ -14953,7 +15139,7 @@
         <v>168</v>
       </c>
       <c r="E54" s="103" t="s">
-        <v>624</v>
+        <v>599</v>
       </c>
       <c r="F54" s="102">
         <v>1</v>
@@ -14986,7 +15172,7 @@
         <v>168</v>
       </c>
       <c r="E55" s="103" t="s">
-        <v>625</v>
+        <v>600</v>
       </c>
       <c r="F55" s="102">
         <v>1</v>
@@ -15019,7 +15205,7 @@
         <v>168</v>
       </c>
       <c r="E56" s="103" t="s">
-        <v>620</v>
+        <v>595</v>
       </c>
       <c r="F56" s="102">
         <v>1</v>
@@ -15052,7 +15238,7 @@
         <v>168</v>
       </c>
       <c r="E57" s="103" t="s">
-        <v>626</v>
+        <v>601</v>
       </c>
       <c r="F57" s="102">
         <v>1</v>

</xml_diff>

<commit_message>
add display direct info card on meeting detail
</commit_message>
<xml_diff>
--- a/db/excel/api-function-granted-users-cdld.xlsx
+++ b/db/excel/api-function-granted-users-cdld.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10613"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0FBA5D4-DC62-5A40-A5C7-03D901824460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CACCC694-E6DC-9E45-B718-D934190C698F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" tabRatio="800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="38400" windowHeight="20060" tabRatio="800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_types" sheetId="27" r:id="rId1"/>
@@ -3456,7 +3456,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -3693,9 +3693,6 @@
     <xf numFmtId="0" fontId="19" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3732,6 +3729,33 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="829">
@@ -5284,7 +5308,7 @@
       <c r="J2" s="90"/>
       <c r="K2" s="90"/>
       <c r="L2" s="90"/>
-      <c r="M2" s="106" t="s">
+      <c r="M2" s="105" t="s">
         <v>188</v>
       </c>
       <c r="N2" s="90">
@@ -5316,7 +5340,7 @@
       <c r="J3" s="86"/>
       <c r="K3" s="86"/>
       <c r="L3" s="86"/>
-      <c r="M3" s="107" t="s">
+      <c r="M3" s="106" t="s">
         <v>188</v>
       </c>
       <c r="N3" s="86">
@@ -5348,7 +5372,7 @@
       <c r="J4" s="86"/>
       <c r="K4" s="86"/>
       <c r="L4" s="86"/>
-      <c r="M4" s="107" t="s">
+      <c r="M4" s="106" t="s">
         <v>188</v>
       </c>
       <c r="N4" s="86">
@@ -5380,7 +5404,7 @@
       <c r="J5" s="86"/>
       <c r="K5" s="86"/>
       <c r="L5" s="86"/>
-      <c r="M5" s="107" t="s">
+      <c r="M5" s="106" t="s">
         <v>188</v>
       </c>
       <c r="N5" s="86">
@@ -5412,7 +5436,7 @@
       <c r="J6" s="86"/>
       <c r="K6" s="86"/>
       <c r="L6" s="86"/>
-      <c r="M6" s="107" t="s">
+      <c r="M6" s="106" t="s">
         <v>188</v>
       </c>
       <c r="N6" s="86">
@@ -5444,7 +5468,7 @@
       <c r="J7" s="86"/>
       <c r="K7" s="86"/>
       <c r="L7" s="86"/>
-      <c r="M7" s="107" t="s">
+      <c r="M7" s="106" t="s">
         <v>188</v>
       </c>
       <c r="N7" s="86">
@@ -5476,7 +5500,7 @@
       <c r="J8" s="86"/>
       <c r="K8" s="86"/>
       <c r="L8" s="86"/>
-      <c r="M8" s="107" t="s">
+      <c r="M8" s="106" t="s">
         <v>188</v>
       </c>
       <c r="N8" s="86">
@@ -5510,7 +5534,7 @@
       <c r="J9" s="90"/>
       <c r="K9" s="90"/>
       <c r="L9" s="90"/>
-      <c r="M9" s="106" t="s">
+      <c r="M9" s="105" t="s">
         <v>188</v>
       </c>
       <c r="N9" s="90">
@@ -5542,7 +5566,7 @@
       <c r="J10" s="88"/>
       <c r="K10" s="86"/>
       <c r="L10" s="86"/>
-      <c r="M10" s="107" t="s">
+      <c r="M10" s="106" t="s">
         <v>188</v>
       </c>
       <c r="N10" s="86">
@@ -5574,7 +5598,7 @@
       <c r="J11" s="86"/>
       <c r="K11" s="86"/>
       <c r="L11" s="86"/>
-      <c r="M11" s="107" t="s">
+      <c r="M11" s="106" t="s">
         <v>188</v>
       </c>
       <c r="N11" s="86">
@@ -5606,7 +5630,7 @@
       <c r="J12" s="86"/>
       <c r="K12" s="86"/>
       <c r="L12" s="86"/>
-      <c r="M12" s="107" t="s">
+      <c r="M12" s="106" t="s">
         <v>188</v>
       </c>
       <c r="N12" s="86">
@@ -5638,7 +5662,7 @@
       <c r="J13" s="86"/>
       <c r="K13" s="86"/>
       <c r="L13" s="86"/>
-      <c r="M13" s="107" t="s">
+      <c r="M13" s="106" t="s">
         <v>188</v>
       </c>
       <c r="N13" s="86">
@@ -5672,7 +5696,7 @@
       <c r="J14" s="90"/>
       <c r="K14" s="90"/>
       <c r="L14" s="90"/>
-      <c r="M14" s="106" t="s">
+      <c r="M14" s="105" t="s">
         <v>188</v>
       </c>
       <c r="N14" s="90">
@@ -5704,7 +5728,7 @@
       <c r="J15" s="88"/>
       <c r="K15" s="86"/>
       <c r="L15" s="86"/>
-      <c r="M15" s="107" t="s">
+      <c r="M15" s="106" t="s">
         <v>188</v>
       </c>
       <c r="N15" s="86">
@@ -5736,7 +5760,7 @@
       <c r="J16" s="90"/>
       <c r="K16" s="90"/>
       <c r="L16" s="90"/>
-      <c r="M16" s="106" t="s">
+      <c r="M16" s="105" t="s">
         <v>188</v>
       </c>
       <c r="N16" s="90">
@@ -6561,11 +6585,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q91"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomRight" activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6744,24 +6768,22 @@
       <c r="Q4" s="57"/>
     </row>
     <row r="5" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="111" t="s">
         <v>257</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="111" t="s">
         <v>297</v>
       </c>
-      <c r="C5" s="50" t="s">
+      <c r="C5" s="111" t="s">
         <v>262</v>
       </c>
-      <c r="D5" s="50" t="s">
+      <c r="D5" s="111" t="s">
         <v>263</v>
       </c>
-      <c r="E5" s="50" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="55">
-        <v>255</v>
-      </c>
+      <c r="E5" s="111" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="112"/>
       <c r="G5" s="55"/>
       <c r="H5" s="55"/>
       <c r="I5" s="55"/>
@@ -7148,24 +7170,22 @@
       <c r="Q16" s="57"/>
     </row>
     <row r="17" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="51" t="s">
+      <c r="A17" s="113" t="s">
         <v>221</v>
       </c>
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="113" t="s">
         <v>297</v>
       </c>
-      <c r="C17" s="51" t="s">
+      <c r="C17" s="113" t="s">
         <v>252</v>
       </c>
-      <c r="D17" s="51" t="s">
+      <c r="D17" s="113" t="s">
         <v>253</v>
       </c>
-      <c r="E17" s="51" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="58">
-        <v>255</v>
-      </c>
+      <c r="E17" s="113" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="114"/>
       <c r="G17" s="58"/>
       <c r="H17" s="58"/>
       <c r="I17" s="58"/>
@@ -7639,382 +7659,382 @@
       <c r="Q31" s="57"/>
     </row>
     <row r="32" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="100" t="s">
+      <c r="A32" s="99" t="s">
         <v>534</v>
       </c>
-      <c r="B32" s="100" t="s">
+      <c r="B32" s="99" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="100" t="s">
+      <c r="C32" s="99" t="s">
         <v>243</v>
       </c>
-      <c r="D32" s="100" t="s">
+      <c r="D32" s="99" t="s">
         <v>544</v>
       </c>
-      <c r="E32" s="100" t="s">
+      <c r="E32" s="99" t="s">
         <v>97</v>
       </c>
-      <c r="F32" s="101"/>
-      <c r="G32" s="101"/>
-      <c r="H32" s="101"/>
-      <c r="I32" s="101"/>
-      <c r="J32" s="101"/>
-      <c r="K32" s="101"/>
-      <c r="L32" s="101"/>
-      <c r="M32" s="101"/>
-      <c r="N32" s="101"/>
-      <c r="O32" s="101"/>
+      <c r="F32" s="100"/>
+      <c r="G32" s="100"/>
+      <c r="H32" s="100"/>
+      <c r="I32" s="100"/>
+      <c r="J32" s="100"/>
+      <c r="K32" s="100"/>
+      <c r="L32" s="100"/>
+      <c r="M32" s="100"/>
+      <c r="N32" s="100"/>
+      <c r="O32" s="100"/>
       <c r="P32" s="56">
         <v>31</v>
       </c>
       <c r="Q32" s="57"/>
     </row>
     <row r="33" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="100" t="s">
+      <c r="A33" s="99" t="s">
         <v>534</v>
       </c>
-      <c r="B33" s="100" t="s">
+      <c r="B33" s="99" t="s">
         <v>222</v>
       </c>
-      <c r="C33" s="100" t="s">
+      <c r="C33" s="99" t="s">
         <v>545</v>
       </c>
-      <c r="D33" s="100" t="s">
+      <c r="D33" s="99" t="s">
         <v>546</v>
       </c>
-      <c r="E33" s="100" t="s">
+      <c r="E33" s="99" t="s">
         <v>97</v>
       </c>
-      <c r="F33" s="101"/>
-      <c r="G33" s="101"/>
-      <c r="H33" s="101"/>
-      <c r="I33" s="101"/>
-      <c r="J33" s="101"/>
-      <c r="K33" s="101"/>
-      <c r="L33" s="101"/>
-      <c r="M33" s="101"/>
-      <c r="N33" s="101"/>
-      <c r="O33" s="101"/>
+      <c r="F33" s="100"/>
+      <c r="G33" s="100"/>
+      <c r="H33" s="100"/>
+      <c r="I33" s="100"/>
+      <c r="J33" s="100"/>
+      <c r="K33" s="100"/>
+      <c r="L33" s="100"/>
+      <c r="M33" s="100"/>
+      <c r="N33" s="100"/>
+      <c r="O33" s="100"/>
       <c r="P33" s="56">
         <v>32</v>
       </c>
       <c r="Q33" s="57"/>
     </row>
     <row r="34" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="100" t="s">
+      <c r="A34" s="99" t="s">
         <v>534</v>
       </c>
-      <c r="B34" s="100" t="s">
+      <c r="B34" s="99" t="s">
         <v>588</v>
       </c>
-      <c r="C34" s="100" t="s">
+      <c r="C34" s="99" t="s">
         <v>589</v>
       </c>
-      <c r="D34" s="100" t="s">
+      <c r="D34" s="99" t="s">
         <v>590</v>
       </c>
-      <c r="E34" s="100" t="s">
+      <c r="E34" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="F34" s="101">
+      <c r="F34" s="100">
         <v>50</v>
       </c>
-      <c r="G34" s="101"/>
-      <c r="H34" s="101"/>
-      <c r="I34" s="101"/>
-      <c r="J34" s="101"/>
-      <c r="K34" s="101"/>
-      <c r="L34" s="101"/>
-      <c r="M34" s="101"/>
-      <c r="N34" s="101"/>
-      <c r="O34" s="101"/>
+      <c r="G34" s="100"/>
+      <c r="H34" s="100"/>
+      <c r="I34" s="100"/>
+      <c r="J34" s="100"/>
+      <c r="K34" s="100"/>
+      <c r="L34" s="100"/>
+      <c r="M34" s="100"/>
+      <c r="N34" s="100"/>
+      <c r="O34" s="100"/>
       <c r="P34" s="56">
         <v>33</v>
       </c>
       <c r="Q34" s="57"/>
     </row>
     <row r="35" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="100" t="s">
+      <c r="A35" s="99" t="s">
         <v>534</v>
       </c>
-      <c r="B35" s="100" t="s">
+      <c r="B35" s="99" t="s">
         <v>227</v>
       </c>
-      <c r="C35" s="100" t="s">
+      <c r="C35" s="99" t="s">
         <v>274</v>
       </c>
-      <c r="D35" s="100" t="s">
+      <c r="D35" s="99" t="s">
         <v>276</v>
       </c>
-      <c r="E35" s="100" t="s">
+      <c r="E35" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="F35" s="101">
+      <c r="F35" s="100">
         <v>500</v>
       </c>
-      <c r="G35" s="101"/>
-      <c r="H35" s="101"/>
-      <c r="I35" s="101"/>
-      <c r="J35" s="101"/>
-      <c r="K35" s="101"/>
-      <c r="L35" s="101"/>
-      <c r="M35" s="101"/>
-      <c r="N35" s="101"/>
-      <c r="O35" s="101"/>
+      <c r="G35" s="100"/>
+      <c r="H35" s="100"/>
+      <c r="I35" s="100"/>
+      <c r="J35" s="100"/>
+      <c r="K35" s="100"/>
+      <c r="L35" s="100"/>
+      <c r="M35" s="100"/>
+      <c r="N35" s="100"/>
+      <c r="O35" s="100"/>
       <c r="P35" s="56">
         <v>34</v>
       </c>
       <c r="Q35" s="57"/>
     </row>
     <row r="36" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="100" t="s">
+      <c r="A36" s="99" t="s">
         <v>534</v>
       </c>
-      <c r="B36" s="100" t="s">
+      <c r="B36" s="99" t="s">
         <v>228</v>
       </c>
-      <c r="C36" s="100" t="s">
+      <c r="C36" s="99" t="s">
         <v>275</v>
       </c>
-      <c r="D36" s="100" t="s">
+      <c r="D36" s="99" t="s">
         <v>277</v>
       </c>
-      <c r="E36" s="100" t="s">
+      <c r="E36" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="F36" s="101">
+      <c r="F36" s="100">
         <v>500</v>
       </c>
-      <c r="G36" s="101"/>
-      <c r="H36" s="101"/>
-      <c r="I36" s="101"/>
-      <c r="J36" s="101"/>
-      <c r="K36" s="101"/>
-      <c r="L36" s="101"/>
-      <c r="M36" s="101"/>
-      <c r="N36" s="101"/>
-      <c r="O36" s="101"/>
+      <c r="G36" s="100"/>
+      <c r="H36" s="100"/>
+      <c r="I36" s="100"/>
+      <c r="J36" s="100"/>
+      <c r="K36" s="100"/>
+      <c r="L36" s="100"/>
+      <c r="M36" s="100"/>
+      <c r="N36" s="100"/>
+      <c r="O36" s="100"/>
       <c r="P36" s="56">
         <v>35</v>
       </c>
       <c r="Q36" s="57"/>
     </row>
     <row r="37" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="100" t="s">
+      <c r="A37" s="99" t="s">
         <v>534</v>
       </c>
-      <c r="B37" s="100" t="s">
+      <c r="B37" s="99" t="s">
         <v>535</v>
       </c>
-      <c r="C37" s="100" t="s">
+      <c r="C37" s="99" t="s">
         <v>536</v>
       </c>
-      <c r="D37" s="100" t="s">
+      <c r="D37" s="99" t="s">
         <v>537</v>
       </c>
-      <c r="E37" s="100" t="s">
+      <c r="E37" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="F37" s="101">
+      <c r="F37" s="100">
         <v>255</v>
       </c>
-      <c r="G37" s="101"/>
-      <c r="H37" s="101"/>
-      <c r="I37" s="101"/>
-      <c r="J37" s="101"/>
-      <c r="K37" s="101"/>
-      <c r="L37" s="101"/>
-      <c r="M37" s="101"/>
-      <c r="N37" s="101"/>
-      <c r="O37" s="101"/>
+      <c r="G37" s="100"/>
+      <c r="H37" s="100"/>
+      <c r="I37" s="100"/>
+      <c r="J37" s="100"/>
+      <c r="K37" s="100"/>
+      <c r="L37" s="100"/>
+      <c r="M37" s="100"/>
+      <c r="N37" s="100"/>
+      <c r="O37" s="100"/>
       <c r="P37" s="56">
         <v>36</v>
       </c>
       <c r="Q37" s="57"/>
     </row>
     <row r="38" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="100" t="s">
+      <c r="A38" s="99" t="s">
         <v>534</v>
       </c>
-      <c r="B38" s="100" t="s">
+      <c r="B38" s="99" t="s">
         <v>540</v>
       </c>
-      <c r="C38" s="100" t="s">
+      <c r="C38" s="99" t="s">
         <v>538</v>
       </c>
-      <c r="D38" s="100" t="s">
+      <c r="D38" s="99" t="s">
         <v>539</v>
       </c>
-      <c r="E38" s="100" t="s">
+      <c r="E38" s="99" t="s">
         <v>97</v>
       </c>
-      <c r="F38" s="101"/>
-      <c r="G38" s="101"/>
-      <c r="H38" s="101"/>
-      <c r="I38" s="101"/>
-      <c r="J38" s="101"/>
-      <c r="K38" s="101"/>
-      <c r="L38" s="101"/>
-      <c r="M38" s="101"/>
-      <c r="N38" s="101"/>
-      <c r="O38" s="101"/>
+      <c r="F38" s="100"/>
+      <c r="G38" s="100"/>
+      <c r="H38" s="100"/>
+      <c r="I38" s="100"/>
+      <c r="J38" s="100"/>
+      <c r="K38" s="100"/>
+      <c r="L38" s="100"/>
+      <c r="M38" s="100"/>
+      <c r="N38" s="100"/>
+      <c r="O38" s="100"/>
       <c r="P38" s="56">
         <v>37</v>
       </c>
       <c r="Q38" s="57"/>
     </row>
     <row r="39" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="100" t="s">
+      <c r="A39" s="99" t="s">
         <v>534</v>
       </c>
-      <c r="B39" s="100" t="s">
+      <c r="B39" s="99" t="s">
         <v>205</v>
       </c>
-      <c r="C39" s="100" t="s">
+      <c r="C39" s="99" t="s">
         <v>237</v>
       </c>
-      <c r="D39" s="100" t="s">
+      <c r="D39" s="99" t="s">
         <v>132</v>
       </c>
-      <c r="E39" s="100" t="s">
+      <c r="E39" s="99" t="s">
         <v>50</v>
       </c>
-      <c r="F39" s="101"/>
-      <c r="G39" s="101"/>
-      <c r="H39" s="101"/>
-      <c r="I39" s="101"/>
-      <c r="J39" s="101"/>
-      <c r="K39" s="101"/>
-      <c r="L39" s="101"/>
-      <c r="M39" s="101"/>
-      <c r="N39" s="101"/>
-      <c r="O39" s="101"/>
+      <c r="F39" s="100"/>
+      <c r="G39" s="100"/>
+      <c r="H39" s="100"/>
+      <c r="I39" s="100"/>
+      <c r="J39" s="100"/>
+      <c r="K39" s="100"/>
+      <c r="L39" s="100"/>
+      <c r="M39" s="100"/>
+      <c r="N39" s="100"/>
+      <c r="O39" s="100"/>
       <c r="P39" s="56">
         <v>38</v>
       </c>
       <c r="Q39" s="57"/>
     </row>
     <row r="40" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="100" t="s">
+      <c r="A40" s="99" t="s">
         <v>534</v>
       </c>
-      <c r="B40" s="100" t="s">
+      <c r="B40" s="99" t="s">
         <v>231</v>
       </c>
-      <c r="C40" s="100" t="s">
+      <c r="C40" s="99" t="s">
         <v>249</v>
       </c>
-      <c r="D40" s="100" t="s">
+      <c r="D40" s="99" t="s">
         <v>296</v>
       </c>
-      <c r="E40" s="100" t="s">
+      <c r="E40" s="99" t="s">
         <v>50</v>
       </c>
-      <c r="F40" s="101"/>
-      <c r="G40" s="101"/>
-      <c r="H40" s="101"/>
-      <c r="I40" s="101"/>
-      <c r="J40" s="101"/>
-      <c r="K40" s="101"/>
-      <c r="L40" s="101"/>
-      <c r="M40" s="101"/>
-      <c r="N40" s="101"/>
-      <c r="O40" s="101"/>
+      <c r="F40" s="100"/>
+      <c r="G40" s="100"/>
+      <c r="H40" s="100"/>
+      <c r="I40" s="100"/>
+      <c r="J40" s="100"/>
+      <c r="K40" s="100"/>
+      <c r="L40" s="100"/>
+      <c r="M40" s="100"/>
+      <c r="N40" s="100"/>
+      <c r="O40" s="100"/>
       <c r="P40" s="56">
         <v>39</v>
       </c>
       <c r="Q40" s="57"/>
     </row>
     <row r="41" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="100" t="s">
+      <c r="A41" s="99" t="s">
         <v>534</v>
       </c>
-      <c r="B41" s="100" t="s">
+      <c r="B41" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="100" t="s">
+      <c r="C41" s="99" t="s">
         <v>238</v>
       </c>
-      <c r="D41" s="100" t="s">
+      <c r="D41" s="99" t="s">
         <v>176</v>
       </c>
-      <c r="E41" s="100" t="s">
+      <c r="E41" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="F41" s="101">
+      <c r="F41" s="100">
         <v>255</v>
       </c>
-      <c r="G41" s="101"/>
-      <c r="H41" s="101"/>
-      <c r="I41" s="101"/>
-      <c r="J41" s="101"/>
-      <c r="K41" s="101"/>
-      <c r="L41" s="101"/>
-      <c r="M41" s="101"/>
-      <c r="N41" s="101"/>
-      <c r="O41" s="101"/>
+      <c r="G41" s="100"/>
+      <c r="H41" s="100"/>
+      <c r="I41" s="100"/>
+      <c r="J41" s="100"/>
+      <c r="K41" s="100"/>
+      <c r="L41" s="100"/>
+      <c r="M41" s="100"/>
+      <c r="N41" s="100"/>
+      <c r="O41" s="100"/>
       <c r="P41" s="56">
         <v>40</v>
       </c>
       <c r="Q41" s="57"/>
     </row>
     <row r="42" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="100" t="s">
+      <c r="A42" s="99" t="s">
         <v>534</v>
       </c>
-      <c r="B42" s="100" t="s">
+      <c r="B42" s="99" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="100" t="s">
+      <c r="C42" s="99" t="s">
         <v>248</v>
       </c>
-      <c r="D42" s="100" t="s">
+      <c r="D42" s="99" t="s">
         <v>177</v>
       </c>
-      <c r="E42" s="100" t="s">
+      <c r="E42" s="99" t="s">
         <v>50</v>
       </c>
-      <c r="F42" s="101"/>
-      <c r="G42" s="101"/>
-      <c r="H42" s="101"/>
-      <c r="I42" s="101"/>
-      <c r="J42" s="101"/>
-      <c r="K42" s="101"/>
-      <c r="L42" s="101"/>
-      <c r="M42" s="101"/>
-      <c r="N42" s="101"/>
-      <c r="O42" s="101"/>
+      <c r="F42" s="100"/>
+      <c r="G42" s="100"/>
+      <c r="H42" s="100"/>
+      <c r="I42" s="100"/>
+      <c r="J42" s="100"/>
+      <c r="K42" s="100"/>
+      <c r="L42" s="100"/>
+      <c r="M42" s="100"/>
+      <c r="N42" s="100"/>
+      <c r="O42" s="100"/>
       <c r="P42" s="56">
         <v>41</v>
       </c>
       <c r="Q42" s="57"/>
     </row>
     <row r="43" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="100" t="s">
+      <c r="A43" s="99" t="s">
         <v>534</v>
       </c>
-      <c r="B43" s="100" t="s">
+      <c r="B43" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="C43" s="100" t="s">
+      <c r="C43" s="99" t="s">
         <v>236</v>
       </c>
-      <c r="D43" s="100" t="s">
+      <c r="D43" s="99" t="s">
         <v>541</v>
       </c>
-      <c r="E43" s="100" t="s">
+      <c r="E43" s="99" t="s">
         <v>97</v>
       </c>
-      <c r="F43" s="101"/>
-      <c r="G43" s="101"/>
-      <c r="H43" s="101"/>
-      <c r="I43" s="101"/>
-      <c r="J43" s="101"/>
-      <c r="K43" s="101"/>
-      <c r="L43" s="101"/>
-      <c r="M43" s="101"/>
-      <c r="N43" s="101"/>
-      <c r="O43" s="101"/>
+      <c r="F43" s="100"/>
+      <c r="G43" s="100"/>
+      <c r="H43" s="100"/>
+      <c r="I43" s="100"/>
+      <c r="J43" s="100"/>
+      <c r="K43" s="100"/>
+      <c r="L43" s="100"/>
+      <c r="M43" s="100"/>
+      <c r="N43" s="100"/>
+      <c r="O43" s="100"/>
       <c r="P43" s="56">
         <v>42</v>
       </c>
@@ -8611,24 +8631,22 @@
       <c r="Q61" s="57"/>
     </row>
     <row r="62" spans="1:17" s="82" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="52" t="s">
+      <c r="A62" s="115" t="s">
         <v>279</v>
       </c>
-      <c r="B62" s="52" t="s">
+      <c r="B62" s="115" t="s">
         <v>297</v>
       </c>
-      <c r="C62" s="52" t="s">
+      <c r="C62" s="115" t="s">
         <v>298</v>
       </c>
-      <c r="D62" s="98" t="s">
+      <c r="D62" s="116" t="s">
         <v>470</v>
       </c>
-      <c r="E62" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="F62" s="46">
-        <v>255</v>
-      </c>
+      <c r="E62" s="115" t="s">
+        <v>16</v>
+      </c>
+      <c r="F62" s="117"/>
       <c r="G62" s="46"/>
       <c r="H62" s="46"/>
       <c r="I62" s="46"/>
@@ -8910,24 +8928,22 @@
       <c r="Q70" s="59"/>
     </row>
     <row r="71" spans="1:17" s="83" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="53" t="s">
+      <c r="A71" s="118" t="s">
         <v>217</v>
       </c>
-      <c r="B71" s="53" t="s">
+      <c r="B71" s="118" t="s">
         <v>297</v>
       </c>
-      <c r="C71" s="53" t="s">
+      <c r="C71" s="118" t="s">
         <v>246</v>
       </c>
-      <c r="D71" s="53" t="s">
+      <c r="D71" s="118" t="s">
         <v>267</v>
       </c>
-      <c r="E71" s="53" t="s">
-        <v>15</v>
-      </c>
-      <c r="F71" s="62">
-        <v>255</v>
-      </c>
+      <c r="E71" s="118" t="s">
+        <v>16</v>
+      </c>
+      <c r="F71" s="119"/>
       <c r="G71" s="62"/>
       <c r="H71" s="62"/>
       <c r="I71" s="62"/>
@@ -9615,7 +9631,7 @@
   </sheetPr>
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -10463,10 +10479,10 @@
       <c r="F32" t="s">
         <v>581</v>
       </c>
-      <c r="I32" s="99" t="s">
+      <c r="I32" s="98" t="s">
         <v>188</v>
       </c>
-      <c r="J32" s="99">
+      <c r="J32" s="98">
         <v>1</v>
       </c>
     </row>
@@ -10489,10 +10505,10 @@
       <c r="F33" t="s">
         <v>582</v>
       </c>
-      <c r="I33" s="99" t="s">
+      <c r="I33" s="98" t="s">
         <v>188</v>
       </c>
-      <c r="J33" s="99">
+      <c r="J33" s="98">
         <v>1</v>
       </c>
     </row>
@@ -10515,10 +10531,10 @@
       <c r="F34" t="s">
         <v>583</v>
       </c>
-      <c r="I34" s="99" t="s">
+      <c r="I34" s="98" t="s">
         <v>188</v>
       </c>
-      <c r="J34" s="99">
+      <c r="J34" s="98">
         <v>1</v>
       </c>
     </row>
@@ -10541,10 +10557,10 @@
       <c r="F35" t="s">
         <v>584</v>
       </c>
-      <c r="I35" s="99" t="s">
+      <c r="I35" s="98" t="s">
         <v>188</v>
       </c>
-      <c r="J35" s="99">
+      <c r="J35" s="98">
         <v>1</v>
       </c>
     </row>
@@ -10567,10 +10583,10 @@
       <c r="F36" t="s">
         <v>585</v>
       </c>
-      <c r="I36" s="99" t="s">
+      <c r="I36" s="98" t="s">
         <v>188</v>
       </c>
-      <c r="J36" s="99">
+      <c r="J36" s="98">
         <v>1</v>
       </c>
     </row>
@@ -10593,10 +10609,10 @@
       <c r="F37" t="s">
         <v>586</v>
       </c>
-      <c r="I37" s="99" t="s">
+      <c r="I37" s="98" t="s">
         <v>188</v>
       </c>
-      <c r="J37" s="99">
+      <c r="J37" s="98">
         <v>1</v>
       </c>
     </row>
@@ -10619,10 +10635,10 @@
       <c r="F38" t="s">
         <v>587</v>
       </c>
-      <c r="I38" s="99" t="s">
+      <c r="I38" s="98" t="s">
         <v>188</v>
       </c>
-      <c r="J38" s="99">
+      <c r="J38" s="98">
         <v>1</v>
       </c>
     </row>
@@ -10671,10 +10687,10 @@
       <c r="F40" t="s">
         <v>585</v>
       </c>
-      <c r="I40" s="99" t="s">
+      <c r="I40" s="98" t="s">
         <v>188</v>
       </c>
-      <c r="J40" s="99">
+      <c r="J40" s="98">
         <v>1</v>
       </c>
     </row>
@@ -10697,10 +10713,10 @@
       <c r="F41" t="s">
         <v>586</v>
       </c>
-      <c r="I41" s="99" t="s">
+      <c r="I41" s="98" t="s">
         <v>188</v>
       </c>
-      <c r="J41" s="99">
+      <c r="J41" s="98">
         <v>1</v>
       </c>
     </row>
@@ -10723,10 +10739,10 @@
       <c r="F42" t="s">
         <v>587</v>
       </c>
-      <c r="I42" s="99" t="s">
+      <c r="I42" s="98" t="s">
         <v>188</v>
       </c>
-      <c r="J42" s="99">
+      <c r="J42" s="98">
         <v>1</v>
       </c>
     </row>
@@ -10749,10 +10765,10 @@
       <c r="F43" t="s">
         <v>584</v>
       </c>
-      <c r="I43" s="99" t="s">
+      <c r="I43" s="98" t="s">
         <v>188</v>
       </c>
-      <c r="J43" s="99">
+      <c r="J43" s="98">
         <v>1</v>
       </c>
     </row>
@@ -14994,268 +15010,268 @@
       <c r="M49" s="3"/>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A50" s="108">
+      <c r="A50" s="107">
         <v>119</v>
       </c>
-      <c r="B50" s="108" t="s">
+      <c r="B50" s="107" t="s">
         <v>22</v>
       </c>
-      <c r="C50" s="108" t="s">
+      <c r="C50" s="107" t="s">
         <v>293</v>
       </c>
-      <c r="D50" s="108" t="s">
+      <c r="D50" s="107" t="s">
         <v>168</v>
       </c>
-      <c r="E50" s="109" t="s">
+      <c r="E50" s="108" t="s">
         <v>547</v>
       </c>
-      <c r="F50" s="108">
-        <v>1</v>
-      </c>
-      <c r="G50" s="108">
-        <v>1</v>
-      </c>
-      <c r="H50" s="108">
-        <v>1</v>
-      </c>
-      <c r="I50" s="110"/>
-      <c r="J50" s="108"/>
-      <c r="K50" s="108"/>
-      <c r="L50" s="111">
-        <v>1</v>
-      </c>
-      <c r="M50" s="110"/>
+      <c r="F50" s="107">
+        <v>1</v>
+      </c>
+      <c r="G50" s="107">
+        <v>1</v>
+      </c>
+      <c r="H50" s="107">
+        <v>1</v>
+      </c>
+      <c r="I50" s="109"/>
+      <c r="J50" s="107"/>
+      <c r="K50" s="107"/>
+      <c r="L50" s="110">
+        <v>1</v>
+      </c>
+      <c r="M50" s="109"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A51" s="102">
+      <c r="A51" s="101">
         <v>120</v>
       </c>
-      <c r="B51" s="102" t="s">
+      <c r="B51" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="C51" s="102" t="s">
+      <c r="C51" s="101" t="s">
         <v>293</v>
       </c>
-      <c r="D51" s="102" t="s">
+      <c r="D51" s="101" t="s">
         <v>168</v>
       </c>
-      <c r="E51" s="103" t="s">
+      <c r="E51" s="102" t="s">
         <v>597</v>
       </c>
-      <c r="F51" s="102">
-        <v>1</v>
-      </c>
-      <c r="G51" s="102">
-        <v>1</v>
-      </c>
-      <c r="H51" s="102">
-        <v>1</v>
-      </c>
-      <c r="I51" s="104"/>
-      <c r="J51" s="102"/>
-      <c r="K51" s="102"/>
-      <c r="L51" s="105">
-        <v>1</v>
-      </c>
-      <c r="M51" s="104"/>
+      <c r="F51" s="101">
+        <v>1</v>
+      </c>
+      <c r="G51" s="101">
+        <v>1</v>
+      </c>
+      <c r="H51" s="101">
+        <v>1</v>
+      </c>
+      <c r="I51" s="103"/>
+      <c r="J51" s="101"/>
+      <c r="K51" s="101"/>
+      <c r="L51" s="104">
+        <v>1</v>
+      </c>
+      <c r="M51" s="103"/>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A52" s="102">
+      <c r="A52" s="101">
         <v>121</v>
       </c>
-      <c r="B52" s="102" t="s">
+      <c r="B52" s="101" t="s">
         <v>22</v>
       </c>
-      <c r="C52" s="102" t="s">
+      <c r="C52" s="101" t="s">
         <v>293</v>
       </c>
-      <c r="D52" s="102" t="s">
+      <c r="D52" s="101" t="s">
         <v>168</v>
       </c>
-      <c r="E52" s="103" t="s">
+      <c r="E52" s="102" t="s">
         <v>598</v>
       </c>
-      <c r="F52" s="102">
-        <v>1</v>
-      </c>
-      <c r="G52" s="102">
-        <v>1</v>
-      </c>
-      <c r="H52" s="102">
-        <v>1</v>
-      </c>
-      <c r="I52" s="104"/>
-      <c r="J52" s="102"/>
-      <c r="K52" s="102"/>
-      <c r="L52" s="105">
-        <v>1</v>
-      </c>
-      <c r="M52" s="104"/>
+      <c r="F52" s="101">
+        <v>1</v>
+      </c>
+      <c r="G52" s="101">
+        <v>1</v>
+      </c>
+      <c r="H52" s="101">
+        <v>1</v>
+      </c>
+      <c r="I52" s="103"/>
+      <c r="J52" s="101"/>
+      <c r="K52" s="101"/>
+      <c r="L52" s="104">
+        <v>1</v>
+      </c>
+      <c r="M52" s="103"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A53" s="102">
+      <c r="A53" s="101">
         <v>122</v>
       </c>
-      <c r="B53" s="102" t="s">
+      <c r="B53" s="101" t="s">
         <v>22</v>
       </c>
-      <c r="C53" s="102" t="s">
+      <c r="C53" s="101" t="s">
         <v>293</v>
       </c>
-      <c r="D53" s="102" t="s">
+      <c r="D53" s="101" t="s">
         <v>168</v>
       </c>
-      <c r="E53" s="103" t="s">
+      <c r="E53" s="102" t="s">
         <v>596</v>
       </c>
-      <c r="F53" s="102">
-        <v>1</v>
-      </c>
-      <c r="G53" s="102">
-        <v>1</v>
-      </c>
-      <c r="H53" s="102">
-        <v>1</v>
-      </c>
-      <c r="I53" s="104"/>
-      <c r="J53" s="102"/>
-      <c r="K53" s="102"/>
-      <c r="L53" s="105">
-        <v>1</v>
-      </c>
-      <c r="M53" s="104"/>
+      <c r="F53" s="101">
+        <v>1</v>
+      </c>
+      <c r="G53" s="101">
+        <v>1</v>
+      </c>
+      <c r="H53" s="101">
+        <v>1</v>
+      </c>
+      <c r="I53" s="103"/>
+      <c r="J53" s="101"/>
+      <c r="K53" s="101"/>
+      <c r="L53" s="104">
+        <v>1</v>
+      </c>
+      <c r="M53" s="103"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A54" s="102">
+      <c r="A54" s="101">
         <v>123</v>
       </c>
-      <c r="B54" s="102" t="s">
+      <c r="B54" s="101" t="s">
         <v>22</v>
       </c>
-      <c r="C54" s="102" t="s">
+      <c r="C54" s="101" t="s">
         <v>293</v>
       </c>
-      <c r="D54" s="102" t="s">
+      <c r="D54" s="101" t="s">
         <v>168</v>
       </c>
-      <c r="E54" s="103" t="s">
+      <c r="E54" s="102" t="s">
         <v>599</v>
       </c>
-      <c r="F54" s="102">
-        <v>1</v>
-      </c>
-      <c r="G54" s="102">
-        <v>1</v>
-      </c>
-      <c r="H54" s="102">
-        <v>1</v>
-      </c>
-      <c r="I54" s="104"/>
-      <c r="J54" s="102"/>
-      <c r="K54" s="102"/>
-      <c r="L54" s="105">
-        <v>1</v>
-      </c>
-      <c r="M54" s="104"/>
+      <c r="F54" s="101">
+        <v>1</v>
+      </c>
+      <c r="G54" s="101">
+        <v>1</v>
+      </c>
+      <c r="H54" s="101">
+        <v>1</v>
+      </c>
+      <c r="I54" s="103"/>
+      <c r="J54" s="101"/>
+      <c r="K54" s="101"/>
+      <c r="L54" s="104">
+        <v>1</v>
+      </c>
+      <c r="M54" s="103"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A55" s="102">
+      <c r="A55" s="101">
         <v>124</v>
       </c>
-      <c r="B55" s="102" t="s">
+      <c r="B55" s="101" t="s">
         <v>22</v>
       </c>
-      <c r="C55" s="102" t="s">
+      <c r="C55" s="101" t="s">
         <v>293</v>
       </c>
-      <c r="D55" s="102" t="s">
+      <c r="D55" s="101" t="s">
         <v>168</v>
       </c>
-      <c r="E55" s="103" t="s">
+      <c r="E55" s="102" t="s">
         <v>600</v>
       </c>
-      <c r="F55" s="102">
-        <v>1</v>
-      </c>
-      <c r="G55" s="102">
-        <v>1</v>
-      </c>
-      <c r="H55" s="102">
-        <v>1</v>
-      </c>
-      <c r="I55" s="104"/>
-      <c r="J55" s="102"/>
-      <c r="K55" s="102"/>
-      <c r="L55" s="105">
-        <v>1</v>
-      </c>
-      <c r="M55" s="104"/>
+      <c r="F55" s="101">
+        <v>1</v>
+      </c>
+      <c r="G55" s="101">
+        <v>1</v>
+      </c>
+      <c r="H55" s="101">
+        <v>1</v>
+      </c>
+      <c r="I55" s="103"/>
+      <c r="J55" s="101"/>
+      <c r="K55" s="101"/>
+      <c r="L55" s="104">
+        <v>1</v>
+      </c>
+      <c r="M55" s="103"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A56" s="102">
+      <c r="A56" s="101">
         <v>125</v>
       </c>
-      <c r="B56" s="102" t="s">
+      <c r="B56" s="101" t="s">
         <v>22</v>
       </c>
-      <c r="C56" s="102" t="s">
+      <c r="C56" s="101" t="s">
         <v>293</v>
       </c>
-      <c r="D56" s="102" t="s">
+      <c r="D56" s="101" t="s">
         <v>168</v>
       </c>
-      <c r="E56" s="103" t="s">
+      <c r="E56" s="102" t="s">
         <v>595</v>
       </c>
-      <c r="F56" s="102">
-        <v>1</v>
-      </c>
-      <c r="G56" s="102">
-        <v>1</v>
-      </c>
-      <c r="H56" s="102">
-        <v>1</v>
-      </c>
-      <c r="I56" s="104"/>
-      <c r="J56" s="102"/>
-      <c r="K56" s="102"/>
-      <c r="L56" s="105">
-        <v>1</v>
-      </c>
-      <c r="M56" s="104"/>
+      <c r="F56" s="101">
+        <v>1</v>
+      </c>
+      <c r="G56" s="101">
+        <v>1</v>
+      </c>
+      <c r="H56" s="101">
+        <v>1</v>
+      </c>
+      <c r="I56" s="103"/>
+      <c r="J56" s="101"/>
+      <c r="K56" s="101"/>
+      <c r="L56" s="104">
+        <v>1</v>
+      </c>
+      <c r="M56" s="103"/>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A57" s="102">
+      <c r="A57" s="101">
         <v>126</v>
       </c>
-      <c r="B57" s="102" t="s">
+      <c r="B57" s="101" t="s">
         <v>22</v>
       </c>
-      <c r="C57" s="102" t="s">
+      <c r="C57" s="101" t="s">
         <v>293</v>
       </c>
-      <c r="D57" s="102" t="s">
+      <c r="D57" s="101" t="s">
         <v>168</v>
       </c>
-      <c r="E57" s="103" t="s">
+      <c r="E57" s="102" t="s">
         <v>601</v>
       </c>
-      <c r="F57" s="102">
-        <v>1</v>
-      </c>
-      <c r="G57" s="102">
-        <v>1</v>
-      </c>
-      <c r="H57" s="102">
-        <v>1</v>
-      </c>
-      <c r="I57" s="104"/>
-      <c r="J57" s="102"/>
-      <c r="K57" s="102"/>
-      <c r="L57" s="105">
-        <v>1</v>
-      </c>
-      <c r="M57" s="104"/>
+      <c r="F57" s="101">
+        <v>1</v>
+      </c>
+      <c r="G57" s="101">
+        <v>1</v>
+      </c>
+      <c r="H57" s="101">
+        <v>1</v>
+      </c>
+      <c r="I57" s="103"/>
+      <c r="J57" s="101"/>
+      <c r="K57" s="101"/>
+      <c r="L57" s="104">
+        <v>1</v>
+      </c>
+      <c r="M57" s="103"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:M16" xr:uid="{00000000-0009-0000-0000-000008000000}"/>

</xml_diff>

<commit_message>
fix direct list render logic in meeting
</commit_message>
<xml_diff>
--- a/db/excel/api-function-granted-users-cdld.xlsx
+++ b/db/excel/api-function-granted-users-cdld.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10613"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA228B50-9733-4526-8869-D465E68B6AD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCBD7AF9-849E-7445-B981-79FC78909D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19460" tabRatio="800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_types" sheetId="27" r:id="rId1"/>
@@ -2388,37 +2388,37 @@
     <t>Màu chữ cho phân loại này</t>
   </si>
   <si>
-    <t>linear-gradient(135deg, #DFEC51 0%,#73AA0A 100%);</t>
-  </si>
-  <si>
-    <t>linear-gradient(135deg, #fad961 0%,#f76b1c 100%);</t>
-  </si>
-  <si>
-    <t>linear-gradient(135deg, #5b247a 0%,#1bcedf 100%);</t>
-  </si>
-  <si>
-    <t>linear-gradient(135deg, #E3E3E3 0%,#5D6874 100%);</t>
-  </si>
-  <si>
-    <t>linear-gradient(135deg, #CE9FFC 0%,#7367F0 100%);</t>
-  </si>
-  <si>
-    <t>linear-gradient(135deg, #F5515F 0%,#A1051D 100%);</t>
-  </si>
-  <si>
-    <t>linear-gradient(135deg, #fcdf8a 0%,#f38381 100%);</t>
-  </si>
-  <si>
-    <t>linear-gradient(135deg, #65799b 0%,#5e2563 100%);</t>
-  </si>
-  <si>
-    <t>linear-gradient(135deg, #184e68 0%,#57ca85 100%);</t>
-  </si>
-  <si>
-    <t>linear-gradient(135deg, #17ead9 0%,#6078ea 100%);</t>
-  </si>
-  <si>
-    <t>linear-gradient(135deg, #13f1fc 0%,#0470dc 100%);</t>
+    <t>linear-gradient(135deg, #fad961 0%,#f76b1c 100%)</t>
+  </si>
+  <si>
+    <t>linear-gradient(135deg, #DFEC51 0%,#73AA0A 100%)</t>
+  </si>
+  <si>
+    <t>linear-gradient(135deg, #5b247a 0%,#1bcedf 100%)</t>
+  </si>
+  <si>
+    <t>linear-gradient(135deg, #E3E3E3 0%,#5D6874 100%)</t>
+  </si>
+  <si>
+    <t>linear-gradient(135deg, #CE9FFC 0%,#7367F0 100%)</t>
+  </si>
+  <si>
+    <t>linear-gradient(135deg, #F5515F 0%,#A1051D 100%)</t>
+  </si>
+  <si>
+    <t>linear-gradient(135deg, #fcdf8a 0%,#f38381 100%)</t>
+  </si>
+  <si>
+    <t>linear-gradient(135deg, #65799b 0%,#5e2563 100%)</t>
+  </si>
+  <si>
+    <t>linear-gradient(135deg, #184e68 0%,#57ca85 100%)</t>
+  </si>
+  <si>
+    <t>linear-gradient(135deg, #17ead9 0%,#6078ea 100%)</t>
+  </si>
+  <si>
+    <t>linear-gradient(135deg, #13f1fc 0%,#0470dc 100%)</t>
   </si>
 </sst>
 </file>
@@ -5092,19 +5092,19 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="9" customWidth="1"/>
     <col min="5" max="5" width="14" style="9" customWidth="1"/>
-    <col min="6" max="6" width="55.42578125" style="9" customWidth="1"/>
-    <col min="7" max="64" width="11.42578125" style="9" customWidth="1"/>
-    <col min="65" max="16384" width="9.140625" style="9"/>
+    <col min="6" max="6" width="55.5" style="9" customWidth="1"/>
+    <col min="7" max="64" width="11.5" style="9" customWidth="1"/>
+    <col min="65" max="16384" width="9.1640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>83</v>
       </c>
@@ -5124,7 +5124,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>15</v>
       </c>
@@ -5144,7 +5144,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>16</v>
       </c>
@@ -5164,7 +5164,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>97</v>
       </c>
@@ -5184,7 +5184,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>17</v>
       </c>
@@ -5204,7 +5204,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>103</v>
       </c>
@@ -5224,7 +5224,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>50</v>
       </c>
@@ -5244,7 +5244,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>106</v>
       </c>
@@ -5286,17 +5286,17 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.28515625" customWidth="1"/>
-    <col min="3" max="3" width="40.140625" customWidth="1"/>
+    <col min="2" max="2" width="48.33203125" customWidth="1"/>
+    <col min="3" max="3" width="40.1640625" customWidth="1"/>
     <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="103" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>18</v>
       </c>
@@ -5316,7 +5316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A2" s="93">
         <v>99</v>
       </c>
@@ -5336,7 +5336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="91">
         <v>21</v>
       </c>
@@ -5375,26 +5375,26 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" style="83" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="83" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" style="83" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" style="83" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" style="83" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" style="83" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" style="83" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" style="87" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" style="87" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" style="87" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21" style="83" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="78.85546875" style="83" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" style="83" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" style="83" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" style="83"/>
-    <col min="12" max="12" width="14.140625" style="83" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" style="83" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.140625" style="83" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="11.42578125" style="83"/>
+    <col min="8" max="8" width="78.83203125" style="83" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="83" customWidth="1"/>
+    <col min="10" max="10" width="12.5" style="83" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" style="83"/>
+    <col min="12" max="12" width="14.1640625" style="83" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" style="83" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.1640625" style="83" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="11.5" style="83"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="82" t="s">
         <v>18</v>
       </c>
@@ -5943,21 +5943,21 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.85546875" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.83203125" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
         <v>1</v>
       </c>
@@ -5992,7 +5992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
         <v>165</v>
       </c>
@@ -6019,7 +6019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
         <v>218</v>
       </c>
@@ -6046,7 +6046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="28" t="s">
         <v>166</v>
       </c>
@@ -6073,7 +6073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="28" t="s">
         <v>167</v>
       </c>
@@ -6122,22 +6122,22 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="40" t="s">
         <v>18</v>
       </c>
@@ -6172,7 +6172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6195,7 +6195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6221,7 +6221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -6247,7 +6247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -6273,7 +6273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -6299,7 +6299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -6325,7 +6325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -6351,7 +6351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -6377,7 +6377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -6403,7 +6403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -6429,7 +6429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -6455,7 +6455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -6481,7 +6481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -6507,7 +6507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -6533,7 +6533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -6559,7 +6559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -6585,7 +6585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -6624,14 +6624,14 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="5" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="5" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="65" t="s">
         <v>18</v>
       </c>
@@ -6648,7 +6648,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6662,7 +6662,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6676,7 +6676,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -6690,7 +6690,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -6704,7 +6704,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -6718,7 +6718,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -6732,7 +6732,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -6746,7 +6746,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -6760,7 +6760,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -6774,7 +6774,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -6804,26 +6804,26 @@
       <selection pane="bottomRight" activeCell="F94" sqref="F94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="72" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="43.42578125" customWidth="1"/>
+    <col min="11" max="11" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="43.5" customWidth="1"/>
     <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="19" customWidth="1"/>
-    <col min="16" max="16" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="54" t="s">
         <v>2</v>
       </c>
@@ -6873,7 +6873,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="50" t="s">
         <v>253</v>
       </c>
@@ -6911,7 +6911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="50" t="s">
         <v>253</v>
       </c>
@@ -6943,7 +6943,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="50" t="s">
         <v>253</v>
       </c>
@@ -6975,7 +6975,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="108" t="s">
         <v>253</v>
       </c>
@@ -7005,7 +7005,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="50" t="s">
         <v>253</v>
       </c>
@@ -7037,7 +7037,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="50" t="s">
         <v>253</v>
       </c>
@@ -7069,7 +7069,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="50" t="s">
         <v>253</v>
       </c>
@@ -7101,7 +7101,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="50" t="s">
         <v>253</v>
       </c>
@@ -7131,7 +7131,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="50" t="s">
         <v>253</v>
       </c>
@@ -7163,7 +7163,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="50" t="s">
         <v>253</v>
       </c>
@@ -7193,7 +7193,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="50" t="s">
         <v>253</v>
       </c>
@@ -7225,7 +7225,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="50" t="s">
         <v>253</v>
       </c>
@@ -7257,7 +7257,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="51" t="s">
         <v>219</v>
       </c>
@@ -7295,7 +7295,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="51" t="s">
         <v>219</v>
       </c>
@@ -7331,7 +7331,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="51" t="s">
         <v>219</v>
       </c>
@@ -7363,7 +7363,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="110" t="s">
         <v>219</v>
       </c>
@@ -7395,7 +7395,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="51" t="s">
         <v>219</v>
       </c>
@@ -7429,7 +7429,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="51" t="s">
         <v>219</v>
       </c>
@@ -7461,7 +7461,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="51" t="s">
         <v>219</v>
       </c>
@@ -7493,7 +7493,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="51" t="s">
         <v>219</v>
       </c>
@@ -7525,7 +7525,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="51" t="s">
         <v>219</v>
       </c>
@@ -7557,7 +7557,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="51" t="s">
         <v>219</v>
       </c>
@@ -7587,7 +7587,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="51" t="s">
         <v>219</v>
       </c>
@@ -7617,7 +7617,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="51" t="s">
         <v>219</v>
       </c>
@@ -7649,7 +7649,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="51" t="s">
         <v>219</v>
       </c>
@@ -7679,7 +7679,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="51" t="s">
         <v>219</v>
       </c>
@@ -7711,7 +7711,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="51" t="s">
         <v>219</v>
       </c>
@@ -7743,7 +7743,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="51" t="s">
         <v>219</v>
       </c>
@@ -7775,7 +7775,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="51" t="s">
         <v>219</v>
       </c>
@@ -7807,7 +7807,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="96" t="s">
         <v>512</v>
       </c>
@@ -7843,7 +7843,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="96" t="s">
         <v>512</v>
       </c>
@@ -7873,7 +7873,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="96" t="s">
         <v>512</v>
       </c>
@@ -7907,7 +7907,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="96" t="s">
         <v>512</v>
       </c>
@@ -7939,7 +7939,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="96" t="s">
         <v>512</v>
       </c>
@@ -7971,7 +7971,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="96" t="s">
         <v>512</v>
       </c>
@@ -8003,7 +8003,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="96" t="s">
         <v>512</v>
       </c>
@@ -8033,7 +8033,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="96" t="s">
         <v>512</v>
       </c>
@@ -8063,7 +8063,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="96" t="s">
         <v>512</v>
       </c>
@@ -8095,7 +8095,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="96" t="s">
         <v>512</v>
       </c>
@@ -8125,7 +8125,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="96" t="s">
         <v>512</v>
       </c>
@@ -8157,7 +8157,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="96" t="s">
         <v>512</v>
       </c>
@@ -8189,7 +8189,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="50" t="s">
         <v>274</v>
       </c>
@@ -8225,7 +8225,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="50" t="s">
         <v>274</v>
       </c>
@@ -8259,7 +8259,7 @@
       <c r="O44" s="55"/>
       <c r="P44" s="56"/>
     </row>
-    <row r="45" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="50" t="s">
         <v>274</v>
       </c>
@@ -8291,7 +8291,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="50" t="s">
         <v>274</v>
       </c>
@@ -8325,7 +8325,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="50" t="s">
         <v>274</v>
       </c>
@@ -8357,7 +8357,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="50" t="s">
         <v>274</v>
       </c>
@@ -8387,7 +8387,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="50" t="s">
         <v>274</v>
       </c>
@@ -8419,7 +8419,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:16" s="117" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" s="117" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="108" t="s">
         <v>274</v>
       </c>
@@ -8451,7 +8451,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="50" t="s">
         <v>274</v>
       </c>
@@ -8483,7 +8483,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="50" t="s">
         <v>274</v>
       </c>
@@ -8515,7 +8515,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="50" t="s">
         <v>274</v>
       </c>
@@ -8545,7 +8545,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" s="118" t="s">
         <v>274</v>
       </c>
@@ -8577,7 +8577,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="50" t="s">
         <v>274</v>
       </c>
@@ -8607,7 +8607,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="50" t="s">
         <v>274</v>
       </c>
@@ -8639,7 +8639,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="50" t="s">
         <v>274</v>
       </c>
@@ -8669,7 +8669,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="50" t="s">
         <v>274</v>
       </c>
@@ -8701,7 +8701,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="50" t="s">
         <v>274</v>
       </c>
@@ -8733,7 +8733,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="52" t="s">
         <v>273</v>
       </c>
@@ -8771,7 +8771,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="52" t="s">
         <v>273</v>
       </c>
@@ -8807,7 +8807,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="52" t="s">
         <v>273</v>
       </c>
@@ -8841,7 +8841,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="52" t="s">
         <v>273</v>
       </c>
@@ -8875,7 +8875,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="52" t="s">
         <v>273</v>
       </c>
@@ -8909,7 +8909,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="52" t="s">
         <v>273</v>
       </c>
@@ -8941,7 +8941,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="52" t="s">
         <v>273</v>
       </c>
@@ -8973,7 +8973,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="112" t="s">
         <v>273</v>
       </c>
@@ -9005,7 +9005,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:16" s="80" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" s="80" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="52" t="s">
         <v>273</v>
       </c>
@@ -9037,7 +9037,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="52" t="s">
         <v>273</v>
       </c>
@@ -9067,7 +9067,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="52" t="s">
         <v>273</v>
       </c>
@@ -9099,7 +9099,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="52" t="s">
         <v>273</v>
       </c>
@@ -9129,7 +9129,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="63" t="s">
         <v>273</v>
       </c>
@@ -9161,7 +9161,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="52" t="s">
         <v>273</v>
       </c>
@@ -9193,7 +9193,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="53" t="s">
         <v>216</v>
       </c>
@@ -9231,7 +9231,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="53" t="s">
         <v>216</v>
       </c>
@@ -9267,7 +9267,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="115" t="s">
         <v>216</v>
       </c>
@@ -9299,7 +9299,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="53" t="s">
         <v>216</v>
       </c>
@@ -9331,7 +9331,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="53" t="s">
         <v>216</v>
       </c>
@@ -9363,7 +9363,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="53" t="s">
         <v>216</v>
       </c>
@@ -9395,7 +9395,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="53" t="s">
         <v>216</v>
       </c>
@@ -9427,7 +9427,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="53" t="s">
         <v>216</v>
       </c>
@@ -9457,7 +9457,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="53" t="s">
         <v>216</v>
       </c>
@@ -9489,7 +9489,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="53" t="s">
         <v>216</v>
       </c>
@@ -9519,7 +9519,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="53" t="s">
         <v>216</v>
       </c>
@@ -9551,7 +9551,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="53" t="s">
         <v>216</v>
       </c>
@@ -9583,7 +9583,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="44" t="s">
         <v>169</v>
       </c>
@@ -9619,7 +9619,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="44" t="s">
         <v>169</v>
       </c>
@@ -9651,7 +9651,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="44" t="s">
         <v>169</v>
       </c>
@@ -9683,7 +9683,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="44" t="s">
         <v>169</v>
       </c>
@@ -9717,7 +9717,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="44" t="s">
         <v>169</v>
       </c>
@@ -9749,7 +9749,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="44" t="s">
         <v>169</v>
       </c>
@@ -9781,7 +9781,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="44" t="s">
         <v>169</v>
       </c>
@@ -9813,7 +9813,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="93" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="44" t="s">
         <v>169</v>
       </c>
@@ -9845,7 +9845,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="94" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="44" t="s">
         <v>169</v>
       </c>
@@ -9875,7 +9875,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="95" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="44" t="s">
         <v>169</v>
       </c>
@@ -9907,7 +9907,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="96" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="44" t="s">
         <v>169</v>
       </c>
@@ -9937,7 +9937,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="97" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="44" t="s">
         <v>169</v>
       </c>
@@ -9969,7 +9969,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="98" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="44" t="s">
         <v>169</v>
       </c>
@@ -10014,26 +10014,26 @@
   </sheetPr>
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="60.5703125" customWidth="1"/>
-    <col min="7" max="7" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60.5" customWidth="1"/>
+    <col min="7" max="7" width="48.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="39" t="s">
         <v>18</v>
       </c>
@@ -10071,7 +10071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="90">
         <v>1</v>
       </c>
@@ -10103,7 +10103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>11</v>
       </c>
@@ -10132,7 +10132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>12</v>
       </c>
@@ -10161,7 +10161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>13</v>
       </c>
@@ -10190,7 +10190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>14</v>
       </c>
@@ -10219,7 +10219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>15</v>
       </c>
@@ -10248,7 +10248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>16</v>
       </c>
@@ -10277,7 +10277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="90">
         <v>2</v>
       </c>
@@ -10309,7 +10309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>21</v>
       </c>
@@ -10338,7 +10338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>22</v>
       </c>
@@ -10367,7 +10367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="90">
         <v>3</v>
       </c>
@@ -10399,7 +10399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>31</v>
       </c>
@@ -10416,7 +10416,7 @@
         <v>391</v>
       </c>
       <c r="G13" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="H13" t="s">
         <v>656</v>
@@ -10428,7 +10428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>32</v>
       </c>
@@ -10445,7 +10445,7 @@
         <v>392</v>
       </c>
       <c r="G14" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="H14" t="s">
         <v>656</v>
@@ -10457,7 +10457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>33</v>
       </c>
@@ -10486,7 +10486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>34</v>
       </c>
@@ -10515,7 +10515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>35</v>
       </c>
@@ -10544,7 +10544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>36</v>
       </c>
@@ -10573,7 +10573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="90">
         <v>4</v>
       </c>
@@ -10605,7 +10605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>41</v>
       </c>
@@ -10634,7 +10634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>42</v>
       </c>
@@ -10663,7 +10663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>43</v>
       </c>
@@ -10692,7 +10692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>44</v>
       </c>
@@ -10721,7 +10721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="90">
         <v>5</v>
       </c>
@@ -10753,7 +10753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>51</v>
       </c>
@@ -10782,7 +10782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>52</v>
       </c>
@@ -10811,7 +10811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>53</v>
       </c>
@@ -10840,7 +10840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>54</v>
       </c>
@@ -10869,7 +10869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>55</v>
       </c>
@@ -10898,7 +10898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>56</v>
       </c>
@@ -10927,7 +10927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>57</v>
       </c>
@@ -10956,7 +10956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>58</v>
       </c>
@@ -10985,7 +10985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>59</v>
       </c>
@@ -11014,7 +11014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>510</v>
       </c>
@@ -11043,7 +11043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>511</v>
       </c>
@@ -11072,7 +11072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>512</v>
       </c>
@@ -11101,7 +11101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>513</v>
       </c>
@@ -11130,7 +11130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>514</v>
       </c>
@@ -11159,7 +11159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="90">
         <v>6</v>
       </c>
@@ -11191,7 +11191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>61</v>
       </c>
@@ -11208,7 +11208,7 @@
         <v>613</v>
       </c>
       <c r="G40" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="H40" t="s">
         <v>656</v>
@@ -11220,7 +11220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>62</v>
       </c>
@@ -11249,7 +11249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>63</v>
       </c>
@@ -11278,7 +11278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>64</v>
       </c>
@@ -11324,16 +11324,16 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
-    <col min="5" max="12" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" customWidth="1"/>
+    <col min="5" max="12" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="38" t="s">
         <v>18</v>
       </c>
@@ -11371,7 +11371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -11407,23 +11407,23 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="61" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="64" t="s">
         <v>18</v>
       </c>
@@ -11464,7 +11464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="41"/>
       <c r="B2" s="41"/>
       <c r="C2" s="41"/>
@@ -11479,7 +11479,7 @@
       <c r="L2" s="41"/>
       <c r="M2" s="41"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="41"/>
       <c r="B3" s="41"/>
       <c r="C3" s="41"/>
@@ -11510,18 +11510,18 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" customWidth="1"/>
+    <col min="6" max="6" width="21.5" customWidth="1"/>
+    <col min="7" max="7" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="64" t="s">
         <v>18</v>
       </c>
@@ -11573,22 +11573,22 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.140625" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.1640625" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="18.5" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="26.42578125" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" customWidth="1"/>
-    <col min="11" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.5" customWidth="1"/>
+    <col min="10" max="10" width="22.83203125" customWidth="1"/>
+    <col min="11" max="12" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="65" t="s">
         <v>18</v>
       </c>
@@ -11643,27 +11643,27 @@
       <selection pane="bottomRight" activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="85.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.42578125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="85.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.1640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.83203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.5" style="17" customWidth="1"/>
     <col min="16" max="16" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -11713,7 +11713,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
@@ -11749,7 +11749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>39</v>
       </c>
@@ -11777,7 +11777,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>39</v>
       </c>
@@ -11807,7 +11807,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>39</v>
       </c>
@@ -11837,7 +11837,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>39</v>
       </c>
@@ -11871,7 +11871,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>39</v>
       </c>
@@ -11899,7 +11899,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>39</v>
       </c>
@@ -11927,7 +11927,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>39</v>
       </c>
@@ -11955,7 +11955,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>39</v>
       </c>
@@ -11983,7 +11983,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>39</v>
       </c>
@@ -12013,7 +12013,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>39</v>
       </c>
@@ -12041,7 +12041,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>39</v>
       </c>
@@ -12071,7 +12071,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>39</v>
       </c>
@@ -12099,7 +12099,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>39</v>
       </c>
@@ -12127,7 +12127,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="77" t="s">
         <v>38</v>
       </c>
@@ -12163,7 +12163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="77" t="s">
         <v>38</v>
       </c>
@@ -12193,7 +12193,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="77" t="s">
         <v>38</v>
       </c>
@@ -12221,7 +12221,7 @@
       <c r="O18" s="78"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="77" t="s">
         <v>38</v>
       </c>
@@ -12251,7 +12251,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="77" t="s">
         <v>38</v>
       </c>
@@ -12279,7 +12279,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="77" t="s">
         <v>38</v>
       </c>
@@ -12307,7 +12307,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="77" t="s">
         <v>38</v>
       </c>
@@ -12337,7 +12337,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="77" t="s">
         <v>38</v>
       </c>
@@ -12367,7 +12367,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>46</v>
       </c>
@@ -12403,7 +12403,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>46</v>
       </c>
@@ -12431,7 +12431,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>46</v>
       </c>
@@ -12461,7 +12461,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>46</v>
       </c>
@@ -12491,7 +12491,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>46</v>
       </c>
@@ -12521,7 +12521,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>46</v>
       </c>
@@ -12551,7 +12551,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>46</v>
       </c>
@@ -12581,7 +12581,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>46</v>
       </c>
@@ -12611,7 +12611,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>46</v>
       </c>
@@ -12639,7 +12639,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>46</v>
       </c>
@@ -12669,7 +12669,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>46</v>
       </c>
@@ -12699,7 +12699,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="77" t="s">
         <v>144</v>
       </c>
@@ -12733,7 +12733,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="77" t="s">
         <v>144</v>
       </c>
@@ -12761,7 +12761,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="77" t="s">
         <v>144</v>
       </c>
@@ -12791,7 +12791,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="77" t="s">
         <v>144</v>
       </c>
@@ -12821,7 +12821,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="77" t="s">
         <v>144</v>
       </c>
@@ -12851,7 +12851,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="77" t="s">
         <v>144</v>
       </c>
@@ -12881,7 +12881,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="77" t="s">
         <v>144</v>
       </c>
@@ -12911,7 +12911,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="77" t="s">
         <v>144</v>
       </c>
@@ -12941,7 +12941,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="77" t="s">
         <v>144</v>
       </c>
@@ -12971,7 +12971,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="77" t="s">
         <v>144</v>
       </c>
@@ -13001,7 +13001,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="77" t="s">
         <v>144</v>
       </c>
@@ -13029,7 +13029,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="77" t="s">
         <v>144</v>
       </c>
@@ -13057,7 +13057,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="77" t="s">
         <v>144</v>
       </c>
@@ -13087,7 +13087,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="77" t="s">
         <v>144</v>
       </c>
@@ -13117,7 +13117,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="42" t="s">
         <v>181</v>
       </c>
@@ -13154,7 +13154,7 @@
       </c>
       <c r="Q49" s="57"/>
     </row>
-    <row r="50" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="42" t="s">
         <v>181</v>
       </c>
@@ -13185,7 +13185,7 @@
       </c>
       <c r="Q50" s="57"/>
     </row>
-    <row r="51" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="42" t="s">
         <v>181</v>
       </c>
@@ -13216,7 +13216,7 @@
       </c>
       <c r="Q51" s="57"/>
     </row>
-    <row r="52" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="42" t="s">
         <v>181</v>
       </c>
@@ -13247,7 +13247,7 @@
       </c>
       <c r="Q52" s="57"/>
     </row>
-    <row r="53" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="42" t="s">
         <v>181</v>
       </c>
@@ -13276,7 +13276,7 @@
       </c>
       <c r="Q53" s="57"/>
     </row>
-    <row r="54" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="42" t="s">
         <v>181</v>
       </c>
@@ -13307,7 +13307,7 @@
       </c>
       <c r="Q54" s="57"/>
     </row>
-    <row r="55" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="42" t="s">
         <v>181</v>
       </c>
@@ -13338,7 +13338,7 @@
       </c>
       <c r="Q55" s="57"/>
     </row>
-    <row r="56" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="42" t="s">
         <v>181</v>
       </c>
@@ -13367,7 +13367,7 @@
       </c>
       <c r="Q56" s="57"/>
     </row>
-    <row r="57" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="42" t="s">
         <v>181</v>
       </c>
@@ -13396,7 +13396,7 @@
       </c>
       <c r="Q57" s="57"/>
     </row>
-    <row r="58" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="42" t="s">
         <v>181</v>
       </c>
@@ -13427,7 +13427,7 @@
       </c>
       <c r="Q58" s="57"/>
     </row>
-    <row r="59" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="42" t="s">
         <v>181</v>
       </c>
@@ -13458,7 +13458,7 @@
       </c>
       <c r="Q59" s="57"/>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" s="66" t="s">
         <v>331</v>
       </c>
@@ -13494,7 +13494,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" s="66" t="s">
         <v>331</v>
       </c>
@@ -13530,7 +13530,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" s="66" t="s">
         <v>331</v>
       </c>
@@ -13560,7 +13560,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" s="66" t="s">
         <v>331</v>
       </c>
@@ -13588,7 +13588,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" s="66" t="s">
         <v>331</v>
       </c>
@@ -13618,7 +13618,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A65" s="66"/>
       <c r="B65" s="66"/>
       <c r="C65" s="66"/>
@@ -13661,25 +13661,25 @@
       <selection pane="bottomRight" activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" customWidth="1"/>
     <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" customWidth="1"/>
+    <col min="7" max="7" width="13.5" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" customWidth="1"/>
+    <col min="9" max="9" width="12.5" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="57" customWidth="1"/>
-    <col min="11" max="11" width="54.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="35.7109375" style="5" customWidth="1"/>
-    <col min="14" max="14" width="51.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="54.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.6640625" style="5" customWidth="1"/>
+    <col min="14" max="14" width="51.1640625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
         <v>18</v>
       </c>
@@ -13723,7 +13723,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="25">
         <v>1</v>
       </c>
@@ -13761,7 +13761,7 @@
       <c r="M2" s="25"/>
       <c r="N2" s="26"/>
     </row>
-    <row r="3" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="25">
         <v>2</v>
       </c>
@@ -13799,7 +13799,7 @@
       <c r="M3" s="25"/>
       <c r="N3" s="26"/>
     </row>
-    <row r="4" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="25">
         <v>3</v>
       </c>
@@ -13837,7 +13837,7 @@
       <c r="M4" s="25"/>
       <c r="N4" s="26"/>
     </row>
-    <row r="5" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="25">
         <v>4</v>
       </c>
@@ -13875,7 +13875,7 @@
       <c r="M5" s="25"/>
       <c r="N5" s="26"/>
     </row>
-    <row r="6" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="25">
         <v>5</v>
       </c>
@@ -13913,7 +13913,7 @@
       <c r="M6" s="25"/>
       <c r="N6" s="26"/>
     </row>
-    <row r="7" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="25">
         <v>6</v>
       </c>
@@ -13951,7 +13951,7 @@
       <c r="M7" s="25"/>
       <c r="N7" s="26"/>
     </row>
-    <row r="8" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="25">
         <v>7</v>
       </c>
@@ -13989,7 +13989,7 @@
       <c r="M8" s="25"/>
       <c r="N8" s="26"/>
     </row>
-    <row r="9" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="25">
         <v>8</v>
       </c>
@@ -14027,7 +14027,7 @@
       <c r="M9" s="25"/>
       <c r="N9" s="26"/>
     </row>
-    <row r="10" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="25">
         <v>9</v>
       </c>
@@ -14065,7 +14065,7 @@
       <c r="M10" s="25"/>
       <c r="N10" s="26"/>
     </row>
-    <row r="11" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="25">
         <v>10</v>
       </c>
@@ -14103,7 +14103,7 @@
       <c r="M11" s="25"/>
       <c r="N11" s="26"/>
     </row>
-    <row r="12" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="25">
         <v>11</v>
       </c>
@@ -14141,7 +14141,7 @@
       <c r="M12" s="25"/>
       <c r="N12" s="26"/>
     </row>
-    <row r="13" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="25">
         <v>12</v>
       </c>
@@ -14179,7 +14179,7 @@
       <c r="M13" s="25"/>
       <c r="N13" s="26"/>
     </row>
-    <row r="14" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="25">
         <v>13</v>
       </c>
@@ -14217,7 +14217,7 @@
       <c r="M14" s="25"/>
       <c r="N14" s="26"/>
     </row>
-    <row r="15" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="25">
         <v>14</v>
       </c>
@@ -14255,7 +14255,7 @@
       <c r="M15" s="25"/>
       <c r="N15" s="26"/>
     </row>
-    <row r="16" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="25">
         <v>15</v>
       </c>
@@ -14293,7 +14293,7 @@
       <c r="M16" s="25"/>
       <c r="N16" s="26"/>
     </row>
-    <row r="17" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="25">
         <v>16</v>
       </c>
@@ -14331,7 +14331,7 @@
       <c r="M17" s="25"/>
       <c r="N17" s="26"/>
     </row>
-    <row r="18" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="25">
         <v>50</v>
       </c>
@@ -14369,7 +14369,7 @@
       <c r="M18" s="25"/>
       <c r="N18" s="26"/>
     </row>
-    <row r="19" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="66">
         <v>51</v>
       </c>
@@ -14403,7 +14403,7 @@
       <c r="M19" s="69"/>
       <c r="N19" s="71"/>
     </row>
-    <row r="20" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="25">
         <v>52</v>
       </c>
@@ -14437,7 +14437,7 @@
       <c r="M20" s="69"/>
       <c r="N20" s="71"/>
     </row>
-    <row r="21" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="66">
         <v>53</v>
       </c>
@@ -14471,7 +14471,7 @@
       <c r="M21" s="69"/>
       <c r="N21" s="71"/>
     </row>
-    <row r="22" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="25">
         <v>54</v>
       </c>
@@ -14505,7 +14505,7 @@
       <c r="M22" s="69"/>
       <c r="N22" s="71"/>
     </row>
-    <row r="23" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="66">
         <v>55</v>
       </c>
@@ -14539,7 +14539,7 @@
       <c r="M23" s="69"/>
       <c r="N23" s="71"/>
     </row>
-    <row r="24" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="25">
         <v>56</v>
       </c>
@@ -14573,7 +14573,7 @@
       <c r="M24" s="69"/>
       <c r="N24" s="71"/>
     </row>
-    <row r="25" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="66">
         <v>57</v>
       </c>
@@ -14607,7 +14607,7 @@
       <c r="M25" s="69"/>
       <c r="N25" s="71"/>
     </row>
-    <row r="26" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="25">
         <v>58</v>
       </c>
@@ -14641,7 +14641,7 @@
       <c r="M26" s="69"/>
       <c r="N26" s="71"/>
     </row>
-    <row r="27" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="66">
         <v>59</v>
       </c>
@@ -14675,7 +14675,7 @@
       <c r="M27" s="69"/>
       <c r="N27" s="71"/>
     </row>
-    <row r="28" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="25">
         <v>60</v>
       </c>
@@ -14709,7 +14709,7 @@
       <c r="M28" s="69"/>
       <c r="N28" s="71"/>
     </row>
-    <row r="29" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="66">
         <v>61</v>
       </c>
@@ -14743,7 +14743,7 @@
       <c r="M29" s="69"/>
       <c r="N29" s="71"/>
     </row>
-    <row r="30" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="25">
         <v>62</v>
       </c>
@@ -14777,7 +14777,7 @@
       <c r="M30" s="69"/>
       <c r="N30" s="71"/>
     </row>
-    <row r="31" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="66">
         <v>63</v>
       </c>
@@ -14811,7 +14811,7 @@
       <c r="M31" s="69"/>
       <c r="N31" s="71"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="34">
         <v>101</v>
       </c>
@@ -14844,7 +14844,7 @@
       </c>
       <c r="M32" s="36"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="34">
         <v>102</v>
       </c>
@@ -14877,7 +14877,7 @@
       </c>
       <c r="M33" s="36"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="34">
         <v>103</v>
       </c>
@@ -14910,7 +14910,7 @@
       </c>
       <c r="M34" s="36"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="34">
         <v>104</v>
       </c>
@@ -14943,7 +14943,7 @@
       </c>
       <c r="M35" s="36"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="34">
         <v>105</v>
       </c>
@@ -14978,7 +14978,7 @@
       </c>
       <c r="M36" s="36"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="34">
         <v>106</v>
       </c>
@@ -15011,7 +15011,7 @@
       </c>
       <c r="M37" s="36"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="34">
         <v>107</v>
       </c>
@@ -15044,7 +15044,7 @@
       </c>
       <c r="M38" s="36"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="34">
         <v>108</v>
       </c>
@@ -15077,7 +15077,7 @@
       </c>
       <c r="M39" s="36"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="34">
         <v>109</v>
       </c>
@@ -15112,7 +15112,7 @@
       </c>
       <c r="M40" s="36"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="34">
         <v>110</v>
       </c>
@@ -15145,7 +15145,7 @@
       </c>
       <c r="M41" s="36"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="34">
         <v>111</v>
       </c>
@@ -15178,7 +15178,7 @@
       </c>
       <c r="M42" s="36"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="34">
         <v>112</v>
       </c>
@@ -15211,7 +15211,7 @@
       </c>
       <c r="M43" s="36"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="34">
         <v>113</v>
       </c>
@@ -15244,7 +15244,7 @@
       </c>
       <c r="M44" s="36"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="34">
         <v>114</v>
       </c>
@@ -15277,7 +15277,7 @@
       </c>
       <c r="M45" s="3"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="34">
         <v>115</v>
       </c>
@@ -15310,7 +15310,7 @@
       </c>
       <c r="M46" s="3"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="34">
         <v>116</v>
       </c>
@@ -15343,7 +15343,7 @@
       </c>
       <c r="M47" s="3"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="34">
         <v>117</v>
       </c>
@@ -15376,7 +15376,7 @@
       </c>
       <c r="M48" s="3"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="34">
         <v>118</v>
       </c>
@@ -15409,7 +15409,7 @@
       </c>
       <c r="M49" s="3"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="104">
         <v>119</v>
       </c>
@@ -15442,7 +15442,7 @@
       </c>
       <c r="M50" s="106"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="98">
         <v>120</v>
       </c>
@@ -15475,7 +15475,7 @@
       </c>
       <c r="M51" s="100"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="98">
         <v>121</v>
       </c>
@@ -15508,7 +15508,7 @@
       </c>
       <c r="M52" s="100"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" s="98">
         <v>122</v>
       </c>
@@ -15541,7 +15541,7 @@
       </c>
       <c r="M53" s="100"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="98">
         <v>123</v>
       </c>
@@ -15574,7 +15574,7 @@
       </c>
       <c r="M54" s="100"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" s="98">
         <v>124</v>
       </c>
@@ -15607,7 +15607,7 @@
       </c>
       <c r="M55" s="100"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" s="98">
         <v>125</v>
       </c>
@@ -15640,7 +15640,7 @@
       </c>
       <c r="M56" s="100"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" s="98">
         <v>126</v>
       </c>

</xml_diff>

<commit_message>
fix unique key direct_orgs and loops
</commit_message>
<xml_diff>
--- a/db/excel/api-function-granted-users-cdld.xlsx
+++ b/db/excel/api-function-granted-users-cdld.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10613"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCBD7AF9-849E-7445-B981-79FC78909D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688BC41E-C904-2348-8439-604712CD97FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19460" tabRatio="800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19460" tabRatio="800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_types" sheetId="27" r:id="rId1"/>
@@ -6797,11 +6797,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P98"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C68" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F94" sqref="F94"/>
+      <selection pane="bottomRight" activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7833,7 +7833,9 @@
       <c r="I31" s="97">
         <v>1</v>
       </c>
-      <c r="J31" s="97"/>
+      <c r="J31" s="97">
+        <v>1</v>
+      </c>
       <c r="K31" s="97"/>
       <c r="L31" s="97"/>
       <c r="M31" s="97"/>
@@ -8215,7 +8217,9 @@
       <c r="I43" s="55">
         <v>1</v>
       </c>
-      <c r="J43" s="55"/>
+      <c r="J43" s="55">
+        <v>1</v>
+      </c>
       <c r="K43" s="55"/>
       <c r="L43" s="55"/>
       <c r="M43" s="55"/>
@@ -10014,7 +10018,7 @@
   </sheetPr>
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add bg to direct meeting and dir org view
</commit_message>
<xml_diff>
--- a/db/excel/api-function-granted-users-cdld.xlsx
+++ b/db/excel/api-function-granted-users-cdld.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10613"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63034DE9-A62E-7244-9DFF-2DB1BFC17509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0BC50B-401D-554C-9DB4-BEAA0381D653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" tabRatio="800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19460" tabRatio="800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_types" sheetId="27" r:id="rId1"/>
@@ -301,7 +301,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1714" uniqueCount="678">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1708" uniqueCount="675">
   <si>
     <t>status</t>
   </si>
@@ -1434,9 +1434,6 @@
     <t>Gia Hạn Lần 1</t>
   </si>
   <si>
-    <t>Gia Hạn Lần 2</t>
-  </si>
-  <si>
     <t>Chỉ Đạo mới được cập nhập và phân cho đơn vị</t>
   </si>
   <si>
@@ -1446,9 +1443,6 @@
     <t>Đơn vị xin gia hạn lần 1</t>
   </si>
   <si>
-    <t>Đơn vị xin gia hạn lần 2</t>
-  </si>
-  <si>
     <t>CMPLT</t>
   </si>
   <si>
@@ -1885,9 +1879,6 @@
   </si>
   <si>
     <t>EXTEND1</t>
-  </si>
-  <si>
-    <t>EXTEND2</t>
   </si>
   <si>
     <t>Chỉ đạo nào là lặp lại thì lưu riêng vào bảng này, mỗi tháng dựa vào cái này để tạo mới bảng directs</t>
@@ -5322,7 +5313,7 @@
         <v>39</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>25</v>
@@ -5339,16 +5330,16 @@
         <v>99</v>
       </c>
       <c r="B2" s="94" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="C2" s="94" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D2" s="93" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="E2" s="93" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="F2" s="93">
         <v>1</v>
@@ -5359,16 +5350,16 @@
         <v>21</v>
       </c>
       <c r="B3" s="92" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="C3" s="92" t="s">
+        <v>431</v>
+      </c>
+      <c r="D3" s="91" t="s">
+        <v>432</v>
+      </c>
+      <c r="E3" s="91" t="s">
         <v>433</v>
-      </c>
-      <c r="D3" s="91" t="s">
-        <v>434</v>
-      </c>
-      <c r="E3" s="91" t="s">
-        <v>435</v>
       </c>
       <c r="F3" s="91">
         <v>1</v>
@@ -5465,7 +5456,7 @@
         <v>344</v>
       </c>
       <c r="D2" s="88" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E2" s="89" t="s">
         <v>344</v>
@@ -5477,7 +5468,7 @@
         <v>345</v>
       </c>
       <c r="H2" s="88" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="I2" s="88"/>
       <c r="J2" s="88"/>
@@ -5506,7 +5497,7 @@
       </c>
       <c r="F3" s="85"/>
       <c r="G3" s="85" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H3" s="84" t="s">
         <v>350</v>
@@ -5538,7 +5529,7 @@
       </c>
       <c r="F4" s="85"/>
       <c r="G4" s="85" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="H4" s="84" t="s">
         <v>351</v>
@@ -5570,7 +5561,7 @@
       </c>
       <c r="F5" s="85"/>
       <c r="G5" s="85" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="H5" s="84" t="s">
         <v>352</v>
@@ -5602,7 +5593,7 @@
       </c>
       <c r="F6" s="85"/>
       <c r="G6" s="85" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="H6" s="84" t="s">
         <v>354</v>
@@ -5634,7 +5625,7 @@
       </c>
       <c r="F7" s="85"/>
       <c r="G7" s="85" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="H7" s="84" t="s">
         <v>356</v>
@@ -5666,7 +5657,7 @@
       </c>
       <c r="F8" s="85"/>
       <c r="G8" s="85" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="H8" s="84" t="s">
         <v>361</v>
@@ -5691,19 +5682,19 @@
         <v>357</v>
       </c>
       <c r="D9" s="88" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="E9" s="89" t="s">
         <v>357</v>
       </c>
       <c r="F9" s="89" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="G9" s="89" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="H9" s="88" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="I9" s="88"/>
       <c r="J9" s="88"/>
@@ -5732,10 +5723,10 @@
       </c>
       <c r="F10" s="85"/>
       <c r="G10" s="85" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="H10" s="84" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="I10" s="84"/>
       <c r="J10" s="86"/>
@@ -5760,14 +5751,14 @@
       </c>
       <c r="D11" s="84"/>
       <c r="E11" s="85" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="F11" s="85"/>
       <c r="G11" s="85" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="H11" s="84" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I11" s="84"/>
       <c r="J11" s="84"/>
@@ -5792,14 +5783,14 @@
       </c>
       <c r="D12" s="84"/>
       <c r="E12" s="85" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="F12" s="85"/>
       <c r="G12" s="85" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="H12" s="84" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="I12" s="84"/>
       <c r="J12" s="84"/>
@@ -5820,18 +5811,18 @@
         <v>2</v>
       </c>
       <c r="C13" s="84" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D13" s="84"/>
       <c r="E13" s="85" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="F13" s="85"/>
       <c r="G13" s="85" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="H13" s="84" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="I13" s="84"/>
       <c r="J13" s="84"/>
@@ -5850,22 +5841,22 @@
       </c>
       <c r="B14" s="88"/>
       <c r="C14" s="88" t="s">
+        <v>406</v>
+      </c>
+      <c r="D14" s="88" t="s">
         <v>408</v>
       </c>
-      <c r="D14" s="88" t="s">
-        <v>410</v>
-      </c>
       <c r="E14" s="89" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="F14" s="89" t="s">
+        <v>436</v>
+      </c>
+      <c r="G14" s="89" t="s">
+        <v>426</v>
+      </c>
+      <c r="H14" s="88" t="s">
         <v>438</v>
-      </c>
-      <c r="G14" s="89" t="s">
-        <v>428</v>
-      </c>
-      <c r="H14" s="88" t="s">
-        <v>440</v>
       </c>
       <c r="I14" s="88"/>
       <c r="J14" s="88"/>
@@ -5886,18 +5877,18 @@
         <v>3</v>
       </c>
       <c r="C15" s="84" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D15" s="84"/>
       <c r="E15" s="85" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="F15" s="85"/>
       <c r="G15" s="85" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="H15" s="84" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="I15" s="84"/>
       <c r="J15" s="86"/>
@@ -5916,20 +5907,20 @@
       </c>
       <c r="B16" s="88"/>
       <c r="C16" s="88" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D16" s="88"/>
       <c r="E16" s="89" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="F16" s="89" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="G16" s="89" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="H16" s="88" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="I16" s="88"/>
       <c r="J16" s="88"/>
@@ -5989,7 +5980,7 @@
         <v>39</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="F1" s="22" t="s">
         <v>140</v>
@@ -6024,7 +6015,7 @@
         <v>138</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="F2" s="30"/>
       <c r="G2" s="30"/>
@@ -6051,7 +6042,7 @@
         <v>138</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="F3" s="30"/>
       <c r="G3" s="30"/>
@@ -6078,7 +6069,7 @@
         <v>138</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="F4" s="28"/>
       <c r="G4" s="28"/>
@@ -6105,7 +6096,7 @@
         <v>138</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="F5" s="28"/>
       <c r="G5" s="28"/>
@@ -6166,10 +6157,10 @@
         <v>240</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="E1" s="40" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="F1" s="40" t="s">
         <v>180</v>
@@ -6198,13 +6189,13 @@
         <v>326</v>
       </c>
       <c r="C2" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="D2" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="E2" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="J2" t="s">
         <v>187</v>
@@ -6224,10 +6215,10 @@
         <v>325</v>
       </c>
       <c r="D3" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="E3" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -6247,13 +6238,13 @@
         <v>189</v>
       </c>
       <c r="C4" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="D4" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E4" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -6273,13 +6264,13 @@
         <v>188</v>
       </c>
       <c r="C5" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="D5" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="E5" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -6299,13 +6290,13 @@
         <v>191</v>
       </c>
       <c r="C6" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="D6" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="E6" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -6325,13 +6316,13 @@
         <v>193</v>
       </c>
       <c r="C7" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="D7" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="E7" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -6351,13 +6342,13 @@
         <v>195</v>
       </c>
       <c r="C8" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="D8" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="E8" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -6377,13 +6368,13 @@
         <v>196</v>
       </c>
       <c r="C9" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="D9" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="E9" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -6403,13 +6394,13 @@
         <v>197</v>
       </c>
       <c r="C10" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="D10" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="E10" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -6429,13 +6420,13 @@
         <v>194</v>
       </c>
       <c r="C11" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="D11" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="E11" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -6455,13 +6446,13 @@
         <v>192</v>
       </c>
       <c r="C12" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="D12" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="E12" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -6481,13 +6472,13 @@
         <v>198</v>
       </c>
       <c r="C13" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="D13" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="E13" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -6507,13 +6498,13 @@
         <v>199</v>
       </c>
       <c r="C14" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="D14" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="E14" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -6533,13 +6524,13 @@
         <v>200</v>
       </c>
       <c r="C15" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="D15" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="E15" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -6559,13 +6550,13 @@
         <v>201</v>
       </c>
       <c r="C16" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="D16" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="E16" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -6585,13 +6576,13 @@
         <v>202</v>
       </c>
       <c r="C17" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="D17" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="E17" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -6611,13 +6602,13 @@
         <v>203</v>
       </c>
       <c r="C18" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="D18" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="E18" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -6702,7 +6693,7 @@
         <v>229</v>
       </c>
       <c r="C4" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="E4" t="s">
         <v>187</v>
@@ -6716,7 +6707,7 @@
         <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E5" t="s">
         <v>187</v>
@@ -6744,7 +6735,7 @@
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="E7" t="s">
         <v>187</v>
@@ -6758,7 +6749,7 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="E8" t="s">
         <v>187</v>
@@ -6786,7 +6777,7 @@
         <v>155</v>
       </c>
       <c r="C10" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="E10" t="s">
         <v>187</v>
@@ -6800,7 +6791,7 @@
         <v>156</v>
       </c>
       <c r="C11" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="E11" t="s">
         <v>187</v>
@@ -6815,8 +6806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C74" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="D88" sqref="D88"/>
@@ -7004,7 +6995,7 @@
         <v>258</v>
       </c>
       <c r="D5" s="108" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="E5" s="108" t="s">
         <v>16</v>
@@ -7318,13 +7309,13 @@
         <v>219</v>
       </c>
       <c r="B15" s="51" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="C15" s="51" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="D15" s="51" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="E15" s="51" t="s">
         <v>16</v>
@@ -7338,7 +7329,7 @@
       <c r="J15" s="58"/>
       <c r="K15" s="58"/>
       <c r="L15" s="59" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="M15" s="58"/>
       <c r="N15" s="58"/>
@@ -7355,10 +7346,10 @@
         <v>316</v>
       </c>
       <c r="C16" s="51" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D16" s="51" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="E16" s="51" t="s">
         <v>15</v>
@@ -7426,7 +7417,7 @@
         <v>250</v>
       </c>
       <c r="D18" s="110" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="E18" s="110" t="s">
         <v>16</v>
@@ -7438,7 +7429,7 @@
       <c r="J18" s="58"/>
       <c r="K18" s="58"/>
       <c r="L18" s="59" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="M18" s="58"/>
       <c r="N18" s="58"/>
@@ -7452,13 +7443,13 @@
         <v>219</v>
       </c>
       <c r="B19" s="51" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C19" s="51" t="s">
+        <v>439</v>
+      </c>
+      <c r="D19" s="51" t="s">
         <v>441</v>
-      </c>
-      <c r="D19" s="51" t="s">
-        <v>443</v>
       </c>
       <c r="E19" s="51" t="s">
         <v>15</v>
@@ -7472,7 +7463,7 @@
       <c r="J19" s="58"/>
       <c r="K19" s="58"/>
       <c r="L19" s="59" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="M19" s="58"/>
       <c r="N19" s="58"/>
@@ -7614,13 +7605,13 @@
         <v>219</v>
       </c>
       <c r="B24" s="51" t="s">
+        <v>442</v>
+      </c>
+      <c r="C24" s="51" t="s">
+        <v>443</v>
+      </c>
+      <c r="D24" s="51" t="s">
         <v>444</v>
-      </c>
-      <c r="C24" s="51" t="s">
-        <v>445</v>
-      </c>
-      <c r="D24" s="51" t="s">
-        <v>446</v>
       </c>
       <c r="E24" s="51" t="s">
         <v>50</v>
@@ -7768,13 +7759,13 @@
         <v>219</v>
       </c>
       <c r="B29" s="51" t="s">
+        <v>445</v>
+      </c>
+      <c r="C29" s="51" t="s">
+        <v>446</v>
+      </c>
+      <c r="D29" s="51" t="s">
         <v>447</v>
-      </c>
-      <c r="C29" s="51" t="s">
-        <v>448</v>
-      </c>
-      <c r="D29" s="51" t="s">
-        <v>449</v>
       </c>
       <c r="E29" s="51" t="s">
         <v>15</v>
@@ -7800,13 +7791,13 @@
         <v>219</v>
       </c>
       <c r="B30" s="51" t="s">
+        <v>485</v>
+      </c>
+      <c r="C30" s="51" t="s">
+        <v>486</v>
+      </c>
+      <c r="D30" s="51" t="s">
         <v>487</v>
-      </c>
-      <c r="C30" s="51" t="s">
-        <v>488</v>
-      </c>
-      <c r="D30" s="51" t="s">
-        <v>489</v>
       </c>
       <c r="E30" s="51" t="s">
         <v>15</v>
@@ -7838,7 +7829,7 @@
         <v>234</v>
       </c>
       <c r="D31" s="51" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="E31" s="51" t="s">
         <v>17</v>
@@ -7861,7 +7852,7 @@
     </row>
     <row r="32" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="96" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B32" s="96" t="s">
         <v>18</v>
@@ -7870,7 +7861,7 @@
         <v>241</v>
       </c>
       <c r="D32" s="96" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="E32" s="96" t="s">
         <v>97</v>
@@ -7899,16 +7890,16 @@
     </row>
     <row r="33" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="96" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B33" s="96" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="C33" s="96" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="D33" s="96" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="E33" s="96" t="s">
         <v>16</v>
@@ -7929,16 +7920,16 @@
     </row>
     <row r="34" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="96" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B34" s="96" t="s">
         <v>220</v>
       </c>
       <c r="C34" s="96" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="D34" s="96" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="E34" s="96" t="s">
         <v>16</v>
@@ -7959,16 +7950,16 @@
     </row>
     <row r="35" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="96" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B35" s="96" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="C35" s="96" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="D35" s="96" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="E35" s="96" t="s">
         <v>15</v>
@@ -7982,7 +7973,7 @@
       <c r="J35" s="97"/>
       <c r="K35" s="97"/>
       <c r="L35" s="59" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="M35" s="97"/>
       <c r="N35" s="97"/>
@@ -7993,7 +7984,7 @@
     </row>
     <row r="36" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="96" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B36" s="96" t="s">
         <v>225</v>
@@ -8002,7 +7993,7 @@
         <v>268</v>
       </c>
       <c r="D36" s="96" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="E36" s="96" t="s">
         <v>15</v>
@@ -8025,7 +8016,7 @@
     </row>
     <row r="37" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="96" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B37" s="96" t="s">
         <v>226</v>
@@ -8034,7 +8025,7 @@
         <v>269</v>
       </c>
       <c r="D37" s="96" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="E37" s="96" t="s">
         <v>15</v>
@@ -8057,16 +8048,16 @@
     </row>
     <row r="38" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="96" t="s">
+        <v>510</v>
+      </c>
+      <c r="B38" s="96" t="s">
+        <v>511</v>
+      </c>
+      <c r="C38" s="96" t="s">
         <v>512</v>
       </c>
-      <c r="B38" s="96" t="s">
+      <c r="D38" s="96" t="s">
         <v>513</v>
-      </c>
-      <c r="C38" s="96" t="s">
-        <v>514</v>
-      </c>
-      <c r="D38" s="96" t="s">
-        <v>515</v>
       </c>
       <c r="E38" s="96" t="s">
         <v>15</v>
@@ -8089,16 +8080,16 @@
     </row>
     <row r="39" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="96" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B39" s="96" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="C39" s="96" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="D39" s="96" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="E39" s="96" t="s">
         <v>97</v>
@@ -8119,7 +8110,7 @@
     </row>
     <row r="40" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="96" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B40" s="96" t="s">
         <v>204</v>
@@ -8149,7 +8140,7 @@
     </row>
     <row r="41" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="96" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B41" s="96" t="s">
         <v>229</v>
@@ -8181,7 +8172,7 @@
     </row>
     <row r="42" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="96" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B42" s="96" t="s">
         <v>19</v>
@@ -8211,7 +8202,7 @@
     </row>
     <row r="43" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="96" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B43" s="96" t="s">
         <v>45</v>
@@ -8243,7 +8234,7 @@
     </row>
     <row r="44" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="96" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B44" s="96" t="s">
         <v>0</v>
@@ -8252,7 +8243,7 @@
         <v>234</v>
       </c>
       <c r="D44" s="96" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="E44" s="96" t="s">
         <v>17</v>
@@ -8319,10 +8310,10 @@
         <v>316</v>
       </c>
       <c r="C46" s="50" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="D46" s="50" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="E46" s="50" t="s">
         <v>15</v>
@@ -8352,13 +8343,13 @@
         <v>274</v>
       </c>
       <c r="B47" s="50" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="C47" s="50" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="D47" s="50" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="E47" s="50" t="s">
         <v>16</v>
@@ -8370,7 +8361,7 @@
       <c r="J47" s="55"/>
       <c r="K47" s="55"/>
       <c r="L47" s="59" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="M47" s="55"/>
       <c r="N47" s="55"/>
@@ -8402,7 +8393,7 @@
       <c r="J48" s="55"/>
       <c r="K48" s="55"/>
       <c r="L48" s="59" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="M48" s="55"/>
       <c r="N48" s="55"/>
@@ -8416,13 +8407,13 @@
         <v>274</v>
       </c>
       <c r="B49" s="50" t="s">
+        <v>562</v>
+      </c>
+      <c r="C49" s="50" t="s">
         <v>565</v>
       </c>
-      <c r="C49" s="50" t="s">
-        <v>568</v>
-      </c>
       <c r="D49" s="50" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="E49" s="50" t="s">
         <v>15</v>
@@ -8436,7 +8427,7 @@
       <c r="J49" s="55"/>
       <c r="K49" s="55"/>
       <c r="L49" s="59" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="M49" s="55"/>
       <c r="N49" s="55"/>
@@ -8468,7 +8459,7 @@
       <c r="J50" s="55"/>
       <c r="K50" s="55"/>
       <c r="L50" s="59" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="M50" s="55"/>
       <c r="N50" s="55"/>
@@ -8488,7 +8479,7 @@
         <v>280</v>
       </c>
       <c r="D51" s="50" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="E51" s="50" t="s">
         <v>16</v>
@@ -8544,13 +8535,13 @@
         <v>274</v>
       </c>
       <c r="B53" s="108" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="C53" s="108" t="s">
         <v>272</v>
       </c>
       <c r="D53" s="108" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E53" s="108" t="s">
         <v>16</v>
@@ -8562,7 +8553,7 @@
       <c r="J53" s="109"/>
       <c r="K53" s="109"/>
       <c r="L53" s="59" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="M53" s="109"/>
       <c r="N53" s="109"/>
@@ -8576,13 +8567,13 @@
         <v>274</v>
       </c>
       <c r="B54" s="50" t="s">
+        <v>445</v>
+      </c>
+      <c r="C54" s="50" t="s">
+        <v>446</v>
+      </c>
+      <c r="D54" s="50" t="s">
         <v>447</v>
-      </c>
-      <c r="C54" s="50" t="s">
-        <v>448</v>
-      </c>
-      <c r="D54" s="50" t="s">
-        <v>449</v>
       </c>
       <c r="E54" s="50" t="s">
         <v>15</v>
@@ -8608,13 +8599,13 @@
         <v>274</v>
       </c>
       <c r="B55" s="50" t="s">
+        <v>482</v>
+      </c>
+      <c r="C55" s="50" t="s">
+        <v>483</v>
+      </c>
+      <c r="D55" s="50" t="s">
         <v>484</v>
-      </c>
-      <c r="C55" s="50" t="s">
-        <v>485</v>
-      </c>
-      <c r="D55" s="50" t="s">
-        <v>486</v>
       </c>
       <c r="E55" s="50" t="s">
         <v>15</v>
@@ -8640,13 +8631,13 @@
         <v>274</v>
       </c>
       <c r="B56" s="50" t="s">
+        <v>442</v>
+      </c>
+      <c r="C56" s="50" t="s">
+        <v>443</v>
+      </c>
+      <c r="D56" s="50" t="s">
         <v>444</v>
-      </c>
-      <c r="C56" s="50" t="s">
-        <v>445</v>
-      </c>
-      <c r="D56" s="50" t="s">
-        <v>446</v>
       </c>
       <c r="E56" s="50" t="s">
         <v>50</v>
@@ -8673,10 +8664,10 @@
         <v>227</v>
       </c>
       <c r="C57" s="118" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="D57" s="118" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="E57" s="118" t="s">
         <v>15</v>
@@ -8832,7 +8823,7 @@
         <v>234</v>
       </c>
       <c r="D62" s="50" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="E62" s="50" t="s">
         <v>17</v>
@@ -8899,10 +8890,10 @@
         <v>316</v>
       </c>
       <c r="C64" s="52" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="D64" s="52" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="E64" s="52" t="s">
         <v>15</v>
@@ -8932,13 +8923,13 @@
         <v>273</v>
       </c>
       <c r="B65" s="52" t="s">
+        <v>562</v>
+      </c>
+      <c r="C65" s="52" t="s">
         <v>565</v>
       </c>
-      <c r="C65" s="52" t="s">
+      <c r="D65" s="52" t="s">
         <v>568</v>
-      </c>
-      <c r="D65" s="52" t="s">
-        <v>571</v>
       </c>
       <c r="E65" s="52" t="s">
         <v>15</v>
@@ -8952,7 +8943,7 @@
       <c r="J65" s="46"/>
       <c r="K65" s="46"/>
       <c r="L65" s="59" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="M65" s="46"/>
       <c r="N65" s="46"/>
@@ -8966,10 +8957,10 @@
         <v>273</v>
       </c>
       <c r="B66" s="52" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="C66" s="52" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="D66" s="52" t="s">
         <v>284</v>
@@ -8986,7 +8977,7 @@
       <c r="J66" s="46"/>
       <c r="K66" s="46"/>
       <c r="L66" s="59" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="M66" s="46"/>
       <c r="N66" s="46"/>
@@ -9020,7 +9011,7 @@
       <c r="J67" s="46"/>
       <c r="K67" s="46"/>
       <c r="L67" s="59" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="M67" s="46"/>
       <c r="N67" s="46"/>
@@ -9104,7 +9095,7 @@
         <v>289</v>
       </c>
       <c r="D70" s="113" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="E70" s="112" t="s">
         <v>16</v>
@@ -9116,7 +9107,7 @@
       <c r="J70" s="46"/>
       <c r="K70" s="46"/>
       <c r="L70" s="59" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="M70" s="46"/>
       <c r="N70" s="46"/>
@@ -9230,7 +9221,7 @@
         <v>236</v>
       </c>
       <c r="D74" s="52" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E74" s="52" t="s">
         <v>50</v>
@@ -9289,10 +9280,10 @@
         <v>0</v>
       </c>
       <c r="C76" s="52" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D76" s="52" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="E76" s="52" t="s">
         <v>17</v>
@@ -9359,10 +9350,10 @@
         <v>316</v>
       </c>
       <c r="C78" s="53" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D78" s="53" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="E78" s="53" t="s">
         <v>15</v>
@@ -9398,7 +9389,7 @@
         <v>244</v>
       </c>
       <c r="D79" s="115" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="E79" s="115" t="s">
         <v>16</v>
@@ -9410,7 +9401,7 @@
       <c r="J79" s="60"/>
       <c r="K79" s="60"/>
       <c r="L79" s="59" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="M79" s="60"/>
       <c r="N79" s="60"/>
@@ -9747,10 +9738,10 @@
         <v>139</v>
       </c>
       <c r="C90" s="44" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D90" s="61" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E90" s="61" t="s">
         <v>16</v>
@@ -9776,13 +9767,13 @@
         <v>169</v>
       </c>
       <c r="B91" s="44" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="C91" s="44" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="D91" s="61" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="E91" s="61" t="s">
         <v>15</v>
@@ -9906,13 +9897,13 @@
         <v>169</v>
       </c>
       <c r="B95" s="44" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="C95" s="44" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="D95" s="61" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="E95" s="61" t="s">
         <v>15</v>
@@ -9938,13 +9929,13 @@
         <v>169</v>
       </c>
       <c r="B96" s="44" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="C96" s="44" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="D96" s="61" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="E96" s="61" t="s">
         <v>15</v>
@@ -10132,10 +10123,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10161,7 +10152,7 @@
         <v>139</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="D1" s="39" t="s">
         <v>240</v>
@@ -10173,10 +10164,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="39" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="H1" s="39" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="I1" s="39" t="s">
         <v>204</v>
@@ -10197,7 +10188,7 @@
       </c>
       <c r="B2" s="90"/>
       <c r="C2" s="90" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D2" s="90" t="s">
         <v>362</v>
@@ -10209,10 +10200,10 @@
         <v>368</v>
       </c>
       <c r="G2" s="90" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="H2" s="90" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="I2" s="90"/>
       <c r="J2" s="90"/>
@@ -10237,13 +10228,13 @@
         <v>364</v>
       </c>
       <c r="F3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G3" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="H3" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K3" t="s">
         <v>187</v>
@@ -10266,13 +10257,13 @@
         <v>367</v>
       </c>
       <c r="F4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G4" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="H4" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K4" t="s">
         <v>187</v>
@@ -10289,19 +10280,19 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
+        <v>373</v>
+      </c>
+      <c r="E5" t="s">
+        <v>374</v>
+      </c>
+      <c r="F5" t="s">
         <v>375</v>
       </c>
-      <c r="E5" t="s">
-        <v>376</v>
-      </c>
-      <c r="F5" t="s">
-        <v>377</v>
-      </c>
       <c r="G5" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="H5" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K5" t="s">
         <v>187</v>
@@ -10318,19 +10309,19 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="E6" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="F6" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="G6" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="H6" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K6" t="s">
         <v>187</v>
@@ -10347,19 +10338,19 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="E7" t="s">
         <v>369</v>
       </c>
       <c r="F7" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G7" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="H7" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K7" t="s">
         <v>187</v>
@@ -10369,87 +10360,87 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>16</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>521</v>
-      </c>
-      <c r="E8" t="s">
-        <v>370</v>
-      </c>
-      <c r="F8" t="s">
-        <v>374</v>
-      </c>
-      <c r="G8" t="s">
-        <v>556</v>
-      </c>
-      <c r="H8" t="s">
-        <v>656</v>
-      </c>
-      <c r="K8" t="s">
+      <c r="A8" s="90">
+        <v>2</v>
+      </c>
+      <c r="B8" s="90"/>
+      <c r="C8" s="90" t="s">
+        <v>641</v>
+      </c>
+      <c r="D8" s="90" t="s">
+        <v>376</v>
+      </c>
+      <c r="E8" s="90" t="s">
+        <v>377</v>
+      </c>
+      <c r="F8" s="90" t="s">
+        <v>384</v>
+      </c>
+      <c r="G8" s="90" t="s">
+        <v>554</v>
+      </c>
+      <c r="H8" s="90" t="s">
+        <v>653</v>
+      </c>
+      <c r="I8" s="90"/>
+      <c r="J8" s="90"/>
+      <c r="K8" s="90" t="s">
         <v>187</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="90">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="90">
+      <c r="A9">
+        <v>21</v>
+      </c>
+      <c r="B9">
         <v>2</v>
       </c>
-      <c r="B9" s="90"/>
-      <c r="C9" s="90" t="s">
-        <v>644</v>
-      </c>
-      <c r="D9" s="90" t="s">
+      <c r="D9" t="s">
         <v>378</v>
       </c>
-      <c r="E9" s="90" t="s">
-        <v>379</v>
-      </c>
-      <c r="F9" s="90" t="s">
-        <v>386</v>
-      </c>
-      <c r="G9" s="90" t="s">
-        <v>557</v>
-      </c>
-      <c r="H9" s="90" t="s">
-        <v>656</v>
-      </c>
-      <c r="I9" s="90"/>
-      <c r="J9" s="90"/>
-      <c r="K9" s="90" t="s">
+      <c r="E9" t="s">
+        <v>381</v>
+      </c>
+      <c r="F9" t="s">
+        <v>382</v>
+      </c>
+      <c r="G9" t="s">
+        <v>552</v>
+      </c>
+      <c r="H9" t="s">
+        <v>653</v>
+      </c>
+      <c r="K9" t="s">
         <v>187</v>
       </c>
-      <c r="L9" s="90">
+      <c r="L9">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
       <c r="D10" t="s">
+        <v>379</v>
+      </c>
+      <c r="E10" t="s">
         <v>380</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>383</v>
       </c>
-      <c r="F10" t="s">
-        <v>384</v>
-      </c>
       <c r="G10" t="s">
-        <v>555</v>
+        <v>548</v>
       </c>
       <c r="H10" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K10" t="s">
         <v>187</v>
@@ -10459,87 +10450,87 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>22</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="D11" t="s">
-        <v>381</v>
-      </c>
-      <c r="E11" t="s">
-        <v>382</v>
-      </c>
-      <c r="F11" t="s">
-        <v>385</v>
-      </c>
-      <c r="G11" t="s">
-        <v>551</v>
-      </c>
-      <c r="H11" t="s">
-        <v>656</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="A11" s="90">
+        <v>3</v>
+      </c>
+      <c r="B11" s="90"/>
+      <c r="C11" s="90" t="s">
+        <v>642</v>
+      </c>
+      <c r="D11" s="90" t="s">
+        <v>473</v>
+      </c>
+      <c r="E11" s="90" t="s">
+        <v>387</v>
+      </c>
+      <c r="F11" s="90" t="s">
+        <v>388</v>
+      </c>
+      <c r="G11" s="90" t="s">
+        <v>547</v>
+      </c>
+      <c r="H11" s="90" t="s">
+        <v>653</v>
+      </c>
+      <c r="I11" s="90"/>
+      <c r="J11" s="90"/>
+      <c r="K11" s="90" t="s">
         <v>187</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="90">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="90">
+      <c r="A12">
+        <v>31</v>
+      </c>
+      <c r="B12">
         <v>3</v>
       </c>
-      <c r="B12" s="90"/>
-      <c r="C12" s="90" t="s">
-        <v>645</v>
-      </c>
-      <c r="D12" s="90" t="s">
-        <v>475</v>
-      </c>
-      <c r="E12" s="90" t="s">
+      <c r="D12" t="s">
+        <v>580</v>
+      </c>
+      <c r="E12" t="s">
+        <v>630</v>
+      </c>
+      <c r="F12" t="s">
         <v>389</v>
       </c>
-      <c r="F12" s="90" t="s">
-        <v>390</v>
-      </c>
-      <c r="G12" s="90" t="s">
-        <v>550</v>
-      </c>
-      <c r="H12" s="90" t="s">
-        <v>656</v>
-      </c>
-      <c r="I12" s="90"/>
-      <c r="J12" s="90"/>
-      <c r="K12" s="90" t="s">
+      <c r="G12" t="s">
+        <v>658</v>
+      </c>
+      <c r="H12" t="s">
+        <v>653</v>
+      </c>
+      <c r="K12" t="s">
         <v>187</v>
       </c>
-      <c r="L12" s="90">
+      <c r="L12">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B13">
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="E13" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="F13" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G13" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="H13" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K13" t="s">
         <v>187</v>
@@ -10550,25 +10541,25 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B14">
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="E14" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="F14" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G14" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="H14" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K14" t="s">
         <v>187</v>
@@ -10579,25 +10570,25 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B15">
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="E15" t="s">
-        <v>635</v>
+        <v>646</v>
       </c>
       <c r="F15" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G15" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="H15" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K15" t="s">
         <v>187</v>
@@ -10608,25 +10599,25 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B16">
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="E16" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="F16" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G16" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="H16" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K16" t="s">
         <v>187</v>
@@ -10637,25 +10628,25 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B17">
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E17" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="F17" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G17" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="H17" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K17" t="s">
         <v>187</v>
@@ -10665,87 +10656,87 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>36</v>
-      </c>
-      <c r="B18">
-        <v>3</v>
-      </c>
-      <c r="D18" t="s">
-        <v>588</v>
-      </c>
-      <c r="E18" t="s">
-        <v>651</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="A18" s="90">
+        <v>4</v>
+      </c>
+      <c r="B18" s="90"/>
+      <c r="C18" s="90" t="s">
+        <v>643</v>
+      </c>
+      <c r="D18" s="90" t="s">
+        <v>474</v>
+      </c>
+      <c r="E18" s="90" t="s">
+        <v>395</v>
+      </c>
+      <c r="F18" s="90" t="s">
         <v>396</v>
       </c>
-      <c r="G18" t="s">
-        <v>666</v>
-      </c>
-      <c r="H18" t="s">
-        <v>656</v>
-      </c>
-      <c r="K18" t="s">
+      <c r="G18" s="90" t="s">
+        <v>554</v>
+      </c>
+      <c r="H18" s="90" t="s">
+        <v>653</v>
+      </c>
+      <c r="I18" s="90"/>
+      <c r="J18" s="90"/>
+      <c r="K18" s="90" t="s">
         <v>187</v>
       </c>
-      <c r="L18">
+      <c r="L18" s="90">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="90">
+      <c r="A19">
+        <v>41</v>
+      </c>
+      <c r="B19">
         <v>4</v>
       </c>
-      <c r="B19" s="90"/>
-      <c r="C19" s="90" t="s">
-        <v>646</v>
-      </c>
-      <c r="D19" s="90" t="s">
-        <v>476</v>
-      </c>
-      <c r="E19" s="90" t="s">
+      <c r="D19" t="s">
+        <v>576</v>
+      </c>
+      <c r="E19" t="s">
         <v>397</v>
       </c>
-      <c r="F19" s="90" t="s">
-        <v>398</v>
-      </c>
-      <c r="G19" s="90" t="s">
-        <v>557</v>
-      </c>
-      <c r="H19" s="90" t="s">
-        <v>656</v>
-      </c>
-      <c r="I19" s="90"/>
-      <c r="J19" s="90"/>
-      <c r="K19" s="90" t="s">
+      <c r="F19" t="s">
+        <v>397</v>
+      </c>
+      <c r="G19" t="s">
+        <v>663</v>
+      </c>
+      <c r="H19" t="s">
+        <v>653</v>
+      </c>
+      <c r="K19" t="s">
         <v>187</v>
       </c>
-      <c r="L19" s="90">
+      <c r="L19">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B20">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="E20" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F20" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G20" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="H20" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K20" t="s">
         <v>187</v>
@@ -10756,25 +10747,25 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B21">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="E21" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F21" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G21" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="H21" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K21" t="s">
         <v>187</v>
@@ -10785,25 +10776,25 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B22">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="E22" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F22" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G22" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="H22" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K22" t="s">
         <v>187</v>
@@ -10813,87 +10804,87 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>44</v>
-      </c>
-      <c r="B23">
-        <v>4</v>
-      </c>
-      <c r="D23" t="s">
-        <v>582</v>
-      </c>
-      <c r="E23" t="s">
-        <v>402</v>
-      </c>
-      <c r="F23" t="s">
-        <v>402</v>
-      </c>
-      <c r="G23" t="s">
-        <v>669</v>
-      </c>
-      <c r="H23" t="s">
-        <v>656</v>
-      </c>
-      <c r="K23" t="s">
+      <c r="A23" s="90">
+        <v>5</v>
+      </c>
+      <c r="B23" s="90"/>
+      <c r="C23" s="90" t="s">
+        <v>644</v>
+      </c>
+      <c r="D23" s="90" t="s">
+        <v>450</v>
+      </c>
+      <c r="E23" s="90" t="s">
+        <v>451</v>
+      </c>
+      <c r="F23" s="90" t="s">
+        <v>396</v>
+      </c>
+      <c r="G23" s="90" t="s">
+        <v>549</v>
+      </c>
+      <c r="H23" s="90" t="s">
+        <v>653</v>
+      </c>
+      <c r="I23" s="90"/>
+      <c r="J23" s="90"/>
+      <c r="K23" s="90" t="s">
         <v>187</v>
       </c>
-      <c r="L23">
+      <c r="L23" s="90">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="90">
+      <c r="A24">
+        <v>51</v>
+      </c>
+      <c r="B24">
         <v>5</v>
       </c>
-      <c r="B24" s="90"/>
-      <c r="C24" s="90" t="s">
-        <v>647</v>
-      </c>
-      <c r="D24" s="90" t="s">
-        <v>452</v>
-      </c>
-      <c r="E24" s="90" t="s">
-        <v>453</v>
-      </c>
-      <c r="F24" s="90" t="s">
-        <v>398</v>
-      </c>
-      <c r="G24" s="90" t="s">
-        <v>552</v>
-      </c>
-      <c r="H24" s="90" t="s">
-        <v>656</v>
-      </c>
-      <c r="I24" s="90"/>
-      <c r="J24" s="90"/>
-      <c r="K24" s="90" t="s">
+      <c r="D24" t="s">
+        <v>507</v>
+      </c>
+      <c r="E24" t="s">
+        <v>508</v>
+      </c>
+      <c r="F24" t="s">
+        <v>509</v>
+      </c>
+      <c r="G24" t="s">
+        <v>550</v>
+      </c>
+      <c r="H24" t="s">
+        <v>653</v>
+      </c>
+      <c r="K24" t="s">
         <v>187</v>
       </c>
-      <c r="L24" s="90">
+      <c r="L24">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B25">
         <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>509</v>
+        <v>452</v>
       </c>
       <c r="E25" t="s">
-        <v>510</v>
+        <v>458</v>
       </c>
       <c r="F25" t="s">
-        <v>511</v>
+        <v>453</v>
       </c>
       <c r="G25" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="H25" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K25" t="s">
         <v>187</v>
@@ -10904,7 +10895,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B26">
         <v>5</v>
@@ -10913,16 +10904,16 @@
         <v>454</v>
       </c>
       <c r="E26" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F26" t="s">
         <v>455</v>
       </c>
       <c r="G26" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="H26" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K26" t="s">
         <v>187</v>
@@ -10933,7 +10924,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B27">
         <v>5</v>
@@ -10942,16 +10933,16 @@
         <v>456</v>
       </c>
       <c r="E27" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F27" t="s">
         <v>457</v>
       </c>
       <c r="G27" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="H27" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K27" t="s">
         <v>187</v>
@@ -10962,25 +10953,25 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B28">
         <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="E28" t="s">
         <v>462</v>
       </c>
       <c r="F28" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="G28" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="H28" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K28" t="s">
         <v>187</v>
@@ -10991,25 +10982,25 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B29">
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="E29" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="F29" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="G29" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="H29" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K29" t="s">
         <v>187</v>
@@ -11020,25 +11011,25 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B30">
         <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="E30" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="F30" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="G30" t="s">
-        <v>555</v>
+        <v>548</v>
       </c>
       <c r="H30" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K30" t="s">
         <v>187</v>
@@ -11049,54 +11040,54 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B31">
         <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="E31" t="s">
+        <v>471</v>
+      </c>
+      <c r="F31" t="s">
         <v>470</v>
       </c>
-      <c r="F31" t="s">
-        <v>471</v>
-      </c>
       <c r="G31" t="s">
-        <v>551</v>
+        <v>555</v>
       </c>
       <c r="H31" t="s">
-        <v>656</v>
-      </c>
-      <c r="K31" t="s">
+        <v>653</v>
+      </c>
+      <c r="K31" s="95" t="s">
         <v>187</v>
       </c>
-      <c r="L31">
+      <c r="L31" s="95">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B32">
         <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>474</v>
+        <v>481</v>
       </c>
       <c r="E32" t="s">
-        <v>473</v>
+        <v>499</v>
       </c>
       <c r="F32" t="s">
-        <v>472</v>
+        <v>500</v>
       </c>
       <c r="G32" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="H32" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K32" s="95" t="s">
         <v>187</v>
@@ -11107,25 +11098,25 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>59</v>
+        <v>510</v>
       </c>
       <c r="B33">
         <v>5</v>
       </c>
       <c r="D33" t="s">
-        <v>483</v>
+        <v>496</v>
       </c>
       <c r="E33" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="F33" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="G33" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="H33" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K33" s="95" t="s">
         <v>187</v>
@@ -11136,25 +11127,25 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B34">
         <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>498</v>
+        <v>488</v>
       </c>
       <c r="E34" t="s">
-        <v>499</v>
+        <v>489</v>
       </c>
       <c r="F34" t="s">
-        <v>500</v>
+        <v>490</v>
       </c>
       <c r="G34" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="H34" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K34" s="95" t="s">
         <v>187</v>
@@ -11165,25 +11156,25 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B35">
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>490</v>
+        <v>475</v>
       </c>
       <c r="E35" t="s">
-        <v>491</v>
+        <v>477</v>
       </c>
       <c r="F35" t="s">
-        <v>492</v>
+        <v>478</v>
       </c>
       <c r="G35" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="H35" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K35" s="95" t="s">
         <v>187</v>
@@ -11194,25 +11185,25 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B36">
         <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="E36" t="s">
+        <v>374</v>
+      </c>
+      <c r="F36" t="s">
         <v>479</v>
       </c>
-      <c r="F36" t="s">
-        <v>480</v>
-      </c>
       <c r="G36" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="H36" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K36" s="95" t="s">
         <v>187</v>
@@ -11223,25 +11214,25 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B37">
         <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>478</v>
+        <v>491</v>
       </c>
       <c r="E37" t="s">
-        <v>376</v>
+        <v>492</v>
       </c>
       <c r="F37" t="s">
-        <v>481</v>
+        <v>493</v>
       </c>
       <c r="G37" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="H37" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K37" s="95" t="s">
         <v>187</v>
@@ -11251,87 +11242,87 @@
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>514</v>
-      </c>
-      <c r="B38">
-        <v>5</v>
-      </c>
-      <c r="D38" t="s">
-        <v>493</v>
-      </c>
-      <c r="E38" t="s">
-        <v>494</v>
-      </c>
-      <c r="F38" t="s">
-        <v>495</v>
-      </c>
-      <c r="G38" t="s">
-        <v>564</v>
-      </c>
-      <c r="H38" t="s">
-        <v>656</v>
-      </c>
-      <c r="K38" s="95" t="s">
+      <c r="A38" s="90">
+        <v>6</v>
+      </c>
+      <c r="B38" s="90"/>
+      <c r="C38" s="90" t="s">
+        <v>645</v>
+      </c>
+      <c r="D38" s="90" t="s">
+        <v>601</v>
+      </c>
+      <c r="E38" s="90" t="s">
+        <v>602</v>
+      </c>
+      <c r="F38" s="90" t="s">
+        <v>603</v>
+      </c>
+      <c r="G38" s="90" t="s">
+        <v>549</v>
+      </c>
+      <c r="H38" s="90" t="s">
+        <v>653</v>
+      </c>
+      <c r="I38" s="90"/>
+      <c r="J38" s="90"/>
+      <c r="K38" s="90" t="s">
         <v>187</v>
       </c>
-      <c r="L38" s="95">
+      <c r="L38" s="90">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" s="90">
+      <c r="A39">
+        <v>61</v>
+      </c>
+      <c r="B39">
         <v>6</v>
       </c>
-      <c r="B39" s="90"/>
-      <c r="C39" s="90" t="s">
-        <v>648</v>
-      </c>
-      <c r="D39" s="90" t="s">
+      <c r="D39" t="s">
         <v>604</v>
       </c>
-      <c r="E39" s="90" t="s">
+      <c r="E39" t="s">
         <v>605</v>
       </c>
-      <c r="F39" s="90" t="s">
-        <v>606</v>
-      </c>
-      <c r="G39" s="90" t="s">
-        <v>552</v>
-      </c>
-      <c r="H39" s="90" t="s">
-        <v>656</v>
-      </c>
-      <c r="I39" s="90"/>
-      <c r="J39" s="90"/>
-      <c r="K39" s="90" t="s">
+      <c r="F39" t="s">
+        <v>610</v>
+      </c>
+      <c r="G39" t="s">
+        <v>658</v>
+      </c>
+      <c r="H39" t="s">
+        <v>653</v>
+      </c>
+      <c r="K39" s="95" t="s">
         <v>187</v>
       </c>
-      <c r="L39" s="90">
+      <c r="L39" s="95">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B40">
         <v>6</v>
       </c>
       <c r="D40" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E40" t="s">
         <v>608</v>
       </c>
       <c r="F40" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="G40" t="s">
-        <v>661</v>
+        <v>667</v>
       </c>
       <c r="H40" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K40" s="95" t="s">
         <v>187</v>
@@ -11342,25 +11333,25 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B41">
         <v>6</v>
       </c>
       <c r="D41" t="s">
+        <v>607</v>
+      </c>
+      <c r="E41" t="s">
         <v>609</v>
       </c>
-      <c r="E41" t="s">
-        <v>611</v>
-      </c>
       <c r="F41" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="G41" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="H41" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K41" s="95" t="s">
         <v>187</v>
@@ -11371,59 +11362,30 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B42">
         <v>6</v>
       </c>
       <c r="D42" t="s">
-        <v>610</v>
+        <v>601</v>
       </c>
       <c r="E42" t="s">
-        <v>612</v>
+        <v>602</v>
       </c>
       <c r="F42" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="G42" t="s">
-        <v>671</v>
+        <v>661</v>
       </c>
       <c r="H42" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K42" s="95" t="s">
         <v>187</v>
       </c>
       <c r="L42" s="95">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>64</v>
-      </c>
-      <c r="B43">
-        <v>6</v>
-      </c>
-      <c r="D43" t="s">
-        <v>604</v>
-      </c>
-      <c r="E43" t="s">
-        <v>605</v>
-      </c>
-      <c r="F43" t="s">
-        <v>616</v>
-      </c>
-      <c r="G43" t="s">
-        <v>664</v>
-      </c>
-      <c r="H43" t="s">
-        <v>656</v>
-      </c>
-      <c r="K43" s="95" t="s">
-        <v>187</v>
-      </c>
-      <c r="L43" s="95">
         <v>1</v>
       </c>
     </row>
@@ -11554,7 +11516,7 @@
         <v>169</v>
       </c>
       <c r="D1" s="64" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E1" s="64" t="s">
         <v>225</v>
@@ -12318,11 +12280,11 @@
         <v>38</v>
       </c>
       <c r="B18" s="77" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C18" s="77"/>
       <c r="D18" s="77" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E18" s="79" t="s">
         <v>15</v>
@@ -12616,11 +12578,11 @@
         <v>46</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>15</v>
@@ -13216,7 +13178,7 @@
       </c>
       <c r="C48" s="77"/>
       <c r="D48" s="77" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="E48" s="77" t="s">
         <v>17</v>
@@ -13401,11 +13363,11 @@
         <v>181</v>
       </c>
       <c r="B54" s="42" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="C54" s="42"/>
       <c r="D54" s="43" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="E54" s="42" t="s">
         <v>15</v>
@@ -13432,11 +13394,11 @@
         <v>181</v>
       </c>
       <c r="B55" s="42" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="C55" s="42"/>
       <c r="D55" s="43" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="E55" s="42" t="s">
         <v>15</v>
@@ -13587,7 +13549,7 @@
       </c>
       <c r="C60" s="66"/>
       <c r="D60" s="70" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="E60" s="66" t="s">
         <v>16</v>
@@ -14741,7 +14703,7 @@
         <v>53</v>
       </c>
       <c r="E26" s="68" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="F26" s="66">
         <v>1</v>
@@ -14775,7 +14737,7 @@
         <v>53</v>
       </c>
       <c r="E27" s="68" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="F27" s="66">
         <v>1</v>
@@ -14809,7 +14771,7 @@
         <v>53</v>
       </c>
       <c r="E28" s="68" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="F28" s="66">
         <v>1</v>
@@ -14843,7 +14805,7 @@
         <v>53</v>
       </c>
       <c r="E29" s="68" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="F29" s="66">
         <v>1</v>
@@ -14877,7 +14839,7 @@
         <v>53</v>
       </c>
       <c r="E30" s="68" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="F30" s="66">
         <v>1</v>
@@ -14911,7 +14873,7 @@
         <v>53</v>
       </c>
       <c r="E31" s="68" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="F31" s="66">
         <v>1</v>
@@ -15543,7 +15505,7 @@
         <v>168</v>
       </c>
       <c r="E50" s="105" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="F50" s="104">
         <v>1</v>
@@ -15576,7 +15538,7 @@
         <v>168</v>
       </c>
       <c r="E51" s="99" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="F51" s="98">
         <v>1</v>
@@ -15609,7 +15571,7 @@
         <v>168</v>
       </c>
       <c r="E52" s="99" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="F52" s="98">
         <v>1</v>
@@ -15642,7 +15604,7 @@
         <v>168</v>
       </c>
       <c r="E53" s="99" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="F53" s="98">
         <v>1</v>
@@ -15675,7 +15637,7 @@
         <v>168</v>
       </c>
       <c r="E54" s="99" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="F54" s="98">
         <v>1</v>
@@ -15708,7 +15670,7 @@
         <v>168</v>
       </c>
       <c r="E55" s="99" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="F55" s="98">
         <v>1</v>
@@ -15741,7 +15703,7 @@
         <v>168</v>
       </c>
       <c r="E56" s="99" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="F56" s="98">
         <v>1</v>
@@ -15774,7 +15736,7 @@
         <v>168</v>
       </c>
       <c r="E57" s="99" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="F57" s="98">
         <v>1</v>

</xml_diff>

<commit_message>
change db for sep exe type and ass type
</commit_message>
<xml_diff>
--- a/db/excel/api-function-granted-users-cdld.xlsx
+++ b/db/excel/api-function-granted-users-cdld.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10613"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2624F4B8-2B1D-B44B-96C4-98EE0EA92FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77CA0AB2-9D78-0C44-9443-79C0AB6C1AD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19460" tabRatio="800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20060" tabRatio="800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_types" sheetId="27" r:id="rId1"/>
@@ -300,7 +300,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1717" uniqueCount="688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1706" uniqueCount="682">
   <si>
     <t>status</t>
   </si>
@@ -1673,36 +1673,15 @@
     <t>Thời gian update history này</t>
   </si>
   <si>
-    <t>EXEC_TYPES</t>
-  </si>
-  <si>
-    <t>Loại lịch sử tác động</t>
-  </si>
-  <si>
-    <t>UPDATE_DEADLINE</t>
-  </si>
-  <si>
     <t>Người đánh giá cập nhập hạn hoàn thành cho chỉ đạo</t>
   </si>
   <si>
-    <t>UPDATE_ASS_CRITERIA</t>
-  </si>
-  <si>
-    <t>Người đánh giá cập nhập chỉ số đánh giá</t>
-  </si>
-  <si>
     <t>UPDATE_EXE_STATUS</t>
   </si>
   <si>
     <t>Người thực hiện cập nhập trạng thái thực hiện</t>
   </si>
   <si>
-    <t>Cập nhập deadline</t>
-  </si>
-  <si>
-    <t>Cập nhập chỉ số</t>
-  </si>
-  <si>
     <t>Cập nhập thực hiện</t>
   </si>
   <si>
@@ -1715,15 +1694,6 @@
     <t>Người thực hiện xin gia hạn lần 1</t>
   </si>
   <si>
-    <t>REQ_EXT2</t>
-  </si>
-  <si>
-    <t>Xin Gia Hạn Lần 2</t>
-  </si>
-  <si>
-    <t>Người thực hiện xin gia hạn lần 2</t>
-  </si>
-  <si>
     <t>ACCEPT_EXT1</t>
   </si>
   <si>
@@ -1733,15 +1703,6 @@
     <t>Người đánh giá đồng ý gia hạn lần 1</t>
   </si>
   <si>
-    <t>Người đánh giá đồng ý gia hạn lần 2</t>
-  </si>
-  <si>
-    <t>Đồng ý GH Lần 2</t>
-  </si>
-  <si>
-    <t>ACCEPT_EXT2</t>
-  </si>
-  <si>
     <t>DIRECT_TYPES</t>
   </si>
   <si>
@@ -1812,9 +1773,6 @@
   </si>
   <si>
     <t>ASS_EXE_CMPLT</t>
-  </si>
-  <si>
-    <t>Đánh Giá Hoàn Thành Thực Hiện</t>
   </si>
   <si>
     <t>Người đánh giá đánh giá hoàn thành thực hiện cho đơn vị thực hiện</t>
@@ -2336,12 +2294,6 @@
     <t>[41,42,43,44]</t>
   </si>
   <si>
-    <t>[51,52,53,54,55,56,57,58,59,510,511,512,513,514]</t>
-  </si>
-  <si>
-    <t>[61,62,63,64]</t>
-  </si>
-  <si>
     <t>Thực hiện 1 lần/tuần</t>
   </si>
   <si>
@@ -2429,9 +2381,6 @@
     <t>Mã Id cuộc họp nơi chỉ đạo này khởi xuất</t>
   </si>
   <si>
-    <t>[71,72,73]</t>
-  </si>
-  <si>
     <t>Ảnh Nền Giao Diện</t>
   </si>
   <si>
@@ -2459,13 +2408,46 @@
     <t>Ảnh nền cho trang quản lý direct org</t>
   </si>
   <si>
-    <t>url(https://images.unsplash.com/photo-1566623357438-90e3406f6c91?ixid=MnwxMjA3fDB8MHxwaG90by1wYWdlfHx8fGVufDB8fHx8&amp;ixlib=rb-1.2.1&amp;auto=format&amp;fit=crop&amp;w=3334&amp;q=80)</t>
-  </si>
-  <si>
     <t>url(https://images.unsplash.com/photo-1608178398319-48f814d0750c?ixlib=rb-1.2.1&amp;ixid=MnwxMjA3fDB8MHxwaG90by1wYWdlfHx8fGVufDB8fHx8&amp;auto=format&amp;fit=crop&amp;w=2406&amp;q=80)</t>
   </si>
   <si>
     <t>url(https://images.unsplash.com/photo-1462331940025-496dfbfc7564?ixid=MnwxMjA3fDB8MHxwaG90by1wYWdlfHx8fGVufDB8fHx8&amp;ixlib=rb-1.2.1&amp;auto=format&amp;fit=crop&amp;w=3454&amp;q=80)</t>
+  </si>
+  <si>
+    <t>[51,52,53,54,55,56,57]</t>
+  </si>
+  <si>
+    <t>[61,62,63,64, 65,66,67]</t>
+  </si>
+  <si>
+    <t>[71,72,73,74]</t>
+  </si>
+  <si>
+    <t>[81,82,83]</t>
+  </si>
+  <si>
+    <t>Loại lịch sử tác động người thực hiện</t>
+  </si>
+  <si>
+    <t>Loại lịch sử tác động người đánh giá</t>
+  </si>
+  <si>
+    <t>Cập nhập deadline, chỉ số</t>
+  </si>
+  <si>
+    <t>UPDATE_CRIT</t>
+  </si>
+  <si>
+    <t>Đánh giá hoàn thành thực hiện</t>
+  </si>
+  <si>
+    <t>ASS_TYPE</t>
+  </si>
+  <si>
+    <t>EXE_TYPE</t>
+  </si>
+  <si>
+    <t>url(https://images.unsplash.com/photo-1548041347-390744c58da6?ixlib=rb-1.2.1&amp;ixid=MnwxMjA3fDB8MHxwaG90by1wYWdlfHx8fGVufDB8fHx8&amp;auto=format&amp;fit=crop&amp;w=1966&amp;q=80)</t>
   </si>
 </sst>
 </file>
@@ -5625,13 +5607,13 @@
         <v>357</v>
       </c>
       <c r="D9" s="87" t="s">
-        <v>538</v>
+        <v>524</v>
       </c>
       <c r="E9" s="88" t="s">
         <v>357</v>
       </c>
       <c r="F9" s="88" t="s">
-        <v>545</v>
+        <v>531</v>
       </c>
       <c r="G9" s="88" t="s">
         <v>419</v>
@@ -5694,7 +5676,7 @@
       </c>
       <c r="D11" s="83"/>
       <c r="E11" s="84" t="s">
-        <v>539</v>
+        <v>525</v>
       </c>
       <c r="F11" s="84"/>
       <c r="G11" s="84" t="s">
@@ -5726,7 +5708,7 @@
       </c>
       <c r="D12" s="83"/>
       <c r="E12" s="84" t="s">
-        <v>535</v>
+        <v>521</v>
       </c>
       <c r="F12" s="84"/>
       <c r="G12" s="84" t="s">
@@ -5758,7 +5740,7 @@
       </c>
       <c r="D13" s="83"/>
       <c r="E13" s="84" t="s">
-        <v>536</v>
+        <v>522</v>
       </c>
       <c r="F13" s="84"/>
       <c r="G13" s="84" t="s">
@@ -5857,7 +5839,7 @@
         <v>410</v>
       </c>
       <c r="F16" s="88" t="s">
-        <v>537</v>
+        <v>523</v>
       </c>
       <c r="G16" s="88" t="s">
         <v>425</v>
@@ -5958,7 +5940,7 @@
         <v>138</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>534</v>
+        <v>520</v>
       </c>
       <c r="F2" s="30"/>
       <c r="G2" s="30"/>
@@ -5985,7 +5967,7 @@
         <v>138</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>534</v>
+        <v>520</v>
       </c>
       <c r="F3" s="30"/>
       <c r="G3" s="30"/>
@@ -6012,7 +5994,7 @@
         <v>138</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>534</v>
+        <v>520</v>
       </c>
       <c r="F4" s="28"/>
       <c r="G4" s="28"/>
@@ -6039,7 +6021,7 @@
         <v>138</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>534</v>
+        <v>520</v>
       </c>
       <c r="F5" s="28"/>
       <c r="G5" s="28"/>
@@ -6100,10 +6082,10 @@
         <v>240</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>649</v>
+        <v>633</v>
       </c>
       <c r="E1" s="40" t="s">
-        <v>650</v>
+        <v>634</v>
       </c>
       <c r="F1" s="40" t="s">
         <v>180</v>
@@ -6132,13 +6114,13 @@
         <v>326</v>
       </c>
       <c r="C2" t="s">
-        <v>586</v>
+        <v>572</v>
       </c>
       <c r="D2" t="s">
-        <v>546</v>
+        <v>532</v>
       </c>
       <c r="E2" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="J2" t="s">
         <v>187</v>
@@ -6158,10 +6140,10 @@
         <v>325</v>
       </c>
       <c r="D3" t="s">
-        <v>547</v>
+        <v>533</v>
       </c>
       <c r="E3" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -6181,13 +6163,13 @@
         <v>189</v>
       </c>
       <c r="C4" t="s">
-        <v>587</v>
+        <v>573</v>
       </c>
       <c r="D4" t="s">
-        <v>548</v>
+        <v>534</v>
       </c>
       <c r="E4" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -6207,13 +6189,13 @@
         <v>188</v>
       </c>
       <c r="C5" t="s">
-        <v>588</v>
+        <v>574</v>
       </c>
       <c r="D5" t="s">
-        <v>549</v>
+        <v>535</v>
       </c>
       <c r="E5" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -6233,13 +6215,13 @@
         <v>191</v>
       </c>
       <c r="C6" t="s">
-        <v>589</v>
+        <v>575</v>
       </c>
       <c r="D6" t="s">
-        <v>550</v>
+        <v>536</v>
       </c>
       <c r="E6" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -6259,13 +6241,13 @@
         <v>193</v>
       </c>
       <c r="C7" t="s">
-        <v>590</v>
+        <v>576</v>
       </c>
       <c r="D7" t="s">
-        <v>551</v>
+        <v>537</v>
       </c>
       <c r="E7" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -6285,13 +6267,13 @@
         <v>195</v>
       </c>
       <c r="C8" t="s">
-        <v>591</v>
+        <v>577</v>
       </c>
       <c r="D8" t="s">
-        <v>552</v>
+        <v>538</v>
       </c>
       <c r="E8" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -6311,13 +6293,13 @@
         <v>196</v>
       </c>
       <c r="C9" t="s">
-        <v>592</v>
+        <v>578</v>
       </c>
       <c r="D9" t="s">
-        <v>553</v>
+        <v>539</v>
       </c>
       <c r="E9" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -6337,13 +6319,13 @@
         <v>197</v>
       </c>
       <c r="C10" t="s">
-        <v>593</v>
+        <v>579</v>
       </c>
       <c r="D10" t="s">
-        <v>554</v>
+        <v>540</v>
       </c>
       <c r="E10" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -6363,13 +6345,13 @@
         <v>194</v>
       </c>
       <c r="C11" t="s">
-        <v>594</v>
+        <v>580</v>
       </c>
       <c r="D11" t="s">
-        <v>555</v>
+        <v>541</v>
       </c>
       <c r="E11" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -6389,13 +6371,13 @@
         <v>192</v>
       </c>
       <c r="C12" t="s">
-        <v>595</v>
+        <v>581</v>
       </c>
       <c r="D12" t="s">
-        <v>555</v>
+        <v>541</v>
       </c>
       <c r="E12" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -6415,13 +6397,13 @@
         <v>198</v>
       </c>
       <c r="C13" t="s">
-        <v>596</v>
+        <v>582</v>
       </c>
       <c r="D13" t="s">
-        <v>555</v>
+        <v>541</v>
       </c>
       <c r="E13" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -6441,13 +6423,13 @@
         <v>199</v>
       </c>
       <c r="C14" t="s">
-        <v>597</v>
+        <v>583</v>
       </c>
       <c r="D14" t="s">
-        <v>555</v>
+        <v>541</v>
       </c>
       <c r="E14" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -6467,13 +6449,13 @@
         <v>200</v>
       </c>
       <c r="C15" t="s">
-        <v>588</v>
+        <v>574</v>
       </c>
       <c r="D15" t="s">
-        <v>555</v>
+        <v>541</v>
       </c>
       <c r="E15" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -6493,13 +6475,13 @@
         <v>201</v>
       </c>
       <c r="C16" t="s">
-        <v>598</v>
+        <v>584</v>
       </c>
       <c r="D16" t="s">
-        <v>555</v>
+        <v>541</v>
       </c>
       <c r="E16" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -6519,13 +6501,13 @@
         <v>202</v>
       </c>
       <c r="C17" t="s">
-        <v>599</v>
+        <v>585</v>
       </c>
       <c r="D17" t="s">
-        <v>555</v>
+        <v>541</v>
       </c>
       <c r="E17" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -6545,13 +6527,13 @@
         <v>203</v>
       </c>
       <c r="C18" t="s">
-        <v>600</v>
+        <v>586</v>
       </c>
       <c r="D18" t="s">
-        <v>555</v>
+        <v>541</v>
       </c>
       <c r="E18" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -6636,7 +6618,7 @@
         <v>229</v>
       </c>
       <c r="C4" t="s">
-        <v>503</v>
+        <v>489</v>
       </c>
       <c r="E4" t="s">
         <v>187</v>
@@ -6650,7 +6632,7 @@
         <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>504</v>
+        <v>490</v>
       </c>
       <c r="E5" t="s">
         <v>187</v>
@@ -6678,7 +6660,7 @@
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>505</v>
+        <v>491</v>
       </c>
       <c r="E7" t="s">
         <v>187</v>
@@ -6692,7 +6674,7 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>506</v>
+        <v>492</v>
       </c>
       <c r="E8" t="s">
         <v>187</v>
@@ -6720,7 +6702,7 @@
         <v>155</v>
       </c>
       <c r="C10" t="s">
-        <v>540</v>
+        <v>526</v>
       </c>
       <c r="E10" t="s">
         <v>187</v>
@@ -6734,7 +6716,7 @@
         <v>156</v>
       </c>
       <c r="C11" t="s">
-        <v>541</v>
+        <v>527</v>
       </c>
       <c r="E11" t="s">
         <v>187</v>
@@ -6749,11 +6731,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C61" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D91" sqref="D91"/>
+      <selection pane="bottomRight" activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6938,7 +6920,7 @@
         <v>258</v>
       </c>
       <c r="D5" s="107" t="s">
-        <v>619</v>
+        <v>605</v>
       </c>
       <c r="E5" s="107" t="s">
         <v>16</v>
@@ -7252,13 +7234,13 @@
         <v>219</v>
       </c>
       <c r="B15" s="50" t="s">
-        <v>669</v>
+        <v>653</v>
       </c>
       <c r="C15" s="50" t="s">
-        <v>670</v>
+        <v>654</v>
       </c>
       <c r="D15" s="50" t="s">
-        <v>671</v>
+        <v>655</v>
       </c>
       <c r="E15" s="50" t="s">
         <v>16</v>
@@ -7272,7 +7254,7 @@
       <c r="J15" s="57"/>
       <c r="K15" s="57"/>
       <c r="L15" s="58" t="s">
-        <v>672</v>
+        <v>656</v>
       </c>
       <c r="M15" s="57"/>
       <c r="N15" s="57"/>
@@ -7289,10 +7271,10 @@
         <v>316</v>
       </c>
       <c r="C16" s="50" t="s">
-        <v>501</v>
+        <v>487</v>
       </c>
       <c r="D16" s="50" t="s">
-        <v>502</v>
+        <v>488</v>
       </c>
       <c r="E16" s="50" t="s">
         <v>15</v>
@@ -7360,7 +7342,7 @@
         <v>250</v>
       </c>
       <c r="D18" s="109" t="s">
-        <v>620</v>
+        <v>606</v>
       </c>
       <c r="E18" s="109" t="s">
         <v>16</v>
@@ -7372,7 +7354,7 @@
       <c r="J18" s="57"/>
       <c r="K18" s="57"/>
       <c r="L18" s="58" t="s">
-        <v>638</v>
+        <v>624</v>
       </c>
       <c r="M18" s="57"/>
       <c r="N18" s="57"/>
@@ -7406,7 +7388,7 @@
       <c r="J19" s="57"/>
       <c r="K19" s="57"/>
       <c r="L19" s="58" t="s">
-        <v>639</v>
+        <v>625</v>
       </c>
       <c r="M19" s="57"/>
       <c r="N19" s="57"/>
@@ -7734,13 +7716,13 @@
         <v>219</v>
       </c>
       <c r="B30" s="50" t="s">
-        <v>485</v>
+        <v>472</v>
       </c>
       <c r="C30" s="50" t="s">
-        <v>486</v>
+        <v>473</v>
       </c>
       <c r="D30" s="50" t="s">
-        <v>487</v>
+        <v>474</v>
       </c>
       <c r="E30" s="50" t="s">
         <v>15</v>
@@ -7772,7 +7754,7 @@
         <v>234</v>
       </c>
       <c r="D31" s="50" t="s">
-        <v>615</v>
+        <v>601</v>
       </c>
       <c r="E31" s="50" t="s">
         <v>17</v>
@@ -7795,7 +7777,7 @@
     </row>
     <row r="32" spans="1:16" s="79" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="95" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
       <c r="B32" s="95" t="s">
         <v>18</v>
@@ -7804,7 +7786,7 @@
         <v>241</v>
       </c>
       <c r="D32" s="95" t="s">
-        <v>519</v>
+        <v>505</v>
       </c>
       <c r="E32" s="95" t="s">
         <v>97</v>
@@ -7833,16 +7815,16 @@
     </row>
     <row r="33" spans="1:16" s="79" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="95" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
       <c r="B33" s="95" t="s">
-        <v>669</v>
+        <v>653</v>
       </c>
       <c r="C33" s="95" t="s">
-        <v>673</v>
+        <v>657</v>
       </c>
       <c r="D33" s="95" t="s">
-        <v>674</v>
+        <v>658</v>
       </c>
       <c r="E33" s="95" t="s">
         <v>16</v>
@@ -7863,16 +7845,16 @@
     </row>
     <row r="34" spans="1:16" s="79" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="95" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
       <c r="B34" s="95" t="s">
         <v>220</v>
       </c>
       <c r="C34" s="95" t="s">
-        <v>520</v>
+        <v>506</v>
       </c>
       <c r="D34" s="95" t="s">
-        <v>521</v>
+        <v>507</v>
       </c>
       <c r="E34" s="95" t="s">
         <v>16</v>
@@ -7893,16 +7875,16 @@
     </row>
     <row r="35" spans="1:16" s="79" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="95" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
       <c r="B35" s="95" t="s">
-        <v>562</v>
+        <v>548</v>
       </c>
       <c r="C35" s="95" t="s">
-        <v>563</v>
+        <v>549</v>
       </c>
       <c r="D35" s="95" t="s">
-        <v>564</v>
+        <v>550</v>
       </c>
       <c r="E35" s="95" t="s">
         <v>15</v>
@@ -7916,7 +7898,7 @@
       <c r="J35" s="96"/>
       <c r="K35" s="96"/>
       <c r="L35" s="58" t="s">
-        <v>634</v>
+        <v>620</v>
       </c>
       <c r="M35" s="96"/>
       <c r="N35" s="96"/>
@@ -7927,7 +7909,7 @@
     </row>
     <row r="36" spans="1:16" s="79" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="95" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
       <c r="B36" s="95" t="s">
         <v>225</v>
@@ -7936,7 +7918,7 @@
         <v>268</v>
       </c>
       <c r="D36" s="95" t="s">
-        <v>621</v>
+        <v>607</v>
       </c>
       <c r="E36" s="95" t="s">
         <v>15</v>
@@ -7959,7 +7941,7 @@
     </row>
     <row r="37" spans="1:16" s="79" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="95" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
       <c r="B37" s="95" t="s">
         <v>226</v>
@@ -7968,7 +7950,7 @@
         <v>269</v>
       </c>
       <c r="D37" s="95" t="s">
-        <v>622</v>
+        <v>608</v>
       </c>
       <c r="E37" s="95" t="s">
         <v>15</v>
@@ -7991,16 +7973,16 @@
     </row>
     <row r="38" spans="1:16" s="79" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="95" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
       <c r="B38" s="95" t="s">
-        <v>511</v>
+        <v>497</v>
       </c>
       <c r="C38" s="95" t="s">
-        <v>512</v>
+        <v>498</v>
       </c>
       <c r="D38" s="95" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E38" s="95" t="s">
         <v>15</v>
@@ -8023,16 +8005,16 @@
     </row>
     <row r="39" spans="1:16" s="79" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="95" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
       <c r="B39" s="95" t="s">
-        <v>516</v>
+        <v>502</v>
       </c>
       <c r="C39" s="95" t="s">
-        <v>514</v>
+        <v>500</v>
       </c>
       <c r="D39" s="95" t="s">
-        <v>515</v>
+        <v>501</v>
       </c>
       <c r="E39" s="95" t="s">
         <v>97</v>
@@ -8053,7 +8035,7 @@
     </row>
     <row r="40" spans="1:16" s="79" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="95" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
       <c r="B40" s="95" t="s">
         <v>204</v>
@@ -8083,7 +8065,7 @@
     </row>
     <row r="41" spans="1:16" s="79" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="95" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
       <c r="B41" s="95" t="s">
         <v>229</v>
@@ -8115,7 +8097,7 @@
     </row>
     <row r="42" spans="1:16" s="79" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="95" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
       <c r="B42" s="95" t="s">
         <v>19</v>
@@ -8145,7 +8127,7 @@
     </row>
     <row r="43" spans="1:16" s="79" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="95" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
       <c r="B43" s="95" t="s">
         <v>45</v>
@@ -8177,7 +8159,7 @@
     </row>
     <row r="44" spans="1:16" s="79" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="95" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
       <c r="B44" s="95" t="s">
         <v>0</v>
@@ -8186,7 +8168,7 @@
         <v>234</v>
       </c>
       <c r="D44" s="95" t="s">
-        <v>517</v>
+        <v>503</v>
       </c>
       <c r="E44" s="95" t="s">
         <v>17</v>
@@ -8253,10 +8235,10 @@
         <v>316</v>
       </c>
       <c r="C46" s="49" t="s">
-        <v>628</v>
+        <v>614</v>
       </c>
       <c r="D46" s="49" t="s">
-        <v>640</v>
+        <v>626</v>
       </c>
       <c r="E46" s="49" t="s">
         <v>15</v>
@@ -8286,13 +8268,13 @@
         <v>274</v>
       </c>
       <c r="B47" s="49" t="s">
-        <v>669</v>
+        <v>653</v>
       </c>
       <c r="C47" s="49" t="s">
-        <v>673</v>
+        <v>657</v>
       </c>
       <c r="D47" s="49" t="s">
-        <v>674</v>
+        <v>658</v>
       </c>
       <c r="E47" s="49" t="s">
         <v>16</v>
@@ -8304,7 +8286,7 @@
       <c r="J47" s="54"/>
       <c r="K47" s="54"/>
       <c r="L47" s="58" t="s">
-        <v>672</v>
+        <v>656</v>
       </c>
       <c r="M47" s="54"/>
       <c r="N47" s="54"/>
@@ -8336,7 +8318,7 @@
       <c r="J48" s="54"/>
       <c r="K48" s="54"/>
       <c r="L48" s="58" t="s">
-        <v>633</v>
+        <v>619</v>
       </c>
       <c r="M48" s="54"/>
       <c r="N48" s="54"/>
@@ -8350,13 +8332,13 @@
         <v>274</v>
       </c>
       <c r="B49" s="49" t="s">
-        <v>562</v>
+        <v>548</v>
       </c>
       <c r="C49" s="49" t="s">
-        <v>565</v>
+        <v>551</v>
       </c>
       <c r="D49" s="49" t="s">
-        <v>566</v>
+        <v>552</v>
       </c>
       <c r="E49" s="49" t="s">
         <v>15</v>
@@ -8370,7 +8352,7 @@
       <c r="J49" s="54"/>
       <c r="K49" s="54"/>
       <c r="L49" s="58" t="s">
-        <v>634</v>
+        <v>620</v>
       </c>
       <c r="M49" s="54"/>
       <c r="N49" s="54"/>
@@ -8402,7 +8384,7 @@
       <c r="J50" s="54"/>
       <c r="K50" s="54"/>
       <c r="L50" s="58" t="s">
-        <v>635</v>
+        <v>621</v>
       </c>
       <c r="M50" s="54"/>
       <c r="N50" s="54"/>
@@ -8422,7 +8404,7 @@
         <v>280</v>
       </c>
       <c r="D51" s="49" t="s">
-        <v>567</v>
+        <v>553</v>
       </c>
       <c r="E51" s="49" t="s">
         <v>16</v>
@@ -8478,13 +8460,13 @@
         <v>274</v>
       </c>
       <c r="B53" s="107" t="s">
-        <v>617</v>
+        <v>603</v>
       </c>
       <c r="C53" s="107" t="s">
         <v>272</v>
       </c>
       <c r="D53" s="107" t="s">
-        <v>614</v>
+        <v>600</v>
       </c>
       <c r="E53" s="107" t="s">
         <v>16</v>
@@ -8496,7 +8478,7 @@
       <c r="J53" s="108"/>
       <c r="K53" s="108"/>
       <c r="L53" s="58" t="s">
-        <v>636</v>
+        <v>622</v>
       </c>
       <c r="M53" s="108"/>
       <c r="N53" s="108"/>
@@ -8542,13 +8524,13 @@
         <v>274</v>
       </c>
       <c r="B55" s="49" t="s">
-        <v>482</v>
+        <v>469</v>
       </c>
       <c r="C55" s="49" t="s">
-        <v>483</v>
+        <v>470</v>
       </c>
       <c r="D55" s="49" t="s">
-        <v>484</v>
+        <v>471</v>
       </c>
       <c r="E55" s="49" t="s">
         <v>15</v>
@@ -8607,10 +8589,10 @@
         <v>227</v>
       </c>
       <c r="C57" s="117" t="s">
-        <v>624</v>
+        <v>610</v>
       </c>
       <c r="D57" s="117" t="s">
-        <v>625</v>
+        <v>611</v>
       </c>
       <c r="E57" s="117" t="s">
         <v>15</v>
@@ -8766,7 +8748,7 @@
         <v>234</v>
       </c>
       <c r="D62" s="49" t="s">
-        <v>616</v>
+        <v>602</v>
       </c>
       <c r="E62" s="49" t="s">
         <v>17</v>
@@ -8833,10 +8815,10 @@
         <v>316</v>
       </c>
       <c r="C64" s="51" t="s">
-        <v>628</v>
+        <v>614</v>
       </c>
       <c r="D64" s="51" t="s">
-        <v>629</v>
+        <v>615</v>
       </c>
       <c r="E64" s="51" t="s">
         <v>15</v>
@@ -8866,13 +8848,13 @@
         <v>273</v>
       </c>
       <c r="B65" s="51" t="s">
-        <v>562</v>
+        <v>548</v>
       </c>
       <c r="C65" s="51" t="s">
-        <v>565</v>
+        <v>551</v>
       </c>
       <c r="D65" s="51" t="s">
-        <v>568</v>
+        <v>554</v>
       </c>
       <c r="E65" s="51" t="s">
         <v>15</v>
@@ -8886,7 +8868,7 @@
       <c r="J65" s="45"/>
       <c r="K65" s="45"/>
       <c r="L65" s="58" t="s">
-        <v>634</v>
+        <v>620</v>
       </c>
       <c r="M65" s="45"/>
       <c r="N65" s="45"/>
@@ -8900,10 +8882,10 @@
         <v>273</v>
       </c>
       <c r="B66" s="51" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="C66" s="51" t="s">
-        <v>627</v>
+        <v>613</v>
       </c>
       <c r="D66" s="51" t="s">
         <v>284</v>
@@ -8920,7 +8902,7 @@
       <c r="J66" s="45"/>
       <c r="K66" s="45"/>
       <c r="L66" s="58" t="s">
-        <v>637</v>
+        <v>623</v>
       </c>
       <c r="M66" s="45"/>
       <c r="N66" s="45"/>
@@ -8954,7 +8936,7 @@
       <c r="J67" s="45"/>
       <c r="K67" s="45"/>
       <c r="L67" s="58" t="s">
-        <v>635</v>
+        <v>621</v>
       </c>
       <c r="M67" s="45"/>
       <c r="N67" s="45"/>
@@ -9038,7 +9020,7 @@
         <v>289</v>
       </c>
       <c r="D70" s="112" t="s">
-        <v>623</v>
+        <v>609</v>
       </c>
       <c r="E70" s="111" t="s">
         <v>16</v>
@@ -9050,7 +9032,7 @@
       <c r="J70" s="45"/>
       <c r="K70" s="45"/>
       <c r="L70" s="58" t="s">
-        <v>638</v>
+        <v>624</v>
       </c>
       <c r="M70" s="45"/>
       <c r="N70" s="45"/>
@@ -9226,7 +9208,7 @@
         <v>448</v>
       </c>
       <c r="D76" s="51" t="s">
-        <v>480</v>
+        <v>467</v>
       </c>
       <c r="E76" s="51" t="s">
         <v>17</v>
@@ -9293,10 +9275,10 @@
         <v>316</v>
       </c>
       <c r="C78" s="52" t="s">
-        <v>501</v>
+        <v>487</v>
       </c>
       <c r="D78" s="52" t="s">
-        <v>502</v>
+        <v>488</v>
       </c>
       <c r="E78" s="52" t="s">
         <v>15</v>
@@ -9332,7 +9314,7 @@
         <v>244</v>
       </c>
       <c r="D79" s="114" t="s">
-        <v>618</v>
+        <v>604</v>
       </c>
       <c r="E79" s="114" t="s">
         <v>16</v>
@@ -9344,7 +9326,7 @@
       <c r="J79" s="59"/>
       <c r="K79" s="59"/>
       <c r="L79" s="58" t="s">
-        <v>638</v>
+        <v>624</v>
       </c>
       <c r="M79" s="59"/>
       <c r="N79" s="59"/>
@@ -9710,13 +9692,13 @@
         <v>169</v>
       </c>
       <c r="B91" s="43" t="s">
-        <v>542</v>
+        <v>528</v>
       </c>
       <c r="C91" s="43" t="s">
-        <v>543</v>
+        <v>529</v>
       </c>
       <c r="D91" s="60" t="s">
-        <v>544</v>
+        <v>530</v>
       </c>
       <c r="E91" s="60" t="s">
         <v>15</v>
@@ -9840,13 +9822,13 @@
         <v>169</v>
       </c>
       <c r="B95" s="43" t="s">
-        <v>649</v>
+        <v>633</v>
       </c>
       <c r="C95" s="43" t="s">
-        <v>654</v>
+        <v>638</v>
       </c>
       <c r="D95" s="60" t="s">
-        <v>655</v>
+        <v>639</v>
       </c>
       <c r="E95" s="60" t="s">
         <v>15</v>
@@ -9872,13 +9854,13 @@
         <v>169</v>
       </c>
       <c r="B96" s="43" t="s">
-        <v>650</v>
+        <v>634</v>
       </c>
       <c r="C96" s="43" t="s">
-        <v>656</v>
+        <v>640</v>
       </c>
       <c r="D96" s="60" t="s">
-        <v>657</v>
+        <v>641</v>
       </c>
       <c r="E96" s="60" t="s">
         <v>15</v>
@@ -10066,17 +10048,17 @@
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:L46"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="60.5" customWidth="1"/>
@@ -10095,7 +10077,7 @@
         <v>139</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>542</v>
+        <v>528</v>
       </c>
       <c r="D1" s="39" t="s">
         <v>240</v>
@@ -10107,10 +10089,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="39" t="s">
-        <v>649</v>
+        <v>633</v>
       </c>
       <c r="H1" s="39" t="s">
-        <v>650</v>
+        <v>634</v>
       </c>
       <c r="I1" s="39" t="s">
         <v>204</v>
@@ -10143,10 +10125,10 @@
         <v>368</v>
       </c>
       <c r="G2" s="89" t="s">
-        <v>547</v>
+        <v>533</v>
       </c>
       <c r="H2" s="89" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="I2" s="89"/>
       <c r="J2" s="89"/>
@@ -10174,10 +10156,10 @@
         <v>370</v>
       </c>
       <c r="G3" t="s">
-        <v>548</v>
+        <v>534</v>
       </c>
       <c r="H3" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="K3" t="s">
         <v>165</v>
@@ -10203,10 +10185,10 @@
         <v>371</v>
       </c>
       <c r="G4" t="s">
-        <v>549</v>
+        <v>535</v>
       </c>
       <c r="H4" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="K4" t="s">
         <v>165</v>
@@ -10232,10 +10214,10 @@
         <v>375</v>
       </c>
       <c r="G5" t="s">
-        <v>550</v>
+        <v>536</v>
       </c>
       <c r="H5" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="K5" t="s">
         <v>165</v>
@@ -10252,19 +10234,19 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>494</v>
+        <v>481</v>
       </c>
       <c r="E6" t="s">
-        <v>477</v>
+        <v>464</v>
       </c>
       <c r="F6" t="s">
-        <v>495</v>
+        <v>482</v>
       </c>
       <c r="G6" t="s">
-        <v>551</v>
+        <v>537</v>
       </c>
       <c r="H6" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="K6" t="s">
         <v>165</v>
@@ -10281,7 +10263,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>518</v>
+        <v>504</v>
       </c>
       <c r="E7" t="s">
         <v>369</v>
@@ -10290,10 +10272,10 @@
         <v>372</v>
       </c>
       <c r="G7" t="s">
-        <v>552</v>
+        <v>538</v>
       </c>
       <c r="H7" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="K7" t="s">
         <v>165</v>
@@ -10308,7 +10290,7 @@
       </c>
       <c r="B8" s="89"/>
       <c r="C8" s="89" t="s">
-        <v>641</v>
+        <v>627</v>
       </c>
       <c r="D8" s="89" t="s">
         <v>376</v>
@@ -10320,10 +10302,10 @@
         <v>384</v>
       </c>
       <c r="G8" s="89" t="s">
-        <v>554</v>
+        <v>540</v>
       </c>
       <c r="H8" s="89" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="I8" s="89"/>
       <c r="J8" s="89"/>
@@ -10351,10 +10333,10 @@
         <v>382</v>
       </c>
       <c r="G9" t="s">
-        <v>552</v>
+        <v>538</v>
       </c>
       <c r="H9" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="K9" t="s">
         <v>165</v>
@@ -10380,10 +10362,10 @@
         <v>383</v>
       </c>
       <c r="G10" t="s">
-        <v>548</v>
+        <v>534</v>
       </c>
       <c r="H10" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="K10" t="s">
         <v>165</v>
@@ -10398,10 +10380,10 @@
       </c>
       <c r="B11" s="89"/>
       <c r="C11" s="89" t="s">
-        <v>642</v>
+        <v>628</v>
       </c>
       <c r="D11" s="89" t="s">
-        <v>473</v>
+        <v>460</v>
       </c>
       <c r="E11" s="89" t="s">
         <v>387</v>
@@ -10410,10 +10392,10 @@
         <v>388</v>
       </c>
       <c r="G11" s="89" t="s">
-        <v>547</v>
+        <v>533</v>
       </c>
       <c r="H11" s="89" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="I11" s="89"/>
       <c r="J11" s="89"/>
@@ -10432,19 +10414,19 @@
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>580</v>
+        <v>566</v>
       </c>
       <c r="E12" t="s">
-        <v>630</v>
+        <v>616</v>
       </c>
       <c r="F12" t="s">
         <v>389</v>
       </c>
       <c r="G12" t="s">
-        <v>658</v>
+        <v>642</v>
       </c>
       <c r="H12" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="K12" t="s">
         <v>165</v>
@@ -10461,19 +10443,19 @@
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>581</v>
+        <v>567</v>
       </c>
       <c r="E13" t="s">
-        <v>631</v>
+        <v>617</v>
       </c>
       <c r="F13" t="s">
         <v>390</v>
       </c>
       <c r="G13" t="s">
-        <v>659</v>
+        <v>643</v>
       </c>
       <c r="H13" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="K13" t="s">
         <v>165</v>
@@ -10490,19 +10472,19 @@
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>582</v>
+        <v>568</v>
       </c>
       <c r="E14" t="s">
-        <v>632</v>
+        <v>618</v>
       </c>
       <c r="F14" t="s">
         <v>391</v>
       </c>
       <c r="G14" t="s">
-        <v>660</v>
+        <v>644</v>
       </c>
       <c r="H14" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="K14" t="s">
         <v>165</v>
@@ -10519,19 +10501,19 @@
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>583</v>
+        <v>569</v>
       </c>
       <c r="E15" t="s">
-        <v>646</v>
+        <v>630</v>
       </c>
       <c r="F15" t="s">
         <v>392</v>
       </c>
       <c r="G15" t="s">
-        <v>661</v>
+        <v>645</v>
       </c>
       <c r="H15" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="K15" t="s">
         <v>165</v>
@@ -10548,19 +10530,19 @@
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>584</v>
+        <v>570</v>
       </c>
       <c r="E16" t="s">
-        <v>647</v>
+        <v>631</v>
       </c>
       <c r="F16" t="s">
         <v>393</v>
       </c>
       <c r="G16" t="s">
-        <v>662</v>
+        <v>646</v>
       </c>
       <c r="H16" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="K16" t="s">
         <v>165</v>
@@ -10577,19 +10559,19 @@
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>585</v>
+        <v>571</v>
       </c>
       <c r="E17" t="s">
-        <v>648</v>
+        <v>632</v>
       </c>
       <c r="F17" t="s">
         <v>394</v>
       </c>
       <c r="G17" t="s">
-        <v>663</v>
+        <v>647</v>
       </c>
       <c r="H17" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="K17" t="s">
         <v>165</v>
@@ -10604,10 +10586,10 @@
       </c>
       <c r="B18" s="89"/>
       <c r="C18" s="89" t="s">
-        <v>643</v>
+        <v>629</v>
       </c>
       <c r="D18" s="89" t="s">
-        <v>474</v>
+        <v>461</v>
       </c>
       <c r="E18" s="89" t="s">
         <v>395</v>
@@ -10616,10 +10598,10 @@
         <v>396</v>
       </c>
       <c r="G18" s="89" t="s">
-        <v>554</v>
+        <v>540</v>
       </c>
       <c r="H18" s="89" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="I18" s="89"/>
       <c r="J18" s="89"/>
@@ -10638,7 +10620,7 @@
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>576</v>
+        <v>562</v>
       </c>
       <c r="E19" t="s">
         <v>397</v>
@@ -10647,10 +10629,10 @@
         <v>397</v>
       </c>
       <c r="G19" t="s">
-        <v>663</v>
+        <v>647</v>
       </c>
       <c r="H19" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="K19" t="s">
         <v>165</v>
@@ -10667,7 +10649,7 @@
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>577</v>
+        <v>563</v>
       </c>
       <c r="E20" t="s">
         <v>398</v>
@@ -10676,10 +10658,10 @@
         <v>398</v>
       </c>
       <c r="G20" t="s">
-        <v>664</v>
+        <v>648</v>
       </c>
       <c r="H20" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="K20" t="s">
         <v>165</v>
@@ -10696,7 +10678,7 @@
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>578</v>
+        <v>564</v>
       </c>
       <c r="E21" t="s">
         <v>399</v>
@@ -10705,10 +10687,10 @@
         <v>399</v>
       </c>
       <c r="G21" t="s">
-        <v>665</v>
+        <v>649</v>
       </c>
       <c r="H21" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="K21" t="s">
         <v>165</v>
@@ -10725,7 +10707,7 @@
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>579</v>
+        <v>565</v>
       </c>
       <c r="E22" t="s">
         <v>400</v>
@@ -10734,10 +10716,10 @@
         <v>400</v>
       </c>
       <c r="G22" t="s">
-        <v>666</v>
+        <v>650</v>
       </c>
       <c r="H22" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="K22" t="s">
         <v>165</v>
@@ -10752,22 +10734,22 @@
       </c>
       <c r="B23" s="89"/>
       <c r="C23" s="89" t="s">
-        <v>644</v>
+        <v>670</v>
       </c>
       <c r="D23" s="89" t="s">
-        <v>450</v>
+        <v>680</v>
       </c>
       <c r="E23" s="89" t="s">
-        <v>451</v>
+        <v>674</v>
       </c>
       <c r="F23" s="89" t="s">
         <v>396</v>
       </c>
       <c r="G23" s="89" t="s">
-        <v>549</v>
+        <v>535</v>
       </c>
       <c r="H23" s="89" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="I23" s="89"/>
       <c r="J23" s="89"/>
@@ -10786,19 +10768,19 @@
         <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>507</v>
+        <v>493</v>
       </c>
       <c r="E24" t="s">
-        <v>508</v>
+        <v>494</v>
       </c>
       <c r="F24" t="s">
-        <v>509</v>
+        <v>495</v>
       </c>
       <c r="G24" t="s">
-        <v>550</v>
+        <v>536</v>
       </c>
       <c r="H24" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="K24" t="s">
         <v>165</v>
@@ -10815,19 +10797,19 @@
         <v>5</v>
       </c>
       <c r="D25" t="s">
+        <v>451</v>
+      </c>
+      <c r="E25" t="s">
+        <v>453</v>
+      </c>
+      <c r="F25" t="s">
         <v>452</v>
       </c>
-      <c r="E25" t="s">
-        <v>458</v>
-      </c>
-      <c r="F25" t="s">
-        <v>453</v>
-      </c>
       <c r="G25" t="s">
-        <v>551</v>
+        <v>539</v>
       </c>
       <c r="H25" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="K25" t="s">
         <v>165</v>
@@ -10844,24 +10826,24 @@
         <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>454</v>
+        <v>462</v>
       </c>
       <c r="E26" t="s">
-        <v>459</v>
+        <v>464</v>
       </c>
       <c r="F26" t="s">
-        <v>455</v>
+        <v>465</v>
       </c>
       <c r="G26" t="s">
-        <v>552</v>
+        <v>545</v>
       </c>
       <c r="H26" t="s">
-        <v>653</v>
-      </c>
-      <c r="K26" t="s">
+        <v>637</v>
+      </c>
+      <c r="K26" s="94" t="s">
         <v>165</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="94">
         <v>1</v>
       </c>
     </row>
@@ -10873,24 +10855,24 @@
         <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>456</v>
+        <v>463</v>
       </c>
       <c r="E27" t="s">
-        <v>460</v>
+        <v>374</v>
       </c>
       <c r="F27" t="s">
-        <v>457</v>
+        <v>466</v>
       </c>
       <c r="G27" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
       <c r="H27" t="s">
-        <v>653</v>
-      </c>
-      <c r="K27" t="s">
+        <v>637</v>
+      </c>
+      <c r="K27" s="94" t="s">
         <v>165</v>
       </c>
-      <c r="L27">
+      <c r="L27" s="94">
         <v>1</v>
       </c>
     </row>
@@ -10902,24 +10884,24 @@
         <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>461</v>
+        <v>475</v>
       </c>
       <c r="E28" t="s">
-        <v>462</v>
+        <v>476</v>
       </c>
       <c r="F28" t="s">
-        <v>463</v>
+        <v>477</v>
       </c>
       <c r="G28" t="s">
-        <v>554</v>
+        <v>544</v>
       </c>
       <c r="H28" t="s">
-        <v>653</v>
-      </c>
-      <c r="K28" t="s">
+        <v>637</v>
+      </c>
+      <c r="K28" s="94" t="s">
         <v>165</v>
       </c>
-      <c r="L28">
+      <c r="L28" s="94">
         <v>1</v>
       </c>
     </row>
@@ -10931,19 +10913,19 @@
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>464</v>
+        <v>454</v>
       </c>
       <c r="E29" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="F29" t="s">
-        <v>466</v>
+        <v>456</v>
       </c>
       <c r="G29" t="s">
-        <v>552</v>
+        <v>540</v>
       </c>
       <c r="H29" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="K29" t="s">
         <v>165</v>
@@ -10953,113 +10935,116 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>57</v>
-      </c>
-      <c r="B30">
-        <v>5</v>
-      </c>
-      <c r="D30" t="s">
-        <v>467</v>
-      </c>
-      <c r="E30" t="s">
-        <v>468</v>
-      </c>
-      <c r="F30" t="s">
-        <v>469</v>
-      </c>
-      <c r="G30" t="s">
-        <v>548</v>
-      </c>
-      <c r="H30" t="s">
-        <v>653</v>
-      </c>
-      <c r="K30" t="s">
+      <c r="A30" s="89">
+        <v>6</v>
+      </c>
+      <c r="B30" s="89"/>
+      <c r="C30" s="89" t="s">
+        <v>671</v>
+      </c>
+      <c r="D30" s="89" t="s">
+        <v>679</v>
+      </c>
+      <c r="E30" s="89" t="s">
+        <v>675</v>
+      </c>
+      <c r="F30" s="89" t="s">
+        <v>589</v>
+      </c>
+      <c r="G30" s="89" t="s">
+        <v>535</v>
+      </c>
+      <c r="H30" s="89" t="s">
+        <v>637</v>
+      </c>
+      <c r="I30" s="89"/>
+      <c r="J30" s="89"/>
+      <c r="K30" s="89" t="s">
         <v>165</v>
       </c>
-      <c r="L30">
+      <c r="L30" s="89">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B31">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D31" t="s">
-        <v>472</v>
+        <v>677</v>
       </c>
       <c r="E31" t="s">
-        <v>471</v>
+        <v>676</v>
       </c>
       <c r="F31" t="s">
-        <v>470</v>
+        <v>450</v>
       </c>
       <c r="G31" t="s">
-        <v>555</v>
+        <v>537</v>
       </c>
       <c r="H31" t="s">
-        <v>653</v>
-      </c>
-      <c r="K31" s="94" t="s">
+        <v>637</v>
+      </c>
+      <c r="K31" t="s">
         <v>165</v>
       </c>
-      <c r="L31" s="94">
+      <c r="L31">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B32">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D32" t="s">
-        <v>481</v>
+        <v>457</v>
       </c>
       <c r="E32" t="s">
-        <v>499</v>
+        <v>458</v>
       </c>
       <c r="F32" t="s">
-        <v>500</v>
+        <v>459</v>
       </c>
       <c r="G32" t="s">
-        <v>556</v>
+        <v>534</v>
       </c>
       <c r="H32" t="s">
-        <v>653</v>
-      </c>
-      <c r="K32" s="94" t="s">
+        <v>637</v>
+      </c>
+      <c r="K32" t="s">
         <v>165</v>
       </c>
-      <c r="L32" s="94">
+      <c r="L32">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>510</v>
+        <v>63</v>
       </c>
       <c r="B33">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D33" t="s">
-        <v>496</v>
+        <v>468</v>
       </c>
       <c r="E33" t="s">
-        <v>497</v>
+        <v>485</v>
       </c>
       <c r="F33" t="s">
-        <v>498</v>
+        <v>486</v>
       </c>
       <c r="G33" t="s">
-        <v>557</v>
+        <v>542</v>
       </c>
       <c r="H33" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="K33" s="94" t="s">
         <v>165</v>
@@ -11070,25 +11055,25 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>511</v>
+        <v>64</v>
       </c>
       <c r="B34">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D34" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="E34" t="s">
-        <v>489</v>
+        <v>678</v>
       </c>
       <c r="F34" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="G34" t="s">
-        <v>558</v>
+        <v>543</v>
       </c>
       <c r="H34" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="K34" s="94" t="s">
         <v>165</v>
@@ -11099,25 +11084,25 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>512</v>
+        <v>65</v>
       </c>
       <c r="B35">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D35" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="E35" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="F35" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="G35" t="s">
-        <v>559</v>
+        <v>547</v>
       </c>
       <c r="H35" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="K35" s="94" t="s">
         <v>165</v>
@@ -11127,55 +11112,58 @@
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>513</v>
-      </c>
-      <c r="B36">
-        <v>5</v>
-      </c>
-      <c r="D36" t="s">
-        <v>476</v>
-      </c>
-      <c r="E36" t="s">
-        <v>374</v>
-      </c>
-      <c r="F36" t="s">
-        <v>479</v>
-      </c>
-      <c r="G36" t="s">
-        <v>560</v>
-      </c>
-      <c r="H36" t="s">
-        <v>653</v>
-      </c>
-      <c r="K36" s="94" t="s">
+      <c r="A36" s="89">
+        <v>7</v>
+      </c>
+      <c r="B36" s="89"/>
+      <c r="C36" s="89" t="s">
+        <v>672</v>
+      </c>
+      <c r="D36" s="89" t="s">
+        <v>587</v>
+      </c>
+      <c r="E36" s="89" t="s">
+        <v>588</v>
+      </c>
+      <c r="F36" s="89" t="s">
+        <v>589</v>
+      </c>
+      <c r="G36" s="89" t="s">
+        <v>535</v>
+      </c>
+      <c r="H36" s="89" t="s">
+        <v>637</v>
+      </c>
+      <c r="I36" s="89"/>
+      <c r="J36" s="89"/>
+      <c r="K36" s="89" t="s">
         <v>165</v>
       </c>
-      <c r="L36" s="94">
+      <c r="L36" s="89">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>514</v>
+        <v>71</v>
       </c>
       <c r="B37">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>491</v>
+        <v>590</v>
       </c>
       <c r="E37" t="s">
-        <v>492</v>
+        <v>591</v>
       </c>
       <c r="F37" t="s">
-        <v>493</v>
+        <v>596</v>
       </c>
       <c r="G37" t="s">
-        <v>561</v>
+        <v>642</v>
       </c>
       <c r="H37" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="K37" s="94" t="s">
         <v>165</v>
@@ -11185,58 +11173,55 @@
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="89">
-        <v>6</v>
-      </c>
-      <c r="B38" s="89"/>
-      <c r="C38" s="89" t="s">
-        <v>645</v>
-      </c>
-      <c r="D38" s="89" t="s">
-        <v>601</v>
-      </c>
-      <c r="E38" s="89" t="s">
-        <v>602</v>
-      </c>
-      <c r="F38" s="89" t="s">
-        <v>603</v>
-      </c>
-      <c r="G38" s="89" t="s">
-        <v>549</v>
-      </c>
-      <c r="H38" s="89" t="s">
-        <v>653</v>
-      </c>
-      <c r="I38" s="89"/>
-      <c r="J38" s="89"/>
-      <c r="K38" s="89" t="s">
+      <c r="A38">
+        <v>72</v>
+      </c>
+      <c r="B38">
+        <v>7</v>
+      </c>
+      <c r="D38" t="s">
+        <v>592</v>
+      </c>
+      <c r="E38" t="s">
+        <v>594</v>
+      </c>
+      <c r="F38" t="s">
+        <v>597</v>
+      </c>
+      <c r="G38" t="s">
+        <v>651</v>
+      </c>
+      <c r="H38" t="s">
+        <v>637</v>
+      </c>
+      <c r="K38" s="94" t="s">
         <v>165</v>
       </c>
-      <c r="L38" s="89">
+      <c r="L38" s="94">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="B39">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>604</v>
+        <v>593</v>
       </c>
       <c r="E39" t="s">
-        <v>605</v>
+        <v>595</v>
       </c>
       <c r="F39" t="s">
-        <v>610</v>
+        <v>598</v>
       </c>
       <c r="G39" t="s">
-        <v>658</v>
+        <v>652</v>
       </c>
       <c r="H39" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="K39" s="94" t="s">
         <v>165</v>
@@ -11247,25 +11232,25 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="B40">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D40" t="s">
-        <v>606</v>
+        <v>587</v>
       </c>
       <c r="E40" t="s">
-        <v>608</v>
+        <v>588</v>
       </c>
       <c r="F40" t="s">
-        <v>611</v>
+        <v>599</v>
       </c>
       <c r="G40" t="s">
-        <v>667</v>
+        <v>645</v>
       </c>
       <c r="H40" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="K40" s="94" t="s">
         <v>165</v>
@@ -11275,55 +11260,55 @@
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>63</v>
-      </c>
-      <c r="B41">
-        <v>6</v>
-      </c>
-      <c r="D41" t="s">
-        <v>607</v>
-      </c>
-      <c r="E41" t="s">
-        <v>609</v>
-      </c>
-      <c r="F41" t="s">
-        <v>612</v>
-      </c>
-      <c r="G41" t="s">
-        <v>668</v>
-      </c>
-      <c r="H41" t="s">
-        <v>653</v>
-      </c>
-      <c r="K41" s="94" t="s">
+      <c r="A41" s="89">
+        <v>8</v>
+      </c>
+      <c r="B41" s="89"/>
+      <c r="C41" s="89" t="s">
+        <v>673</v>
+      </c>
+      <c r="D41" s="89" t="s">
+        <v>660</v>
+      </c>
+      <c r="E41" s="89" t="s">
+        <v>659</v>
+      </c>
+      <c r="F41" s="89" t="s">
+        <v>661</v>
+      </c>
+      <c r="G41" s="89" t="s">
+        <v>637</v>
+      </c>
+      <c r="H41" s="89" t="s">
+        <v>637</v>
+      </c>
+      <c r="I41" s="89"/>
+      <c r="J41" s="89"/>
+      <c r="K41" s="89" t="s">
         <v>165</v>
       </c>
-      <c r="L41" s="94">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L41" s="89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="B42">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D42" t="s">
-        <v>601</v>
+        <v>662</v>
       </c>
       <c r="E42" t="s">
-        <v>602</v>
-      </c>
-      <c r="F42" t="s">
-        <v>613</v>
-      </c>
-      <c r="G42" t="s">
-        <v>661</v>
+        <v>665</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>669</v>
       </c>
       <c r="H42" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="K42" s="94" t="s">
         <v>165</v>
@@ -11332,113 +11317,55 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43" s="89">
-        <v>7</v>
-      </c>
-      <c r="B43" s="89"/>
-      <c r="C43" s="89" t="s">
-        <v>675</v>
-      </c>
-      <c r="D43" s="89" t="s">
-        <v>677</v>
-      </c>
-      <c r="E43" s="89" t="s">
-        <v>676</v>
-      </c>
-      <c r="F43" s="89" t="s">
-        <v>678</v>
-      </c>
-      <c r="G43" s="89" t="s">
-        <v>653</v>
-      </c>
-      <c r="H43" s="89" t="s">
-        <v>653</v>
-      </c>
-      <c r="I43" s="89"/>
-      <c r="J43" s="89"/>
-      <c r="K43" s="89" t="s">
+    <row r="43" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>82</v>
+      </c>
+      <c r="B43">
+        <v>8</v>
+      </c>
+      <c r="D43" t="s">
+        <v>663</v>
+      </c>
+      <c r="E43" t="s">
+        <v>666</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>668</v>
+      </c>
+      <c r="H43" t="s">
+        <v>637</v>
+      </c>
+      <c r="K43" s="94" t="s">
         <v>165</v>
       </c>
-      <c r="L43" s="89">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="L43" s="94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="52" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="B44">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D44" t="s">
-        <v>679</v>
+        <v>664</v>
       </c>
       <c r="E44" t="s">
-        <v>682</v>
+        <v>667</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>687</v>
+        <v>681</v>
       </c>
       <c r="H44" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="K44" s="94" t="s">
         <v>165</v>
       </c>
       <c r="L44" s="94">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" ht="64" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>72</v>
-      </c>
-      <c r="B45">
-        <v>7</v>
-      </c>
-      <c r="D45" t="s">
-        <v>680</v>
-      </c>
-      <c r="E45" t="s">
-        <v>683</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>686</v>
-      </c>
-      <c r="H45" t="s">
-        <v>653</v>
-      </c>
-      <c r="K45" s="94" t="s">
-        <v>165</v>
-      </c>
-      <c r="L45" s="94">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" ht="48" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>73</v>
-      </c>
-      <c r="B46">
-        <v>7</v>
-      </c>
-      <c r="D46" t="s">
-        <v>681</v>
-      </c>
-      <c r="E46" t="s">
-        <v>684</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>685</v>
-      </c>
-      <c r="H46" t="s">
-        <v>653</v>
-      </c>
-      <c r="K46" s="94" t="s">
-        <v>165</v>
-      </c>
-      <c r="L46" s="94">
         <v>1</v>
       </c>
     </row>
@@ -12532,7 +12459,7 @@
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4" t="s">
-        <v>532</v>
+        <v>518</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>15</v>
@@ -13313,11 +13240,11 @@
         <v>181</v>
       </c>
       <c r="B54" s="41" t="s">
-        <v>649</v>
+        <v>633</v>
       </c>
       <c r="C54" s="41"/>
       <c r="D54" s="42" t="s">
-        <v>651</v>
+        <v>635</v>
       </c>
       <c r="E54" s="41" t="s">
         <v>15</v>
@@ -13344,11 +13271,11 @@
         <v>181</v>
       </c>
       <c r="B55" s="41" t="s">
-        <v>650</v>
+        <v>634</v>
       </c>
       <c r="C55" s="41"/>
       <c r="D55" s="42" t="s">
-        <v>652</v>
+        <v>636</v>
       </c>
       <c r="E55" s="41" t="s">
         <v>15</v>
@@ -13499,7 +13426,7 @@
       </c>
       <c r="C60" s="65"/>
       <c r="D60" s="69" t="s">
-        <v>531</v>
+        <v>517</v>
       </c>
       <c r="E60" s="65" t="s">
         <v>16</v>
@@ -14653,7 +14580,7 @@
         <v>53</v>
       </c>
       <c r="E26" s="67" t="s">
-        <v>525</v>
+        <v>511</v>
       </c>
       <c r="F26" s="65">
         <v>1</v>
@@ -14687,7 +14614,7 @@
         <v>53</v>
       </c>
       <c r="E27" s="67" t="s">
-        <v>526</v>
+        <v>512</v>
       </c>
       <c r="F27" s="65">
         <v>1</v>
@@ -14721,7 +14648,7 @@
         <v>53</v>
       </c>
       <c r="E28" s="67" t="s">
-        <v>527</v>
+        <v>513</v>
       </c>
       <c r="F28" s="65">
         <v>1</v>
@@ -14755,7 +14682,7 @@
         <v>53</v>
       </c>
       <c r="E29" s="67" t="s">
-        <v>528</v>
+        <v>514</v>
       </c>
       <c r="F29" s="65">
         <v>1</v>
@@ -14789,7 +14716,7 @@
         <v>53</v>
       </c>
       <c r="E30" s="67" t="s">
-        <v>529</v>
+        <v>515</v>
       </c>
       <c r="F30" s="65">
         <v>1</v>
@@ -14823,7 +14750,7 @@
         <v>53</v>
       </c>
       <c r="E31" s="67" t="s">
-        <v>530</v>
+        <v>516</v>
       </c>
       <c r="F31" s="65">
         <v>1</v>
@@ -15455,7 +15382,7 @@
         <v>168</v>
       </c>
       <c r="E50" s="104" t="s">
-        <v>522</v>
+        <v>508</v>
       </c>
       <c r="F50" s="103">
         <v>1</v>
@@ -15488,7 +15415,7 @@
         <v>168</v>
       </c>
       <c r="E51" s="98" t="s">
-        <v>571</v>
+        <v>557</v>
       </c>
       <c r="F51" s="97">
         <v>1</v>
@@ -15521,7 +15448,7 @@
         <v>168</v>
       </c>
       <c r="E52" s="98" t="s">
-        <v>572</v>
+        <v>558</v>
       </c>
       <c r="F52" s="97">
         <v>1</v>
@@ -15554,7 +15481,7 @@
         <v>168</v>
       </c>
       <c r="E53" s="98" t="s">
-        <v>570</v>
+        <v>556</v>
       </c>
       <c r="F53" s="97">
         <v>1</v>
@@ -15587,7 +15514,7 @@
         <v>168</v>
       </c>
       <c r="E54" s="98" t="s">
-        <v>573</v>
+        <v>559</v>
       </c>
       <c r="F54" s="97">
         <v>1</v>
@@ -15620,7 +15547,7 @@
         <v>168</v>
       </c>
       <c r="E55" s="98" t="s">
-        <v>574</v>
+        <v>560</v>
       </c>
       <c r="F55" s="97">
         <v>1</v>
@@ -15653,7 +15580,7 @@
         <v>168</v>
       </c>
       <c r="E56" s="98" t="s">
-        <v>569</v>
+        <v>555</v>
       </c>
       <c r="F56" s="97">
         <v>1</v>
@@ -15686,7 +15613,7 @@
         <v>168</v>
       </c>
       <c r="E57" s="98" t="s">
-        <v>575</v>
+        <v>561</v>
       </c>
       <c r="F57" s="97">
         <v>1</v>
@@ -15763,13 +15690,13 @@
         <v>99</v>
       </c>
       <c r="B2" s="93" t="s">
-        <v>523</v>
+        <v>509</v>
       </c>
       <c r="C2" s="93" t="s">
         <v>430</v>
       </c>
       <c r="D2" s="92" t="s">
-        <v>533</v>
+        <v>519</v>
       </c>
       <c r="E2" s="92" t="s">
         <v>429</v>
@@ -15783,7 +15710,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="91" t="s">
-        <v>524</v>
+        <v>510</v>
       </c>
       <c r="C3" s="91" t="s">
         <v>431</v>

</xml_diff>

<commit_message>
change cat datatype in direct_executes
</commit_message>
<xml_diff>
--- a/db/excel/api-function-granted-users-cdld.xlsx
+++ b/db/excel/api-function-granted-users-cdld.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10711"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2085528-406F-2A41-813E-77B683B55EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B9FA57-F35C-1C47-B4C2-BADCFFC1DEE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" tabRatio="800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6709,10 +6709,10 @@
   <dimension ref="A1:P99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C54" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C43" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B73" sqref="B73"/>
+      <selection pane="bottomRight" activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
push get dx by dos api
</commit_message>
<xml_diff>
--- a/db/excel/api-function-granted-users-cdld.xlsx
+++ b/db/excel/api-function-granted-users-cdld.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10711"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B9FA57-F35C-1C47-B4C2-BADCFFC1DEE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8261661-E7A8-A84B-9875-68B57C8B0813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" tabRatio="800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19480" tabRatio="800" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_types" sheetId="27" r:id="rId1"/>
@@ -1214,13 +1214,7 @@
     <t>/update-direct</t>
   </si>
   <si>
-    <t>/get-direct-org</t>
-  </si>
-  <si>
     <t>Lấy Chỉ Đạo Đơn Vị Theo Mã Đơn Vị (organization-id)</t>
-  </si>
-  <si>
-    <t>/get-direct-by-org</t>
   </si>
   <si>
     <t>/get-direct-org-all</t>
@@ -2454,6 +2448,12 @@
   </si>
   <si>
     <t>/update-direct-org-exec-status</t>
+  </si>
+  <si>
+    <t>/get-direct-org-detail</t>
+  </si>
+  <si>
+    <t>/get-direct-exe-by-dos</t>
   </si>
 </sst>
 </file>
@@ -5372,22 +5372,22 @@
       </c>
       <c r="B2" s="83"/>
       <c r="C2" s="83" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D2" s="83" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E2" s="84" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F2" s="84" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="G2" s="84" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="H2" s="83" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="I2" s="83"/>
       <c r="J2" s="83"/>
@@ -5408,18 +5408,18 @@
         <v>1</v>
       </c>
       <c r="C3" s="79" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D3" s="79"/>
       <c r="E3" s="80" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="F3" s="80"/>
       <c r="G3" s="80" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="H3" s="79" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="I3" s="79"/>
       <c r="J3" s="79"/>
@@ -5440,18 +5440,18 @@
         <v>1</v>
       </c>
       <c r="C4" s="79" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D4" s="79"/>
       <c r="E4" s="80" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F4" s="80"/>
       <c r="G4" s="80" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H4" s="79" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="I4" s="79"/>
       <c r="J4" s="79"/>
@@ -5472,18 +5472,18 @@
         <v>1</v>
       </c>
       <c r="C5" s="79" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D5" s="79"/>
       <c r="E5" s="80" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F5" s="80"/>
       <c r="G5" s="80" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="H5" s="79" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="I5" s="79"/>
       <c r="J5" s="79"/>
@@ -5504,18 +5504,18 @@
         <v>1</v>
       </c>
       <c r="C6" s="79" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D6" s="79"/>
       <c r="E6" s="80" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F6" s="80"/>
       <c r="G6" s="80" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="H6" s="79" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="I6" s="79"/>
       <c r="J6" s="79"/>
@@ -5536,18 +5536,18 @@
         <v>1</v>
       </c>
       <c r="C7" s="79" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D7" s="79"/>
       <c r="E7" s="80" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F7" s="80"/>
       <c r="G7" s="80" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="H7" s="79" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="I7" s="79"/>
       <c r="J7" s="79"/>
@@ -5568,18 +5568,18 @@
         <v>1</v>
       </c>
       <c r="C8" s="79" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D8" s="79"/>
       <c r="E8" s="80" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="F8" s="80"/>
       <c r="G8" s="80" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="H8" s="79" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="I8" s="79"/>
       <c r="J8" s="79"/>
@@ -5598,22 +5598,22 @@
       </c>
       <c r="B9" s="83"/>
       <c r="C9" s="83" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D9" s="83" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="E9" s="84" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F9" s="84" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="G9" s="84" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="H9" s="83" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="I9" s="83"/>
       <c r="J9" s="83"/>
@@ -5634,18 +5634,18 @@
         <v>2</v>
       </c>
       <c r="C10" s="79" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D10" s="79"/>
       <c r="E10" s="80" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F10" s="80"/>
       <c r="G10" s="80" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="H10" s="79" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="I10" s="79"/>
       <c r="J10" s="81"/>
@@ -5666,18 +5666,18 @@
         <v>2</v>
       </c>
       <c r="C11" s="79" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D11" s="79"/>
       <c r="E11" s="80" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="F11" s="80"/>
       <c r="G11" s="80" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H11" s="79" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="I11" s="79"/>
       <c r="J11" s="79"/>
@@ -5698,18 +5698,18 @@
         <v>2</v>
       </c>
       <c r="C12" s="79" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D12" s="79"/>
       <c r="E12" s="80" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="F12" s="80"/>
       <c r="G12" s="80" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H12" s="79" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="I12" s="79"/>
       <c r="J12" s="79"/>
@@ -5730,18 +5730,18 @@
         <v>2</v>
       </c>
       <c r="C13" s="79" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D13" s="79"/>
       <c r="E13" s="80" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="F13" s="80"/>
       <c r="G13" s="80" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="H13" s="79" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="I13" s="79"/>
       <c r="J13" s="79"/>
@@ -5760,22 +5760,22 @@
       </c>
       <c r="B14" s="83"/>
       <c r="C14" s="83" t="s">
+        <v>396</v>
+      </c>
+      <c r="D14" s="83" t="s">
         <v>398</v>
       </c>
-      <c r="D14" s="83" t="s">
-        <v>400</v>
-      </c>
       <c r="E14" s="84" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F14" s="84" t="s">
+        <v>426</v>
+      </c>
+      <c r="G14" s="84" t="s">
+        <v>416</v>
+      </c>
+      <c r="H14" s="83" t="s">
         <v>428</v>
-      </c>
-      <c r="G14" s="84" t="s">
-        <v>418</v>
-      </c>
-      <c r="H14" s="83" t="s">
-        <v>430</v>
       </c>
       <c r="I14" s="83"/>
       <c r="J14" s="83"/>
@@ -5796,18 +5796,18 @@
         <v>3</v>
       </c>
       <c r="C15" s="79" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D15" s="79"/>
       <c r="E15" s="80" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="F15" s="80"/>
       <c r="G15" s="80" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="H15" s="79" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I15" s="79"/>
       <c r="J15" s="81"/>
@@ -5826,20 +5826,20 @@
       </c>
       <c r="B16" s="83"/>
       <c r="C16" s="83" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D16" s="83"/>
       <c r="E16" s="84" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F16" s="84" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="G16" s="84" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="H16" s="83" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="I16" s="83"/>
       <c r="J16" s="83"/>
@@ -5890,7 +5890,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C1" s="22" t="s">
         <v>38</v>
@@ -5899,7 +5899,7 @@
         <v>39</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="F1" s="22" t="s">
         <v>139</v>
@@ -5931,10 +5931,10 @@
         <v>109</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F2" s="29"/>
       <c r="G2" s="29"/>
@@ -5958,10 +5958,10 @@
         <v>109</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F3" s="29"/>
       <c r="G3" s="29"/>
@@ -5985,10 +5985,10 @@
         <v>109</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F4" s="28"/>
       <c r="G4" s="28"/>
@@ -6012,10 +6012,10 @@
         <v>109</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F5" s="28"/>
       <c r="G5" s="28"/>
@@ -6030,7 +6030,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="28" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="B6" s="28">
         <v>5</v>
@@ -6039,10 +6039,10 @@
         <v>109</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F6" s="28"/>
       <c r="G6" s="28"/>
@@ -6057,7 +6057,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="28" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B7" s="28">
         <v>3</v>
@@ -6066,10 +6066,10 @@
         <v>109</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
@@ -6130,10 +6130,10 @@
         <v>233</v>
       </c>
       <c r="D1" s="39" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="E1" s="39" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F1" s="39" t="s">
         <v>178</v>
@@ -6162,13 +6162,13 @@
         <v>187</v>
       </c>
       <c r="C2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D2" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="E2" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="J2" t="s">
         <v>185</v>
@@ -6185,13 +6185,13 @@
         <v>186</v>
       </c>
       <c r="C3" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="D3" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="E3" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="J3" t="s">
         <v>185</v>
@@ -6208,13 +6208,13 @@
         <v>188</v>
       </c>
       <c r="C4" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="D4" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="E4" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="J4" t="s">
         <v>185</v>
@@ -6228,16 +6228,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="C5" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="D5" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="E5" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="J5" t="s">
         <v>185</v>
@@ -6251,16 +6251,16 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="C6" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="D6" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="E6" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="J6" t="s">
         <v>185</v>
@@ -6274,16 +6274,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="C7" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="D7" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="E7" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="J7" t="s">
         <v>185</v>
@@ -6297,16 +6297,16 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="C8" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="D8" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="E8" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="J8" t="s">
         <v>185</v>
@@ -6320,16 +6320,16 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="C9" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="D9" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="E9" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="J9" t="s">
         <v>185</v>
@@ -6346,13 +6346,13 @@
         <v>195</v>
       </c>
       <c r="C10" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="D10" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="E10" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="J10" t="s">
         <v>185</v>
@@ -6369,13 +6369,13 @@
         <v>193</v>
       </c>
       <c r="C11" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="D11" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="E11" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="J11" t="s">
         <v>185</v>
@@ -6392,13 +6392,13 @@
         <v>190</v>
       </c>
       <c r="C12" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="D12" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="E12" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="J12" t="s">
         <v>185</v>
@@ -6415,13 +6415,13 @@
         <v>189</v>
       </c>
       <c r="C13" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="D13" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="E13" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="J13" t="s">
         <v>185</v>
@@ -6438,13 +6438,13 @@
         <v>192</v>
       </c>
       <c r="C14" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="D14" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="E14" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="J14" t="s">
         <v>185</v>
@@ -6461,13 +6461,13 @@
         <v>191</v>
       </c>
       <c r="C15" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="D15" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="E15" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="J15" t="s">
         <v>185</v>
@@ -6484,13 +6484,13 @@
         <v>194</v>
       </c>
       <c r="C16" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="D16" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="E16" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="J16" t="s">
         <v>185</v>
@@ -6507,13 +6507,13 @@
         <v>196</v>
       </c>
       <c r="C17" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="D17" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="E17" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="J17" t="s">
         <v>185</v>
@@ -6547,10 +6547,10 @@
         <v>18</v>
       </c>
       <c r="B1" s="61" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C1" s="61" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D1" s="61" t="s">
         <v>19</v>
@@ -6595,7 +6595,7 @@
         <v>222</v>
       </c>
       <c r="C4" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E4" t="s">
         <v>185</v>
@@ -6609,7 +6609,7 @@
         <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="E5" t="s">
         <v>185</v>
@@ -6637,7 +6637,7 @@
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E7" t="s">
         <v>185</v>
@@ -6651,7 +6651,7 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="E8" t="s">
         <v>185</v>
@@ -6679,7 +6679,7 @@
         <v>154</v>
       </c>
       <c r="C10" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="E10" t="s">
         <v>185</v>
@@ -6693,7 +6693,7 @@
         <v>155</v>
       </c>
       <c r="C11" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="E11" t="s">
         <v>185</v>
@@ -6708,11 +6708,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C43" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C70" sqref="C70"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6775,10 +6775,10 @@
         <v>13</v>
       </c>
       <c r="N1" s="51" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="O1" s="51" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="P1" s="51" t="s">
         <v>14</v>
@@ -6897,7 +6897,7 @@
         <v>251</v>
       </c>
       <c r="D5" s="103" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="E5" s="103" t="s">
         <v>16</v>
@@ -7209,13 +7209,13 @@
         <v>212</v>
       </c>
       <c r="B15" s="48" t="s">
+        <v>633</v>
+      </c>
+      <c r="C15" s="48" t="s">
+        <v>634</v>
+      </c>
+      <c r="D15" s="48" t="s">
         <v>635</v>
-      </c>
-      <c r="C15" s="48" t="s">
-        <v>636</v>
-      </c>
-      <c r="D15" s="48" t="s">
-        <v>637</v>
       </c>
       <c r="E15" s="48" t="s">
         <v>16</v>
@@ -7229,7 +7229,7 @@
       <c r="J15" s="55"/>
       <c r="K15" s="55"/>
       <c r="L15" s="56" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="M15" s="55"/>
       <c r="N15" s="55"/>
@@ -7243,13 +7243,13 @@
         <v>212</v>
       </c>
       <c r="B16" s="48" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C16" s="48" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D16" s="48" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E16" s="48" t="s">
         <v>15</v>
@@ -7321,7 +7321,7 @@
         <v>243</v>
       </c>
       <c r="D18" s="105" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="E18" s="105" t="s">
         <v>16</v>
@@ -7335,7 +7335,7 @@
       <c r="J18" s="55"/>
       <c r="K18" s="55"/>
       <c r="L18" s="56" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="M18" s="55"/>
       <c r="N18" s="55"/>
@@ -7349,13 +7349,13 @@
         <v>212</v>
       </c>
       <c r="B19" s="48" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C19" s="48" t="s">
+        <v>429</v>
+      </c>
+      <c r="D19" s="48" t="s">
         <v>431</v>
-      </c>
-      <c r="D19" s="48" t="s">
-        <v>433</v>
       </c>
       <c r="E19" s="48" t="s">
         <v>15</v>
@@ -7371,7 +7371,7 @@
       <c r="J19" s="55"/>
       <c r="K19" s="55"/>
       <c r="L19" s="56" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="M19" s="55"/>
       <c r="N19" s="55"/>
@@ -7481,13 +7481,13 @@
         <v>212</v>
       </c>
       <c r="B23" s="48" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="C23" s="48" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D23" s="48" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="E23" s="48" t="s">
         <v>50</v>
@@ -7635,13 +7635,13 @@
         <v>212</v>
       </c>
       <c r="B28" s="48" t="s">
+        <v>434</v>
+      </c>
+      <c r="C28" s="48" t="s">
+        <v>435</v>
+      </c>
+      <c r="D28" s="48" t="s">
         <v>436</v>
-      </c>
-      <c r="C28" s="48" t="s">
-        <v>437</v>
-      </c>
-      <c r="D28" s="48" t="s">
-        <v>438</v>
       </c>
       <c r="E28" s="48" t="s">
         <v>15</v>
@@ -7667,13 +7667,13 @@
         <v>212</v>
       </c>
       <c r="B29" s="48" t="s">
+        <v>460</v>
+      </c>
+      <c r="C29" s="48" t="s">
+        <v>461</v>
+      </c>
+      <c r="D29" s="48" t="s">
         <v>462</v>
-      </c>
-      <c r="C29" s="48" t="s">
-        <v>463</v>
-      </c>
-      <c r="D29" s="48" t="s">
-        <v>464</v>
       </c>
       <c r="E29" s="48" t="s">
         <v>15</v>
@@ -7705,7 +7705,7 @@
         <v>227</v>
       </c>
       <c r="D30" s="48" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="E30" s="48" t="s">
         <v>17</v>
@@ -7728,7 +7728,7 @@
     </row>
     <row r="31" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="91" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B31" s="91" t="s">
         <v>18</v>
@@ -7737,7 +7737,7 @@
         <v>234</v>
       </c>
       <c r="D31" s="91" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="E31" s="91" t="s">
         <v>97</v>
@@ -7766,16 +7766,16 @@
     </row>
     <row r="32" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="91" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B32" s="91" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="C32" s="91" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="D32" s="91" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="E32" s="91" t="s">
         <v>16</v>
@@ -7796,16 +7796,16 @@
     </row>
     <row r="33" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="91" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B33" s="91" t="s">
         <v>213</v>
       </c>
       <c r="C33" s="91" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="D33" s="91" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="E33" s="91" t="s">
         <v>16</v>
@@ -7826,16 +7826,16 @@
     </row>
     <row r="34" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="91" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B34" s="91" t="s">
+        <v>534</v>
+      </c>
+      <c r="C34" s="91" t="s">
+        <v>535</v>
+      </c>
+      <c r="D34" s="91" t="s">
         <v>536</v>
-      </c>
-      <c r="C34" s="91" t="s">
-        <v>537</v>
-      </c>
-      <c r="D34" s="91" t="s">
-        <v>538</v>
       </c>
       <c r="E34" s="91" t="s">
         <v>15</v>
@@ -7849,7 +7849,7 @@
       <c r="J34" s="92"/>
       <c r="K34" s="92"/>
       <c r="L34" s="56" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="M34" s="92"/>
       <c r="N34" s="92"/>
@@ -7860,7 +7860,7 @@
     </row>
     <row r="35" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="91" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B35" s="91" t="s">
         <v>218</v>
@@ -7869,7 +7869,7 @@
         <v>261</v>
       </c>
       <c r="D35" s="91" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="E35" s="91" t="s">
         <v>15</v>
@@ -7892,7 +7892,7 @@
     </row>
     <row r="36" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="91" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B36" s="91" t="s">
         <v>219</v>
@@ -7901,7 +7901,7 @@
         <v>262</v>
       </c>
       <c r="D36" s="91" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="E36" s="91" t="s">
         <v>15</v>
@@ -7924,16 +7924,16 @@
     </row>
     <row r="37" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="91" t="s">
+        <v>484</v>
+      </c>
+      <c r="B37" s="91" t="s">
+        <v>485</v>
+      </c>
+      <c r="C37" s="91" t="s">
         <v>486</v>
       </c>
-      <c r="B37" s="91" t="s">
+      <c r="D37" s="91" t="s">
         <v>487</v>
-      </c>
-      <c r="C37" s="91" t="s">
-        <v>488</v>
-      </c>
-      <c r="D37" s="91" t="s">
-        <v>489</v>
       </c>
       <c r="E37" s="91" t="s">
         <v>15</v>
@@ -7956,16 +7956,16 @@
     </row>
     <row r="38" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="91" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B38" s="91" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C38" s="91" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D38" s="91" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="E38" s="91" t="s">
         <v>97</v>
@@ -7986,7 +7986,7 @@
     </row>
     <row r="39" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="91" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B39" s="91" t="s">
         <v>197</v>
@@ -8016,7 +8016,7 @@
     </row>
     <row r="40" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="91" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B40" s="91" t="s">
         <v>222</v>
@@ -8048,7 +8048,7 @@
     </row>
     <row r="41" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="91" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B41" s="91" t="s">
         <v>19</v>
@@ -8078,7 +8078,7 @@
     </row>
     <row r="42" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="91" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B42" s="91" t="s">
         <v>45</v>
@@ -8110,7 +8110,7 @@
     </row>
     <row r="43" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="91" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B43" s="91" t="s">
         <v>0</v>
@@ -8119,7 +8119,7 @@
         <v>227</v>
       </c>
       <c r="D43" s="91" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="E43" s="91" t="s">
         <v>17</v>
@@ -8179,13 +8179,13 @@
         <v>267</v>
       </c>
       <c r="B45" s="47" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C45" s="47" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="D45" s="47" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="E45" s="47" t="s">
         <v>15</v>
@@ -8217,13 +8217,13 @@
         <v>267</v>
       </c>
       <c r="B46" s="47" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="C46" s="47" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="D46" s="47" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="E46" s="47" t="s">
         <v>16</v>
@@ -8237,7 +8237,7 @@
       <c r="J46" s="52"/>
       <c r="K46" s="52"/>
       <c r="L46" s="56" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="M46" s="52"/>
       <c r="N46" s="52"/>
@@ -8257,7 +8257,7 @@
         <v>269</v>
       </c>
       <c r="D47" s="47" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E47" s="47" t="s">
         <v>16</v>
@@ -8271,7 +8271,7 @@
       <c r="J47" s="52"/>
       <c r="K47" s="52"/>
       <c r="L47" s="56" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="M47" s="52"/>
       <c r="N47" s="52"/>
@@ -8285,13 +8285,13 @@
         <v>267</v>
       </c>
       <c r="B48" s="47" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C48" s="47" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="D48" s="47" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="E48" s="47" t="s">
         <v>15</v>
@@ -8307,7 +8307,7 @@
       <c r="J48" s="52"/>
       <c r="K48" s="52"/>
       <c r="L48" s="56" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="M48" s="52"/>
       <c r="N48" s="52"/>
@@ -8341,7 +8341,7 @@
       <c r="J49" s="52"/>
       <c r="K49" s="52"/>
       <c r="L49" s="56" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="M49" s="52"/>
       <c r="N49" s="52"/>
@@ -8361,7 +8361,7 @@
         <v>273</v>
       </c>
       <c r="D50" s="47" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="E50" s="47" t="s">
         <v>16</v>
@@ -8393,7 +8393,7 @@
         <v>242</v>
       </c>
       <c r="D51" s="47" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="E51" s="47" t="s">
         <v>15</v>
@@ -8451,13 +8451,13 @@
         <v>267</v>
       </c>
       <c r="B53" s="103" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="C53" s="103" t="s">
         <v>265</v>
       </c>
       <c r="D53" s="103" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="E53" s="103" t="s">
         <v>16</v>
@@ -8469,7 +8469,7 @@
       <c r="J53" s="104"/>
       <c r="K53" s="104"/>
       <c r="L53" s="56" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="M53" s="104"/>
       <c r="N53" s="104"/>
@@ -8483,13 +8483,13 @@
         <v>267</v>
       </c>
       <c r="B54" s="47" t="s">
+        <v>434</v>
+      </c>
+      <c r="C54" s="47" t="s">
+        <v>435</v>
+      </c>
+      <c r="D54" s="47" t="s">
         <v>436</v>
-      </c>
-      <c r="C54" s="47" t="s">
-        <v>437</v>
-      </c>
-      <c r="D54" s="47" t="s">
-        <v>438</v>
       </c>
       <c r="E54" s="47" t="s">
         <v>15</v>
@@ -8515,13 +8515,13 @@
         <v>267</v>
       </c>
       <c r="B55" s="47" t="s">
+        <v>457</v>
+      </c>
+      <c r="C55" s="47" t="s">
+        <v>458</v>
+      </c>
+      <c r="D55" s="47" t="s">
         <v>459</v>
-      </c>
-      <c r="C55" s="47" t="s">
-        <v>460</v>
-      </c>
-      <c r="D55" s="47" t="s">
-        <v>461</v>
       </c>
       <c r="E55" s="47" t="s">
         <v>15</v>
@@ -8547,13 +8547,13 @@
         <v>267</v>
       </c>
       <c r="B56" s="47" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="C56" s="47" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D56" s="47" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="E56" s="47" t="s">
         <v>50</v>
@@ -8580,10 +8580,10 @@
         <v>220</v>
       </c>
       <c r="C57" s="113" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="D57" s="113" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="E57" s="113" t="s">
         <v>15</v>
@@ -8739,7 +8739,7 @@
         <v>227</v>
       </c>
       <c r="D62" s="47" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="E62" s="47" t="s">
         <v>17</v>
@@ -8799,13 +8799,13 @@
         <v>266</v>
       </c>
       <c r="B64" s="49" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C64" s="49" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="D64" s="49" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="E64" s="49" t="s">
         <v>15</v>
@@ -8837,13 +8837,13 @@
         <v>266</v>
       </c>
       <c r="B65" s="49" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C65" s="49" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="D65" s="49" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="E65" s="49" t="s">
         <v>15</v>
@@ -8859,7 +8859,7 @@
       <c r="J65" s="44"/>
       <c r="K65" s="44"/>
       <c r="L65" s="56" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="M65" s="44"/>
       <c r="N65" s="44"/>
@@ -8873,10 +8873,10 @@
         <v>266</v>
       </c>
       <c r="B66" s="49" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="C66" s="49" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="D66" s="49" t="s">
         <v>277</v>
@@ -8895,7 +8895,7 @@
       <c r="J66" s="44"/>
       <c r="K66" s="44"/>
       <c r="L66" s="56" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="M66" s="44"/>
       <c r="N66" s="44"/>
@@ -8929,7 +8929,7 @@
       <c r="J67" s="44"/>
       <c r="K67" s="44"/>
       <c r="L67" s="56" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="M67" s="44"/>
       <c r="N67" s="44"/>
@@ -9013,7 +9013,7 @@
         <v>282</v>
       </c>
       <c r="D70" s="108" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="E70" s="107" t="s">
         <v>16</v>
@@ -9027,7 +9027,7 @@
       <c r="J70" s="44"/>
       <c r="K70" s="44"/>
       <c r="L70" s="56" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="M70" s="44"/>
       <c r="N70" s="44"/>
@@ -9138,10 +9138,10 @@
         <v>0</v>
       </c>
       <c r="C74" s="49" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D74" s="49" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E74" s="49" t="s">
         <v>17</v>
@@ -9203,13 +9203,13 @@
         <v>209</v>
       </c>
       <c r="B76" s="50" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C76" s="50" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D76" s="50" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E76" s="50" t="s">
         <v>15</v>
@@ -9247,7 +9247,7 @@
         <v>237</v>
       </c>
       <c r="D77" s="110" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E77" s="110" t="s">
         <v>16</v>
@@ -9259,7 +9259,7 @@
       <c r="J77" s="57"/>
       <c r="K77" s="57"/>
       <c r="L77" s="56" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="M77" s="57"/>
       <c r="N77" s="57"/>
@@ -9596,10 +9596,10 @@
         <v>138</v>
       </c>
       <c r="C88" s="42" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D88" s="58" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E88" s="58" t="s">
         <v>16</v>
@@ -9625,13 +9625,13 @@
         <v>168</v>
       </c>
       <c r="B89" s="42" t="s">
+        <v>515</v>
+      </c>
+      <c r="C89" s="42" t="s">
+        <v>516</v>
+      </c>
+      <c r="D89" s="58" t="s">
         <v>517</v>
-      </c>
-      <c r="C89" s="42" t="s">
-        <v>518</v>
-      </c>
-      <c r="D89" s="58" t="s">
-        <v>519</v>
       </c>
       <c r="E89" s="58" t="s">
         <v>15</v>
@@ -9755,13 +9755,13 @@
         <v>168</v>
       </c>
       <c r="B93" s="42" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="C93" s="42" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="D93" s="58" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="E93" s="58" t="s">
         <v>15</v>
@@ -9787,13 +9787,13 @@
         <v>168</v>
       </c>
       <c r="B94" s="42" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="C94" s="42" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="D94" s="58" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="E94" s="58" t="s">
         <v>15</v>
@@ -10010,7 +10010,7 @@
         <v>138</v>
       </c>
       <c r="C1" s="38" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D1" s="38" t="s">
         <v>233</v>
@@ -10022,10 +10022,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="38" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="H1" s="38" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="I1" s="38" t="s">
         <v>197</v>
@@ -10046,22 +10046,22 @@
       </c>
       <c r="B2" s="85"/>
       <c r="C2" s="85" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D2" s="85" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E2" s="85" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F2" s="85" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G2" s="85" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="H2" s="85" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="I2" s="85"/>
       <c r="J2" s="85"/>
@@ -10080,19 +10080,19 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E3" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="F3" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G3" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="H3" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K3" t="s">
         <v>164</v>
@@ -10109,19 +10109,19 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E4" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="F4" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="G4" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="H4" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K4" t="s">
         <v>164</v>
@@ -10138,19 +10138,19 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
+        <v>363</v>
+      </c>
+      <c r="E5" t="s">
+        <v>364</v>
+      </c>
+      <c r="F5" t="s">
         <v>365</v>
       </c>
-      <c r="E5" t="s">
-        <v>366</v>
-      </c>
-      <c r="F5" t="s">
-        <v>367</v>
-      </c>
       <c r="G5" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="H5" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K5" t="s">
         <v>164</v>
@@ -10167,19 +10167,19 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="E6" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="F6" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="G6" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="H6" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K6" t="s">
         <v>164</v>
@@ -10196,19 +10196,19 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="E7" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="F7" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G7" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="H7" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K7" t="s">
         <v>164</v>
@@ -10223,22 +10223,22 @@
       </c>
       <c r="B8" s="85"/>
       <c r="C8" s="85" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="D8" s="85" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E8" s="85" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="F8" s="85" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="G8" s="85" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="H8" s="85" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="I8" s="85"/>
       <c r="J8" s="85"/>
@@ -10257,19 +10257,19 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E9" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F9" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="G9" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="H9" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K9" t="s">
         <v>164</v>
@@ -10286,19 +10286,19 @@
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="F10" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="G10" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="H10" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K10" t="s">
         <v>164</v>
@@ -10313,22 +10313,22 @@
       </c>
       <c r="B11" s="85"/>
       <c r="C11" s="85" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="D11" s="85" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="E11" s="85" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F11" s="85" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="G11" s="85" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="H11" s="85" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="I11" s="85"/>
       <c r="J11" s="85"/>
@@ -10347,19 +10347,19 @@
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="E12" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="F12" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="G12" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="H12" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K12" t="s">
         <v>164</v>
@@ -10376,19 +10376,19 @@
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="E13" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="F13" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="G13" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="H13" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K13" t="s">
         <v>164</v>
@@ -10405,19 +10405,19 @@
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="E14" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="F14" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="G14" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="H14" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K14" t="s">
         <v>164</v>
@@ -10434,19 +10434,19 @@
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="E15" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="F15" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="G15" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="H15" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K15" t="s">
         <v>164</v>
@@ -10463,19 +10463,19 @@
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="E16" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="F16" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="G16" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="H16" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K16" t="s">
         <v>164</v>
@@ -10492,19 +10492,19 @@
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="E17" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="F17" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="G17" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="H17" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K17" t="s">
         <v>164</v>
@@ -10519,22 +10519,22 @@
       </c>
       <c r="B18" s="85"/>
       <c r="C18" s="85" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="D18" s="85" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E18" s="85" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="F18" s="85" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="G18" s="85" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="H18" s="85" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="I18" s="85"/>
       <c r="J18" s="85"/>
@@ -10553,19 +10553,19 @@
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="E19" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F19" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="G19" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="H19" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K19" t="s">
         <v>164</v>
@@ -10582,19 +10582,19 @@
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="E20" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="F20" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="G20" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="H20" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K20" t="s">
         <v>164</v>
@@ -10611,19 +10611,19 @@
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="E21" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F21" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="G21" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="H21" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K21" t="s">
         <v>164</v>
@@ -10640,19 +10640,19 @@
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="E22" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F22" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="G22" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="H22" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K22" t="s">
         <v>164</v>
@@ -10667,22 +10667,22 @@
       </c>
       <c r="B23" s="85"/>
       <c r="C23" s="85" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="D23" s="85" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="E23" s="85" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="F23" s="85" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="G23" s="85" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="H23" s="85" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="I23" s="85"/>
       <c r="J23" s="85"/>
@@ -10701,19 +10701,19 @@
         <v>5</v>
       </c>
       <c r="D24" t="s">
+        <v>481</v>
+      </c>
+      <c r="E24" t="s">
+        <v>482</v>
+      </c>
+      <c r="F24" t="s">
         <v>483</v>
       </c>
-      <c r="E24" t="s">
-        <v>484</v>
-      </c>
-      <c r="F24" t="s">
-        <v>485</v>
-      </c>
       <c r="G24" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="H24" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K24" t="s">
         <v>164</v>
@@ -10730,19 +10730,19 @@
         <v>5</v>
       </c>
       <c r="D25" t="s">
+        <v>439</v>
+      </c>
+      <c r="E25" t="s">
         <v>441</v>
       </c>
-      <c r="E25" t="s">
-        <v>443</v>
-      </c>
       <c r="F25" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="G25" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="H25" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K25" t="s">
         <v>164</v>
@@ -10759,19 +10759,19 @@
         <v>5</v>
       </c>
       <c r="D26" t="s">
+        <v>450</v>
+      </c>
+      <c r="E26" t="s">
         <v>452</v>
       </c>
-      <c r="E26" t="s">
-        <v>454</v>
-      </c>
       <c r="F26" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="G26" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="H26" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K26" s="90" t="s">
         <v>164</v>
@@ -10788,19 +10788,19 @@
         <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E27" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="F27" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="G27" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="H27" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K27" s="90" t="s">
         <v>164</v>
@@ -10817,19 +10817,19 @@
         <v>5</v>
       </c>
       <c r="D28" t="s">
+        <v>463</v>
+      </c>
+      <c r="E28" t="s">
+        <v>464</v>
+      </c>
+      <c r="F28" t="s">
         <v>465</v>
       </c>
-      <c r="E28" t="s">
-        <v>466</v>
-      </c>
-      <c r="F28" t="s">
-        <v>467</v>
-      </c>
       <c r="G28" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="H28" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K28" s="90" t="s">
         <v>164</v>
@@ -10846,19 +10846,19 @@
         <v>5</v>
       </c>
       <c r="D29" t="s">
+        <v>442</v>
+      </c>
+      <c r="E29" t="s">
+        <v>443</v>
+      </c>
+      <c r="F29" t="s">
         <v>444</v>
       </c>
-      <c r="E29" t="s">
-        <v>445</v>
-      </c>
-      <c r="F29" t="s">
-        <v>446</v>
-      </c>
       <c r="G29" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="H29" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K29" t="s">
         <v>164</v>
@@ -10873,22 +10873,22 @@
       </c>
       <c r="B30" s="85"/>
       <c r="C30" s="85" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D30" s="85" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="E30" s="85" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="F30" s="85" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="G30" s="85" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="H30" s="85" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="I30" s="85"/>
       <c r="J30" s="85"/>
@@ -10907,19 +10907,19 @@
         <v>6</v>
       </c>
       <c r="D31" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="E31" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="F31" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="G31" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="H31" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K31" t="s">
         <v>164</v>
@@ -10936,19 +10936,19 @@
         <v>6</v>
       </c>
       <c r="D32" t="s">
+        <v>445</v>
+      </c>
+      <c r="E32" t="s">
+        <v>446</v>
+      </c>
+      <c r="F32" t="s">
         <v>447</v>
       </c>
-      <c r="E32" t="s">
-        <v>448</v>
-      </c>
-      <c r="F32" t="s">
-        <v>449</v>
-      </c>
       <c r="G32" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="H32" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K32" t="s">
         <v>164</v>
@@ -10965,19 +10965,19 @@
         <v>6</v>
       </c>
       <c r="D33" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="E33" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="F33" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="G33" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="H33" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K33" s="90" t="s">
         <v>164</v>
@@ -10994,19 +10994,19 @@
         <v>6</v>
       </c>
       <c r="D34" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="E34" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="F34" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="G34" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="H34" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K34" s="90" t="s">
         <v>164</v>
@@ -11023,19 +11023,19 @@
         <v>6</v>
       </c>
       <c r="D35" t="s">
+        <v>466</v>
+      </c>
+      <c r="E35" t="s">
+        <v>467</v>
+      </c>
+      <c r="F35" t="s">
         <v>468</v>
       </c>
-      <c r="E35" t="s">
-        <v>469</v>
-      </c>
-      <c r="F35" t="s">
-        <v>470</v>
-      </c>
       <c r="G35" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="H35" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K35" s="90" t="s">
         <v>164</v>
@@ -11050,22 +11050,22 @@
       </c>
       <c r="B36" s="85"/>
       <c r="C36" s="85" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="D36" s="85" t="s">
+        <v>572</v>
+      </c>
+      <c r="E36" s="85" t="s">
+        <v>573</v>
+      </c>
+      <c r="F36" s="85" t="s">
         <v>574</v>
       </c>
-      <c r="E36" s="85" t="s">
-        <v>575</v>
-      </c>
-      <c r="F36" s="85" t="s">
-        <v>576</v>
-      </c>
       <c r="G36" s="85" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="H36" s="85" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="I36" s="85"/>
       <c r="J36" s="85"/>
@@ -11084,19 +11084,19 @@
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E37" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="F37" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="G37" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="H37" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K37" s="90" t="s">
         <v>164</v>
@@ -11113,19 +11113,19 @@
         <v>7</v>
       </c>
       <c r="D38" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="E38" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="F38" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="G38" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="H38" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K38" s="90" t="s">
         <v>164</v>
@@ -11142,19 +11142,19 @@
         <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="E39" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="F39" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="G39" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="H39" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K39" s="90" t="s">
         <v>164</v>
@@ -11171,19 +11171,19 @@
         <v>7</v>
       </c>
       <c r="D40" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="E40" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="F40" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="G40" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="H40" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K40" s="90" t="s">
         <v>164</v>
@@ -11198,22 +11198,22 @@
       </c>
       <c r="B41" s="85"/>
       <c r="C41" s="85" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="D41" s="85" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="E41" s="85" t="s">
+        <v>639</v>
+      </c>
+      <c r="F41" s="85" t="s">
         <v>641</v>
       </c>
-      <c r="F41" s="85" t="s">
-        <v>643</v>
-      </c>
       <c r="G41" s="85" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="H41" s="85" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="I41" s="85"/>
       <c r="J41" s="85"/>
@@ -11232,16 +11232,16 @@
         <v>8</v>
       </c>
       <c r="D42" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="E42" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="H42" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K42" s="90" t="s">
         <v>164</v>
@@ -11258,16 +11258,16 @@
         <v>8</v>
       </c>
       <c r="D43" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="E43" t="s">
+        <v>646</v>
+      </c>
+      <c r="F43" s="5" t="s">
         <v>648</v>
       </c>
-      <c r="F43" s="5" t="s">
-        <v>650</v>
-      </c>
       <c r="H43" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K43" s="90" t="s">
         <v>164</v>
@@ -11284,16 +11284,16 @@
         <v>8</v>
       </c>
       <c r="D44" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="E44" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="H44" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="K44" s="90" t="s">
         <v>164</v>
@@ -11596,10 +11596,10 @@
         <v>13</v>
       </c>
       <c r="N1" s="69" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="O1" s="69" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="P1" s="20" t="s">
         <v>14</v>
@@ -12090,11 +12090,11 @@
         <v>38</v>
       </c>
       <c r="B18" s="72" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C18" s="72"/>
       <c r="D18" s="72" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E18" s="74" t="s">
         <v>15</v>
@@ -12208,7 +12208,7 @@
       </c>
       <c r="C22" s="72"/>
       <c r="D22" s="72" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E22" s="74" t="s">
         <v>15</v>
@@ -12300,11 +12300,11 @@
         <v>46</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>16</v>
@@ -12388,11 +12388,11 @@
         <v>46</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>15</v>
@@ -12540,7 +12540,7 @@
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>15</v>
@@ -12752,7 +12752,7 @@
       </c>
       <c r="C40" s="72"/>
       <c r="D40" s="72" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E40" s="72" t="s">
         <v>15</v>
@@ -12930,7 +12930,7 @@
       </c>
       <c r="C46" s="72"/>
       <c r="D46" s="72" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E46" s="72" t="s">
         <v>50</v>
@@ -12958,7 +12958,7 @@
       </c>
       <c r="C47" s="72"/>
       <c r="D47" s="72" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E47" s="72" t="s">
         <v>15</v>
@@ -12988,7 +12988,7 @@
       </c>
       <c r="C48" s="72"/>
       <c r="D48" s="72" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E48" s="72" t="s">
         <v>17</v>
@@ -13086,7 +13086,7 @@
       </c>
       <c r="C51" s="40"/>
       <c r="D51" s="41" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E51" s="40" t="s">
         <v>15</v>
@@ -13117,7 +13117,7 @@
       </c>
       <c r="C52" s="40"/>
       <c r="D52" s="41" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E52" s="40" t="s">
         <v>15</v>
@@ -13173,11 +13173,11 @@
         <v>179</v>
       </c>
       <c r="B54" s="40" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="C54" s="40"/>
       <c r="D54" s="41" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="E54" s="40" t="s">
         <v>15</v>
@@ -13204,11 +13204,11 @@
         <v>179</v>
       </c>
       <c r="B55" s="40" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="C55" s="40"/>
       <c r="D55" s="41" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E55" s="40" t="s">
         <v>15</v>
@@ -13352,14 +13352,14 @@
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" s="62" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B60" s="62" t="s">
         <v>18</v>
       </c>
       <c r="C60" s="62"/>
       <c r="D60" s="66" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="E60" s="62" t="s">
         <v>16</v>
@@ -13388,14 +13388,14 @@
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" s="62" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B61" s="62" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C61" s="62"/>
       <c r="D61" s="66" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E61" s="62" t="s">
         <v>15</v>
@@ -13424,14 +13424,14 @@
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" s="62" t="s">
+        <v>321</v>
+      </c>
+      <c r="B62" s="62" t="s">
         <v>323</v>
-      </c>
-      <c r="B62" s="62" t="s">
-        <v>325</v>
       </c>
       <c r="C62" s="62"/>
       <c r="D62" s="66" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E62" s="62" t="s">
         <v>15</v>
@@ -13454,14 +13454,14 @@
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" s="62" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B63" s="62" t="s">
         <v>19</v>
       </c>
       <c r="C63" s="62"/>
       <c r="D63" s="66" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E63" s="66" t="s">
         <v>50</v>
@@ -13482,14 +13482,14 @@
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" s="62" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B64" s="62" t="s">
         <v>45</v>
       </c>
       <c r="C64" s="62"/>
       <c r="D64" s="66" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E64" s="66" t="s">
         <v>15</v>
@@ -13528,11 +13528,11 @@
   </sheetPr>
   <dimension ref="A1:N71"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H38" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="7" ySplit="1" topLeftCell="H22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E62" sqref="E62"/>
+      <selection pane="bottomRight" activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14257,7 +14257,7 @@
         <v>53</v>
       </c>
       <c r="E19" s="64" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F19" s="62">
         <v>1</v>
@@ -14291,7 +14291,7 @@
         <v>53</v>
       </c>
       <c r="E20" s="64" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F20" s="62">
         <v>1</v>
@@ -14325,7 +14325,7 @@
         <v>53</v>
       </c>
       <c r="E21" s="64" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="F21" s="62">
         <v>1</v>
@@ -14359,7 +14359,7 @@
         <v>53</v>
       </c>
       <c r="E22" s="64" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F22" s="62">
         <v>1</v>
@@ -14393,7 +14393,7 @@
         <v>53</v>
       </c>
       <c r="E23" s="64" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="F23" s="62">
         <v>1</v>
@@ -14427,7 +14427,7 @@
         <v>53</v>
       </c>
       <c r="E24" s="64" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F24" s="62">
         <v>1</v>
@@ -14461,7 +14461,7 @@
         <v>53</v>
       </c>
       <c r="E25" s="64" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F25" s="62">
         <v>1</v>
@@ -14495,7 +14495,7 @@
         <v>53</v>
       </c>
       <c r="E26" s="64" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F26" s="62">
         <v>1</v>
@@ -14529,7 +14529,7 @@
         <v>53</v>
       </c>
       <c r="E27" s="64" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="F27" s="62">
         <v>1</v>
@@ -14563,7 +14563,7 @@
         <v>53</v>
       </c>
       <c r="E28" s="64" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="F28" s="62">
         <v>1</v>
@@ -14597,7 +14597,7 @@
         <v>53</v>
       </c>
       <c r="E29" s="64" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="F29" s="62">
         <v>1</v>
@@ -14631,7 +14631,7 @@
         <v>53</v>
       </c>
       <c r="E30" s="64" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="F30" s="62">
         <v>1</v>
@@ -14665,7 +14665,7 @@
         <v>53</v>
       </c>
       <c r="E31" s="64" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="F31" s="62">
         <v>1</v>
@@ -14932,7 +14932,7 @@
         <v>167</v>
       </c>
       <c r="E39" s="46" t="s">
-        <v>297</v>
+        <v>682</v>
       </c>
       <c r="F39" s="33">
         <v>1</v>
@@ -14965,7 +14965,7 @@
         <v>167</v>
       </c>
       <c r="E40" s="46" t="s">
-        <v>299</v>
+        <v>683</v>
       </c>
       <c r="F40" s="33">
         <v>1</v>
@@ -14978,7 +14978,7 @@
       </c>
       <c r="I40" s="35"/>
       <c r="J40" s="33" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="K40" s="33"/>
       <c r="L40" s="35">
@@ -15000,7 +15000,7 @@
         <v>167</v>
       </c>
       <c r="E41" s="46" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F41" s="33">
         <v>1</v>
@@ -15033,7 +15033,7 @@
         <v>167</v>
       </c>
       <c r="E42" s="46" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F42" s="33">
         <v>1</v>
@@ -15066,7 +15066,7 @@
         <v>167</v>
       </c>
       <c r="E43" s="46" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F43" s="33">
         <v>1</v>
@@ -15099,7 +15099,7 @@
         <v>167</v>
       </c>
       <c r="E44" s="46" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F44" s="33">
         <v>1</v>
@@ -15132,7 +15132,7 @@
         <v>167</v>
       </c>
       <c r="E45" s="46" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F45" s="33">
         <v>1</v>
@@ -15165,7 +15165,7 @@
         <v>167</v>
       </c>
       <c r="E46" s="46" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F46" s="33">
         <v>1</v>
@@ -15198,7 +15198,7 @@
         <v>167</v>
       </c>
       <c r="E47" s="46" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F47" s="33">
         <v>1</v>
@@ -15231,7 +15231,7 @@
         <v>167</v>
       </c>
       <c r="E48" s="46" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F48" s="33">
         <v>1</v>
@@ -15264,7 +15264,7 @@
         <v>167</v>
       </c>
       <c r="E49" s="46" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F49" s="33">
         <v>1</v>
@@ -15297,7 +15297,7 @@
         <v>167</v>
       </c>
       <c r="E50" s="100" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="F50" s="99">
         <v>1</v>
@@ -15330,7 +15330,7 @@
         <v>167</v>
       </c>
       <c r="E51" s="100" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="F51" s="99">
         <v>1</v>
@@ -15363,7 +15363,7 @@
         <v>167</v>
       </c>
       <c r="E52" s="94" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="F52" s="93">
         <v>1</v>
@@ -15396,7 +15396,7 @@
         <v>167</v>
       </c>
       <c r="E53" s="94" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="F53" s="93">
         <v>1</v>
@@ -15429,7 +15429,7 @@
         <v>167</v>
       </c>
       <c r="E54" s="94" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="F54" s="93">
         <v>1</v>
@@ -15462,7 +15462,7 @@
         <v>167</v>
       </c>
       <c r="E55" s="94" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="F55" s="93">
         <v>1</v>
@@ -15495,7 +15495,7 @@
         <v>167</v>
       </c>
       <c r="E56" s="94" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="F56" s="93">
         <v>1</v>
@@ -15528,7 +15528,7 @@
         <v>167</v>
       </c>
       <c r="E57" s="94" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="F57" s="93">
         <v>1</v>
@@ -15561,7 +15561,7 @@
         <v>167</v>
       </c>
       <c r="E58" s="94" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="F58" s="93">
         <v>1</v>
@@ -15594,7 +15594,7 @@
         <v>167</v>
       </c>
       <c r="E59" s="94" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="F59" s="93">
         <v>1</v>
@@ -15627,7 +15627,7 @@
         <v>167</v>
       </c>
       <c r="E60" s="94" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="F60" s="93">
         <v>1</v>
@@ -15660,7 +15660,7 @@
         <v>167</v>
       </c>
       <c r="E61" s="94" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="F61" s="93">
         <v>1</v>
@@ -15693,7 +15693,7 @@
         <v>167</v>
       </c>
       <c r="E62" s="94" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="F62" s="93">
         <v>1</v>
@@ -16032,7 +16032,7 @@
         <v>39</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>25</v>
@@ -16049,16 +16049,16 @@
         <v>99</v>
       </c>
       <c r="B2" s="89" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C2" s="89" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D2" s="88" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="E2" s="88" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F2" s="88">
         <v>1</v>
@@ -16069,16 +16069,16 @@
         <v>21</v>
       </c>
       <c r="B3" s="87" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C3" s="87" t="s">
+        <v>421</v>
+      </c>
+      <c r="D3" s="86" t="s">
+        <v>422</v>
+      </c>
+      <c r="E3" s="86" t="s">
         <v>423</v>
-      </c>
-      <c r="D3" s="86" t="s">
-        <v>424</v>
-      </c>
-      <c r="E3" s="86" t="s">
-        <v>425</v>
       </c>
       <c r="F3" s="86">
         <v>1</v>

</xml_diff>

<commit_message>
api add filter helper method
</commit_message>
<xml_diff>
--- a/db/excel/api-function-granted-users-cdld.xlsx
+++ b/db/excel/api-function-granted-users-cdld.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10711"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8261661-E7A8-A84B-9875-68B57C8B0813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C90CB5-8CB9-E141-BD31-0A6EB25ED51D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19480" tabRatio="800" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" tabRatio="800" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_types" sheetId="27" r:id="rId1"/>
@@ -300,7 +300,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1748" uniqueCount="684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1750" uniqueCount="686">
   <si>
     <t>status</t>
   </si>
@@ -2454,6 +2454,12 @@
   </si>
   <si>
     <t>/get-direct-exe-by-dos</t>
+  </si>
+  <si>
+    <t>/get-filter-meeting</t>
+  </si>
+  <si>
+    <t>/get-filter-direct-org</t>
   </si>
 </sst>
 </file>
@@ -6709,10 +6715,10 @@
   <dimension ref="A1:P99"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11529,10 +11535,10 @@
   <dimension ref="A1:Q64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D64" sqref="D64"/>
+      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13529,10 +13535,10 @@
   <dimension ref="A1:N71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="H32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E41" sqref="E41"/>
+      <selection pane="bottomRight" activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15725,7 +15731,9 @@
       <c r="D63" s="93" t="s">
         <v>167</v>
       </c>
-      <c r="E63" s="94"/>
+      <c r="E63" s="94" t="s">
+        <v>685</v>
+      </c>
       <c r="F63" s="93">
         <v>1</v>
       </c>
@@ -15756,7 +15764,9 @@
       <c r="D64" s="93" t="s">
         <v>167</v>
       </c>
-      <c r="E64" s="94"/>
+      <c r="E64" s="94" t="s">
+        <v>684</v>
+      </c>
       <c r="F64" s="93">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
commit code pre working day 16 07
</commit_message>
<xml_diff>
--- a/db/excel/api-function-granted-users-cdld.xlsx
+++ b/db/excel/api-function-granted-users-cdld.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10711"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C90CB5-8CB9-E141-BD31-0A6EB25ED51D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D65821D-E39C-F042-8408-1E715BE0349E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" tabRatio="800" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" tabRatio="800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_types" sheetId="27" r:id="rId1"/>
@@ -6107,7 +6107,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9989,8 +9989,8 @@
   </sheetPr>
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13534,11 +13534,11 @@
   </sheetPr>
   <dimension ref="A1:N71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="7" ySplit="1" topLeftCell="H32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E64" sqref="E64"/>
+      <selection pane="bottomRight" activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add hook to check user menus
</commit_message>
<xml_diff>
--- a/db/excel/api-function-granted-users-cdld.xlsx
+++ b/db/excel/api-function-granted-users-cdld.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10711"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3CD1E9B-DE00-1648-816F-248838AB890D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E6E841-D486-D04A-A947-40E4B44A386D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" tabRatio="800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" tabRatio="800" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_types" sheetId="27" r:id="rId1"/>
@@ -1583,9 +1583,6 @@
     <t>[1,11,12,13,14,15,16,2,21,22,23,24,3,31,4]</t>
   </si>
   <si>
-    <t>[2,21,22,23,24,3,31,4]</t>
-  </si>
-  <si>
     <t>Nhóm user người dùng toàn quyền</t>
   </si>
   <si>
@@ -2481,6 +2478,9 @@
   </si>
   <si>
     <t>Mảng chứa chỉ số Đơn vị đánh giá nhập</t>
+  </si>
+  <si>
+    <t>[2,21,22,23,24,25,26,3,31,4]</t>
   </si>
 </sst>
 </file>
@@ -5334,10 +5334,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <sheetPr>
+    <tabColor theme="3" tint="0.79998168889431442"/>
+  </sheetPr>
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5403,7 +5406,7 @@
         <v>0</v>
       </c>
       <c r="O1" s="77" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -5419,7 +5422,7 @@
         <v>399</v>
       </c>
       <c r="F2" s="84" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G2" s="84" t="s">
         <v>414</v>
@@ -5450,7 +5453,7 @@
         <v>334</v>
       </c>
       <c r="D3" s="83" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="E3" s="84" t="s">
         <v>334</v>
@@ -5665,7 +5668,7 @@
       </c>
       <c r="D9" s="79"/>
       <c r="E9" s="80" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="F9" s="80"/>
       <c r="G9" s="80" t="s">
@@ -5697,19 +5700,19 @@
         <v>347</v>
       </c>
       <c r="D10" s="83" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="E10" s="84" t="s">
         <v>347</v>
       </c>
       <c r="F10" s="84" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G10" s="84" t="s">
         <v>408</v>
       </c>
       <c r="H10" s="83" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="I10" s="83"/>
       <c r="J10" s="83"/>
@@ -5772,7 +5775,7 @@
       </c>
       <c r="D12" s="79"/>
       <c r="E12" s="80" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F12" s="80"/>
       <c r="G12" s="80" t="s">
@@ -5807,7 +5810,7 @@
       </c>
       <c r="D13" s="79"/>
       <c r="E13" s="80" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F13" s="80"/>
       <c r="G13" s="80" t="s">
@@ -5842,7 +5845,7 @@
       </c>
       <c r="D14" s="79"/>
       <c r="E14" s="80" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F14" s="80"/>
       <c r="G14" s="80" t="s">
@@ -5874,19 +5877,19 @@
         <v>396</v>
       </c>
       <c r="D15" s="83" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="E15" s="84" t="s">
         <v>396</v>
       </c>
       <c r="F15" s="84" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G15" s="84" t="s">
         <v>415</v>
       </c>
       <c r="H15" s="83" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="I15" s="83"/>
       <c r="J15" s="83"/>
@@ -6016,10 +6019,10 @@
         <v>109</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="F2" s="29"/>
       <c r="G2" s="29"/>
@@ -6043,10 +6046,10 @@
         <v>109</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="F3" s="29"/>
       <c r="G3" s="29"/>
@@ -6070,10 +6073,10 @@
         <v>109</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="F4" s="28"/>
       <c r="G4" s="28"/>
@@ -6097,10 +6100,10 @@
         <v>109</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="F5" s="28"/>
       <c r="G5" s="28"/>
@@ -6115,7 +6118,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="28" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B6" s="28">
         <v>5</v>
@@ -6124,10 +6127,10 @@
         <v>109</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="F6" s="28"/>
       <c r="G6" s="28"/>
@@ -6142,7 +6145,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="28" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B7" s="28">
         <v>3</v>
@@ -6151,10 +6154,10 @@
         <v>109</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
@@ -6215,10 +6218,10 @@
         <v>233</v>
       </c>
       <c r="D1" s="39" t="s">
+        <v>610</v>
+      </c>
+      <c r="E1" s="39" t="s">
         <v>611</v>
-      </c>
-      <c r="E1" s="39" t="s">
-        <v>612</v>
       </c>
       <c r="F1" s="39" t="s">
         <v>178</v>
@@ -6250,10 +6253,10 @@
         <v>316</v>
       </c>
       <c r="D2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E2" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="J2" t="s">
         <v>185</v>
@@ -6270,13 +6273,13 @@
         <v>186</v>
       </c>
       <c r="C3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="J3" t="s">
         <v>185</v>
@@ -6293,13 +6296,13 @@
         <v>188</v>
       </c>
       <c r="C4" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="E4" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="J4" t="s">
         <v>185</v>
@@ -6313,16 +6316,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="C5" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D5" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E5" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="J5" t="s">
         <v>185</v>
@@ -6336,16 +6339,16 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C6" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D6" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="E6" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="J6" t="s">
         <v>185</v>
@@ -6359,16 +6362,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C7" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D7" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="E7" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="J7" t="s">
         <v>185</v>
@@ -6382,16 +6385,16 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="C8" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D8" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="E8" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="J8" t="s">
         <v>185</v>
@@ -6405,16 +6408,16 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C9" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D9" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E9" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="J9" t="s">
         <v>185</v>
@@ -6431,13 +6434,13 @@
         <v>195</v>
       </c>
       <c r="C10" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D10" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E10" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="J10" t="s">
         <v>185</v>
@@ -6454,13 +6457,13 @@
         <v>193</v>
       </c>
       <c r="C11" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D11" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E11" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="J11" t="s">
         <v>185</v>
@@ -6477,13 +6480,13 @@
         <v>190</v>
       </c>
       <c r="C12" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D12" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E12" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="J12" t="s">
         <v>185</v>
@@ -6500,13 +6503,13 @@
         <v>189</v>
       </c>
       <c r="C13" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D13" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E13" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="J13" t="s">
         <v>185</v>
@@ -6523,13 +6526,13 @@
         <v>192</v>
       </c>
       <c r="C14" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D14" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E14" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="J14" t="s">
         <v>185</v>
@@ -6546,13 +6549,13 @@
         <v>191</v>
       </c>
       <c r="C15" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D15" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E15" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="J15" t="s">
         <v>185</v>
@@ -6569,13 +6572,13 @@
         <v>194</v>
       </c>
       <c r="C16" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D16" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E16" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="J16" t="s">
         <v>185</v>
@@ -6592,13 +6595,13 @@
         <v>196</v>
       </c>
       <c r="C17" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D17" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E17" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="J17" t="s">
         <v>185</v>
@@ -6680,7 +6683,7 @@
         <v>222</v>
       </c>
       <c r="C4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E4" t="s">
         <v>185</v>
@@ -6694,7 +6697,7 @@
         <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="E5" t="s">
         <v>185</v>
@@ -6722,7 +6725,7 @@
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E7" t="s">
         <v>185</v>
@@ -6736,7 +6739,7 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="E8" t="s">
         <v>185</v>
@@ -6764,7 +6767,7 @@
         <v>154</v>
       </c>
       <c r="C10" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E10" t="s">
         <v>185</v>
@@ -6778,7 +6781,7 @@
         <v>155</v>
       </c>
       <c r="C11" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E11" t="s">
         <v>185</v>
@@ -6793,8 +6796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="D27" sqref="D27"/>
@@ -6982,7 +6985,7 @@
         <v>251</v>
       </c>
       <c r="D5" s="103" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="E5" s="103" t="s">
         <v>16</v>
@@ -7294,13 +7297,13 @@
         <v>212</v>
       </c>
       <c r="B15" s="48" t="s">
+        <v>630</v>
+      </c>
+      <c r="C15" s="48" t="s">
         <v>631</v>
       </c>
-      <c r="C15" s="48" t="s">
+      <c r="D15" s="48" t="s">
         <v>632</v>
-      </c>
-      <c r="D15" s="48" t="s">
-        <v>633</v>
       </c>
       <c r="E15" s="48" t="s">
         <v>16</v>
@@ -7314,7 +7317,7 @@
       <c r="J15" s="55"/>
       <c r="K15" s="55"/>
       <c r="L15" s="56" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="M15" s="55"/>
       <c r="N15" s="55"/>
@@ -7331,10 +7334,10 @@
         <v>307</v>
       </c>
       <c r="C16" s="48" t="s">
+        <v>473</v>
+      </c>
+      <c r="D16" s="48" t="s">
         <v>474</v>
-      </c>
-      <c r="D16" s="48" t="s">
-        <v>475</v>
       </c>
       <c r="E16" s="48" t="s">
         <v>15</v>
@@ -7406,7 +7409,7 @@
         <v>243</v>
       </c>
       <c r="D18" s="105" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E18" s="105" t="s">
         <v>16</v>
@@ -7420,7 +7423,7 @@
       <c r="J18" s="55"/>
       <c r="K18" s="55"/>
       <c r="L18" s="56" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="M18" s="55"/>
       <c r="N18" s="55"/>
@@ -7434,13 +7437,13 @@
         <v>212</v>
       </c>
       <c r="B19" s="48" t="s">
+        <v>428</v>
+      </c>
+      <c r="C19" s="48" t="s">
+        <v>427</v>
+      </c>
+      <c r="D19" s="48" t="s">
         <v>429</v>
-      </c>
-      <c r="C19" s="48" t="s">
-        <v>428</v>
-      </c>
-      <c r="D19" s="48" t="s">
-        <v>430</v>
       </c>
       <c r="E19" s="48" t="s">
         <v>16</v>
@@ -7454,7 +7457,7 @@
       <c r="J19" s="55"/>
       <c r="K19" s="55"/>
       <c r="L19" s="56" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="M19" s="55"/>
       <c r="N19" s="55"/>
@@ -7564,13 +7567,13 @@
         <v>212</v>
       </c>
       <c r="B23" s="48" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C23" s="48" t="s">
+        <v>430</v>
+      </c>
+      <c r="D23" s="48" t="s">
         <v>431</v>
-      </c>
-      <c r="D23" s="48" t="s">
-        <v>432</v>
       </c>
       <c r="E23" s="48" t="s">
         <v>50</v>
@@ -7718,13 +7721,13 @@
         <v>212</v>
       </c>
       <c r="B28" s="116" t="s">
+        <v>683</v>
+      </c>
+      <c r="C28" s="116" t="s">
         <v>684</v>
       </c>
-      <c r="C28" s="116" t="s">
-        <v>685</v>
-      </c>
       <c r="D28" s="116" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="E28" s="116" t="s">
         <v>15</v>
@@ -7750,13 +7753,13 @@
         <v>212</v>
       </c>
       <c r="B29" s="48" t="s">
+        <v>432</v>
+      </c>
+      <c r="C29" s="48" t="s">
         <v>433</v>
       </c>
-      <c r="C29" s="48" t="s">
+      <c r="D29" s="48" t="s">
         <v>434</v>
-      </c>
-      <c r="D29" s="48" t="s">
-        <v>435</v>
       </c>
       <c r="E29" s="48" t="s">
         <v>15</v>
@@ -7782,13 +7785,13 @@
         <v>212</v>
       </c>
       <c r="B30" s="48" t="s">
+        <v>458</v>
+      </c>
+      <c r="C30" s="48" t="s">
         <v>459</v>
       </c>
-      <c r="C30" s="48" t="s">
+      <c r="D30" s="48" t="s">
         <v>460</v>
-      </c>
-      <c r="D30" s="48" t="s">
-        <v>461</v>
       </c>
       <c r="E30" s="48" t="s">
         <v>15</v>
@@ -7820,7 +7823,7 @@
         <v>227</v>
       </c>
       <c r="D31" s="48" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="E31" s="48" t="s">
         <v>17</v>
@@ -7843,7 +7846,7 @@
     </row>
     <row r="32" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="91" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B32" s="91" t="s">
         <v>18</v>
@@ -7852,7 +7855,7 @@
         <v>234</v>
       </c>
       <c r="D32" s="91" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E32" s="91" t="s">
         <v>97</v>
@@ -7881,16 +7884,16 @@
     </row>
     <row r="33" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="91" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B33" s="91" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C33" s="91" t="s">
+        <v>634</v>
+      </c>
+      <c r="D33" s="91" t="s">
         <v>635</v>
-      </c>
-      <c r="D33" s="91" t="s">
-        <v>636</v>
       </c>
       <c r="E33" s="91" t="s">
         <v>16</v>
@@ -7911,16 +7914,16 @@
     </row>
     <row r="34" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="91" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B34" s="91" t="s">
         <v>213</v>
       </c>
       <c r="C34" s="91" t="s">
+        <v>492</v>
+      </c>
+      <c r="D34" s="91" t="s">
         <v>493</v>
-      </c>
-      <c r="D34" s="91" t="s">
-        <v>494</v>
       </c>
       <c r="E34" s="91" t="s">
         <v>16</v>
@@ -7941,16 +7944,16 @@
     </row>
     <row r="35" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="91" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B35" s="91" t="s">
+        <v>531</v>
+      </c>
+      <c r="C35" s="91" t="s">
         <v>532</v>
       </c>
-      <c r="C35" s="91" t="s">
+      <c r="D35" s="91" t="s">
         <v>533</v>
-      </c>
-      <c r="D35" s="91" t="s">
-        <v>534</v>
       </c>
       <c r="E35" s="91" t="s">
         <v>15</v>
@@ -7964,7 +7967,7 @@
       <c r="J35" s="92"/>
       <c r="K35" s="92"/>
       <c r="L35" s="56" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="M35" s="92"/>
       <c r="N35" s="92"/>
@@ -7975,7 +7978,7 @@
     </row>
     <row r="36" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="91" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B36" s="91" t="s">
         <v>218</v>
@@ -7984,7 +7987,7 @@
         <v>261</v>
       </c>
       <c r="D36" s="91" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="E36" s="91" t="s">
         <v>15</v>
@@ -8007,7 +8010,7 @@
     </row>
     <row r="37" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="91" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B37" s="91" t="s">
         <v>219</v>
@@ -8016,7 +8019,7 @@
         <v>262</v>
       </c>
       <c r="D37" s="91" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="E37" s="91" t="s">
         <v>15</v>
@@ -8039,16 +8042,16 @@
     </row>
     <row r="38" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="91" t="s">
+        <v>482</v>
+      </c>
+      <c r="B38" s="91" t="s">
         <v>483</v>
       </c>
-      <c r="B38" s="91" t="s">
+      <c r="C38" s="91" t="s">
         <v>484</v>
       </c>
-      <c r="C38" s="91" t="s">
+      <c r="D38" s="91" t="s">
         <v>485</v>
-      </c>
-      <c r="D38" s="91" t="s">
-        <v>486</v>
       </c>
       <c r="E38" s="91" t="s">
         <v>15</v>
@@ -8071,16 +8074,16 @@
     </row>
     <row r="39" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="91" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B39" s="91" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C39" s="91" t="s">
+        <v>486</v>
+      </c>
+      <c r="D39" s="91" t="s">
         <v>487</v>
-      </c>
-      <c r="D39" s="91" t="s">
-        <v>488</v>
       </c>
       <c r="E39" s="91" t="s">
         <v>97</v>
@@ -8101,7 +8104,7 @@
     </row>
     <row r="40" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="91" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B40" s="91" t="s">
         <v>197</v>
@@ -8131,7 +8134,7 @@
     </row>
     <row r="41" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="91" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B41" s="91" t="s">
         <v>222</v>
@@ -8163,7 +8166,7 @@
     </row>
     <row r="42" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="91" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B42" s="91" t="s">
         <v>19</v>
@@ -8193,7 +8196,7 @@
     </row>
     <row r="43" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="91" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B43" s="91" t="s">
         <v>45</v>
@@ -8225,7 +8228,7 @@
     </row>
     <row r="44" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="91" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B44" s="91" t="s">
         <v>0</v>
@@ -8234,7 +8237,7 @@
         <v>227</v>
       </c>
       <c r="D44" s="91" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E44" s="91" t="s">
         <v>17</v>
@@ -8297,10 +8300,10 @@
         <v>307</v>
       </c>
       <c r="C46" s="47" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D46" s="47" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="E46" s="47" t="s">
         <v>15</v>
@@ -8332,13 +8335,13 @@
         <v>267</v>
       </c>
       <c r="B47" s="47" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C47" s="47" t="s">
+        <v>634</v>
+      </c>
+      <c r="D47" s="47" t="s">
         <v>635</v>
-      </c>
-      <c r="D47" s="47" t="s">
-        <v>636</v>
       </c>
       <c r="E47" s="47" t="s">
         <v>16</v>
@@ -8352,7 +8355,7 @@
       <c r="J47" s="52"/>
       <c r="K47" s="52"/>
       <c r="L47" s="56" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="M47" s="52"/>
       <c r="N47" s="52"/>
@@ -8386,7 +8389,7 @@
       <c r="J48" s="52"/>
       <c r="K48" s="52"/>
       <c r="L48" s="56" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="M48" s="52"/>
       <c r="N48" s="52"/>
@@ -8400,13 +8403,13 @@
         <v>267</v>
       </c>
       <c r="B49" s="47" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C49" s="47" t="s">
+        <v>534</v>
+      </c>
+      <c r="D49" s="47" t="s">
         <v>535</v>
-      </c>
-      <c r="D49" s="47" t="s">
-        <v>536</v>
       </c>
       <c r="E49" s="47" t="s">
         <v>15</v>
@@ -8422,7 +8425,7 @@
       <c r="J49" s="52"/>
       <c r="K49" s="52"/>
       <c r="L49" s="56" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="M49" s="52"/>
       <c r="N49" s="52"/>
@@ -8456,7 +8459,7 @@
       <c r="J50" s="52"/>
       <c r="K50" s="52"/>
       <c r="L50" s="56" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="M50" s="52"/>
       <c r="N50" s="52"/>
@@ -8476,7 +8479,7 @@
         <v>273</v>
       </c>
       <c r="D51" s="47" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E51" s="47" t="s">
         <v>16</v>
@@ -8508,7 +8511,7 @@
         <v>242</v>
       </c>
       <c r="D52" s="47" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="E52" s="47" t="s">
         <v>15</v>
@@ -8566,13 +8569,13 @@
         <v>267</v>
       </c>
       <c r="B54" s="103" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C54" s="103" t="s">
         <v>265</v>
       </c>
       <c r="D54" s="103" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="E54" s="103" t="s">
         <v>16</v>
@@ -8584,7 +8587,7 @@
       <c r="J54" s="104"/>
       <c r="K54" s="104"/>
       <c r="L54" s="56" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="M54" s="104"/>
       <c r="N54" s="104"/>
@@ -8598,13 +8601,13 @@
         <v>267</v>
       </c>
       <c r="B55" s="47" t="s">
+        <v>432</v>
+      </c>
+      <c r="C55" s="47" t="s">
         <v>433</v>
       </c>
-      <c r="C55" s="47" t="s">
+      <c r="D55" s="47" t="s">
         <v>434</v>
-      </c>
-      <c r="D55" s="47" t="s">
-        <v>435</v>
       </c>
       <c r="E55" s="47" t="s">
         <v>15</v>
@@ -8630,13 +8633,13 @@
         <v>267</v>
       </c>
       <c r="B56" s="47" t="s">
+        <v>455</v>
+      </c>
+      <c r="C56" s="47" t="s">
         <v>456</v>
       </c>
-      <c r="C56" s="47" t="s">
+      <c r="D56" s="47" t="s">
         <v>457</v>
-      </c>
-      <c r="D56" s="47" t="s">
-        <v>458</v>
       </c>
       <c r="E56" s="47" t="s">
         <v>15</v>
@@ -8662,13 +8665,13 @@
         <v>267</v>
       </c>
       <c r="B57" s="47" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C57" s="47" t="s">
+        <v>430</v>
+      </c>
+      <c r="D57" s="47" t="s">
         <v>431</v>
-      </c>
-      <c r="D57" s="47" t="s">
-        <v>432</v>
       </c>
       <c r="E57" s="47" t="s">
         <v>50</v>
@@ -8695,10 +8698,10 @@
         <v>220</v>
       </c>
       <c r="C58" s="113" t="s">
+        <v>588</v>
+      </c>
+      <c r="D58" s="113" t="s">
         <v>589</v>
-      </c>
-      <c r="D58" s="113" t="s">
-        <v>590</v>
       </c>
       <c r="E58" s="113" t="s">
         <v>15</v>
@@ -8854,7 +8857,7 @@
         <v>227</v>
       </c>
       <c r="D63" s="47" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E63" s="47" t="s">
         <v>17</v>
@@ -8917,10 +8920,10 @@
         <v>307</v>
       </c>
       <c r="C65" s="49" t="s">
+        <v>591</v>
+      </c>
+      <c r="D65" s="49" t="s">
         <v>592</v>
-      </c>
-      <c r="D65" s="49" t="s">
-        <v>593</v>
       </c>
       <c r="E65" s="49" t="s">
         <v>15</v>
@@ -8952,13 +8955,13 @@
         <v>266</v>
       </c>
       <c r="B66" s="49" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C66" s="49" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D66" s="49" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E66" s="49" t="s">
         <v>15</v>
@@ -8974,7 +8977,7 @@
       <c r="J66" s="44"/>
       <c r="K66" s="44"/>
       <c r="L66" s="56" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="M66" s="44"/>
       <c r="N66" s="44"/>
@@ -8988,10 +8991,10 @@
         <v>266</v>
       </c>
       <c r="B67" s="49" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C67" s="49" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D67" s="49" t="s">
         <v>277</v>
@@ -9010,7 +9013,7 @@
       <c r="J67" s="44"/>
       <c r="K67" s="44"/>
       <c r="L67" s="56" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="M67" s="44"/>
       <c r="N67" s="44"/>
@@ -9044,7 +9047,7 @@
       <c r="J68" s="44"/>
       <c r="K68" s="44"/>
       <c r="L68" s="56" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="M68" s="44"/>
       <c r="N68" s="44"/>
@@ -9128,7 +9131,7 @@
         <v>282</v>
       </c>
       <c r="D71" s="108" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="E71" s="107" t="s">
         <v>16</v>
@@ -9142,7 +9145,7 @@
       <c r="J71" s="44"/>
       <c r="K71" s="44"/>
       <c r="L71" s="56" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="M71" s="44"/>
       <c r="N71" s="44"/>
@@ -9253,10 +9256,10 @@
         <v>0</v>
       </c>
       <c r="C75" s="49" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D75" s="49" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E75" s="49" t="s">
         <v>17</v>
@@ -9321,10 +9324,10 @@
         <v>307</v>
       </c>
       <c r="C77" s="50" t="s">
+        <v>473</v>
+      </c>
+      <c r="D77" s="50" t="s">
         <v>474</v>
-      </c>
-      <c r="D77" s="50" t="s">
-        <v>475</v>
       </c>
       <c r="E77" s="50" t="s">
         <v>15</v>
@@ -9362,7 +9365,7 @@
         <v>237</v>
       </c>
       <c r="D78" s="110" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E78" s="110" t="s">
         <v>16</v>
@@ -9374,7 +9377,7 @@
       <c r="J78" s="57"/>
       <c r="K78" s="57"/>
       <c r="L78" s="56" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="M78" s="57"/>
       <c r="N78" s="57"/>
@@ -9740,13 +9743,13 @@
         <v>168</v>
       </c>
       <c r="B90" s="42" t="s">
+        <v>512</v>
+      </c>
+      <c r="C90" s="42" t="s">
         <v>513</v>
       </c>
-      <c r="C90" s="42" t="s">
+      <c r="D90" s="58" t="s">
         <v>514</v>
-      </c>
-      <c r="D90" s="58" t="s">
-        <v>515</v>
       </c>
       <c r="E90" s="58" t="s">
         <v>15</v>
@@ -9870,13 +9873,13 @@
         <v>168</v>
       </c>
       <c r="B94" s="42" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C94" s="42" t="s">
+        <v>615</v>
+      </c>
+      <c r="D94" s="58" t="s">
         <v>616</v>
-      </c>
-      <c r="D94" s="58" t="s">
-        <v>617</v>
       </c>
       <c r="E94" s="58" t="s">
         <v>15</v>
@@ -9902,13 +9905,13 @@
         <v>168</v>
       </c>
       <c r="B95" s="42" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C95" s="42" t="s">
+        <v>617</v>
+      </c>
+      <c r="D95" s="58" t="s">
         <v>618</v>
-      </c>
-      <c r="D95" s="58" t="s">
-        <v>619</v>
       </c>
       <c r="E95" s="58" t="s">
         <v>15</v>
@@ -10125,7 +10128,7 @@
         <v>138</v>
       </c>
       <c r="C1" s="38" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D1" s="38" t="s">
         <v>233</v>
@@ -10137,10 +10140,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="38" t="s">
+        <v>610</v>
+      </c>
+      <c r="H1" s="38" t="s">
         <v>611</v>
-      </c>
-      <c r="H1" s="38" t="s">
-        <v>612</v>
       </c>
       <c r="I1" s="38" t="s">
         <v>197</v>
@@ -10173,10 +10176,10 @@
         <v>358</v>
       </c>
       <c r="G2" s="85" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="H2" s="85" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="I2" s="85"/>
       <c r="J2" s="85"/>
@@ -10204,10 +10207,10 @@
         <v>360</v>
       </c>
       <c r="G3" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="H3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K3" t="s">
         <v>164</v>
@@ -10233,10 +10236,10 @@
         <v>361</v>
       </c>
       <c r="G4" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="H4" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K4" t="s">
         <v>164</v>
@@ -10262,10 +10265,10 @@
         <v>365</v>
       </c>
       <c r="G5" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="H5" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K5" t="s">
         <v>164</v>
@@ -10282,19 +10285,19 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
+        <v>467</v>
+      </c>
+      <c r="E6" t="s">
+        <v>450</v>
+      </c>
+      <c r="F6" t="s">
         <v>468</v>
       </c>
-      <c r="E6" t="s">
-        <v>451</v>
-      </c>
-      <c r="F6" t="s">
-        <v>469</v>
-      </c>
       <c r="G6" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="H6" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K6" t="s">
         <v>164</v>
@@ -10311,7 +10314,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E7" t="s">
         <v>359</v>
@@ -10320,10 +10323,10 @@
         <v>362</v>
       </c>
       <c r="G7" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="H7" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K7" t="s">
         <v>164</v>
@@ -10338,7 +10341,7 @@
       </c>
       <c r="B8" s="85"/>
       <c r="C8" s="85" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="D8" s="85" t="s">
         <v>366</v>
@@ -10350,10 +10353,10 @@
         <v>374</v>
       </c>
       <c r="G8" s="85" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H8" s="85" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="I8" s="85"/>
       <c r="J8" s="85"/>
@@ -10381,10 +10384,10 @@
         <v>372</v>
       </c>
       <c r="G9" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="H9" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K9" t="s">
         <v>164</v>
@@ -10410,10 +10413,10 @@
         <v>373</v>
       </c>
       <c r="G10" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="H10" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K10" t="s">
         <v>164</v>
@@ -10428,10 +10431,10 @@
       </c>
       <c r="B11" s="85"/>
       <c r="C11" s="85" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D11" s="85" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E11" s="85" t="s">
         <v>377</v>
@@ -10440,10 +10443,10 @@
         <v>378</v>
       </c>
       <c r="G11" s="85" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="H11" s="85" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="I11" s="85"/>
       <c r="J11" s="85"/>
@@ -10462,19 +10465,19 @@
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="E12" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="F12" t="s">
         <v>379</v>
       </c>
       <c r="G12" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="H12" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K12" t="s">
         <v>164</v>
@@ -10491,19 +10494,19 @@
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="E13" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="F13" t="s">
         <v>380</v>
       </c>
       <c r="G13" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="H13" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K13" t="s">
         <v>164</v>
@@ -10520,19 +10523,19 @@
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E14" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="F14" t="s">
         <v>381</v>
       </c>
       <c r="G14" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="H14" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K14" t="s">
         <v>164</v>
@@ -10549,19 +10552,19 @@
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E15" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="F15" t="s">
         <v>382</v>
       </c>
       <c r="G15" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H15" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K15" t="s">
         <v>164</v>
@@ -10578,19 +10581,19 @@
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E16" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F16" t="s">
         <v>383</v>
       </c>
       <c r="G16" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="H16" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K16" t="s">
         <v>164</v>
@@ -10607,19 +10610,19 @@
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E17" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="F17" t="s">
         <v>384</v>
       </c>
       <c r="G17" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="H17" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K17" t="s">
         <v>164</v>
@@ -10634,10 +10637,10 @@
       </c>
       <c r="B18" s="85"/>
       <c r="C18" s="85" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D18" s="85" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E18" s="85" t="s">
         <v>385</v>
@@ -10646,10 +10649,10 @@
         <v>386</v>
       </c>
       <c r="G18" s="85" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H18" s="85" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="I18" s="85"/>
       <c r="J18" s="85"/>
@@ -10668,7 +10671,7 @@
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E19" t="s">
         <v>387</v>
@@ -10677,10 +10680,10 @@
         <v>387</v>
       </c>
       <c r="G19" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="H19" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K19" t="s">
         <v>164</v>
@@ -10697,7 +10700,7 @@
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E20" t="s">
         <v>388</v>
@@ -10706,10 +10709,10 @@
         <v>388</v>
       </c>
       <c r="G20" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="H20" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K20" t="s">
         <v>164</v>
@@ -10726,7 +10729,7 @@
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E21" t="s">
         <v>389</v>
@@ -10735,10 +10738,10 @@
         <v>389</v>
       </c>
       <c r="G21" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="H21" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K21" t="s">
         <v>164</v>
@@ -10755,7 +10758,7 @@
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="E22" t="s">
         <v>390</v>
@@ -10764,10 +10767,10 @@
         <v>390</v>
       </c>
       <c r="G22" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="H22" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K22" t="s">
         <v>164</v>
@@ -10782,22 +10785,22 @@
       </c>
       <c r="B23" s="85"/>
       <c r="C23" s="85" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D23" s="85" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="E23" s="85" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="F23" s="85" t="s">
         <v>386</v>
       </c>
       <c r="G23" s="85" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="H23" s="85" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="I23" s="85"/>
       <c r="J23" s="85"/>
@@ -10816,19 +10819,19 @@
         <v>5</v>
       </c>
       <c r="D24" t="s">
+        <v>479</v>
+      </c>
+      <c r="E24" t="s">
         <v>480</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>481</v>
       </c>
-      <c r="F24" t="s">
-        <v>482</v>
-      </c>
       <c r="G24" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="H24" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K24" t="s">
         <v>164</v>
@@ -10845,19 +10848,19 @@
         <v>5</v>
       </c>
       <c r="D25" t="s">
+        <v>437</v>
+      </c>
+      <c r="E25" t="s">
+        <v>439</v>
+      </c>
+      <c r="F25" t="s">
         <v>438</v>
       </c>
-      <c r="E25" t="s">
-        <v>440</v>
-      </c>
-      <c r="F25" t="s">
-        <v>439</v>
-      </c>
       <c r="G25" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H25" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K25" t="s">
         <v>164</v>
@@ -10874,19 +10877,19 @@
         <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E26" t="s">
+        <v>450</v>
+      </c>
+      <c r="F26" t="s">
         <v>451</v>
       </c>
-      <c r="F26" t="s">
-        <v>452</v>
-      </c>
       <c r="G26" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="H26" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K26" s="90" t="s">
         <v>164</v>
@@ -10903,19 +10906,19 @@
         <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E27" t="s">
         <v>364</v>
       </c>
       <c r="F27" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="G27" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="H27" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K27" s="90" t="s">
         <v>164</v>
@@ -10932,19 +10935,19 @@
         <v>5</v>
       </c>
       <c r="D28" t="s">
+        <v>461</v>
+      </c>
+      <c r="E28" t="s">
         <v>462</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>463</v>
       </c>
-      <c r="F28" t="s">
-        <v>464</v>
-      </c>
       <c r="G28" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="H28" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K28" s="90" t="s">
         <v>164</v>
@@ -10961,19 +10964,19 @@
         <v>5</v>
       </c>
       <c r="D29" t="s">
+        <v>440</v>
+      </c>
+      <c r="E29" t="s">
         <v>441</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>442</v>
       </c>
-      <c r="F29" t="s">
-        <v>443</v>
-      </c>
       <c r="G29" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H29" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K29" t="s">
         <v>164</v>
@@ -10988,22 +10991,22 @@
       </c>
       <c r="B30" s="85"/>
       <c r="C30" s="85" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D30" s="85" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="E30" s="85" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="F30" s="85" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="G30" s="85" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="H30" s="85" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="I30" s="85"/>
       <c r="J30" s="85"/>
@@ -11022,19 +11025,19 @@
         <v>6</v>
       </c>
       <c r="D31" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="E31" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="F31" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G31" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="H31" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K31" t="s">
         <v>164</v>
@@ -11051,19 +11054,19 @@
         <v>6</v>
       </c>
       <c r="D32" t="s">
+        <v>443</v>
+      </c>
+      <c r="E32" t="s">
         <v>444</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>445</v>
       </c>
-      <c r="F32" t="s">
-        <v>446</v>
-      </c>
       <c r="G32" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="H32" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K32" t="s">
         <v>164</v>
@@ -11080,19 +11083,19 @@
         <v>6</v>
       </c>
       <c r="D33" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E33" t="s">
+        <v>471</v>
+      </c>
+      <c r="F33" t="s">
         <v>472</v>
       </c>
-      <c r="F33" t="s">
-        <v>473</v>
-      </c>
       <c r="G33" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="H33" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K33" s="90" t="s">
         <v>164</v>
@@ -11109,19 +11112,19 @@
         <v>6</v>
       </c>
       <c r="D34" t="s">
+        <v>469</v>
+      </c>
+      <c r="E34" t="s">
+        <v>655</v>
+      </c>
+      <c r="F34" t="s">
         <v>470</v>
       </c>
-      <c r="E34" t="s">
-        <v>656</v>
-      </c>
-      <c r="F34" t="s">
-        <v>471</v>
-      </c>
       <c r="G34" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="H34" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K34" s="90" t="s">
         <v>164</v>
@@ -11138,19 +11141,19 @@
         <v>6</v>
       </c>
       <c r="D35" t="s">
+        <v>464</v>
+      </c>
+      <c r="E35" t="s">
         <v>465</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>466</v>
       </c>
-      <c r="F35" t="s">
-        <v>467</v>
-      </c>
       <c r="G35" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="H35" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K35" s="90" t="s">
         <v>164</v>
@@ -11165,22 +11168,22 @@
       </c>
       <c r="B36" s="85"/>
       <c r="C36" s="85" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D36" s="85" t="s">
+        <v>569</v>
+      </c>
+      <c r="E36" s="85" t="s">
         <v>570</v>
       </c>
-      <c r="E36" s="85" t="s">
+      <c r="F36" s="85" t="s">
         <v>571</v>
       </c>
-      <c r="F36" s="85" t="s">
-        <v>572</v>
-      </c>
       <c r="G36" s="85" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="H36" s="85" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="I36" s="85"/>
       <c r="J36" s="85"/>
@@ -11199,19 +11202,19 @@
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E37" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="F37" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="G37" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="H37" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K37" s="90" t="s">
         <v>164</v>
@@ -11228,19 +11231,19 @@
         <v>7</v>
       </c>
       <c r="D38" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E38" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="F38" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="G38" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="H38" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K38" s="90" t="s">
         <v>164</v>
@@ -11257,19 +11260,19 @@
         <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E39" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="F39" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="G39" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="H39" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K39" s="90" t="s">
         <v>164</v>
@@ -11286,19 +11289,19 @@
         <v>7</v>
       </c>
       <c r="D40" t="s">
+        <v>569</v>
+      </c>
+      <c r="E40" t="s">
         <v>570</v>
       </c>
-      <c r="E40" t="s">
-        <v>571</v>
-      </c>
       <c r="F40" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="G40" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H40" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K40" s="90" t="s">
         <v>164</v>
@@ -11313,22 +11316,22 @@
       </c>
       <c r="B41" s="85"/>
       <c r="C41" s="85" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="D41" s="85" t="s">
+        <v>637</v>
+      </c>
+      <c r="E41" s="85" t="s">
+        <v>636</v>
+      </c>
+      <c r="F41" s="85" t="s">
         <v>638</v>
       </c>
-      <c r="E41" s="85" t="s">
-        <v>637</v>
-      </c>
-      <c r="F41" s="85" t="s">
-        <v>639</v>
-      </c>
       <c r="G41" s="85" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="H41" s="85" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="I41" s="85"/>
       <c r="J41" s="85"/>
@@ -11347,16 +11350,16 @@
         <v>8</v>
       </c>
       <c r="D42" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="E42" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="H42" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K42" s="90" t="s">
         <v>164</v>
@@ -11373,16 +11376,16 @@
         <v>8</v>
       </c>
       <c r="D43" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E43" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="H43" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K43" s="90" t="s">
         <v>164</v>
@@ -11399,16 +11402,16 @@
         <v>8</v>
       </c>
       <c r="D44" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="E44" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="H44" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K44" s="90" t="s">
         <v>164</v>
@@ -12209,7 +12212,7 @@
       </c>
       <c r="C18" s="72"/>
       <c r="D18" s="72" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E18" s="74" t="s">
         <v>15</v>
@@ -12507,7 +12510,7 @@
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>15</v>
@@ -13099,11 +13102,11 @@
         <v>143</v>
       </c>
       <c r="B48" s="72" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C48" s="72"/>
       <c r="D48" s="72" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="E48" s="72" t="s">
         <v>16</v>
@@ -13131,7 +13134,7 @@
       </c>
       <c r="C49" s="72"/>
       <c r="D49" s="72" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E49" s="72" t="s">
         <v>17</v>
@@ -13316,11 +13319,11 @@
         <v>179</v>
       </c>
       <c r="B55" s="40" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C55" s="40"/>
       <c r="D55" s="41" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E55" s="40" t="s">
         <v>15</v>
@@ -13347,11 +13350,11 @@
         <v>179</v>
       </c>
       <c r="B56" s="40" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C56" s="40"/>
       <c r="D56" s="41" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E56" s="40" t="s">
         <v>15</v>
@@ -13502,7 +13505,7 @@
       </c>
       <c r="C61" s="62"/>
       <c r="D61" s="66" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E61" s="62" t="s">
         <v>16</v>
@@ -14638,7 +14641,7 @@
         <v>53</v>
       </c>
       <c r="E26" s="64" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F26" s="62">
         <v>1</v>
@@ -14672,7 +14675,7 @@
         <v>53</v>
       </c>
       <c r="E27" s="64" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F27" s="62">
         <v>1</v>
@@ -14706,7 +14709,7 @@
         <v>53</v>
       </c>
       <c r="E28" s="64" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F28" s="62">
         <v>1</v>
@@ -14740,7 +14743,7 @@
         <v>53</v>
       </c>
       <c r="E29" s="64" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F29" s="62">
         <v>1</v>
@@ -14774,7 +14777,7 @@
         <v>53</v>
       </c>
       <c r="E30" s="64" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F30" s="62">
         <v>1</v>
@@ -14808,7 +14811,7 @@
         <v>53</v>
       </c>
       <c r="E31" s="64" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F31" s="62">
         <v>1</v>
@@ -15075,7 +15078,7 @@
         <v>167</v>
       </c>
       <c r="E39" s="46" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="F39" s="33">
         <v>1</v>
@@ -15108,7 +15111,7 @@
         <v>167</v>
       </c>
       <c r="E40" s="46" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="F40" s="33">
         <v>1</v>
@@ -15440,7 +15443,7 @@
         <v>167</v>
       </c>
       <c r="E50" s="100" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="F50" s="99">
         <v>1</v>
@@ -15473,7 +15476,7 @@
         <v>167</v>
       </c>
       <c r="E51" s="100" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="F51" s="99">
         <v>1</v>
@@ -15506,7 +15509,7 @@
         <v>167</v>
       </c>
       <c r="E52" s="94" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F52" s="93">
         <v>1</v>
@@ -15539,7 +15542,7 @@
         <v>167</v>
       </c>
       <c r="E53" s="94" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="F53" s="93">
         <v>1</v>
@@ -15572,7 +15575,7 @@
         <v>167</v>
       </c>
       <c r="E54" s="94" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="F54" s="93">
         <v>1</v>
@@ -15605,7 +15608,7 @@
         <v>167</v>
       </c>
       <c r="E55" s="94" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F55" s="93">
         <v>1</v>
@@ -15638,7 +15641,7 @@
         <v>167</v>
       </c>
       <c r="E56" s="94" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F56" s="93">
         <v>1</v>
@@ -15671,7 +15674,7 @@
         <v>167</v>
       </c>
       <c r="E57" s="94" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="F57" s="93">
         <v>1</v>
@@ -15704,7 +15707,7 @@
         <v>167</v>
       </c>
       <c r="E58" s="94" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="F58" s="93">
         <v>1</v>
@@ -15737,7 +15740,7 @@
         <v>167</v>
       </c>
       <c r="E59" s="94" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F59" s="93">
         <v>1</v>
@@ -15770,7 +15773,7 @@
         <v>167</v>
       </c>
       <c r="E60" s="94" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="F60" s="93">
         <v>1</v>
@@ -15803,7 +15806,7 @@
         <v>167</v>
       </c>
       <c r="E61" s="94" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="F61" s="93">
         <v>1</v>
@@ -15836,7 +15839,7 @@
         <v>167</v>
       </c>
       <c r="E62" s="94" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="F62" s="93">
         <v>1</v>
@@ -15869,7 +15872,7 @@
         <v>167</v>
       </c>
       <c r="E63" s="94" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="F63" s="93">
         <v>1</v>
@@ -15902,7 +15905,7 @@
         <v>167</v>
       </c>
       <c r="E64" s="94" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="F64" s="93">
         <v>1</v>
@@ -16158,7 +16161,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16196,13 +16199,13 @@
         <v>99</v>
       </c>
       <c r="B2" s="89" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C2" s="89" t="s">
         <v>419</v>
       </c>
       <c r="D2" s="88" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E2" s="88" t="s">
         <v>418</v>
@@ -16216,16 +16219,16 @@
         <v>21</v>
       </c>
       <c r="B3" s="87" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C3" s="87" t="s">
+        <v>692</v>
+      </c>
+      <c r="D3" s="86" t="s">
         <v>420</v>
       </c>
-      <c r="D3" s="86" t="s">
+      <c r="E3" s="86" t="s">
         <v>421</v>
-      </c>
-      <c r="E3" s="86" t="s">
-        <v>422</v>
       </c>
       <c r="F3" s="86">
         <v>1</v>

</xml_diff>

<commit_message>
add date picker in board not cmplt
</commit_message>
<xml_diff>
--- a/db/excel/api-function-granted-users-cdld.xlsx
+++ b/db/excel/api-function-granted-users-cdld.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10711"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D733442-6859-EA41-8DA6-2F862C60530D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F76C20-625A-B141-B128-D6F7FB078300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19460" tabRatio="800" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19460" tabRatio="800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_types" sheetId="27" r:id="rId1"/>
@@ -300,7 +300,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1780" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1785" uniqueCount="710">
   <si>
     <t>status</t>
   </si>
@@ -2523,6 +2523,15 @@
   </si>
   <si>
     <t>Báo cáo dashboard</t>
+  </si>
+  <si>
+    <t>Ảnh nền cho trang quản lý direct org ass</t>
+  </si>
+  <si>
+    <t>BG_DI_ORG_ASS</t>
+  </si>
+  <si>
+    <t>url(https://images.unsplash.com/photo-1599158150601-1417ebbaafdd?ixlib=rb-1.2.1&amp;ixid=MnwxMjA3fDB8MHxwaG90by1wYWdlfHx8fGVufDB8fHx8&amp;auto=format&amp;fit=crop&amp;w=1920&amp;q=40)</t>
   </si>
 </sst>
 </file>
@@ -5396,8 +5405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10241,10 +10250,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11559,6 +11568,32 @@
         <v>164</v>
       </c>
       <c r="L44" s="88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>84</v>
+      </c>
+      <c r="B45">
+        <v>8</v>
+      </c>
+      <c r="D45" t="s">
+        <v>708</v>
+      </c>
+      <c r="E45" t="s">
+        <v>707</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>709</v>
+      </c>
+      <c r="H45" t="s">
+        <v>607</v>
+      </c>
+      <c r="K45" s="88" t="s">
+        <v>164</v>
+      </c>
+      <c r="L45" s="88">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add view and logic direct crit deadline view
</commit_message>
<xml_diff>
--- a/db/excel/api-function-granted-users-cdld.xlsx
+++ b/db/excel/api-function-granted-users-cdld.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10711"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439CA746-8F99-0D4A-83EE-0CA79FA3C887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E8319B-F97A-5B47-B73B-3C319DF414B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="520" windowWidth="33600" windowHeight="19480" tabRatio="800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" tabRatio="800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_types" sheetId="27" r:id="rId1"/>
@@ -300,7 +300,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1992" uniqueCount="749">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2029" uniqueCount="768">
   <si>
     <t>status</t>
   </si>
@@ -2003,9 +2003,6 @@
     <t>Chỉ đạo chung của cả Ban Giám Đốc</t>
   </si>
   <si>
-    <t>Bản ghi này hoạt động hay không hoạt động</t>
-  </si>
-  <si>
     <t>Trạng thái của bản ghi này</t>
   </si>
   <si>
@@ -2649,6 +2646,66 @@
   </si>
   <si>
     <t>Trang đánh giá thực hiện chỉ đạo của các đơn vị (người đánh giá)</t>
+  </si>
+  <si>
+    <t>[91,92,93]</t>
+  </si>
+  <si>
+    <t>DIRECT_STATUS</t>
+  </si>
+  <si>
+    <t>D_NEW</t>
+  </si>
+  <si>
+    <t>Danh mục trạng thái của chỉ đạo (bảng directs)</t>
+  </si>
+  <si>
+    <t>Danh mục các trạng thái của chỉ đạo</t>
+  </si>
+  <si>
+    <t>D_U_CRIT</t>
+  </si>
+  <si>
+    <t>D_U_CMT</t>
+  </si>
+  <si>
+    <t>D_DEL</t>
+  </si>
+  <si>
+    <t>Đã Cập Nhập Bình Luận Lãnh Đạo</t>
+  </si>
+  <si>
+    <t>Không hoạt động</t>
+  </si>
+  <si>
+    <t>Chỉ đạo được tạo mới thì có trạng thái này</t>
+  </si>
+  <si>
+    <t>Chỉ đạo mới (1)</t>
+  </si>
+  <si>
+    <t>Khi đơn vị đánh giá cập nhập chỉ số thì có trạng thái này</t>
+  </si>
+  <si>
+    <t>Khi P.TH thêm ý kiến của lãnh đạo thì có trạng thái này</t>
+  </si>
+  <si>
+    <t>Nếu xoá đi thì có trạng thái này</t>
+  </si>
+  <si>
+    <t>Bản ghi này hoạt động hay không hoạt động (lấy từ categories)</t>
+  </si>
+  <si>
+    <t>Đã Cập Nhập Deadlne, Chỉ Số (2)</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>Giá Trị</t>
+  </si>
+  <si>
+    <t>Gía trị khi lưu db của dữ liệu này</t>
   </si>
 </sst>
 </file>
@@ -5617,7 +5674,7 @@
         <v>4</v>
       </c>
       <c r="I1" s="77" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="J1" s="77" t="s">
         <v>158</v>
@@ -5632,7 +5689,7 @@
         <v>0</v>
       </c>
       <c r="N1" s="77" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
@@ -5678,7 +5735,7 @@
         <v>343</v>
       </c>
       <c r="D3" s="115" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="E3" s="116" t="s">
         <v>343</v>
@@ -5713,18 +5770,18 @@
         <v>3</v>
       </c>
       <c r="C4" s="79" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="D4" s="79"/>
       <c r="E4" s="80" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="F4" s="80"/>
       <c r="G4" s="80" t="s">
+        <v>745</v>
+      </c>
+      <c r="H4" s="79" t="s">
         <v>746</v>
-      </c>
-      <c r="H4" s="79" t="s">
-        <v>747</v>
       </c>
       <c r="I4" s="79"/>
       <c r="J4" s="79"/>
@@ -5747,18 +5804,18 @@
         <v>3</v>
       </c>
       <c r="C5" s="79" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="D5" s="79"/>
       <c r="E5" s="80" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="F5" s="80"/>
       <c r="G5" s="80" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="H5" s="79" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="I5" s="79"/>
       <c r="J5" s="79"/>
@@ -5813,22 +5870,22 @@
       </c>
       <c r="B7" s="115"/>
       <c r="C7" s="115" t="s">
+        <v>668</v>
+      </c>
+      <c r="D7" s="115" t="s">
+        <v>683</v>
+      </c>
+      <c r="E7" s="116" t="s">
+        <v>668</v>
+      </c>
+      <c r="F7" s="116" t="s">
+        <v>680</v>
+      </c>
+      <c r="G7" s="116" t="s">
         <v>669</v>
       </c>
-      <c r="D7" s="115" t="s">
-        <v>684</v>
-      </c>
-      <c r="E7" s="116" t="s">
-        <v>669</v>
-      </c>
-      <c r="F7" s="116" t="s">
-        <v>681</v>
-      </c>
-      <c r="G7" s="116" t="s">
-        <v>670</v>
-      </c>
       <c r="H7" s="115" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="I7" s="115"/>
       <c r="J7" s="115"/>
@@ -5919,18 +5976,18 @@
         <v>4</v>
       </c>
       <c r="C10" s="79" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="D10" s="79"/>
       <c r="E10" s="80" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="F10" s="80"/>
       <c r="G10" s="80" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="H10" s="79" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="I10" s="79"/>
       <c r="J10" s="81"/>
@@ -5954,7 +6011,7 @@
         <v>388</v>
       </c>
       <c r="D11" s="115" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="E11" s="116" t="s">
         <v>388</v>
@@ -5989,18 +6046,18 @@
         <v>5</v>
       </c>
       <c r="C12" s="79" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="D12" s="79"/>
       <c r="E12" s="80" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="F12" s="80"/>
       <c r="G12" s="80" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="H12" s="79" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="I12" s="79"/>
       <c r="J12" s="81"/>
@@ -6058,7 +6115,7 @@
         <v>331</v>
       </c>
       <c r="D14" s="115" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="E14" s="116" t="s">
         <v>331</v>
@@ -6067,7 +6124,7 @@
         <v>335</v>
       </c>
       <c r="G14" s="116" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="H14" s="115" t="s">
         <v>402</v>
@@ -6101,7 +6158,7 @@
       </c>
       <c r="F15" s="80"/>
       <c r="G15" s="80" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="H15" s="79" t="s">
         <v>336</v>
@@ -6135,7 +6192,7 @@
       </c>
       <c r="F16" s="80"/>
       <c r="G16" s="80" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="H16" s="79" t="s">
         <v>337</v>
@@ -6169,7 +6226,7 @@
       </c>
       <c r="F17" s="80"/>
       <c r="G17" s="80" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="H17" s="79" t="s">
         <v>338</v>
@@ -6267,11 +6324,11 @@
       </c>
       <c r="D20" s="79"/>
       <c r="E20" s="80" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="F20" s="80"/>
       <c r="G20" s="80" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="H20" s="79" t="s">
         <v>346</v>
@@ -6368,10 +6425,10 @@
         <v>109</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="F2" s="29"/>
       <c r="G2" s="29"/>
@@ -6395,10 +6452,10 @@
         <v>109</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="F3" s="29"/>
       <c r="G3" s="29"/>
@@ -6422,10 +6479,10 @@
         <v>109</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="F4" s="28"/>
       <c r="G4" s="28"/>
@@ -6449,10 +6506,10 @@
         <v>109</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="F5" s="28"/>
       <c r="G5" s="28"/>
@@ -6467,7 +6524,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="28" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B6" s="28">
         <v>5</v>
@@ -6476,10 +6533,10 @@
         <v>109</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="F6" s="28"/>
       <c r="G6" s="28"/>
@@ -6494,7 +6551,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="28" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B7" s="28">
         <v>3</v>
@@ -6503,10 +6560,10 @@
         <v>109</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
@@ -6567,10 +6624,10 @@
         <v>233</v>
       </c>
       <c r="D1" s="39" t="s">
+        <v>589</v>
+      </c>
+      <c r="E1" s="39" t="s">
         <v>590</v>
-      </c>
-      <c r="E1" s="39" t="s">
-        <v>591</v>
       </c>
       <c r="F1" s="39" t="s">
         <v>178</v>
@@ -6605,7 +6662,7 @@
         <v>498</v>
       </c>
       <c r="E2" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="J2" t="s">
         <v>185</v>
@@ -6628,7 +6685,7 @@
         <v>500</v>
       </c>
       <c r="E3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="J3" t="s">
         <v>185</v>
@@ -6651,7 +6708,7 @@
         <v>501</v>
       </c>
       <c r="E4" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="J4" t="s">
         <v>185</v>
@@ -6665,7 +6722,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="C5" t="s">
         <v>536</v>
@@ -6674,7 +6731,7 @@
         <v>499</v>
       </c>
       <c r="E5" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="J5" t="s">
         <v>185</v>
@@ -6688,7 +6745,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C6" t="s">
         <v>540</v>
@@ -6697,7 +6754,7 @@
         <v>503</v>
       </c>
       <c r="E6" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="J6" t="s">
         <v>185</v>
@@ -6711,7 +6768,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="C7" t="s">
         <v>539</v>
@@ -6720,7 +6777,7 @@
         <v>502</v>
       </c>
       <c r="E7" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="J7" t="s">
         <v>185</v>
@@ -6734,7 +6791,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C8" t="s">
         <v>541</v>
@@ -6743,7 +6800,7 @@
         <v>504</v>
       </c>
       <c r="E8" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="J8" t="s">
         <v>185</v>
@@ -6757,7 +6814,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="C9" t="s">
         <v>542</v>
@@ -6766,7 +6823,7 @@
         <v>505</v>
       </c>
       <c r="E9" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="J9" t="s">
         <v>185</v>
@@ -6789,7 +6846,7 @@
         <v>506</v>
       </c>
       <c r="E10" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="J10" t="s">
         <v>185</v>
@@ -6812,7 +6869,7 @@
         <v>506</v>
       </c>
       <c r="E11" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="J11" t="s">
         <v>185</v>
@@ -6835,7 +6892,7 @@
         <v>506</v>
       </c>
       <c r="E12" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="J12" t="s">
         <v>185</v>
@@ -6858,7 +6915,7 @@
         <v>506</v>
       </c>
       <c r="E13" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="J13" t="s">
         <v>185</v>
@@ -6881,7 +6938,7 @@
         <v>506</v>
       </c>
       <c r="E14" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="J14" t="s">
         <v>185</v>
@@ -6904,7 +6961,7 @@
         <v>506</v>
       </c>
       <c r="E15" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="J15" t="s">
         <v>185</v>
@@ -6927,7 +6984,7 @@
         <v>506</v>
       </c>
       <c r="E16" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="J16" t="s">
         <v>185</v>
@@ -6950,7 +7007,7 @@
         <v>506</v>
       </c>
       <c r="E17" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="J17" t="s">
         <v>185</v>
@@ -7143,13 +7200,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P134"/>
+  <dimension ref="A1:P135"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C94" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A18" sqref="A18"/>
+      <selection pane="bottomRight" activeCell="G125" sqref="G125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7334,7 +7391,7 @@
         <v>251</v>
       </c>
       <c r="D5" s="100" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="E5" s="100" t="s">
         <v>16</v>
@@ -7646,13 +7703,13 @@
         <v>212</v>
       </c>
       <c r="B15" s="48" t="s">
+        <v>609</v>
+      </c>
+      <c r="C15" s="48" t="s">
         <v>610</v>
       </c>
-      <c r="C15" s="48" t="s">
+      <c r="D15" s="48" t="s">
         <v>611</v>
-      </c>
-      <c r="D15" s="48" t="s">
-        <v>612</v>
       </c>
       <c r="E15" s="48" t="s">
         <v>16</v>
@@ -7666,7 +7723,7 @@
       <c r="J15" s="55"/>
       <c r="K15" s="55"/>
       <c r="L15" s="56" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="M15" s="55"/>
       <c r="N15" s="55"/>
@@ -7758,7 +7815,7 @@
         <v>243</v>
       </c>
       <c r="D18" s="102" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="E18" s="102" t="s">
         <v>16</v>
@@ -7772,7 +7829,7 @@
       <c r="J18" s="55"/>
       <c r="K18" s="55"/>
       <c r="L18" s="56" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="M18" s="55"/>
       <c r="N18" s="55"/>
@@ -7806,7 +7863,7 @@
       <c r="J19" s="55"/>
       <c r="K19" s="55"/>
       <c r="L19" s="56" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="M19" s="55"/>
       <c r="N19" s="55"/>
@@ -7916,7 +7973,7 @@
         <v>212</v>
       </c>
       <c r="B23" s="112" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C23" s="112" t="s">
         <v>415</v>
@@ -8070,13 +8127,13 @@
         <v>212</v>
       </c>
       <c r="B28" s="112" t="s">
+        <v>661</v>
+      </c>
+      <c r="C28" s="112" t="s">
         <v>662</v>
       </c>
-      <c r="C28" s="112" t="s">
-        <v>663</v>
-      </c>
       <c r="D28" s="112" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="E28" s="112" t="s">
         <v>15</v>
@@ -8162,20 +8219,20 @@
       </c>
     </row>
     <row r="31" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="48" t="s">
+      <c r="A31" s="102" t="s">
         <v>212</v>
       </c>
-      <c r="B31" s="48" t="s">
+      <c r="B31" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="C31" s="48" t="s">
+      <c r="C31" s="102" t="s">
         <v>227</v>
       </c>
-      <c r="D31" s="48" t="s">
-        <v>560</v>
-      </c>
-      <c r="E31" s="48" t="s">
-        <v>17</v>
+      <c r="D31" s="102" t="s">
+        <v>763</v>
+      </c>
+      <c r="E31" s="102" t="s">
+        <v>16</v>
       </c>
       <c r="F31" s="55"/>
       <c r="G31" s="55"/>
@@ -8195,7 +8252,7 @@
     </row>
     <row r="32" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="47" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B32" s="47" t="s">
         <v>305</v>
@@ -8233,16 +8290,16 @@
     </row>
     <row r="33" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="47" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B33" s="47" t="s">
         <v>513</v>
       </c>
       <c r="C33" s="47" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="D33" s="47" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="E33" s="47" t="s">
         <v>15</v>
@@ -8258,7 +8315,7 @@
       <c r="J33" s="52"/>
       <c r="K33" s="52"/>
       <c r="L33" s="56" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="M33" s="52"/>
       <c r="N33" s="52"/>
@@ -8269,16 +8326,16 @@
     </row>
     <row r="34" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="47" t="s">
+        <v>728</v>
+      </c>
+      <c r="B34" s="47" t="s">
         <v>729</v>
       </c>
-      <c r="B34" s="47" t="s">
-        <v>730</v>
-      </c>
       <c r="C34" s="47" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="D34" s="47" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E34" s="47" t="s">
         <v>15</v>
@@ -8301,16 +8358,16 @@
     </row>
     <row r="35" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="47" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B35" s="47" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C35" s="47" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D35" s="47" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E35" s="47" t="s">
         <v>15</v>
@@ -8333,16 +8390,16 @@
     </row>
     <row r="36" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="47" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B36" s="47" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C36" s="47" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="D36" s="47" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E36" s="47" t="s">
         <v>15</v>
@@ -8365,16 +8422,16 @@
     </row>
     <row r="37" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="47" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B37" s="47" t="s">
         <v>45</v>
       </c>
       <c r="C37" s="47" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="D37" s="47" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E37" s="47" t="s">
         <v>15</v>
@@ -8397,16 +8454,16 @@
     </row>
     <row r="38" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="47" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B38" s="47" t="s">
         <v>19</v>
       </c>
       <c r="C38" s="47" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="D38" s="47" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E38" s="47" t="s">
         <v>50</v>
@@ -8427,16 +8484,16 @@
     </row>
     <row r="39" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="47" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B39" s="47" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="C39" s="47" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="D39" s="47" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="E39" s="47" t="s">
         <v>15</v>
@@ -8500,13 +8557,13 @@
         <v>467</v>
       </c>
       <c r="B41" s="89" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C41" s="89" t="s">
+        <v>613</v>
+      </c>
+      <c r="D41" s="89" t="s">
         <v>614</v>
-      </c>
-      <c r="D41" s="89" t="s">
-        <v>615</v>
       </c>
       <c r="E41" s="89" t="s">
         <v>16</v>
@@ -8580,7 +8637,7 @@
       <c r="J43" s="90"/>
       <c r="K43" s="90"/>
       <c r="L43" s="56" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="M43" s="90"/>
       <c r="N43" s="90"/>
@@ -8600,7 +8657,7 @@
         <v>261</v>
       </c>
       <c r="D44" s="89" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="E44" s="89" t="s">
         <v>15</v>
@@ -8632,7 +8689,7 @@
         <v>262</v>
       </c>
       <c r="D45" s="89" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="E45" s="89" t="s">
         <v>15</v>
@@ -8913,10 +8970,10 @@
         <v>305</v>
       </c>
       <c r="C54" s="47" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D54" s="47" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E54" s="47" t="s">
         <v>15</v>
@@ -8948,13 +9005,13 @@
         <v>267</v>
       </c>
       <c r="B55" s="47" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C55" s="47" t="s">
+        <v>613</v>
+      </c>
+      <c r="D55" s="47" t="s">
         <v>614</v>
-      </c>
-      <c r="D55" s="47" t="s">
-        <v>615</v>
       </c>
       <c r="E55" s="47" t="s">
         <v>16</v>
@@ -8968,7 +9025,7 @@
       <c r="J55" s="52"/>
       <c r="K55" s="52"/>
       <c r="L55" s="56" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="M55" s="52"/>
       <c r="N55" s="52"/>
@@ -9004,7 +9061,7 @@
       <c r="J56" s="52"/>
       <c r="K56" s="52"/>
       <c r="L56" s="56" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="M56" s="52"/>
       <c r="N56" s="52"/>
@@ -9038,7 +9095,7 @@
       <c r="J57" s="52"/>
       <c r="K57" s="52"/>
       <c r="L57" s="56" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="M57" s="52"/>
       <c r="N57" s="52"/>
@@ -9084,13 +9141,13 @@
         <v>267</v>
       </c>
       <c r="B59" s="100" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C59" s="100" t="s">
         <v>265</v>
       </c>
       <c r="D59" s="100" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="E59" s="100" t="s">
         <v>16</v>
@@ -9102,7 +9159,7 @@
       <c r="J59" s="101"/>
       <c r="K59" s="101"/>
       <c r="L59" s="56" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="M59" s="101"/>
       <c r="N59" s="101"/>
@@ -9180,7 +9237,7 @@
         <v>267</v>
       </c>
       <c r="B62" s="47" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C62" s="47" t="s">
         <v>415</v>
@@ -9213,10 +9270,10 @@
         <v>220</v>
       </c>
       <c r="C63" s="110" t="s">
+        <v>568</v>
+      </c>
+      <c r="D63" s="110" t="s">
         <v>569</v>
-      </c>
-      <c r="D63" s="110" t="s">
-        <v>570</v>
       </c>
       <c r="E63" s="110" t="s">
         <v>15</v>
@@ -9372,7 +9429,7 @@
         <v>227</v>
       </c>
       <c r="D68" s="47" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="E68" s="47" t="s">
         <v>17</v>
@@ -9435,10 +9492,10 @@
         <v>305</v>
       </c>
       <c r="C70" s="49" t="s">
+        <v>571</v>
+      </c>
+      <c r="D70" s="49" t="s">
         <v>572</v>
-      </c>
-      <c r="D70" s="49" t="s">
-        <v>573</v>
       </c>
       <c r="E70" s="49" t="s">
         <v>15</v>
@@ -9492,7 +9549,7 @@
       <c r="J71" s="44"/>
       <c r="K71" s="44"/>
       <c r="L71" s="56" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="M71" s="44"/>
       <c r="N71" s="44"/>
@@ -9506,10 +9563,10 @@
         <v>266</v>
       </c>
       <c r="B72" s="49" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C72" s="49" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D72" s="49" t="s">
         <v>275</v>
@@ -9528,7 +9585,7 @@
       <c r="J72" s="44"/>
       <c r="K72" s="44"/>
       <c r="L72" s="56" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="M72" s="44"/>
       <c r="N72" s="44"/>
@@ -9562,7 +9619,7 @@
       <c r="J73" s="44"/>
       <c r="K73" s="44"/>
       <c r="L73" s="56" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="M73" s="44"/>
       <c r="N73" s="44"/>
@@ -9576,13 +9633,13 @@
         <v>266</v>
       </c>
       <c r="B74" s="49" t="s">
+        <v>719</v>
+      </c>
+      <c r="C74" s="49" t="s">
         <v>720</v>
       </c>
-      <c r="C74" s="49" t="s">
+      <c r="D74" s="49" t="s">
         <v>721</v>
-      </c>
-      <c r="D74" s="49" t="s">
-        <v>722</v>
       </c>
       <c r="E74" s="49" t="s">
         <v>16</v>
@@ -9614,7 +9671,7 @@
         <v>280</v>
       </c>
       <c r="D75" s="105" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="E75" s="104" t="s">
         <v>16</v>
@@ -9628,7 +9685,7 @@
       <c r="J75" s="44"/>
       <c r="K75" s="44"/>
       <c r="L75" s="56" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="M75" s="44"/>
       <c r="N75" s="44"/>
@@ -9736,13 +9793,13 @@
         <v>266</v>
       </c>
       <c r="B79" s="49" t="s">
+        <v>724</v>
+      </c>
+      <c r="C79" s="49" t="s">
         <v>725</v>
       </c>
-      <c r="C79" s="49" t="s">
-        <v>726</v>
-      </c>
       <c r="D79" s="49" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="E79" s="49" t="s">
         <v>17</v>
@@ -9772,7 +9829,7 @@
         <v>420</v>
       </c>
       <c r="D80" s="49" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="E80" s="49" t="s">
         <v>17</v>
@@ -9795,7 +9852,7 @@
     </row>
     <row r="81" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="25" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B81" s="25" t="s">
         <v>18</v>
@@ -9829,16 +9886,16 @@
     </row>
     <row r="82" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="25" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B82" s="25" t="s">
         <v>305</v>
       </c>
       <c r="C82" s="25" t="s">
+        <v>571</v>
+      </c>
+      <c r="D82" s="25" t="s">
         <v>572</v>
-      </c>
-      <c r="D82" s="25" t="s">
-        <v>573</v>
       </c>
       <c r="E82" s="25" t="s">
         <v>15</v>
@@ -9867,16 +9924,16 @@
     </row>
     <row r="83" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="25" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B83" s="47" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C83" s="47" t="s">
+        <v>613</v>
+      </c>
+      <c r="D83" s="47" t="s">
         <v>614</v>
-      </c>
-      <c r="D83" s="47" t="s">
-        <v>615</v>
       </c>
       <c r="E83" s="47" t="s">
         <v>16</v>
@@ -9890,7 +9947,7 @@
       <c r="J83" s="52"/>
       <c r="K83" s="52"/>
       <c r="L83" s="56" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="M83" s="52"/>
       <c r="N83" s="52"/>
@@ -9901,7 +9958,7 @@
     </row>
     <row r="84" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="25" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B84" s="25" t="s">
         <v>513</v>
@@ -9926,7 +9983,7 @@
       <c r="J84" s="119"/>
       <c r="K84" s="119"/>
       <c r="L84" s="56" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="M84" s="119"/>
       <c r="N84" s="119"/>
@@ -9937,13 +9994,13 @@
     </row>
     <row r="85" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="25" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B85" s="25" t="s">
         <v>182</v>
       </c>
       <c r="C85" s="25" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D85" s="25" t="s">
         <v>281</v>
@@ -9960,7 +10017,7 @@
       <c r="J85" s="119"/>
       <c r="K85" s="119"/>
       <c r="L85" s="56" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="M85" s="119"/>
       <c r="N85" s="119"/>
@@ -9971,13 +10028,13 @@
     </row>
     <row r="86" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="25" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B86" s="25" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C86" s="25" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D86" s="25" t="s">
         <v>282</v>
@@ -10003,7 +10060,7 @@
     </row>
     <row r="87" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="25" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B87" s="25" t="s">
         <v>4</v>
@@ -10035,16 +10092,16 @@
     </row>
     <row r="88" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="120" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B88" s="100" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C88" s="100" t="s">
         <v>265</v>
       </c>
       <c r="D88" s="100" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="E88" s="120" t="s">
         <v>16</v>
@@ -10058,7 +10115,7 @@
       <c r="J88" s="119"/>
       <c r="K88" s="119"/>
       <c r="L88" s="56" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="M88" s="119"/>
       <c r="N88" s="119"/>
@@ -10069,16 +10126,16 @@
     </row>
     <row r="89" spans="1:16" s="76" customFormat="1" ht="28" x14ac:dyDescent="0.2">
       <c r="A89" s="124" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B89" s="125" t="s">
+        <v>716</v>
+      </c>
+      <c r="C89" s="125" t="s">
         <v>717</v>
       </c>
-      <c r="C89" s="125" t="s">
+      <c r="D89" s="126" t="s">
         <v>718</v>
-      </c>
-      <c r="D89" s="126" t="s">
-        <v>719</v>
       </c>
       <c r="E89" s="127" t="s">
         <v>15</v>
@@ -10101,7 +10158,7 @@
     </row>
     <row r="90" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="25" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B90" s="25" t="s">
         <v>209</v>
@@ -10133,7 +10190,7 @@
     </row>
     <row r="91" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="25" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B91" s="25" t="s">
         <v>197</v>
@@ -10163,7 +10220,7 @@
     </row>
     <row r="92" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="25" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B92" s="25" t="s">
         <v>222</v>
@@ -10195,16 +10252,16 @@
     </row>
     <row r="93" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="25" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B93" s="25" t="s">
+        <v>724</v>
+      </c>
+      <c r="C93" s="25" t="s">
         <v>725</v>
       </c>
-      <c r="C93" s="25" t="s">
-        <v>726</v>
-      </c>
       <c r="D93" s="25" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="E93" s="25" t="s">
         <v>17</v>
@@ -10225,7 +10282,7 @@
     </row>
     <row r="94" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="25" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B94" s="25" t="s">
         <v>0</v>
@@ -10257,7 +10314,7 @@
     </row>
     <row r="95" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="58" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B95" s="58" t="s">
         <v>18</v>
@@ -10291,16 +10348,16 @@
     </row>
     <row r="96" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="58" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B96" s="58" t="s">
         <v>305</v>
       </c>
       <c r="C96" s="58" t="s">
+        <v>571</v>
+      </c>
+      <c r="D96" s="58" t="s">
         <v>572</v>
-      </c>
-      <c r="D96" s="58" t="s">
-        <v>573</v>
       </c>
       <c r="E96" s="58" t="s">
         <v>15</v>
@@ -10329,7 +10386,7 @@
     </row>
     <row r="97" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="58" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B97" s="58" t="s">
         <v>513</v>
@@ -10354,7 +10411,7 @@
       <c r="J97" s="43"/>
       <c r="K97" s="43"/>
       <c r="L97" s="58" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="M97" s="43"/>
       <c r="N97" s="43"/>
@@ -10365,13 +10422,13 @@
     </row>
     <row r="98" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="58" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B98" s="58" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C98" s="58" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D98" s="58" t="s">
         <v>275</v>
@@ -10390,7 +10447,7 @@
       <c r="J98" s="43"/>
       <c r="K98" s="43"/>
       <c r="L98" s="58" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="M98" s="43"/>
       <c r="N98" s="43"/>
@@ -10401,16 +10458,16 @@
     </row>
     <row r="99" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="58" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B99" s="58" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="C99" s="58" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="D99" s="58" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="E99" s="58" t="s">
         <v>15</v>
@@ -10433,13 +10490,13 @@
     </row>
     <row r="100" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A100" s="58" t="s">
+        <v>706</v>
+      </c>
+      <c r="B100" s="58" t="s">
+        <v>709</v>
+      </c>
+      <c r="C100" s="58" t="s">
         <v>707</v>
-      </c>
-      <c r="B100" s="58" t="s">
-        <v>710</v>
-      </c>
-      <c r="C100" s="58" t="s">
-        <v>708</v>
       </c>
       <c r="D100" s="58" t="s">
         <v>281</v>
@@ -10456,7 +10513,7 @@
       <c r="J100" s="43"/>
       <c r="K100" s="43"/>
       <c r="L100" s="58" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="M100" s="43"/>
       <c r="N100" s="43"/>
@@ -10467,13 +10524,13 @@
     </row>
     <row r="101" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A101" s="58" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B101" s="58" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C101" s="58" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D101" s="58" t="s">
         <v>282</v>
@@ -10499,16 +10556,16 @@
     </row>
     <row r="102" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A102" s="58" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B102" s="58" t="s">
+        <v>711</v>
+      </c>
+      <c r="C102" s="58" t="s">
+        <v>704</v>
+      </c>
+      <c r="D102" s="58" t="s">
         <v>712</v>
-      </c>
-      <c r="C102" s="58" t="s">
-        <v>705</v>
-      </c>
-      <c r="D102" s="58" t="s">
-        <v>713</v>
       </c>
       <c r="E102" s="58" t="s">
         <v>16</v>
@@ -10531,16 +10588,16 @@
     </row>
     <row r="103" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A103" s="58" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B103" s="58" t="s">
         <v>4</v>
       </c>
       <c r="C103" s="58" t="s">
+        <v>713</v>
+      </c>
+      <c r="D103" s="58" t="s">
         <v>714</v>
-      </c>
-      <c r="D103" s="58" t="s">
-        <v>715</v>
       </c>
       <c r="E103" s="58" t="s">
         <v>15</v>
@@ -10563,16 +10620,16 @@
     </row>
     <row r="104" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="58" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B104" s="58" t="s">
+        <v>719</v>
+      </c>
+      <c r="C104" s="58" t="s">
         <v>720</v>
       </c>
-      <c r="C104" s="58" t="s">
+      <c r="D104" s="58" t="s">
         <v>721</v>
-      </c>
-      <c r="D104" s="58" t="s">
-        <v>722</v>
       </c>
       <c r="E104" s="58" t="s">
         <v>16</v>
@@ -10595,16 +10652,16 @@
     </row>
     <row r="105" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A105" s="122" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B105" s="122" t="s">
         <v>279</v>
       </c>
       <c r="C105" s="122" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="D105" s="122" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="E105" s="122" t="s">
         <v>16</v>
@@ -10618,7 +10675,7 @@
       <c r="J105" s="43"/>
       <c r="K105" s="43"/>
       <c r="L105" s="58" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="M105" s="43"/>
       <c r="N105" s="43"/>
@@ -10629,7 +10686,7 @@
     </row>
     <row r="106" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A106" s="58" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B106" s="58" t="s">
         <v>209</v>
@@ -10661,7 +10718,7 @@
     </row>
     <row r="107" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A107" s="58" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B107" s="58" t="s">
         <v>197</v>
@@ -10691,7 +10748,7 @@
     </row>
     <row r="108" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A108" s="58" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B108" s="58" t="s">
         <v>222</v>
@@ -10723,7 +10780,7 @@
     </row>
     <row r="109" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A109" s="58" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B109" s="58" t="s">
         <v>0</v>
@@ -10838,7 +10895,7 @@
         <v>237</v>
       </c>
       <c r="D112" s="107" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="E112" s="107" t="s">
         <v>16</v>
@@ -10850,7 +10907,7 @@
       <c r="J112" s="57"/>
       <c r="K112" s="57"/>
       <c r="L112" s="56" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="M112" s="57"/>
       <c r="N112" s="57"/>
@@ -11248,20 +11305,18 @@
         <v>168</v>
       </c>
       <c r="B125" s="42" t="s">
-        <v>233</v>
+        <v>765</v>
       </c>
       <c r="C125" s="42" t="s">
-        <v>235</v>
+        <v>766</v>
       </c>
       <c r="D125" s="58" t="s">
-        <v>283</v>
+        <v>767</v>
       </c>
       <c r="E125" s="58" t="s">
-        <v>15</v>
-      </c>
-      <c r="F125" s="43">
-        <v>50</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="F125" s="43"/>
       <c r="G125" s="43">
         <v>1</v>
       </c>
@@ -11282,13 +11337,13 @@
         <v>168</v>
       </c>
       <c r="B126" s="42" t="s">
-        <v>25</v>
+        <v>233</v>
       </c>
       <c r="C126" s="42" t="s">
-        <v>199</v>
+        <v>235</v>
       </c>
       <c r="D126" s="58" t="s">
-        <v>260</v>
+        <v>283</v>
       </c>
       <c r="E126" s="58" t="s">
         <v>15</v>
@@ -11296,7 +11351,9 @@
       <c r="F126" s="43">
         <v>50</v>
       </c>
-      <c r="G126" s="43"/>
+      <c r="G126" s="43">
+        <v>1</v>
+      </c>
       <c r="H126" s="43"/>
       <c r="I126" s="43"/>
       <c r="J126" s="43"/>
@@ -11306,7 +11363,7 @@
       <c r="N126" s="43"/>
       <c r="O126" s="43"/>
       <c r="P126" s="53">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="127" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
@@ -11314,19 +11371,19 @@
         <v>168</v>
       </c>
       <c r="B127" s="42" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="C127" s="42" t="s">
-        <v>236</v>
+        <v>199</v>
       </c>
       <c r="D127" s="58" t="s">
-        <v>225</v>
+        <v>260</v>
       </c>
       <c r="E127" s="58" t="s">
         <v>15</v>
       </c>
       <c r="F127" s="43">
-        <v>255</v>
+        <v>50</v>
       </c>
       <c r="G127" s="43"/>
       <c r="H127" s="43"/>
@@ -11338,7 +11395,7 @@
       <c r="N127" s="43"/>
       <c r="O127" s="43"/>
       <c r="P127" s="53">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="128" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
@@ -11346,19 +11403,19 @@
         <v>168</v>
       </c>
       <c r="B128" s="42" t="s">
-        <v>590</v>
+        <v>4</v>
       </c>
       <c r="C128" s="42" t="s">
-        <v>595</v>
+        <v>236</v>
       </c>
       <c r="D128" s="58" t="s">
-        <v>596</v>
+        <v>225</v>
       </c>
       <c r="E128" s="58" t="s">
         <v>15</v>
       </c>
       <c r="F128" s="43">
-        <v>100</v>
+        <v>255</v>
       </c>
       <c r="G128" s="43"/>
       <c r="H128" s="43"/>
@@ -11370,7 +11427,7 @@
       <c r="N128" s="43"/>
       <c r="O128" s="43"/>
       <c r="P128" s="53">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="129" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
@@ -11378,19 +11435,19 @@
         <v>168</v>
       </c>
       <c r="B129" s="42" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="C129" s="42" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="D129" s="58" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="E129" s="58" t="s">
         <v>15</v>
       </c>
       <c r="F129" s="43">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G129" s="43"/>
       <c r="H129" s="43"/>
@@ -11402,7 +11459,7 @@
       <c r="N129" s="43"/>
       <c r="O129" s="43"/>
       <c r="P129" s="53">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="130" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
@@ -11410,18 +11467,20 @@
         <v>168</v>
       </c>
       <c r="B130" s="42" t="s">
-        <v>197</v>
+        <v>590</v>
       </c>
       <c r="C130" s="42" t="s">
-        <v>228</v>
+        <v>596</v>
       </c>
       <c r="D130" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="E130" s="59" t="s">
+        <v>597</v>
+      </c>
+      <c r="E130" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="F130" s="43">
         <v>50</v>
       </c>
-      <c r="F130" s="43"/>
       <c r="G130" s="43"/>
       <c r="H130" s="43"/>
       <c r="I130" s="43"/>
@@ -11432,7 +11491,7 @@
       <c r="N130" s="43"/>
       <c r="O130" s="43"/>
       <c r="P130" s="53">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="131" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
@@ -11440,20 +11499,18 @@
         <v>168</v>
       </c>
       <c r="B131" s="42" t="s">
-        <v>222</v>
+        <v>197</v>
       </c>
       <c r="C131" s="42" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="D131" s="58" t="s">
-        <v>232</v>
+        <v>132</v>
       </c>
       <c r="E131" s="59" t="s">
-        <v>15</v>
-      </c>
-      <c r="F131" s="43">
-        <v>255</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="F131" s="43"/>
       <c r="G131" s="43"/>
       <c r="H131" s="43"/>
       <c r="I131" s="43"/>
@@ -11464,7 +11521,7 @@
       <c r="N131" s="43"/>
       <c r="O131" s="43"/>
       <c r="P131" s="53">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="132" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
@@ -11472,18 +11529,20 @@
         <v>168</v>
       </c>
       <c r="B132" s="42" t="s">
-        <v>19</v>
+        <v>222</v>
       </c>
       <c r="C132" s="42" t="s">
-        <v>229</v>
+        <v>240</v>
       </c>
       <c r="D132" s="58" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="E132" s="59" t="s">
-        <v>50</v>
-      </c>
-      <c r="F132" s="43"/>
+        <v>15</v>
+      </c>
+      <c r="F132" s="43">
+        <v>255</v>
+      </c>
       <c r="G132" s="43"/>
       <c r="H132" s="43"/>
       <c r="I132" s="43"/>
@@ -11494,7 +11553,7 @@
       <c r="N132" s="43"/>
       <c r="O132" s="43"/>
       <c r="P132" s="53">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="133" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
@@ -11502,20 +11561,18 @@
         <v>168</v>
       </c>
       <c r="B133" s="42" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="C133" s="42" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="D133" s="58" t="s">
-        <v>170</v>
+        <v>238</v>
       </c>
       <c r="E133" s="59" t="s">
-        <v>15</v>
-      </c>
-      <c r="F133" s="43">
         <v>50</v>
       </c>
+      <c r="F133" s="43"/>
       <c r="G133" s="43"/>
       <c r="H133" s="43"/>
       <c r="I133" s="43"/>
@@ -11526,7 +11583,7 @@
       <c r="N133" s="43"/>
       <c r="O133" s="43"/>
       <c r="P133" s="53">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="134" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
@@ -11534,30 +11591,62 @@
         <v>168</v>
       </c>
       <c r="B134" s="42" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="C134" s="42" t="s">
-        <v>227</v>
+        <v>239</v>
       </c>
       <c r="D134" s="58" t="s">
-        <v>171</v>
-      </c>
-      <c r="E134" s="58" t="s">
-        <v>17</v>
-      </c>
-      <c r="F134" s="43"/>
+        <v>170</v>
+      </c>
+      <c r="E134" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="F134" s="43">
+        <v>50</v>
+      </c>
       <c r="G134" s="43"/>
       <c r="H134" s="43"/>
       <c r="I134" s="43"/>
       <c r="J134" s="43"/>
       <c r="K134" s="43"/>
       <c r="L134" s="43"/>
-      <c r="M134" s="43">
-        <v>1</v>
-      </c>
+      <c r="M134" s="43"/>
       <c r="N134" s="43"/>
       <c r="O134" s="43"/>
       <c r="P134" s="53">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="135" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="42" t="s">
+        <v>168</v>
+      </c>
+      <c r="B135" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C135" s="42" t="s">
+        <v>227</v>
+      </c>
+      <c r="D135" s="58" t="s">
+        <v>171</v>
+      </c>
+      <c r="E135" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="F135" s="43"/>
+      <c r="G135" s="43"/>
+      <c r="H135" s="43"/>
+      <c r="I135" s="43"/>
+      <c r="J135" s="43"/>
+      <c r="K135" s="43"/>
+      <c r="L135" s="43"/>
+      <c r="M135" s="43">
+        <v>1</v>
+      </c>
+      <c r="N135" s="43"/>
+      <c r="O135" s="43"/>
+      <c r="P135" s="53">
         <v>133</v>
       </c>
     </row>
@@ -11572,10 +11661,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:L49"/>
+  <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11583,17 +11672,18 @@
     <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="60.5" customWidth="1"/>
-    <col min="7" max="7" width="48.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.5" customWidth="1"/>
+    <col min="8" max="8" width="48.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="38" t="s">
         <v>18</v>
       </c>
@@ -11604,211 +11694,215 @@
         <v>494</v>
       </c>
       <c r="D1" s="38" t="s">
+        <v>765</v>
+      </c>
+      <c r="E1" s="38" t="s">
         <v>233</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="F1" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="38" t="s">
+      <c r="G1" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="H1" s="38" t="s">
+        <v>589</v>
+      </c>
+      <c r="I1" s="38" t="s">
         <v>590</v>
       </c>
-      <c r="H1" s="38" t="s">
-        <v>591</v>
-      </c>
-      <c r="I1" s="38" t="s">
+      <c r="J1" s="38" t="s">
         <v>197</v>
       </c>
-      <c r="J1" s="38" t="s">
+      <c r="K1" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="38" t="s">
+      <c r="L1" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="38" t="s">
+      <c r="M1" s="38" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="83">
         <v>1</v>
       </c>
       <c r="B2" s="83"/>
       <c r="C2" s="83" t="s">
+        <v>697</v>
+      </c>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83" t="s">
         <v>698</v>
       </c>
-      <c r="D2" s="83" t="s">
-        <v>699</v>
-      </c>
-      <c r="E2" s="83" t="s">
-        <v>723</v>
-      </c>
       <c r="F2" s="83" t="s">
+        <v>722</v>
+      </c>
+      <c r="G2" s="83" t="s">
         <v>351</v>
       </c>
-      <c r="G2" s="83" t="s">
+      <c r="H2" s="83" t="s">
         <v>498</v>
       </c>
-      <c r="H2" s="83" t="s">
-        <v>594</v>
-      </c>
-      <c r="I2" s="83"/>
+      <c r="I2" s="83" t="s">
+        <v>593</v>
+      </c>
       <c r="J2" s="83"/>
-      <c r="K2" s="83" t="s">
+      <c r="K2" s="83"/>
+      <c r="L2" s="83" t="s">
         <v>164</v>
       </c>
-      <c r="L2" s="83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" s="83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>11</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>348</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>347</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>353</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>499</v>
       </c>
-      <c r="H3" t="s">
-        <v>594</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="I3" t="s">
+        <v>593</v>
+      </c>
+      <c r="L3" t="s">
         <v>164</v>
       </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>12</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>349</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>350</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>354</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>500</v>
       </c>
-      <c r="H4" t="s">
-        <v>594</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="I4" t="s">
+        <v>593</v>
+      </c>
+      <c r="L4" t="s">
         <v>164</v>
       </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>13</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>452</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>435</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>453</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>501</v>
       </c>
-      <c r="H5" t="s">
-        <v>594</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="I5" t="s">
+        <v>593</v>
+      </c>
+      <c r="L5" t="s">
         <v>164</v>
       </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>14</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>356</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>357</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>358</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>502</v>
       </c>
-      <c r="H6" t="s">
-        <v>594</v>
-      </c>
-      <c r="K6" t="s">
+      <c r="I6" t="s">
+        <v>593</v>
+      </c>
+      <c r="L6" t="s">
         <v>164</v>
       </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>15</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="D7" t="s">
-        <v>701</v>
-      </c>
       <c r="E7" t="s">
+        <v>700</v>
+      </c>
+      <c r="F7" t="s">
         <v>352</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>355</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>503</v>
       </c>
-      <c r="H7" t="s">
-        <v>594</v>
-      </c>
-      <c r="K7" t="s">
+      <c r="I7" t="s">
+        <v>593</v>
+      </c>
+      <c r="L7" t="s">
         <v>164</v>
       </c>
-      <c r="L7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="118">
         <v>111</v>
       </c>
@@ -11816,31 +11910,32 @@
         <v>1</v>
       </c>
       <c r="C8" s="118"/>
-      <c r="D8" s="118" t="s">
-        <v>696</v>
-      </c>
+      <c r="D8" s="118"/>
       <c r="E8" s="118" t="s">
-        <v>633</v>
+        <v>695</v>
       </c>
       <c r="F8" s="118" t="s">
+        <v>632</v>
+      </c>
+      <c r="G8" s="118" t="s">
         <v>421</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>500</v>
       </c>
-      <c r="H8" t="s">
-        <v>594</v>
-      </c>
-      <c r="I8" s="118"/>
+      <c r="I8" t="s">
+        <v>593</v>
+      </c>
       <c r="J8" s="118"/>
-      <c r="K8" t="s">
+      <c r="K8" s="118"/>
+      <c r="L8" t="s">
         <v>164</v>
       </c>
-      <c r="L8" s="118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M8" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="118">
         <v>112</v>
       </c>
@@ -11848,31 +11943,32 @@
         <v>1</v>
       </c>
       <c r="C9" s="118"/>
-      <c r="D9" s="118" t="s">
+      <c r="D9" s="118"/>
+      <c r="E9" s="118" t="s">
         <v>439</v>
       </c>
-      <c r="E9" s="118" t="s">
+      <c r="F9" s="118" t="s">
         <v>456</v>
       </c>
-      <c r="F9" s="118" t="s">
+      <c r="G9" s="118" t="s">
         <v>457</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>502</v>
       </c>
-      <c r="H9" t="s">
-        <v>594</v>
-      </c>
-      <c r="I9" s="118"/>
+      <c r="I9" t="s">
+        <v>593</v>
+      </c>
       <c r="J9" s="118"/>
-      <c r="K9" t="s">
+      <c r="K9" s="118"/>
+      <c r="L9" t="s">
         <v>164</v>
       </c>
-      <c r="L9" s="118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M9" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="118">
         <v>114</v>
       </c>
@@ -11880,31 +11976,32 @@
         <v>1</v>
       </c>
       <c r="C10" s="118"/>
-      <c r="D10" s="118" t="s">
+      <c r="D10" s="118"/>
+      <c r="E10" s="118" t="s">
         <v>454</v>
       </c>
-      <c r="E10" s="118" t="s">
-        <v>700</v>
-      </c>
       <c r="F10" s="118" t="s">
+        <v>699</v>
+      </c>
+      <c r="G10" s="118" t="s">
         <v>455</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>503</v>
       </c>
-      <c r="H10" t="s">
-        <v>594</v>
-      </c>
-      <c r="I10" s="118"/>
+      <c r="I10" t="s">
+        <v>593</v>
+      </c>
       <c r="J10" s="118"/>
-      <c r="K10" t="s">
+      <c r="K10" s="118"/>
+      <c r="L10" t="s">
         <v>164</v>
       </c>
-      <c r="L10" s="118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M10" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="118">
         <v>115</v>
       </c>
@@ -11912,1038 +12009,1046 @@
         <v>1</v>
       </c>
       <c r="C11" s="118"/>
-      <c r="D11" s="118" t="s">
-        <v>697</v>
-      </c>
+      <c r="D11" s="118"/>
       <c r="E11" s="118" t="s">
+        <v>696</v>
+      </c>
+      <c r="F11" s="118" t="s">
         <v>429</v>
       </c>
-      <c r="F11" s="118" t="s">
+      <c r="G11" s="118" t="s">
         <v>430</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>501</v>
       </c>
-      <c r="H11" t="s">
-        <v>594</v>
-      </c>
-      <c r="I11" s="118"/>
+      <c r="I11" t="s">
+        <v>593</v>
+      </c>
       <c r="J11" s="118"/>
-      <c r="K11" t="s">
+      <c r="K11" s="118"/>
+      <c r="L11" t="s">
         <v>164</v>
       </c>
-      <c r="L11" s="118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M11" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="83">
         <v>2</v>
       </c>
       <c r="B12" s="83"/>
       <c r="C12" s="83" t="s">
-        <v>584</v>
-      </c>
-      <c r="D12" s="83" t="s">
+        <v>583</v>
+      </c>
+      <c r="D12" s="83"/>
+      <c r="E12" s="83" t="s">
         <v>359</v>
       </c>
-      <c r="E12" s="83" t="s">
+      <c r="F12" s="83" t="s">
         <v>360</v>
       </c>
-      <c r="F12" s="83" t="s">
+      <c r="G12" s="83" t="s">
         <v>367</v>
       </c>
-      <c r="G12" s="83" t="s">
+      <c r="H12" s="83" t="s">
         <v>505</v>
       </c>
-      <c r="H12" s="83" t="s">
-        <v>594</v>
-      </c>
-      <c r="I12" s="83"/>
+      <c r="I12" s="83" t="s">
+        <v>593</v>
+      </c>
       <c r="J12" s="83"/>
-      <c r="K12" s="83" t="s">
+      <c r="K12" s="83"/>
+      <c r="L12" s="83" t="s">
         <v>164</v>
       </c>
-      <c r="L12" s="83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M12" s="83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>21</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>361</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>364</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>365</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>503</v>
       </c>
-      <c r="H13" t="s">
-        <v>594</v>
-      </c>
-      <c r="K13" t="s">
+      <c r="I13" t="s">
+        <v>593</v>
+      </c>
+      <c r="L13" t="s">
         <v>164</v>
       </c>
-      <c r="L13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>22</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>362</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>363</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>366</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>499</v>
       </c>
-      <c r="H14" t="s">
-        <v>594</v>
-      </c>
-      <c r="K14" t="s">
+      <c r="I14" t="s">
+        <v>593</v>
+      </c>
+      <c r="L14" t="s">
         <v>164</v>
       </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="83">
         <v>3</v>
       </c>
       <c r="B15" s="83"/>
       <c r="C15" s="83" t="s">
-        <v>585</v>
-      </c>
-      <c r="D15" s="83" t="s">
+        <v>584</v>
+      </c>
+      <c r="D15" s="83"/>
+      <c r="E15" s="83" t="s">
         <v>431</v>
       </c>
-      <c r="E15" s="83" t="s">
+      <c r="F15" s="83" t="s">
         <v>370</v>
       </c>
-      <c r="F15" s="83" t="s">
+      <c r="G15" s="83" t="s">
         <v>371</v>
       </c>
-      <c r="G15" s="83" t="s">
+      <c r="H15" s="83" t="s">
         <v>498</v>
       </c>
-      <c r="H15" s="83" t="s">
-        <v>594</v>
-      </c>
-      <c r="I15" s="83"/>
+      <c r="I15" s="83" t="s">
+        <v>593</v>
+      </c>
       <c r="J15" s="83"/>
-      <c r="K15" s="83" t="s">
+      <c r="K15" s="83"/>
+      <c r="L15" s="83" t="s">
         <v>164</v>
       </c>
-      <c r="L15" s="83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M15" s="83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>31</v>
       </c>
       <c r="B16">
         <v>3</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>530</v>
       </c>
-      <c r="E16" t="s">
-        <v>574</v>
-      </c>
       <c r="F16" t="s">
+        <v>573</v>
+      </c>
+      <c r="G16" t="s">
         <v>372</v>
       </c>
-      <c r="G16" t="s">
-        <v>599</v>
-      </c>
       <c r="H16" t="s">
-        <v>594</v>
-      </c>
-      <c r="K16" t="s">
+        <v>598</v>
+      </c>
+      <c r="I16" t="s">
+        <v>593</v>
+      </c>
+      <c r="L16" t="s">
         <v>164</v>
       </c>
-      <c r="L16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>32</v>
       </c>
       <c r="B17">
         <v>3</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>531</v>
       </c>
-      <c r="E17" t="s">
-        <v>575</v>
-      </c>
       <c r="F17" t="s">
+        <v>574</v>
+      </c>
+      <c r="G17" t="s">
         <v>373</v>
       </c>
-      <c r="G17" t="s">
-        <v>600</v>
-      </c>
       <c r="H17" t="s">
-        <v>594</v>
-      </c>
-      <c r="K17" t="s">
+        <v>599</v>
+      </c>
+      <c r="I17" t="s">
+        <v>593</v>
+      </c>
+      <c r="L17" t="s">
         <v>164</v>
       </c>
-      <c r="L17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>33</v>
       </c>
       <c r="B18">
         <v>3</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>532</v>
       </c>
-      <c r="E18" t="s">
-        <v>576</v>
-      </c>
       <c r="F18" t="s">
+        <v>575</v>
+      </c>
+      <c r="G18" t="s">
         <v>374</v>
       </c>
-      <c r="G18" t="s">
-        <v>601</v>
-      </c>
       <c r="H18" t="s">
-        <v>594</v>
-      </c>
-      <c r="K18" t="s">
+        <v>600</v>
+      </c>
+      <c r="I18" t="s">
+        <v>593</v>
+      </c>
+      <c r="L18" t="s">
         <v>164</v>
       </c>
-      <c r="L18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>34</v>
       </c>
       <c r="B19">
         <v>3</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>533</v>
       </c>
-      <c r="E19" t="s">
-        <v>587</v>
-      </c>
       <c r="F19" t="s">
+        <v>586</v>
+      </c>
+      <c r="G19" t="s">
         <v>375</v>
       </c>
-      <c r="G19" t="s">
-        <v>602</v>
-      </c>
       <c r="H19" t="s">
-        <v>594</v>
-      </c>
-      <c r="K19" t="s">
+        <v>601</v>
+      </c>
+      <c r="I19" t="s">
+        <v>593</v>
+      </c>
+      <c r="L19" t="s">
         <v>164</v>
       </c>
-      <c r="L19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>35</v>
       </c>
       <c r="B20">
         <v>3</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>534</v>
       </c>
-      <c r="E20" t="s">
-        <v>588</v>
-      </c>
       <c r="F20" t="s">
+        <v>587</v>
+      </c>
+      <c r="G20" t="s">
         <v>376</v>
       </c>
-      <c r="G20" t="s">
-        <v>603</v>
-      </c>
       <c r="H20" t="s">
-        <v>594</v>
-      </c>
-      <c r="K20" t="s">
+        <v>602</v>
+      </c>
+      <c r="I20" t="s">
+        <v>593</v>
+      </c>
+      <c r="L20" t="s">
         <v>164</v>
       </c>
-      <c r="L20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>36</v>
       </c>
       <c r="B21">
         <v>3</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>535</v>
       </c>
-      <c r="E21" t="s">
-        <v>589</v>
-      </c>
       <c r="F21" t="s">
+        <v>588</v>
+      </c>
+      <c r="G21" t="s">
         <v>377</v>
       </c>
-      <c r="G21" t="s">
-        <v>604</v>
-      </c>
       <c r="H21" t="s">
-        <v>594</v>
-      </c>
-      <c r="K21" t="s">
+        <v>603</v>
+      </c>
+      <c r="I21" t="s">
+        <v>593</v>
+      </c>
+      <c r="L21" t="s">
         <v>164</v>
       </c>
-      <c r="L21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="83">
         <v>4</v>
       </c>
       <c r="B22" s="83"/>
       <c r="C22" s="83" t="s">
-        <v>586</v>
-      </c>
-      <c r="D22" s="83" t="s">
+        <v>585</v>
+      </c>
+      <c r="D22" s="83"/>
+      <c r="E22" s="83" t="s">
         <v>432</v>
       </c>
-      <c r="E22" s="83" t="s">
+      <c r="F22" s="83" t="s">
         <v>378</v>
       </c>
-      <c r="F22" s="83" t="s">
+      <c r="G22" s="83" t="s">
         <v>379</v>
       </c>
-      <c r="G22" s="83" t="s">
+      <c r="H22" s="83" t="s">
         <v>505</v>
       </c>
-      <c r="H22" s="83" t="s">
-        <v>594</v>
-      </c>
-      <c r="I22" s="83"/>
+      <c r="I22" s="83" t="s">
+        <v>593</v>
+      </c>
       <c r="J22" s="83"/>
-      <c r="K22" s="83" t="s">
+      <c r="K22" s="83"/>
+      <c r="L22" s="83" t="s">
         <v>164</v>
       </c>
-      <c r="L22" s="83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M22" s="83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>41</v>
       </c>
       <c r="B23">
         <v>4</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>526</v>
-      </c>
-      <c r="E23" t="s">
-        <v>380</v>
       </c>
       <c r="F23" t="s">
         <v>380</v>
       </c>
       <c r="G23" t="s">
-        <v>604</v>
+        <v>380</v>
       </c>
       <c r="H23" t="s">
-        <v>594</v>
-      </c>
-      <c r="K23" t="s">
+        <v>603</v>
+      </c>
+      <c r="I23" t="s">
+        <v>593</v>
+      </c>
+      <c r="L23" t="s">
         <v>164</v>
       </c>
-      <c r="L23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>42</v>
       </c>
       <c r="B24">
         <v>4</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>527</v>
-      </c>
-      <c r="E24" t="s">
-        <v>381</v>
       </c>
       <c r="F24" t="s">
         <v>381</v>
       </c>
       <c r="G24" t="s">
-        <v>605</v>
+        <v>381</v>
       </c>
       <c r="H24" t="s">
-        <v>594</v>
-      </c>
-      <c r="K24" t="s">
+        <v>604</v>
+      </c>
+      <c r="I24" t="s">
+        <v>593</v>
+      </c>
+      <c r="L24" t="s">
         <v>164</v>
       </c>
-      <c r="L24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>43</v>
       </c>
       <c r="B25">
         <v>4</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>528</v>
-      </c>
-      <c r="E25" t="s">
-        <v>382</v>
       </c>
       <c r="F25" t="s">
         <v>382</v>
       </c>
       <c r="G25" t="s">
-        <v>606</v>
+        <v>382</v>
       </c>
       <c r="H25" t="s">
-        <v>594</v>
-      </c>
-      <c r="K25" t="s">
+        <v>605</v>
+      </c>
+      <c r="I25" t="s">
+        <v>593</v>
+      </c>
+      <c r="L25" t="s">
         <v>164</v>
       </c>
-      <c r="L25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>44</v>
       </c>
       <c r="B26">
         <v>4</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>529</v>
-      </c>
-      <c r="E26" t="s">
-        <v>383</v>
       </c>
       <c r="F26" t="s">
         <v>383</v>
       </c>
       <c r="G26" t="s">
-        <v>607</v>
+        <v>383</v>
       </c>
       <c r="H26" t="s">
-        <v>594</v>
-      </c>
-      <c r="K26" t="s">
+        <v>606</v>
+      </c>
+      <c r="I26" t="s">
+        <v>593</v>
+      </c>
+      <c r="L26" t="s">
         <v>164</v>
       </c>
-      <c r="L26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="83">
         <v>5</v>
       </c>
       <c r="B27" s="83"/>
       <c r="C27" s="83" t="s">
-        <v>627</v>
-      </c>
-      <c r="D27" s="83" t="s">
-        <v>637</v>
-      </c>
+        <v>626</v>
+      </c>
+      <c r="D27" s="83"/>
       <c r="E27" s="83" t="s">
-        <v>631</v>
+        <v>636</v>
       </c>
       <c r="F27" s="83" t="s">
+        <v>630</v>
+      </c>
+      <c r="G27" s="83" t="s">
         <v>379</v>
       </c>
-      <c r="G27" s="83" t="s">
+      <c r="H27" s="83" t="s">
         <v>500</v>
       </c>
-      <c r="H27" s="83" t="s">
-        <v>594</v>
-      </c>
-      <c r="I27" s="83"/>
+      <c r="I27" s="83" t="s">
+        <v>593</v>
+      </c>
       <c r="J27" s="83"/>
-      <c r="K27" s="83" t="s">
+      <c r="K27" s="83"/>
+      <c r="L27" s="83" t="s">
         <v>164</v>
       </c>
-      <c r="L27" s="83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M27" s="83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>51</v>
       </c>
       <c r="B28">
         <v>5</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>464</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>465</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>466</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>501</v>
       </c>
-      <c r="H28" t="s">
-        <v>594</v>
-      </c>
-      <c r="K28" t="s">
+      <c r="I28" t="s">
+        <v>593</v>
+      </c>
+      <c r="L28" t="s">
         <v>164</v>
       </c>
-      <c r="L28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>52</v>
       </c>
       <c r="B29">
         <v>5</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>422</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>424</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>423</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>504</v>
       </c>
-      <c r="H29" t="s">
-        <v>594</v>
-      </c>
-      <c r="K29" t="s">
+      <c r="I29" t="s">
+        <v>593</v>
+      </c>
+      <c r="L29" t="s">
         <v>164</v>
       </c>
-      <c r="L29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>53</v>
       </c>
       <c r="B30">
         <v>5</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>433</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>435</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>436</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>510</v>
       </c>
-      <c r="H30" t="s">
-        <v>594</v>
-      </c>
-      <c r="K30" s="88" t="s">
+      <c r="I30" t="s">
+        <v>593</v>
+      </c>
+      <c r="L30" s="88" t="s">
         <v>164</v>
       </c>
-      <c r="L30" s="88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M30" s="88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>54</v>
       </c>
       <c r="B31">
         <v>5</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>434</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>357</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>437</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>511</v>
       </c>
-      <c r="H31" t="s">
-        <v>594</v>
-      </c>
-      <c r="K31" s="88" t="s">
+      <c r="I31" t="s">
+        <v>593</v>
+      </c>
+      <c r="L31" s="88" t="s">
         <v>164</v>
       </c>
-      <c r="L31" s="88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M31" s="88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>55</v>
       </c>
       <c r="B32">
         <v>5</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>425</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>426</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>427</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>505</v>
       </c>
-      <c r="H32" t="s">
-        <v>594</v>
-      </c>
-      <c r="K32" t="s">
+      <c r="I32" t="s">
+        <v>593</v>
+      </c>
+      <c r="L32" t="s">
         <v>164</v>
       </c>
-      <c r="L32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>56</v>
       </c>
       <c r="B33">
         <v>5</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>446</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>447</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>448</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>509</v>
       </c>
-      <c r="H33" t="s">
-        <v>594</v>
-      </c>
-      <c r="K33" s="88" t="s">
+      <c r="I33" t="s">
+        <v>593</v>
+      </c>
+      <c r="L33" s="88" t="s">
         <v>164</v>
       </c>
-      <c r="L33" s="88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M33" s="88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="83">
         <v>6</v>
       </c>
       <c r="B34" s="83"/>
       <c r="C34" s="83" t="s">
-        <v>628</v>
-      </c>
-      <c r="D34" s="83" t="s">
-        <v>636</v>
-      </c>
+        <v>627</v>
+      </c>
+      <c r="D34" s="83"/>
       <c r="E34" s="83" t="s">
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="F34" s="83" t="s">
+        <v>631</v>
+      </c>
+      <c r="G34" s="83" t="s">
         <v>552</v>
       </c>
-      <c r="G34" s="83" t="s">
+      <c r="H34" s="83" t="s">
         <v>500</v>
       </c>
-      <c r="H34" s="83" t="s">
-        <v>594</v>
-      </c>
-      <c r="I34" s="83"/>
+      <c r="I34" s="83" t="s">
+        <v>593</v>
+      </c>
       <c r="J34" s="83"/>
-      <c r="K34" s="83" t="s">
+      <c r="K34" s="83"/>
+      <c r="L34" s="83" t="s">
         <v>164</v>
       </c>
-      <c r="L34" s="83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M34" s="83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>61</v>
       </c>
       <c r="B35">
         <v>6</v>
       </c>
-      <c r="D35" t="s">
-        <v>634</v>
-      </c>
       <c r="E35" t="s">
         <v>633</v>
       </c>
       <c r="F35" t="s">
+        <v>632</v>
+      </c>
+      <c r="G35" t="s">
         <v>421</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>502</v>
       </c>
-      <c r="H35" t="s">
-        <v>594</v>
-      </c>
-      <c r="K35" t="s">
+      <c r="I35" t="s">
+        <v>593</v>
+      </c>
+      <c r="L35" t="s">
         <v>164</v>
       </c>
-      <c r="L35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>62</v>
       </c>
       <c r="B36">
         <v>6</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>439</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>456</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>457</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>507</v>
       </c>
-      <c r="H36" t="s">
-        <v>594</v>
-      </c>
-      <c r="K36" s="88" t="s">
+      <c r="I36" t="s">
+        <v>593</v>
+      </c>
+      <c r="L36" s="88" t="s">
         <v>164</v>
       </c>
-      <c r="L36" s="88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M36" s="88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>63</v>
       </c>
       <c r="B37">
         <v>6</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>454</v>
       </c>
-      <c r="E37" t="s">
-        <v>635</v>
-      </c>
       <c r="F37" t="s">
+        <v>634</v>
+      </c>
+      <c r="G37" t="s">
         <v>455</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>508</v>
       </c>
-      <c r="H37" t="s">
-        <v>594</v>
-      </c>
-      <c r="K37" s="88" t="s">
+      <c r="I37" t="s">
+        <v>593</v>
+      </c>
+      <c r="L37" s="88" t="s">
         <v>164</v>
       </c>
-      <c r="L37" s="88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M37" s="88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>64</v>
       </c>
       <c r="B38">
         <v>6</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>428</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>429</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>430</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>499</v>
       </c>
-      <c r="H38" t="s">
-        <v>594</v>
-      </c>
-      <c r="K38" t="s">
+      <c r="I38" t="s">
+        <v>593</v>
+      </c>
+      <c r="L38" t="s">
         <v>164</v>
       </c>
-      <c r="L38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>65</v>
       </c>
       <c r="B39">
         <v>6</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>449</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>450</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>451</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>512</v>
       </c>
-      <c r="H39" t="s">
-        <v>594</v>
-      </c>
-      <c r="K39" s="88" t="s">
+      <c r="I39" t="s">
+        <v>593</v>
+      </c>
+      <c r="L39" s="88" t="s">
         <v>164</v>
       </c>
-      <c r="L39" s="88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M39" s="88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="83">
         <v>7</v>
       </c>
       <c r="B40" s="83"/>
       <c r="C40" s="83" t="s">
-        <v>629</v>
-      </c>
-      <c r="D40" s="83" t="s">
+        <v>628</v>
+      </c>
+      <c r="D40" s="83"/>
+      <c r="E40" s="83" t="s">
         <v>550</v>
       </c>
-      <c r="E40" s="83" t="s">
+      <c r="F40" s="83" t="s">
         <v>551</v>
       </c>
-      <c r="F40" s="83" t="s">
+      <c r="G40" s="83" t="s">
         <v>552</v>
       </c>
-      <c r="G40" s="83" t="s">
+      <c r="H40" s="83" t="s">
         <v>500</v>
       </c>
-      <c r="H40" s="83" t="s">
-        <v>594</v>
-      </c>
-      <c r="I40" s="83"/>
+      <c r="I40" s="83" t="s">
+        <v>593</v>
+      </c>
       <c r="J40" s="83"/>
-      <c r="K40" s="83" t="s">
+      <c r="K40" s="83"/>
+      <c r="L40" s="83" t="s">
         <v>164</v>
       </c>
-      <c r="L40" s="83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M40" s="83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>71</v>
       </c>
       <c r="B41">
         <v>7</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>553</v>
       </c>
-      <c r="E41" t="s">
-        <v>645</v>
-      </c>
       <c r="F41" t="s">
+        <v>644</v>
+      </c>
+      <c r="G41" t="s">
         <v>556</v>
       </c>
-      <c r="G41" t="s">
-        <v>599</v>
-      </c>
       <c r="H41" t="s">
-        <v>594</v>
-      </c>
-      <c r="K41" s="88" t="s">
+        <v>598</v>
+      </c>
+      <c r="I41" t="s">
+        <v>593</v>
+      </c>
+      <c r="L41" s="88" t="s">
         <v>164</v>
       </c>
-      <c r="L41" s="88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M41" s="88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>72</v>
       </c>
       <c r="B42">
         <v>7</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>554</v>
       </c>
-      <c r="E42" t="s">
-        <v>646</v>
-      </c>
       <c r="F42" t="s">
+        <v>645</v>
+      </c>
+      <c r="G42" t="s">
         <v>557</v>
       </c>
-      <c r="G42" t="s">
-        <v>608</v>
-      </c>
       <c r="H42" t="s">
-        <v>594</v>
-      </c>
-      <c r="K42" s="88" t="s">
+        <v>607</v>
+      </c>
+      <c r="I42" t="s">
+        <v>593</v>
+      </c>
+      <c r="L42" s="88" t="s">
         <v>164</v>
       </c>
-      <c r="L42" s="88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M42" s="88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>73</v>
       </c>
       <c r="B43">
         <v>7</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>555</v>
       </c>
-      <c r="E43" t="s">
-        <v>647</v>
-      </c>
       <c r="F43" t="s">
+        <v>646</v>
+      </c>
+      <c r="G43" t="s">
         <v>558</v>
       </c>
-      <c r="G43" t="s">
-        <v>609</v>
-      </c>
       <c r="H43" t="s">
-        <v>594</v>
-      </c>
-      <c r="K43" s="88" t="s">
+        <v>608</v>
+      </c>
+      <c r="I43" t="s">
+        <v>593</v>
+      </c>
+      <c r="L43" s="88" t="s">
         <v>164</v>
       </c>
-      <c r="L43" s="88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M43" s="88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>74</v>
       </c>
       <c r="B44">
         <v>7</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>550</v>
       </c>
-      <c r="E44" t="s">
+      <c r="F44" t="s">
         <v>551</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>559</v>
       </c>
-      <c r="G44" t="s">
-        <v>602</v>
-      </c>
       <c r="H44" t="s">
-        <v>594</v>
-      </c>
-      <c r="K44" s="88" t="s">
+        <v>601</v>
+      </c>
+      <c r="I44" t="s">
+        <v>593</v>
+      </c>
+      <c r="L44" s="88" t="s">
         <v>164</v>
       </c>
-      <c r="L44" s="88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M44" s="88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="83">
         <v>8</v>
       </c>
       <c r="B45" s="83"/>
       <c r="C45" s="83" t="s">
-        <v>630</v>
-      </c>
-      <c r="D45" s="83" t="s">
-        <v>617</v>
-      </c>
+        <v>629</v>
+      </c>
+      <c r="D45" s="83"/>
       <c r="E45" s="83" t="s">
         <v>616</v>
       </c>
       <c r="F45" s="83" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="G45" s="83" t="s">
-        <v>594</v>
+        <v>617</v>
       </c>
       <c r="H45" s="83" t="s">
-        <v>594</v>
-      </c>
-      <c r="I45" s="83"/>
+        <v>593</v>
+      </c>
+      <c r="I45" s="83" t="s">
+        <v>593</v>
+      </c>
       <c r="J45" s="83"/>
-      <c r="K45" s="83" t="s">
+      <c r="K45" s="83"/>
+      <c r="L45" s="83" t="s">
         <v>164</v>
       </c>
-      <c r="L45" s="83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M45" s="83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="18">
         <v>81</v>
       </c>
@@ -12951,29 +13056,30 @@
         <v>8</v>
       </c>
       <c r="C46" s="18"/>
-      <c r="D46" s="18" t="s">
-        <v>619</v>
-      </c>
+      <c r="D46" s="18"/>
       <c r="E46" s="18" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="F46" s="18" t="s">
-        <v>626</v>
-      </c>
-      <c r="G46" s="18"/>
-      <c r="H46" s="18" t="s">
-        <v>594</v>
-      </c>
-      <c r="I46" s="18"/>
+        <v>621</v>
+      </c>
+      <c r="G46" s="18" t="s">
+        <v>625</v>
+      </c>
+      <c r="H46" s="18"/>
+      <c r="I46" s="18" t="s">
+        <v>593</v>
+      </c>
       <c r="J46" s="18"/>
-      <c r="K46" s="129" t="s">
+      <c r="K46" s="18"/>
+      <c r="L46" s="129" t="s">
         <v>164</v>
       </c>
-      <c r="L46" s="129">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M46" s="129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="18">
         <v>82</v>
       </c>
@@ -12981,29 +13087,30 @@
         <v>8</v>
       </c>
       <c r="C47" s="18"/>
-      <c r="D47" s="18" t="s">
-        <v>620</v>
-      </c>
+      <c r="D47" s="18"/>
       <c r="E47" s="18" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="F47" s="18" t="s">
-        <v>625</v>
-      </c>
-      <c r="G47" s="18"/>
-      <c r="H47" s="18" t="s">
-        <v>594</v>
-      </c>
-      <c r="I47" s="18"/>
+        <v>622</v>
+      </c>
+      <c r="G47" s="18" t="s">
+        <v>624</v>
+      </c>
+      <c r="H47" s="18"/>
+      <c r="I47" s="18" t="s">
+        <v>593</v>
+      </c>
       <c r="J47" s="18"/>
-      <c r="K47" s="129" t="s">
+      <c r="K47" s="18"/>
+      <c r="L47" s="129" t="s">
         <v>164</v>
       </c>
-      <c r="L47" s="129">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M47" s="129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="18">
         <v>83</v>
       </c>
@@ -13011,29 +13118,30 @@
         <v>8</v>
       </c>
       <c r="C48" s="18"/>
-      <c r="D48" s="18" t="s">
-        <v>621</v>
-      </c>
+      <c r="D48" s="18"/>
       <c r="E48" s="18" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="F48" s="18" t="s">
-        <v>638</v>
-      </c>
-      <c r="G48" s="18"/>
-      <c r="H48" s="18" t="s">
-        <v>594</v>
-      </c>
-      <c r="I48" s="18"/>
+        <v>623</v>
+      </c>
+      <c r="G48" s="18" t="s">
+        <v>637</v>
+      </c>
+      <c r="H48" s="18"/>
+      <c r="I48" s="18" t="s">
+        <v>593</v>
+      </c>
       <c r="J48" s="18"/>
-      <c r="K48" s="129" t="s">
+      <c r="K48" s="18"/>
+      <c r="L48" s="129" t="s">
         <v>164</v>
       </c>
-      <c r="L48" s="129">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M48" s="129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="18">
         <v>84</v>
       </c>
@@ -13041,25 +13149,199 @@
         <v>8</v>
       </c>
       <c r="C49" s="18"/>
-      <c r="D49" s="18" t="s">
-        <v>694</v>
-      </c>
+      <c r="D49" s="18"/>
       <c r="E49" s="18" t="s">
         <v>693</v>
       </c>
       <c r="F49" s="18" t="s">
-        <v>695</v>
-      </c>
-      <c r="G49" s="18"/>
-      <c r="H49" s="18" t="s">
-        <v>594</v>
-      </c>
-      <c r="I49" s="18"/>
+        <v>692</v>
+      </c>
+      <c r="G49" s="18" t="s">
+        <v>694</v>
+      </c>
+      <c r="H49" s="18"/>
+      <c r="I49" s="18" t="s">
+        <v>593</v>
+      </c>
       <c r="J49" s="18"/>
-      <c r="K49" s="129" t="s">
+      <c r="K49" s="18"/>
+      <c r="L49" s="129" t="s">
         <v>164</v>
       </c>
-      <c r="L49" s="129">
+      <c r="M49" s="129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A50" s="83">
+        <v>9</v>
+      </c>
+      <c r="B50" s="83"/>
+      <c r="C50" s="83" t="s">
+        <v>748</v>
+      </c>
+      <c r="D50" s="83"/>
+      <c r="E50" s="83" t="s">
+        <v>749</v>
+      </c>
+      <c r="F50" s="83" t="s">
+        <v>751</v>
+      </c>
+      <c r="G50" s="83" t="s">
+        <v>752</v>
+      </c>
+      <c r="H50" s="83" t="s">
+        <v>593</v>
+      </c>
+      <c r="I50" s="83" t="s">
+        <v>593</v>
+      </c>
+      <c r="J50" s="83"/>
+      <c r="K50" s="83"/>
+      <c r="L50" s="83" t="s">
+        <v>164</v>
+      </c>
+      <c r="M50" s="83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A51" s="18">
+        <v>90</v>
+      </c>
+      <c r="B51" s="18">
+        <v>9</v>
+      </c>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18">
+        <v>0</v>
+      </c>
+      <c r="E51" s="18" t="s">
+        <v>755</v>
+      </c>
+      <c r="F51" s="18" t="s">
+        <v>757</v>
+      </c>
+      <c r="G51" s="18" t="s">
+        <v>762</v>
+      </c>
+      <c r="H51" t="s">
+        <v>502</v>
+      </c>
+      <c r="I51" s="18" t="s">
+        <v>593</v>
+      </c>
+      <c r="J51" s="18"/>
+      <c r="K51" s="18"/>
+      <c r="L51" s="129" t="s">
+        <v>164</v>
+      </c>
+      <c r="M51" s="129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A52" s="18">
+        <v>91</v>
+      </c>
+      <c r="B52" s="18">
+        <v>9</v>
+      </c>
+      <c r="C52" s="18"/>
+      <c r="D52" s="18">
+        <v>1</v>
+      </c>
+      <c r="E52" s="18" t="s">
+        <v>750</v>
+      </c>
+      <c r="F52" s="18" t="s">
+        <v>759</v>
+      </c>
+      <c r="G52" s="18" t="s">
+        <v>758</v>
+      </c>
+      <c r="H52" t="s">
+        <v>499</v>
+      </c>
+      <c r="I52" s="18" t="s">
+        <v>593</v>
+      </c>
+      <c r="J52" s="18"/>
+      <c r="K52" s="18"/>
+      <c r="L52" s="129" t="s">
+        <v>164</v>
+      </c>
+      <c r="M52" s="129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A53" s="18">
+        <v>92</v>
+      </c>
+      <c r="B53" s="18">
+        <v>9</v>
+      </c>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18">
+        <v>2</v>
+      </c>
+      <c r="E53" s="18" t="s">
+        <v>753</v>
+      </c>
+      <c r="F53" s="18" t="s">
+        <v>764</v>
+      </c>
+      <c r="G53" s="18" t="s">
+        <v>760</v>
+      </c>
+      <c r="H53" t="s">
+        <v>500</v>
+      </c>
+      <c r="I53" s="18" t="s">
+        <v>593</v>
+      </c>
+      <c r="J53" s="18"/>
+      <c r="K53" s="18"/>
+      <c r="L53" s="129" t="s">
+        <v>164</v>
+      </c>
+      <c r="M53" s="129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A54" s="18">
+        <v>93</v>
+      </c>
+      <c r="B54" s="18">
+        <v>9</v>
+      </c>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18">
+        <v>3</v>
+      </c>
+      <c r="E54" s="18" t="s">
+        <v>754</v>
+      </c>
+      <c r="F54" s="18" t="s">
+        <v>756</v>
+      </c>
+      <c r="G54" s="18" t="s">
+        <v>761</v>
+      </c>
+      <c r="H54" t="s">
+        <v>501</v>
+      </c>
+      <c r="I54" s="18" t="s">
+        <v>593</v>
+      </c>
+      <c r="J54" s="18"/>
+      <c r="K54" s="18"/>
+      <c r="L54" s="129" t="s">
+        <v>164</v>
+      </c>
+      <c r="M54" s="129">
         <v>1</v>
       </c>
     </row>
@@ -14745,11 +15027,11 @@
         <v>143</v>
       </c>
       <c r="B48" s="72" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C48" s="72"/>
       <c r="D48" s="72" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="E48" s="72" t="s">
         <v>17</v>
@@ -14771,11 +15053,11 @@
         <v>143</v>
       </c>
       <c r="B49" s="72" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="C49" s="72"/>
       <c r="D49" s="72" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="E49" s="72" t="s">
         <v>16</v>
@@ -14988,11 +15270,11 @@
         <v>179</v>
       </c>
       <c r="B56" s="40" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C56" s="40"/>
       <c r="D56" s="41" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E56" s="40" t="s">
         <v>15</v>
@@ -15019,11 +15301,11 @@
         <v>179</v>
       </c>
       <c r="B57" s="40" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C57" s="40"/>
       <c r="D57" s="41" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E57" s="40" t="s">
         <v>15</v>
@@ -16747,7 +17029,7 @@
         <v>167</v>
       </c>
       <c r="E39" s="46" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="F39" s="33">
         <v>1</v>
@@ -16780,7 +17062,7 @@
         <v>167</v>
       </c>
       <c r="E40" s="46" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="F40" s="33">
         <v>1</v>
@@ -17343,7 +17625,7 @@
         <v>167</v>
       </c>
       <c r="E57" s="92" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="F57" s="91">
         <v>1</v>
@@ -17376,7 +17658,7 @@
         <v>167</v>
       </c>
       <c r="E58" s="92" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="F58" s="91">
         <v>1</v>
@@ -17442,7 +17724,7 @@
         <v>167</v>
       </c>
       <c r="E60" s="92" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="F60" s="91">
         <v>1</v>
@@ -17475,7 +17757,7 @@
         <v>167</v>
       </c>
       <c r="E61" s="92" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="F61" s="91">
         <v>1</v>
@@ -17508,7 +17790,7 @@
         <v>167</v>
       </c>
       <c r="E62" s="92" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="F62" s="91">
         <v>1</v>
@@ -17541,7 +17823,7 @@
         <v>167</v>
       </c>
       <c r="E63" s="92" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="F63" s="91">
         <v>1</v>
@@ -17574,7 +17856,7 @@
         <v>167</v>
       </c>
       <c r="E64" s="92" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="F64" s="91">
         <v>1</v>
@@ -17871,7 +18153,7 @@
         <v>479</v>
       </c>
       <c r="C2" s="87" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="D2" s="86" t="s">
         <v>488</v>
@@ -17888,10 +18170,10 @@
         <v>21</v>
       </c>
       <c r="B3" s="85" t="s">
+        <v>686</v>
+      </c>
+      <c r="C3" s="85" t="s">
         <v>687</v>
-      </c>
-      <c r="C3" s="85" t="s">
-        <v>688</v>
       </c>
       <c r="D3" s="84" t="s">
         <v>405</v>

</xml_diff>

<commit_message>
add edit crit logic to view org direct crit
</commit_message>
<xml_diff>
--- a/db/excel/api-function-granted-users-cdld.xlsx
+++ b/db/excel/api-function-granted-users-cdld.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E8319B-F97A-5B47-B73B-3C319DF414B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE0E7D7C-463C-42B9-BC13-6A3D42C8507E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" tabRatio="800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_types" sheetId="27" r:id="rId1"/>
@@ -5439,19 +5439,19 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" style="9" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="9" customWidth="1"/>
     <col min="5" max="5" width="14" style="9" customWidth="1"/>
-    <col min="6" max="6" width="55.5" style="9" customWidth="1"/>
-    <col min="7" max="64" width="11.5" style="9" customWidth="1"/>
-    <col min="65" max="16384" width="9.1640625" style="9"/>
+    <col min="6" max="6" width="55.42578125" style="9" customWidth="1"/>
+    <col min="7" max="64" width="11.42578125" style="9" customWidth="1"/>
+    <col min="65" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>83</v>
       </c>
@@ -5471,7 +5471,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>15</v>
       </c>
@@ -5491,7 +5491,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>16</v>
       </c>
@@ -5511,7 +5511,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>97</v>
       </c>
@@ -5531,7 +5531,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>17</v>
       </c>
@@ -5551,7 +5551,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>103</v>
       </c>
@@ -5571,7 +5571,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>50</v>
       </c>
@@ -5591,7 +5591,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>106</v>
       </c>
@@ -5630,25 +5630,25 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" style="78" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" style="78" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5" style="78" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" style="78" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" style="82" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" style="82" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.6640625" style="78" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="78.83203125" style="78" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="78" customWidth="1"/>
-    <col min="10" max="10" width="12.5" style="78" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.1640625" style="78" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" style="78" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.1640625" style="78" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="11.5" style="78"/>
+    <col min="1" max="1" width="4.140625" style="78" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="78" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" style="78" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="78" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" style="82" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" style="82" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" style="78" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="78.85546875" style="78" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" style="78" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="78" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" style="78" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" style="78" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.140625" style="78" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="11.42578125" style="78"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="77" t="s">
         <v>18</v>
       </c>
@@ -5692,7 +5692,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A2" s="115">
         <v>1</v>
       </c>
@@ -5726,7 +5726,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A3" s="115">
         <v>3</v>
       </c>
@@ -5762,7 +5762,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A4" s="79">
         <v>31</v>
       </c>
@@ -5796,7 +5796,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A5" s="79">
         <v>32</v>
       </c>
@@ -5830,7 +5830,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A6" s="79">
         <v>33</v>
       </c>
@@ -5864,7 +5864,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A7" s="115">
         <v>4</v>
       </c>
@@ -5900,7 +5900,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A8" s="79">
         <v>41</v>
       </c>
@@ -5934,7 +5934,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A9" s="79">
         <v>42</v>
       </c>
@@ -5968,7 +5968,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A10" s="79">
         <v>43</v>
       </c>
@@ -6002,7 +6002,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A11" s="115">
         <v>5</v>
       </c>
@@ -6038,7 +6038,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A12" s="79">
         <v>51</v>
       </c>
@@ -6072,7 +6072,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A13" s="79">
         <v>52</v>
       </c>
@@ -6106,7 +6106,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A14" s="115">
         <v>2</v>
       </c>
@@ -6142,7 +6142,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A15" s="79">
         <v>21</v>
       </c>
@@ -6176,7 +6176,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A16" s="79">
         <v>22</v>
       </c>
@@ -6210,7 +6210,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A17" s="79">
         <v>23</v>
       </c>
@@ -6244,7 +6244,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A18" s="79">
         <v>24</v>
       </c>
@@ -6278,7 +6278,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A19" s="79">
         <v>25</v>
       </c>
@@ -6312,7 +6312,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A20" s="79">
         <v>26</v>
       </c>
@@ -6365,21 +6365,21 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.83203125" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>1</v>
       </c>
@@ -6414,7 +6414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>164</v>
       </c>
@@ -6441,7 +6441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
         <v>211</v>
       </c>
@@ -6468,7 +6468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
         <v>165</v>
       </c>
@@ -6495,7 +6495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>166</v>
       </c>
@@ -6522,7 +6522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
         <v>640</v>
       </c>
@@ -6549,7 +6549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
         <v>641</v>
       </c>
@@ -6598,22 +6598,22 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" customWidth="1"/>
-    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="39" t="s">
         <v>18</v>
       </c>
@@ -6648,7 +6648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6671,7 +6671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6694,7 +6694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -6717,7 +6717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -6740,7 +6740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -6763,7 +6763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -6786,7 +6786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -6809,7 +6809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -6832,7 +6832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -6855,7 +6855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -6878,7 +6878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -6901,7 +6901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -6924,7 +6924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -6947,7 +6947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -6970,7 +6970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -6993,7 +6993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -7029,14 +7029,14 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.1640625" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="5" width="19.1640625" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="5" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="61" t="s">
         <v>18</v>
       </c>
@@ -7053,7 +7053,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7067,7 +7067,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -7081,7 +7081,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -7095,7 +7095,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -7109,7 +7109,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -7123,7 +7123,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -7137,7 +7137,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -7151,7 +7151,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -7165,7 +7165,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -7179,7 +7179,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -7203,32 +7203,32 @@
   <dimension ref="A1:P135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C94" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G125" sqref="G125"/>
+      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="72" customWidth="1"/>
-    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="43.5" customWidth="1"/>
+    <col min="11" max="11" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="43.42578125" customWidth="1"/>
     <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="19" customWidth="1"/>
-    <col min="16" max="16" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="51" t="s">
         <v>2</v>
       </c>
@@ -7278,7 +7278,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
         <v>246</v>
       </c>
@@ -7316,7 +7316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
         <v>246</v>
       </c>
@@ -7348,7 +7348,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
         <v>246</v>
       </c>
@@ -7380,7 +7380,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="100" t="s">
         <v>246</v>
       </c>
@@ -7410,7 +7410,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="47" t="s">
         <v>246</v>
       </c>
@@ -7442,7 +7442,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="47" t="s">
         <v>246</v>
       </c>
@@ -7474,7 +7474,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="47" t="s">
         <v>246</v>
       </c>
@@ -7506,7 +7506,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="47" t="s">
         <v>246</v>
       </c>
@@ -7536,7 +7536,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="47" t="s">
         <v>246</v>
       </c>
@@ -7568,7 +7568,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="47" t="s">
         <v>246</v>
       </c>
@@ -7598,7 +7598,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="47" t="s">
         <v>246</v>
       </c>
@@ -7630,7 +7630,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="47" t="s">
         <v>246</v>
       </c>
@@ -7662,7 +7662,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="48" t="s">
         <v>212</v>
       </c>
@@ -7698,7 +7698,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="48" t="s">
         <v>212</v>
       </c>
@@ -7732,7 +7732,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="48" t="s">
         <v>212</v>
       </c>
@@ -7770,7 +7770,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="48" t="s">
         <v>212</v>
       </c>
@@ -7804,7 +7804,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="102" t="s">
         <v>212</v>
       </c>
@@ -7838,7 +7838,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="48" t="s">
         <v>212</v>
       </c>
@@ -7872,7 +7872,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="48" t="s">
         <v>212</v>
       </c>
@@ -7904,7 +7904,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="48" t="s">
         <v>212</v>
       </c>
@@ -7936,7 +7936,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="48" t="s">
         <v>212</v>
       </c>
@@ -7968,7 +7968,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="112" t="s">
         <v>212</v>
       </c>
@@ -7998,7 +7998,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="48" t="s">
         <v>212</v>
       </c>
@@ -8028,7 +8028,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="48" t="s">
         <v>212</v>
       </c>
@@ -8060,7 +8060,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="48" t="s">
         <v>212</v>
       </c>
@@ -8090,7 +8090,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="48" t="s">
         <v>212</v>
       </c>
@@ -8122,7 +8122,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:16" s="114" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" s="114" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="112" t="s">
         <v>212</v>
       </c>
@@ -8139,7 +8139,7 @@
         <v>15</v>
       </c>
       <c r="F28" s="113">
-        <v>500</v>
+        <v>2000</v>
       </c>
       <c r="G28" s="113"/>
       <c r="H28" s="113"/>
@@ -8154,7 +8154,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="48" t="s">
         <v>212</v>
       </c>
@@ -8186,7 +8186,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="48" t="s">
         <v>212</v>
       </c>
@@ -8218,7 +8218,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="102" t="s">
         <v>212</v>
       </c>
@@ -8250,7 +8250,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="47" t="s">
         <v>728</v>
       </c>
@@ -8288,7 +8288,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="47" t="s">
         <v>728</v>
       </c>
@@ -8324,7 +8324,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="47" t="s">
         <v>728</v>
       </c>
@@ -8356,7 +8356,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="47" t="s">
         <v>728</v>
       </c>
@@ -8388,7 +8388,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="47" t="s">
         <v>728</v>
       </c>
@@ -8420,7 +8420,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="47" t="s">
         <v>728</v>
       </c>
@@ -8452,7 +8452,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="47" t="s">
         <v>728</v>
       </c>
@@ -8482,7 +8482,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="47" t="s">
         <v>728</v>
       </c>
@@ -8514,7 +8514,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="89" t="s">
         <v>467</v>
       </c>
@@ -8552,7 +8552,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="89" t="s">
         <v>467</v>
       </c>
@@ -8582,7 +8582,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="89" t="s">
         <v>467</v>
       </c>
@@ -8612,7 +8612,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="89" t="s">
         <v>467</v>
       </c>
@@ -8646,7 +8646,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="89" t="s">
         <v>467</v>
       </c>
@@ -8678,7 +8678,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="89" t="s">
         <v>467</v>
       </c>
@@ -8710,7 +8710,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="89" t="s">
         <v>467</v>
       </c>
@@ -8742,7 +8742,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="89" t="s">
         <v>467</v>
       </c>
@@ -8772,7 +8772,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="89" t="s">
         <v>467</v>
       </c>
@@ -8802,7 +8802,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="89" t="s">
         <v>467</v>
       </c>
@@ -8834,7 +8834,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="89" t="s">
         <v>467</v>
       </c>
@@ -8864,7 +8864,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="89" t="s">
         <v>467</v>
       </c>
@@ -8896,7 +8896,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="89" t="s">
         <v>467</v>
       </c>
@@ -8928,7 +8928,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="47" t="s">
         <v>267</v>
       </c>
@@ -8962,7 +8962,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="47" t="s">
         <v>267</v>
       </c>
@@ -9000,7 +9000,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="47" t="s">
         <v>267</v>
       </c>
@@ -9034,7 +9034,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="47" t="s">
         <v>267</v>
       </c>
@@ -9070,7 +9070,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="47" t="s">
         <v>267</v>
       </c>
@@ -9104,7 +9104,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="47" t="s">
         <v>267</v>
       </c>
@@ -9136,7 +9136,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:16" s="109" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" s="109" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="100" t="s">
         <v>267</v>
       </c>
@@ -9168,7 +9168,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="47" t="s">
         <v>267</v>
       </c>
@@ -9200,7 +9200,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="47" t="s">
         <v>267</v>
       </c>
@@ -9232,7 +9232,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="47" t="s">
         <v>267</v>
       </c>
@@ -9262,7 +9262,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="110" t="s">
         <v>267</v>
       </c>
@@ -9294,7 +9294,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="47" t="s">
         <v>267</v>
       </c>
@@ -9324,7 +9324,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="47" t="s">
         <v>267</v>
       </c>
@@ -9356,7 +9356,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="47" t="s">
         <v>267</v>
       </c>
@@ -9386,7 +9386,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="47" t="s">
         <v>267</v>
       </c>
@@ -9418,7 +9418,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="47" t="s">
         <v>267</v>
       </c>
@@ -9450,7 +9450,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="49" t="s">
         <v>266</v>
       </c>
@@ -9484,7 +9484,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="49" t="s">
         <v>266</v>
       </c>
@@ -9522,7 +9522,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="49" t="s">
         <v>266</v>
       </c>
@@ -9558,7 +9558,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="49" t="s">
         <v>266</v>
       </c>
@@ -9594,7 +9594,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="49" t="s">
         <v>266</v>
       </c>
@@ -9628,7 +9628,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="49" t="s">
         <v>266</v>
       </c>
@@ -9660,7 +9660,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="104" t="s">
         <v>266</v>
       </c>
@@ -9694,7 +9694,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="49" t="s">
         <v>266</v>
       </c>
@@ -9726,7 +9726,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="49" t="s">
         <v>266</v>
       </c>
@@ -9756,7 +9756,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="49" t="s">
         <v>266</v>
       </c>
@@ -9788,7 +9788,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="49" t="s">
         <v>266</v>
       </c>
@@ -9818,7 +9818,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="49" t="s">
         <v>266</v>
       </c>
@@ -9850,7 +9850,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="25" t="s">
         <v>701</v>
       </c>
@@ -9884,7 +9884,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="25" t="s">
         <v>701</v>
       </c>
@@ -9922,7 +9922,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="25" t="s">
         <v>701</v>
       </c>
@@ -9956,7 +9956,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="25" t="s">
         <v>701</v>
       </c>
@@ -9992,7 +9992,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="25" t="s">
         <v>701</v>
       </c>
@@ -10026,7 +10026,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="25" t="s">
         <v>701</v>
       </c>
@@ -10058,7 +10058,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="25" t="s">
         <v>701</v>
       </c>
@@ -10090,7 +10090,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="120" t="s">
         <v>701</v>
       </c>
@@ -10124,7 +10124,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:16" s="76" customFormat="1" ht="28" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:16" s="76" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A89" s="124" t="s">
         <v>701</v>
       </c>
@@ -10156,7 +10156,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="25" t="s">
         <v>701</v>
       </c>
@@ -10188,7 +10188,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="25" t="s">
         <v>701</v>
       </c>
@@ -10218,7 +10218,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="25" t="s">
         <v>701</v>
       </c>
@@ -10250,7 +10250,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="25" t="s">
         <v>701</v>
       </c>
@@ -10280,7 +10280,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="25" t="s">
         <v>701</v>
       </c>
@@ -10312,7 +10312,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="58" t="s">
         <v>706</v>
       </c>
@@ -10346,7 +10346,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="58" t="s">
         <v>706</v>
       </c>
@@ -10384,7 +10384,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="58" t="s">
         <v>706</v>
       </c>
@@ -10420,7 +10420,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="58" t="s">
         <v>706</v>
       </c>
@@ -10456,7 +10456,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="58" t="s">
         <v>706</v>
       </c>
@@ -10488,7 +10488,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="58" t="s">
         <v>706</v>
       </c>
@@ -10522,7 +10522,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="58" t="s">
         <v>706</v>
       </c>
@@ -10554,7 +10554,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="58" t="s">
         <v>706</v>
       </c>
@@ -10586,7 +10586,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="58" t="s">
         <v>706</v>
       </c>
@@ -10618,7 +10618,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="58" t="s">
         <v>701</v>
       </c>
@@ -10650,7 +10650,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="122" t="s">
         <v>706</v>
       </c>
@@ -10684,7 +10684,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="58" t="s">
         <v>706</v>
       </c>
@@ -10716,7 +10716,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="58" t="s">
         <v>706</v>
       </c>
@@ -10746,7 +10746,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="58" t="s">
         <v>706</v>
       </c>
@@ -10778,7 +10778,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="58" t="s">
         <v>706</v>
       </c>
@@ -10810,7 +10810,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="50" t="s">
         <v>209</v>
       </c>
@@ -10846,7 +10846,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="50" t="s">
         <v>209</v>
       </c>
@@ -10884,7 +10884,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="107" t="s">
         <v>209</v>
       </c>
@@ -10916,7 +10916,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="50" t="s">
         <v>209</v>
       </c>
@@ -10948,7 +10948,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="50" t="s">
         <v>209</v>
       </c>
@@ -10980,7 +10980,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="50" t="s">
         <v>209</v>
       </c>
@@ -11012,7 +11012,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="50" t="s">
         <v>209</v>
       </c>
@@ -11044,7 +11044,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="50" t="s">
         <v>209</v>
       </c>
@@ -11074,7 +11074,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="50" t="s">
         <v>209</v>
       </c>
@@ -11106,7 +11106,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="50" t="s">
         <v>209</v>
       </c>
@@ -11136,7 +11136,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="50" t="s">
         <v>209</v>
       </c>
@@ -11168,7 +11168,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="50" t="s">
         <v>209</v>
       </c>
@@ -11200,7 +11200,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="42" t="s">
         <v>168</v>
       </c>
@@ -11236,7 +11236,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="42" t="s">
         <v>168</v>
       </c>
@@ -11268,7 +11268,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="42" t="s">
         <v>168</v>
       </c>
@@ -11300,7 +11300,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="42" t="s">
         <v>168</v>
       </c>
@@ -11332,7 +11332,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="42" t="s">
         <v>168</v>
       </c>
@@ -11366,7 +11366,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="127" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="42" t="s">
         <v>168</v>
       </c>
@@ -11398,7 +11398,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="128" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="42" t="s">
         <v>168</v>
       </c>
@@ -11430,7 +11430,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="129" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="42" t="s">
         <v>168</v>
       </c>
@@ -11462,7 +11462,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="130" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="42" t="s">
         <v>168</v>
       </c>
@@ -11494,7 +11494,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="131" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="42" t="s">
         <v>168</v>
       </c>
@@ -11524,7 +11524,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="132" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="42" t="s">
         <v>168</v>
       </c>
@@ -11556,7 +11556,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="133" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="42" t="s">
         <v>168</v>
       </c>
@@ -11586,7 +11586,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="134" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="42" t="s">
         <v>168</v>
       </c>
@@ -11618,7 +11618,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="135" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="42" t="s">
         <v>168</v>
       </c>
@@ -11667,23 +11667,23 @@
       <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.5" customWidth="1"/>
-    <col min="8" max="8" width="48.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.42578125" customWidth="1"/>
+    <col min="8" max="8" width="48.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
         <v>18</v>
       </c>
@@ -11724,7 +11724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="83">
         <v>1</v>
       </c>
@@ -11757,7 +11757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>11</v>
       </c>
@@ -11786,7 +11786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>12</v>
       </c>
@@ -11815,7 +11815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>13</v>
       </c>
@@ -11844,7 +11844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>14</v>
       </c>
@@ -11873,7 +11873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>15</v>
       </c>
@@ -11902,7 +11902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="118">
         <v>111</v>
       </c>
@@ -11935,7 +11935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="118">
         <v>112</v>
       </c>
@@ -11968,7 +11968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="118">
         <v>114</v>
       </c>
@@ -12001,7 +12001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="118">
         <v>115</v>
       </c>
@@ -12034,7 +12034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="83">
         <v>2</v>
       </c>
@@ -12067,7 +12067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>21</v>
       </c>
@@ -12096,7 +12096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>22</v>
       </c>
@@ -12125,7 +12125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="83">
         <v>3</v>
       </c>
@@ -12158,7 +12158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>31</v>
       </c>
@@ -12187,7 +12187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>32</v>
       </c>
@@ -12216,7 +12216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>33</v>
       </c>
@@ -12245,7 +12245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>34</v>
       </c>
@@ -12274,7 +12274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>35</v>
       </c>
@@ -12303,7 +12303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>36</v>
       </c>
@@ -12332,7 +12332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="83">
         <v>4</v>
       </c>
@@ -12365,7 +12365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>41</v>
       </c>
@@ -12394,7 +12394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>42</v>
       </c>
@@ -12423,7 +12423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>43</v>
       </c>
@@ -12452,7 +12452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>44</v>
       </c>
@@ -12481,7 +12481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="83">
         <v>5</v>
       </c>
@@ -12514,7 +12514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>51</v>
       </c>
@@ -12543,7 +12543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>52</v>
       </c>
@@ -12572,7 +12572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>53</v>
       </c>
@@ -12601,7 +12601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>54</v>
       </c>
@@ -12630,7 +12630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>55</v>
       </c>
@@ -12659,7 +12659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>56</v>
       </c>
@@ -12688,7 +12688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="83">
         <v>6</v>
       </c>
@@ -12721,7 +12721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>61</v>
       </c>
@@ -12750,7 +12750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>62</v>
       </c>
@@ -12779,7 +12779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>63</v>
       </c>
@@ -12808,7 +12808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>64</v>
       </c>
@@ -12837,7 +12837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>65</v>
       </c>
@@ -12866,7 +12866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="83">
         <v>7</v>
       </c>
@@ -12899,7 +12899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>71</v>
       </c>
@@ -12928,7 +12928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>72</v>
       </c>
@@ -12957,7 +12957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>73</v>
       </c>
@@ -12986,7 +12986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>74</v>
       </c>
@@ -13015,7 +13015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="83">
         <v>8</v>
       </c>
@@ -13048,7 +13048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="18">
         <v>81</v>
       </c>
@@ -13079,7 +13079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="18">
         <v>82</v>
       </c>
@@ -13110,7 +13110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="18">
         <v>83</v>
       </c>
@@ -13141,7 +13141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="18">
         <v>84</v>
       </c>
@@ -13172,7 +13172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="83">
         <v>9</v>
       </c>
@@ -13205,7 +13205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="18">
         <v>90</v>
       </c>
@@ -13240,7 +13240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="18">
         <v>91</v>
       </c>
@@ -13275,7 +13275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="18">
         <v>92</v>
       </c>
@@ -13310,7 +13310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="18">
         <v>93</v>
       </c>
@@ -13362,16 +13362,16 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" customWidth="1"/>
-    <col min="5" max="12" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="5" max="12" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>18</v>
       </c>
@@ -13409,7 +13409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -13445,18 +13445,18 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.6640625" customWidth="1"/>
-    <col min="6" max="6" width="21.5" customWidth="1"/>
-    <col min="7" max="7" width="24.5" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="60" t="s">
         <v>18</v>
       </c>
@@ -13508,22 +13508,22 @@
       <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.1640625" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" customWidth="1"/>
-    <col min="7" max="7" width="18.5" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="26.5" customWidth="1"/>
-    <col min="10" max="10" width="22.83203125" customWidth="1"/>
-    <col min="11" max="12" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.42578125" customWidth="1"/>
+    <col min="10" max="10" width="22.85546875" customWidth="1"/>
+    <col min="11" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="61" t="s">
         <v>18</v>
       </c>
@@ -13578,27 +13578,27 @@
       <selection pane="bottomRight" activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="85.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" style="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" style="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.6640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.1640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.83203125" style="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.6640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.5" style="17" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="85.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" style="17" customWidth="1"/>
     <col min="16" max="16" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -13648,7 +13648,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
@@ -13684,7 +13684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>39</v>
       </c>
@@ -13712,7 +13712,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>39</v>
       </c>
@@ -13742,7 +13742,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>39</v>
       </c>
@@ -13772,7 +13772,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>39</v>
       </c>
@@ -13806,7 +13806,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>39</v>
       </c>
@@ -13834,7 +13834,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>39</v>
       </c>
@@ -13862,7 +13862,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>39</v>
       </c>
@@ -13890,7 +13890,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>39</v>
       </c>
@@ -13918,7 +13918,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>39</v>
       </c>
@@ -13948,7 +13948,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>39</v>
       </c>
@@ -13976,7 +13976,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>39</v>
       </c>
@@ -14006,7 +14006,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>39</v>
       </c>
@@ -14034,7 +14034,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>39</v>
       </c>
@@ -14062,7 +14062,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="72" t="s">
         <v>38</v>
       </c>
@@ -14098,7 +14098,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="72" t="s">
         <v>38</v>
       </c>
@@ -14128,7 +14128,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="72" t="s">
         <v>38</v>
       </c>
@@ -14156,7 +14156,7 @@
       <c r="O18" s="73"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="72" t="s">
         <v>38</v>
       </c>
@@ -14186,7 +14186,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="72" t="s">
         <v>38</v>
       </c>
@@ -14214,7 +14214,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="72" t="s">
         <v>38</v>
       </c>
@@ -14242,7 +14242,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="72" t="s">
         <v>38</v>
       </c>
@@ -14272,7 +14272,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="72" t="s">
         <v>38</v>
       </c>
@@ -14302,7 +14302,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>46</v>
       </c>
@@ -14338,7 +14338,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>46</v>
       </c>
@@ -14366,7 +14366,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>46</v>
       </c>
@@ -14396,7 +14396,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>46</v>
       </c>
@@ -14426,7 +14426,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>46</v>
       </c>
@@ -14456,7 +14456,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>46</v>
       </c>
@@ -14486,7 +14486,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>46</v>
       </c>
@@ -14516,7 +14516,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>46</v>
       </c>
@@ -14546,7 +14546,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>46</v>
       </c>
@@ -14574,7 +14574,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>46</v>
       </c>
@@ -14604,7 +14604,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>46</v>
       </c>
@@ -14634,7 +14634,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="72" t="s">
         <v>143</v>
       </c>
@@ -14668,7 +14668,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="72" t="s">
         <v>143</v>
       </c>
@@ -14696,7 +14696,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="72" t="s">
         <v>143</v>
       </c>
@@ -14726,7 +14726,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="72" t="s">
         <v>143</v>
       </c>
@@ -14756,7 +14756,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="72" t="s">
         <v>143</v>
       </c>
@@ -14786,7 +14786,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="72" t="s">
         <v>143</v>
       </c>
@@ -14816,7 +14816,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="72" t="s">
         <v>143</v>
       </c>
@@ -14846,7 +14846,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="72" t="s">
         <v>143</v>
       </c>
@@ -14876,7 +14876,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="72" t="s">
         <v>143</v>
       </c>
@@ -14906,7 +14906,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="72" t="s">
         <v>143</v>
       </c>
@@ -14936,7 +14936,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="72" t="s">
         <v>143</v>
       </c>
@@ -14964,7 +14964,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="72" t="s">
         <v>143</v>
       </c>
@@ -14992,7 +14992,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="72" t="s">
         <v>143</v>
       </c>
@@ -15022,7 +15022,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="72" t="s">
         <v>143</v>
       </c>
@@ -15048,7 +15048,7 @@
       <c r="O48" s="73"/>
       <c r="P48" s="1"/>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="72" t="s">
         <v>143</v>
       </c>
@@ -15076,7 +15076,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="72" t="s">
         <v>143</v>
       </c>
@@ -15106,7 +15106,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="40" t="s">
         <v>179</v>
       </c>
@@ -15143,7 +15143,7 @@
       </c>
       <c r="Q51" s="54"/>
     </row>
-    <row r="52" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="40" t="s">
         <v>179</v>
       </c>
@@ -15174,7 +15174,7 @@
       </c>
       <c r="Q52" s="54"/>
     </row>
-    <row r="53" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="40" t="s">
         <v>179</v>
       </c>
@@ -15205,7 +15205,7 @@
       </c>
       <c r="Q53" s="54"/>
     </row>
-    <row r="54" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="40" t="s">
         <v>179</v>
       </c>
@@ -15236,7 +15236,7 @@
       </c>
       <c r="Q54" s="54"/>
     </row>
-    <row r="55" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="40" t="s">
         <v>179</v>
       </c>
@@ -15265,7 +15265,7 @@
       </c>
       <c r="Q55" s="54"/>
     </row>
-    <row r="56" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="40" t="s">
         <v>179</v>
       </c>
@@ -15296,7 +15296,7 @@
       </c>
       <c r="Q56" s="54"/>
     </row>
-    <row r="57" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="40" t="s">
         <v>179</v>
       </c>
@@ -15327,7 +15327,7 @@
       </c>
       <c r="Q57" s="54"/>
     </row>
-    <row r="58" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="40" t="s">
         <v>179</v>
       </c>
@@ -15356,7 +15356,7 @@
       </c>
       <c r="Q58" s="54"/>
     </row>
-    <row r="59" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="40" t="s">
         <v>179</v>
       </c>
@@ -15385,7 +15385,7 @@
       </c>
       <c r="Q59" s="54"/>
     </row>
-    <row r="60" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="40" t="s">
         <v>179</v>
       </c>
@@ -15416,7 +15416,7 @@
       </c>
       <c r="Q60" s="54"/>
     </row>
-    <row r="61" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="40" t="s">
         <v>179</v>
       </c>
@@ -15447,7 +15447,7 @@
       </c>
       <c r="Q61" s="54"/>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="62" t="s">
         <v>319</v>
       </c>
@@ -15483,7 +15483,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="62" t="s">
         <v>319</v>
       </c>
@@ -15519,7 +15519,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="62" t="s">
         <v>319</v>
       </c>
@@ -15549,7 +15549,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="62" t="s">
         <v>319</v>
       </c>
@@ -15577,7 +15577,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="62" t="s">
         <v>319</v>
       </c>
@@ -15632,25 +15632,25 @@
       <selection pane="bottomRight" activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.5" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
     <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" customWidth="1"/>
-    <col min="7" max="7" width="13.5" customWidth="1"/>
-    <col min="8" max="8" width="9.83203125" customWidth="1"/>
-    <col min="9" max="9" width="12.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="57" customWidth="1"/>
-    <col min="11" max="11" width="54.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="35.6640625" style="5" customWidth="1"/>
-    <col min="14" max="14" width="51.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="54.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.7109375" style="5" customWidth="1"/>
+    <col min="14" max="14" width="51.140625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>18</v>
       </c>
@@ -15694,7 +15694,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25">
         <v>1</v>
       </c>
@@ -15732,7 +15732,7 @@
       <c r="M2" s="25"/>
       <c r="N2" s="26"/>
     </row>
-    <row r="3" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="25">
         <v>2</v>
       </c>
@@ -15770,7 +15770,7 @@
       <c r="M3" s="25"/>
       <c r="N3" s="26"/>
     </row>
-    <row r="4" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25">
         <v>3</v>
       </c>
@@ -15808,7 +15808,7 @@
       <c r="M4" s="25"/>
       <c r="N4" s="26"/>
     </row>
-    <row r="5" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25">
         <v>4</v>
       </c>
@@ -15846,7 +15846,7 @@
       <c r="M5" s="25"/>
       <c r="N5" s="26"/>
     </row>
-    <row r="6" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25">
         <v>5</v>
       </c>
@@ -15884,7 +15884,7 @@
       <c r="M6" s="25"/>
       <c r="N6" s="26"/>
     </row>
-    <row r="7" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="25">
         <v>6</v>
       </c>
@@ -15922,7 +15922,7 @@
       <c r="M7" s="25"/>
       <c r="N7" s="26"/>
     </row>
-    <row r="8" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="25">
         <v>7</v>
       </c>
@@ -15960,7 +15960,7 @@
       <c r="M8" s="25"/>
       <c r="N8" s="26"/>
     </row>
-    <row r="9" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25">
         <v>8</v>
       </c>
@@ -15998,7 +15998,7 @@
       <c r="M9" s="25"/>
       <c r="N9" s="26"/>
     </row>
-    <row r="10" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="25">
         <v>9</v>
       </c>
@@ -16036,7 +16036,7 @@
       <c r="M10" s="25"/>
       <c r="N10" s="26"/>
     </row>
-    <row r="11" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="25">
         <v>10</v>
       </c>
@@ -16074,7 +16074,7 @@
       <c r="M11" s="25"/>
       <c r="N11" s="26"/>
     </row>
-    <row r="12" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="25">
         <v>11</v>
       </c>
@@ -16112,7 +16112,7 @@
       <c r="M12" s="25"/>
       <c r="N12" s="26"/>
     </row>
-    <row r="13" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="25">
         <v>12</v>
       </c>
@@ -16150,7 +16150,7 @@
       <c r="M13" s="25"/>
       <c r="N13" s="26"/>
     </row>
-    <row r="14" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="25">
         <v>13</v>
       </c>
@@ -16188,7 +16188,7 @@
       <c r="M14" s="25"/>
       <c r="N14" s="26"/>
     </row>
-    <row r="15" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="25">
         <v>14</v>
       </c>
@@ -16226,7 +16226,7 @@
       <c r="M15" s="25"/>
       <c r="N15" s="26"/>
     </row>
-    <row r="16" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="25">
         <v>15</v>
       </c>
@@ -16264,7 +16264,7 @@
       <c r="M16" s="25"/>
       <c r="N16" s="26"/>
     </row>
-    <row r="17" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="25">
         <v>16</v>
       </c>
@@ -16302,7 +16302,7 @@
       <c r="M17" s="25"/>
       <c r="N17" s="26"/>
     </row>
-    <row r="18" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="25">
         <v>50</v>
       </c>
@@ -16340,7 +16340,7 @@
       <c r="M18" s="25"/>
       <c r="N18" s="26"/>
     </row>
-    <row r="19" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="62">
         <v>51</v>
       </c>
@@ -16374,7 +16374,7 @@
       <c r="M19" s="65"/>
       <c r="N19" s="67"/>
     </row>
-    <row r="20" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="25">
         <v>52</v>
       </c>
@@ -16408,7 +16408,7 @@
       <c r="M20" s="65"/>
       <c r="N20" s="67"/>
     </row>
-    <row r="21" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="62">
         <v>53</v>
       </c>
@@ -16442,7 +16442,7 @@
       <c r="M21" s="65"/>
       <c r="N21" s="67"/>
     </row>
-    <row r="22" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="25">
         <v>54</v>
       </c>
@@ -16476,7 +16476,7 @@
       <c r="M22" s="65"/>
       <c r="N22" s="67"/>
     </row>
-    <row r="23" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="62">
         <v>55</v>
       </c>
@@ -16510,7 +16510,7 @@
       <c r="M23" s="65"/>
       <c r="N23" s="67"/>
     </row>
-    <row r="24" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="25">
         <v>56</v>
       </c>
@@ -16544,7 +16544,7 @@
       <c r="M24" s="65"/>
       <c r="N24" s="67"/>
     </row>
-    <row r="25" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="62">
         <v>57</v>
       </c>
@@ -16578,7 +16578,7 @@
       <c r="M25" s="65"/>
       <c r="N25" s="67"/>
     </row>
-    <row r="26" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="25">
         <v>58</v>
       </c>
@@ -16612,7 +16612,7 @@
       <c r="M26" s="65"/>
       <c r="N26" s="67"/>
     </row>
-    <row r="27" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="62">
         <v>59</v>
       </c>
@@ -16646,7 +16646,7 @@
       <c r="M27" s="65"/>
       <c r="N27" s="67"/>
     </row>
-    <row r="28" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="25">
         <v>60</v>
       </c>
@@ -16680,7 +16680,7 @@
       <c r="M28" s="65"/>
       <c r="N28" s="67"/>
     </row>
-    <row r="29" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="62">
         <v>61</v>
       </c>
@@ -16714,7 +16714,7 @@
       <c r="M29" s="65"/>
       <c r="N29" s="67"/>
     </row>
-    <row r="30" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="25">
         <v>62</v>
       </c>
@@ -16748,7 +16748,7 @@
       <c r="M30" s="65"/>
       <c r="N30" s="67"/>
     </row>
-    <row r="31" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="62">
         <v>63</v>
       </c>
@@ -16782,7 +16782,7 @@
       <c r="M31" s="65"/>
       <c r="N31" s="67"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="33">
         <v>101</v>
       </c>
@@ -16815,7 +16815,7 @@
       </c>
       <c r="M32" s="35"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="33">
         <v>102</v>
       </c>
@@ -16848,7 +16848,7 @@
       </c>
       <c r="M33" s="35"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="33">
         <v>103</v>
       </c>
@@ -16881,7 +16881,7 @@
       </c>
       <c r="M34" s="35"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="33">
         <v>104</v>
       </c>
@@ -16914,7 +16914,7 @@
       </c>
       <c r="M35" s="35"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="33">
         <v>105</v>
       </c>
@@ -16949,7 +16949,7 @@
       </c>
       <c r="M36" s="35"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="33">
         <v>106</v>
       </c>
@@ -16982,7 +16982,7 @@
       </c>
       <c r="M37" s="35"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="33">
         <v>107</v>
       </c>
@@ -17015,7 +17015,7 @@
       </c>
       <c r="M38" s="35"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="33">
         <v>108</v>
       </c>
@@ -17048,7 +17048,7 @@
       </c>
       <c r="M39" s="35"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="33">
         <v>109</v>
       </c>
@@ -17083,7 +17083,7 @@
       </c>
       <c r="M40" s="35"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="33">
         <v>110</v>
       </c>
@@ -17116,7 +17116,7 @@
       </c>
       <c r="M41" s="35"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="33">
         <v>111</v>
       </c>
@@ -17149,7 +17149,7 @@
       </c>
       <c r="M42" s="35"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="33">
         <v>112</v>
       </c>
@@ -17182,7 +17182,7 @@
       </c>
       <c r="M43" s="35"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="33">
         <v>113</v>
       </c>
@@ -17215,7 +17215,7 @@
       </c>
       <c r="M44" s="35"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="33">
         <v>114</v>
       </c>
@@ -17248,7 +17248,7 @@
       </c>
       <c r="M45" s="3"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="33">
         <v>115</v>
       </c>
@@ -17281,7 +17281,7 @@
       </c>
       <c r="M46" s="3"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="33">
         <v>116</v>
       </c>
@@ -17314,7 +17314,7 @@
       </c>
       <c r="M47" s="3"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="33">
         <v>117</v>
       </c>
@@ -17347,7 +17347,7 @@
       </c>
       <c r="M48" s="3"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="33">
         <v>118</v>
       </c>
@@ -17380,7 +17380,7 @@
       </c>
       <c r="M49" s="3"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="96">
         <v>119</v>
       </c>
@@ -17413,7 +17413,7 @@
       </c>
       <c r="M50" s="98"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="96">
         <v>120</v>
       </c>
@@ -17446,7 +17446,7 @@
       </c>
       <c r="M51" s="98"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="91">
         <v>121</v>
       </c>
@@ -17479,7 +17479,7 @@
       </c>
       <c r="M52" s="93"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="91">
         <v>122</v>
       </c>
@@ -17512,7 +17512,7 @@
       </c>
       <c r="M53" s="93"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="91">
         <v>123</v>
       </c>
@@ -17545,7 +17545,7 @@
       </c>
       <c r="M54" s="93"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="91">
         <v>124</v>
       </c>
@@ -17578,7 +17578,7 @@
       </c>
       <c r="M55" s="93"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="91">
         <v>125</v>
       </c>
@@ -17611,7 +17611,7 @@
       </c>
       <c r="M56" s="93"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="91">
         <v>126</v>
       </c>
@@ -17644,7 +17644,7 @@
       </c>
       <c r="M57" s="93"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="91">
         <v>127</v>
       </c>
@@ -17677,7 +17677,7 @@
       </c>
       <c r="M58" s="93"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="91">
         <v>128</v>
       </c>
@@ -17710,7 +17710,7 @@
       </c>
       <c r="M59" s="93"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="91">
         <v>129</v>
       </c>
@@ -17743,7 +17743,7 @@
       </c>
       <c r="M60" s="93"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="91">
         <v>130</v>
       </c>
@@ -17776,7 +17776,7 @@
       </c>
       <c r="M61" s="93"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="91">
         <v>131</v>
       </c>
@@ -17809,7 +17809,7 @@
       </c>
       <c r="M62" s="93"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="91">
         <v>132</v>
       </c>
@@ -17842,7 +17842,7 @@
       </c>
       <c r="M63" s="93"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="91">
         <v>133</v>
       </c>
@@ -17875,7 +17875,7 @@
       </c>
       <c r="M64" s="93"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="91">
         <v>134</v>
       </c>
@@ -17906,7 +17906,7 @@
       </c>
       <c r="M65" s="93"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="91">
         <v>135</v>
       </c>
@@ -17937,7 +17937,7 @@
       </c>
       <c r="M66" s="93"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="91">
         <v>136</v>
       </c>
@@ -17968,7 +17968,7 @@
       </c>
       <c r="M67" s="93"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="91">
         <v>137</v>
       </c>
@@ -17999,7 +17999,7 @@
       </c>
       <c r="M68" s="93"/>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="91">
         <v>138</v>
       </c>
@@ -18030,7 +18030,7 @@
       </c>
       <c r="M69" s="93"/>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="91">
         <v>139</v>
       </c>
@@ -18061,7 +18061,7 @@
       </c>
       <c r="M70" s="93"/>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="91">
         <v>140</v>
       </c>
@@ -18115,17 +18115,17 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.33203125" customWidth="1"/>
-    <col min="3" max="3" width="40.1640625" customWidth="1"/>
+    <col min="2" max="2" width="48.28515625" customWidth="1"/>
+    <col min="3" max="3" width="40.140625" customWidth="1"/>
     <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="103" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>18</v>
       </c>
@@ -18145,7 +18145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="86">
         <v>99</v>
       </c>
@@ -18165,7 +18165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="84">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
add update DO and update DA as well
</commit_message>
<xml_diff>
--- a/db/excel/api-function-granted-users-cdld.xlsx
+++ b/db/excel/api-function-granted-users-cdld.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE0E7D7C-463C-42B9-BC13-6A3D42C8507E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC4207C-4E0D-4D4E-AD59-34F9C120D539}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_types" sheetId="27" r:id="rId1"/>
@@ -300,7 +300,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2029" uniqueCount="768">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2029" uniqueCount="767">
   <si>
     <t>status</t>
   </si>
@@ -2283,9 +2283,6 @@
   </si>
   <si>
     <t>UPDATE_CRIT</t>
-  </si>
-  <si>
-    <t>Đánh giá hoàn thành thực hiện</t>
   </si>
   <si>
     <t>ASS_TYPE</t>
@@ -5674,7 +5671,7 @@
         <v>4</v>
       </c>
       <c r="I1" s="77" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="J1" s="77" t="s">
         <v>158</v>
@@ -5689,10 +5686,10 @@
         <v>0</v>
       </c>
       <c r="N1" s="77" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="115">
         <v>1</v>
       </c>
@@ -5726,7 +5723,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="115">
         <v>3</v>
       </c>
@@ -5735,7 +5732,7 @@
         <v>343</v>
       </c>
       <c r="D3" s="115" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="E3" s="116" t="s">
         <v>343</v>
@@ -5762,7 +5759,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="79">
         <v>31</v>
       </c>
@@ -5770,18 +5767,18 @@
         <v>3</v>
       </c>
       <c r="C4" s="79" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="D4" s="79"/>
       <c r="E4" s="80" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="F4" s="80"/>
       <c r="G4" s="80" t="s">
+        <v>744</v>
+      </c>
+      <c r="H4" s="79" t="s">
         <v>745</v>
-      </c>
-      <c r="H4" s="79" t="s">
-        <v>746</v>
       </c>
       <c r="I4" s="79"/>
       <c r="J4" s="79"/>
@@ -5796,7 +5793,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="79">
         <v>32</v>
       </c>
@@ -5804,18 +5801,18 @@
         <v>3</v>
       </c>
       <c r="C5" s="79" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="D5" s="79"/>
       <c r="E5" s="80" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="F5" s="80"/>
       <c r="G5" s="80" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="H5" s="79" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="I5" s="79"/>
       <c r="J5" s="79"/>
@@ -5830,7 +5827,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="79">
         <v>33</v>
       </c>
@@ -5864,28 +5861,28 @@
         <v>203</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="115">
         <v>4</v>
       </c>
       <c r="B7" s="115"/>
       <c r="C7" s="115" t="s">
+        <v>667</v>
+      </c>
+      <c r="D7" s="115" t="s">
+        <v>682</v>
+      </c>
+      <c r="E7" s="116" t="s">
+        <v>667</v>
+      </c>
+      <c r="F7" s="116" t="s">
+        <v>679</v>
+      </c>
+      <c r="G7" s="116" t="s">
         <v>668</v>
       </c>
-      <c r="D7" s="115" t="s">
-        <v>683</v>
-      </c>
-      <c r="E7" s="116" t="s">
-        <v>668</v>
-      </c>
-      <c r="F7" s="116" t="s">
-        <v>680</v>
-      </c>
-      <c r="G7" s="116" t="s">
-        <v>669</v>
-      </c>
       <c r="H7" s="115" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="I7" s="115"/>
       <c r="J7" s="115"/>
@@ -5900,7 +5897,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="79">
         <v>41</v>
       </c>
@@ -5934,7 +5931,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="79">
         <v>42</v>
       </c>
@@ -5968,7 +5965,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="79">
         <v>43</v>
       </c>
@@ -5976,18 +5973,18 @@
         <v>4</v>
       </c>
       <c r="C10" s="79" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="D10" s="79"/>
       <c r="E10" s="80" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="F10" s="80"/>
       <c r="G10" s="80" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="H10" s="79" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="I10" s="79"/>
       <c r="J10" s="81"/>
@@ -6002,7 +5999,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="115">
         <v>5</v>
       </c>
@@ -6011,7 +6008,7 @@
         <v>388</v>
       </c>
       <c r="D11" s="115" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="E11" s="116" t="s">
         <v>388</v>
@@ -6038,7 +6035,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="79">
         <v>51</v>
       </c>
@@ -6046,18 +6043,18 @@
         <v>5</v>
       </c>
       <c r="C12" s="79" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="D12" s="79"/>
       <c r="E12" s="80" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="F12" s="80"/>
       <c r="G12" s="80" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H12" s="79" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="I12" s="79"/>
       <c r="J12" s="81"/>
@@ -6072,7 +6069,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="79">
         <v>52</v>
       </c>
@@ -6106,7 +6103,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="115">
         <v>2</v>
       </c>
@@ -6115,7 +6112,7 @@
         <v>331</v>
       </c>
       <c r="D14" s="115" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="E14" s="116" t="s">
         <v>331</v>
@@ -6124,7 +6121,7 @@
         <v>335</v>
       </c>
       <c r="G14" s="116" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="H14" s="115" t="s">
         <v>402</v>
@@ -6142,7 +6139,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="79">
         <v>21</v>
       </c>
@@ -6158,7 +6155,7 @@
       </c>
       <c r="F15" s="80"/>
       <c r="G15" s="80" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="H15" s="79" t="s">
         <v>336</v>
@@ -6176,7 +6173,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="79">
         <v>22</v>
       </c>
@@ -6192,7 +6189,7 @@
       </c>
       <c r="F16" s="80"/>
       <c r="G16" s="80" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="H16" s="79" t="s">
         <v>337</v>
@@ -6210,7 +6207,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="79">
         <v>23</v>
       </c>
@@ -6226,7 +6223,7 @@
       </c>
       <c r="F17" s="80"/>
       <c r="G17" s="80" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="H17" s="79" t="s">
         <v>338</v>
@@ -6244,7 +6241,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="79">
         <v>24</v>
       </c>
@@ -6278,7 +6275,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="79">
         <v>25</v>
       </c>
@@ -6312,7 +6309,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="79">
         <v>26</v>
       </c>
@@ -6324,11 +6321,11 @@
       </c>
       <c r="D20" s="79"/>
       <c r="E20" s="80" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="F20" s="80"/>
       <c r="G20" s="80" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="H20" s="79" t="s">
         <v>346</v>
@@ -6425,10 +6422,10 @@
         <v>109</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="F2" s="29"/>
       <c r="G2" s="29"/>
@@ -6452,10 +6449,10 @@
         <v>109</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="F3" s="29"/>
       <c r="G3" s="29"/>
@@ -6479,10 +6476,10 @@
         <v>109</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="F4" s="28"/>
       <c r="G4" s="28"/>
@@ -6506,10 +6503,10 @@
         <v>109</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="F5" s="28"/>
       <c r="G5" s="28"/>
@@ -6524,7 +6521,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B6" s="28">
         <v>5</v>
@@ -6533,10 +6530,10 @@
         <v>109</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="F6" s="28"/>
       <c r="G6" s="28"/>
@@ -6551,7 +6548,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B7" s="28">
         <v>3</v>
@@ -6560,10 +6557,10 @@
         <v>109</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
@@ -6722,7 +6719,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C5" t="s">
         <v>536</v>
@@ -6745,7 +6742,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C6" t="s">
         <v>540</v>
@@ -6768,7 +6765,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="C7" t="s">
         <v>539</v>
@@ -6791,7 +6788,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="C8" t="s">
         <v>541</v>
@@ -6814,7 +6811,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C9" t="s">
         <v>542</v>
@@ -7202,16 +7199,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P135"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C74" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
+      <selection pane="bottomRight" activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="72" customWidth="1"/>
@@ -7973,7 +7970,7 @@
         <v>212</v>
       </c>
       <c r="B23" s="112" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="C23" s="112" t="s">
         <v>415</v>
@@ -8127,13 +8124,13 @@
         <v>212</v>
       </c>
       <c r="B28" s="112" t="s">
+        <v>660</v>
+      </c>
+      <c r="C28" s="112" t="s">
         <v>661</v>
       </c>
-      <c r="C28" s="112" t="s">
-        <v>662</v>
-      </c>
       <c r="D28" s="112" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="E28" s="112" t="s">
         <v>15</v>
@@ -8229,7 +8226,7 @@
         <v>227</v>
       </c>
       <c r="D31" s="102" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="E31" s="102" t="s">
         <v>16</v>
@@ -8252,7 +8249,7 @@
     </row>
     <row r="32" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="47" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B32" s="47" t="s">
         <v>305</v>
@@ -8290,16 +8287,16 @@
     </row>
     <row r="33" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="47" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B33" s="47" t="s">
         <v>513</v>
       </c>
       <c r="C33" s="47" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="D33" s="47" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E33" s="47" t="s">
         <v>15</v>
@@ -8326,16 +8323,16 @@
     </row>
     <row r="34" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="47" t="s">
+        <v>727</v>
+      </c>
+      <c r="B34" s="47" t="s">
         <v>728</v>
       </c>
-      <c r="B34" s="47" t="s">
-        <v>729</v>
-      </c>
       <c r="C34" s="47" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="D34" s="47" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="E34" s="47" t="s">
         <v>15</v>
@@ -8358,16 +8355,16 @@
     </row>
     <row r="35" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="47" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B35" s="47" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C35" s="47" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="D35" s="47" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E35" s="47" t="s">
         <v>15</v>
@@ -8390,16 +8387,16 @@
     </row>
     <row r="36" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="47" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B36" s="47" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C36" s="47" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D36" s="47" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E36" s="47" t="s">
         <v>15</v>
@@ -8422,16 +8419,16 @@
     </row>
     <row r="37" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="47" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B37" s="47" t="s">
         <v>45</v>
       </c>
       <c r="C37" s="47" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="D37" s="47" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E37" s="47" t="s">
         <v>15</v>
@@ -8454,16 +8451,16 @@
     </row>
     <row r="38" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="47" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B38" s="47" t="s">
         <v>19</v>
       </c>
       <c r="C38" s="47" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="D38" s="47" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E38" s="47" t="s">
         <v>50</v>
@@ -8484,16 +8481,16 @@
     </row>
     <row r="39" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="47" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B39" s="47" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C39" s="47" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="D39" s="47" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E39" s="47" t="s">
         <v>15</v>
@@ -9147,7 +9144,7 @@
         <v>265</v>
       </c>
       <c r="D59" s="100" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="E59" s="100" t="s">
         <v>16</v>
@@ -9237,7 +9234,7 @@
         <v>267</v>
       </c>
       <c r="B62" s="47" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="C62" s="47" t="s">
         <v>415</v>
@@ -9563,7 +9560,7 @@
         <v>266</v>
       </c>
       <c r="B72" s="49" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C72" s="49" t="s">
         <v>570</v>
@@ -9633,13 +9630,13 @@
         <v>266</v>
       </c>
       <c r="B74" s="49" t="s">
+        <v>718</v>
+      </c>
+      <c r="C74" s="49" t="s">
         <v>719</v>
       </c>
-      <c r="C74" s="49" t="s">
+      <c r="D74" s="49" t="s">
         <v>720</v>
-      </c>
-      <c r="D74" s="49" t="s">
-        <v>721</v>
       </c>
       <c r="E74" s="49" t="s">
         <v>16</v>
@@ -9793,13 +9790,13 @@
         <v>266</v>
       </c>
       <c r="B79" s="49" t="s">
+        <v>723</v>
+      </c>
+      <c r="C79" s="49" t="s">
         <v>724</v>
       </c>
-      <c r="C79" s="49" t="s">
-        <v>725</v>
-      </c>
       <c r="D79" s="49" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="E79" s="49" t="s">
         <v>17</v>
@@ -9829,7 +9826,7 @@
         <v>420</v>
       </c>
       <c r="D80" s="49" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="E80" s="49" t="s">
         <v>17</v>
@@ -9852,7 +9849,7 @@
     </row>
     <row r="81" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="25" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B81" s="25" t="s">
         <v>18</v>
@@ -9886,7 +9883,7 @@
     </row>
     <row r="82" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="25" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B82" s="25" t="s">
         <v>305</v>
@@ -9924,7 +9921,7 @@
     </row>
     <row r="83" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="25" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B83" s="47" t="s">
         <v>609</v>
@@ -9958,7 +9955,7 @@
     </row>
     <row r="84" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="25" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B84" s="25" t="s">
         <v>513</v>
@@ -9994,13 +9991,13 @@
     </row>
     <row r="85" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="25" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B85" s="25" t="s">
         <v>182</v>
       </c>
       <c r="C85" s="25" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D85" s="25" t="s">
         <v>281</v>
@@ -10028,13 +10025,13 @@
     </row>
     <row r="86" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="25" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B86" s="25" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="C86" s="25" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D86" s="25" t="s">
         <v>282</v>
@@ -10060,7 +10057,7 @@
     </row>
     <row r="87" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="25" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B87" s="25" t="s">
         <v>4</v>
@@ -10092,7 +10089,7 @@
     </row>
     <row r="88" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="120" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B88" s="100" t="s">
         <v>561</v>
@@ -10101,7 +10098,7 @@
         <v>265</v>
       </c>
       <c r="D88" s="100" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="E88" s="120" t="s">
         <v>16</v>
@@ -10126,16 +10123,16 @@
     </row>
     <row r="89" spans="1:16" s="76" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A89" s="124" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B89" s="125" t="s">
+        <v>715</v>
+      </c>
+      <c r="C89" s="125" t="s">
         <v>716</v>
       </c>
-      <c r="C89" s="125" t="s">
+      <c r="D89" s="126" t="s">
         <v>717</v>
-      </c>
-      <c r="D89" s="126" t="s">
-        <v>718</v>
       </c>
       <c r="E89" s="127" t="s">
         <v>15</v>
@@ -10158,7 +10155,7 @@
     </row>
     <row r="90" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="25" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B90" s="25" t="s">
         <v>209</v>
@@ -10190,7 +10187,7 @@
     </row>
     <row r="91" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="25" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B91" s="25" t="s">
         <v>197</v>
@@ -10220,7 +10217,7 @@
     </row>
     <row r="92" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="25" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B92" s="25" t="s">
         <v>222</v>
@@ -10252,16 +10249,16 @@
     </row>
     <row r="93" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="25" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B93" s="25" t="s">
+        <v>723</v>
+      </c>
+      <c r="C93" s="25" t="s">
         <v>724</v>
       </c>
-      <c r="C93" s="25" t="s">
-        <v>725</v>
-      </c>
       <c r="D93" s="25" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="E93" s="25" t="s">
         <v>17</v>
@@ -10282,7 +10279,7 @@
     </row>
     <row r="94" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="25" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B94" s="25" t="s">
         <v>0</v>
@@ -10314,7 +10311,7 @@
     </row>
     <row r="95" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="58" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B95" s="58" t="s">
         <v>18</v>
@@ -10348,7 +10345,7 @@
     </row>
     <row r="96" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="58" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B96" s="58" t="s">
         <v>305</v>
@@ -10386,7 +10383,7 @@
     </row>
     <row r="97" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="58" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B97" s="58" t="s">
         <v>513</v>
@@ -10422,10 +10419,10 @@
     </row>
     <row r="98" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="58" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B98" s="58" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C98" s="58" t="s">
         <v>570</v>
@@ -10458,16 +10455,16 @@
     </row>
     <row r="99" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="58" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B99" s="58" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="C99" s="58" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="D99" s="58" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E99" s="58" t="s">
         <v>15</v>
@@ -10490,13 +10487,13 @@
     </row>
     <row r="100" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="58" t="s">
+        <v>705</v>
+      </c>
+      <c r="B100" s="58" t="s">
+        <v>708</v>
+      </c>
+      <c r="C100" s="58" t="s">
         <v>706</v>
-      </c>
-      <c r="B100" s="58" t="s">
-        <v>709</v>
-      </c>
-      <c r="C100" s="58" t="s">
-        <v>707</v>
       </c>
       <c r="D100" s="58" t="s">
         <v>281</v>
@@ -10524,13 +10521,13 @@
     </row>
     <row r="101" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="58" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B101" s="58" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="C101" s="58" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D101" s="58" t="s">
         <v>282</v>
@@ -10556,16 +10553,16 @@
     </row>
     <row r="102" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="58" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B102" s="58" t="s">
+        <v>710</v>
+      </c>
+      <c r="C102" s="58" t="s">
+        <v>703</v>
+      </c>
+      <c r="D102" s="58" t="s">
         <v>711</v>
-      </c>
-      <c r="C102" s="58" t="s">
-        <v>704</v>
-      </c>
-      <c r="D102" s="58" t="s">
-        <v>712</v>
       </c>
       <c r="E102" s="58" t="s">
         <v>16</v>
@@ -10588,16 +10585,16 @@
     </row>
     <row r="103" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="58" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B103" s="58" t="s">
         <v>4</v>
       </c>
       <c r="C103" s="58" t="s">
+        <v>712</v>
+      </c>
+      <c r="D103" s="58" t="s">
         <v>713</v>
-      </c>
-      <c r="D103" s="58" t="s">
-        <v>714</v>
       </c>
       <c r="E103" s="58" t="s">
         <v>15</v>
@@ -10620,16 +10617,16 @@
     </row>
     <row r="104" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="58" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B104" s="58" t="s">
+        <v>718</v>
+      </c>
+      <c r="C104" s="58" t="s">
         <v>719</v>
       </c>
-      <c r="C104" s="58" t="s">
+      <c r="D104" s="58" t="s">
         <v>720</v>
-      </c>
-      <c r="D104" s="58" t="s">
-        <v>721</v>
       </c>
       <c r="E104" s="58" t="s">
         <v>16</v>
@@ -10652,16 +10649,16 @@
     </row>
     <row r="105" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="122" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B105" s="122" t="s">
         <v>279</v>
       </c>
       <c r="C105" s="122" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D105" s="122" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="E105" s="122" t="s">
         <v>16</v>
@@ -10686,7 +10683,7 @@
     </row>
     <row r="106" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="58" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B106" s="58" t="s">
         <v>209</v>
@@ -10718,7 +10715,7 @@
     </row>
     <row r="107" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="58" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B107" s="58" t="s">
         <v>197</v>
@@ -10748,7 +10745,7 @@
     </row>
     <row r="108" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="58" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B108" s="58" t="s">
         <v>222</v>
@@ -10780,7 +10777,7 @@
     </row>
     <row r="109" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="58" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B109" s="58" t="s">
         <v>0</v>
@@ -11305,13 +11302,13 @@
         <v>168</v>
       </c>
       <c r="B125" s="42" t="s">
+        <v>764</v>
+      </c>
+      <c r="C125" s="42" t="s">
         <v>765</v>
       </c>
-      <c r="C125" s="42" t="s">
+      <c r="D125" s="58" t="s">
         <v>766</v>
-      </c>
-      <c r="D125" s="58" t="s">
-        <v>767</v>
       </c>
       <c r="E125" s="58" t="s">
         <v>16</v>
@@ -11663,8 +11660,8 @@
   </sheetPr>
   <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11694,7 +11691,7 @@
         <v>494</v>
       </c>
       <c r="D1" s="38" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="E1" s="38" t="s">
         <v>233</v>
@@ -11730,14 +11727,14 @@
       </c>
       <c r="B2" s="83"/>
       <c r="C2" s="83" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="D2" s="83"/>
       <c r="E2" s="83" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="F2" s="83" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="G2" s="83" t="s">
         <v>351</v>
@@ -11881,7 +11878,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="F7" t="s">
         <v>352</v>
@@ -11912,7 +11909,7 @@
       <c r="C8" s="118"/>
       <c r="D8" s="118"/>
       <c r="E8" s="118" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="F8" s="118" t="s">
         <v>632</v>
@@ -11981,7 +11978,7 @@
         <v>454</v>
       </c>
       <c r="F10" s="118" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="G10" s="118" t="s">
         <v>455</v>
@@ -12011,7 +12008,7 @@
       <c r="C11" s="118"/>
       <c r="D11" s="118"/>
       <c r="E11" s="118" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="F11" s="118" t="s">
         <v>429</v>
@@ -12491,7 +12488,7 @@
       </c>
       <c r="D27" s="83"/>
       <c r="E27" s="83" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="F27" s="83" t="s">
         <v>630</v>
@@ -12698,7 +12695,7 @@
       </c>
       <c r="D34" s="83"/>
       <c r="E34" s="83" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="F34" s="83" t="s">
         <v>631</v>
@@ -12781,7 +12778,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B37">
         <v>6</v>
@@ -12790,7 +12787,7 @@
         <v>454</v>
       </c>
       <c r="F37" t="s">
-        <v>634</v>
+        <v>698</v>
       </c>
       <c r="G37" t="s">
         <v>455</v>
@@ -12810,7 +12807,7 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B38">
         <v>6</v>
@@ -12839,7 +12836,7 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B39">
         <v>6</v>
@@ -12910,7 +12907,7 @@
         <v>553</v>
       </c>
       <c r="F41" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="G41" t="s">
         <v>556</v>
@@ -12939,7 +12936,7 @@
         <v>554</v>
       </c>
       <c r="F42" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="G42" t="s">
         <v>557</v>
@@ -12968,7 +12965,7 @@
         <v>555</v>
       </c>
       <c r="F43" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="G43" t="s">
         <v>558</v>
@@ -13126,7 +13123,7 @@
         <v>623</v>
       </c>
       <c r="G48" s="18" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="H48" s="18"/>
       <c r="I48" s="18" t="s">
@@ -13151,13 +13148,13 @@
       <c r="C49" s="18"/>
       <c r="D49" s="18"/>
       <c r="E49" s="18" t="s">
+        <v>692</v>
+      </c>
+      <c r="F49" s="18" t="s">
+        <v>691</v>
+      </c>
+      <c r="G49" s="18" t="s">
         <v>693</v>
-      </c>
-      <c r="F49" s="18" t="s">
-        <v>692</v>
-      </c>
-      <c r="G49" s="18" t="s">
-        <v>694</v>
       </c>
       <c r="H49" s="18"/>
       <c r="I49" s="18" t="s">
@@ -13178,17 +13175,17 @@
       </c>
       <c r="B50" s="83"/>
       <c r="C50" s="83" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="D50" s="83"/>
       <c r="E50" s="83" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="F50" s="83" t="s">
+        <v>750</v>
+      </c>
+      <c r="G50" s="83" t="s">
         <v>751</v>
-      </c>
-      <c r="G50" s="83" t="s">
-        <v>752</v>
       </c>
       <c r="H50" s="83" t="s">
         <v>593</v>
@@ -13217,13 +13214,13 @@
         <v>0</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="F51" s="18" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="G51" s="18" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="H51" t="s">
         <v>502</v>
@@ -13252,13 +13249,13 @@
         <v>1</v>
       </c>
       <c r="E52" s="18" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="F52" s="18" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="G52" s="18" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="H52" t="s">
         <v>499</v>
@@ -13287,13 +13284,13 @@
         <v>2</v>
       </c>
       <c r="E53" s="18" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="F53" s="18" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="G53" s="18" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="H53" t="s">
         <v>500</v>
@@ -13322,13 +13319,13 @@
         <v>3</v>
       </c>
       <c r="E54" s="18" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="F54" s="18" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="G54" s="18" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="H54" t="s">
         <v>501</v>
@@ -15027,11 +15024,11 @@
         <v>143</v>
       </c>
       <c r="B48" s="72" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C48" s="72"/>
       <c r="D48" s="72" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="E48" s="72" t="s">
         <v>17</v>
@@ -15053,11 +15050,11 @@
         <v>143</v>
       </c>
       <c r="B49" s="72" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C49" s="72"/>
       <c r="D49" s="72" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="E49" s="72" t="s">
         <v>16</v>
@@ -17029,7 +17026,7 @@
         <v>167</v>
       </c>
       <c r="E39" s="46" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="F39" s="33">
         <v>1</v>
@@ -17062,7 +17059,7 @@
         <v>167</v>
       </c>
       <c r="E40" s="46" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="F40" s="33">
         <v>1</v>
@@ -17625,7 +17622,7 @@
         <v>167</v>
       </c>
       <c r="E57" s="92" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="F57" s="91">
         <v>1</v>
@@ -17658,7 +17655,7 @@
         <v>167</v>
       </c>
       <c r="E58" s="92" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="F58" s="91">
         <v>1</v>
@@ -17724,7 +17721,7 @@
         <v>167</v>
       </c>
       <c r="E60" s="92" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="F60" s="91">
         <v>1</v>
@@ -17757,7 +17754,7 @@
         <v>167</v>
       </c>
       <c r="E61" s="92" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="F61" s="91">
         <v>1</v>
@@ -17790,7 +17787,7 @@
         <v>167</v>
       </c>
       <c r="E62" s="92" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="F62" s="91">
         <v>1</v>
@@ -17823,7 +17820,7 @@
         <v>167</v>
       </c>
       <c r="E63" s="92" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="F63" s="91">
         <v>1</v>
@@ -17856,7 +17853,7 @@
         <v>167</v>
       </c>
       <c r="E64" s="92" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="F64" s="91">
         <v>1</v>
@@ -18153,7 +18150,7 @@
         <v>479</v>
       </c>
       <c r="C2" s="87" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="D2" s="86" t="s">
         <v>488</v>
@@ -18170,10 +18167,10 @@
         <v>21</v>
       </c>
       <c r="B3" s="85" t="s">
+        <v>685</v>
+      </c>
+      <c r="C3" s="85" t="s">
         <v>686</v>
-      </c>
-      <c r="C3" s="85" t="s">
-        <v>687</v>
       </c>
       <c r="D3" s="84" t="s">
         <v>405</v>

</xml_diff>

<commit_message>
add complete report agg and detail
</commit_message>
<xml_diff>
--- a/db/excel/api-function-granted-users-cdld.xlsx
+++ b/db/excel/api-function-granted-users-cdld.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10808"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0B8638-ED39-3743-A899-B6CC93338D52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1208B5-E99B-AC4B-8D94-1494E1C34587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19460" tabRatio="800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19460" tabRatio="800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_types" sheetId="27" r:id="rId1"/>
@@ -228,7 +228,7 @@
     <definedName name="yyjy_ukyu" localSheetId="0">{"'Sheet1'!$L$16"}</definedName>
     <definedName name="yyjy_ukyu">{"'Sheet1'!$L$16"}</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -300,7 +300,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2035" uniqueCount="768">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2041" uniqueCount="770">
   <si>
     <t>status</t>
   </si>
@@ -2706,6 +2706,12 @@
   </si>
   <si>
     <t>Đã thực hiện đánh giá (đánh giá gì thì khi đánh giá xong cũng chuyển trạng thái qua 116 này)</t>
+  </si>
+  <si>
+    <t>Thứ tự sắp xếp</t>
+  </si>
+  <si>
+    <t>Thứ Tự</t>
   </si>
 </sst>
 </file>
@@ -7200,13 +7206,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P135"/>
+  <dimension ref="A1:P136"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C49" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C112" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C90" sqref="C90"/>
+      <selection pane="bottomRight" activeCell="C136" sqref="C136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9689,7 +9695,7 @@
       <c r="N75" s="49"/>
       <c r="O75" s="49"/>
       <c r="P75" s="53">
-        <v>102</v>
+        <v>74</v>
       </c>
     </row>
     <row r="76" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
@@ -9723,7 +9729,7 @@
       <c r="N76" s="44"/>
       <c r="O76" s="44"/>
       <c r="P76" s="53">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="77" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
@@ -9755,7 +9761,7 @@
       <c r="N77" s="44"/>
       <c r="O77" s="44"/>
       <c r="P77" s="53">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="78" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
@@ -9785,7 +9791,7 @@
       <c r="N78" s="44"/>
       <c r="O78" s="44"/>
       <c r="P78" s="53">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="79" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
@@ -9817,7 +9823,7 @@
       <c r="N79" s="44"/>
       <c r="O79" s="44"/>
       <c r="P79" s="53">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="80" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
@@ -9847,7 +9853,7 @@
       <c r="N80" s="44"/>
       <c r="O80" s="44"/>
       <c r="P80" s="53">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="81" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
@@ -9879,7 +9885,7 @@
       <c r="N81" s="44"/>
       <c r="O81" s="44"/>
       <c r="P81" s="53">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="82" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
@@ -9913,7 +9919,7 @@
       <c r="N82" s="119"/>
       <c r="O82" s="119"/>
       <c r="P82" s="53">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="83" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
@@ -9951,7 +9957,7 @@
       <c r="N83" s="119"/>
       <c r="O83" s="119"/>
       <c r="P83" s="53">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="84" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
@@ -9985,7 +9991,7 @@
       <c r="N84" s="52"/>
       <c r="O84" s="52"/>
       <c r="P84" s="53">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="85" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
@@ -10021,7 +10027,7 @@
       <c r="N85" s="119"/>
       <c r="O85" s="119"/>
       <c r="P85" s="53">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="86" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
@@ -10055,7 +10061,7 @@
       <c r="N86" s="119"/>
       <c r="O86" s="119"/>
       <c r="P86" s="53">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="87" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
@@ -10087,7 +10093,7 @@
       <c r="N87" s="119"/>
       <c r="O87" s="119"/>
       <c r="P87" s="53">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="88" spans="1:16" s="76" customFormat="1" x14ac:dyDescent="0.2">
@@ -11367,7 +11373,7 @@
       <c r="N126" s="43"/>
       <c r="O126" s="43"/>
       <c r="P126" s="53">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="127" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
@@ -11399,7 +11405,7 @@
       <c r="N127" s="43"/>
       <c r="O127" s="43"/>
       <c r="P127" s="53">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="128" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
@@ -11431,7 +11437,7 @@
       <c r="N128" s="43"/>
       <c r="O128" s="43"/>
       <c r="P128" s="53">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="129" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
@@ -11463,7 +11469,7 @@
       <c r="N129" s="43"/>
       <c r="O129" s="43"/>
       <c r="P129" s="53">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="130" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
@@ -11495,7 +11501,7 @@
       <c r="N130" s="43"/>
       <c r="O130" s="43"/>
       <c r="P130" s="53">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="131" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
@@ -11525,7 +11531,7 @@
       <c r="N131" s="43"/>
       <c r="O131" s="43"/>
       <c r="P131" s="53">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="132" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
@@ -11557,7 +11563,7 @@
       <c r="N132" s="43"/>
       <c r="O132" s="43"/>
       <c r="P132" s="53">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="133" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
@@ -11587,7 +11593,7 @@
       <c r="N133" s="43"/>
       <c r="O133" s="43"/>
       <c r="P133" s="53">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="134" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
@@ -11619,7 +11625,7 @@
       <c r="N134" s="43"/>
       <c r="O134" s="43"/>
       <c r="P134" s="53">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="135" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
@@ -11627,16 +11633,16 @@
         <v>168</v>
       </c>
       <c r="B135" s="42" t="s">
-        <v>0</v>
+        <v>662</v>
       </c>
       <c r="C135" s="42" t="s">
-        <v>226</v>
+        <v>769</v>
       </c>
       <c r="D135" s="58" t="s">
-        <v>171</v>
+        <v>768</v>
       </c>
       <c r="E135" s="58" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F135" s="43"/>
       <c r="G135" s="43"/>
@@ -11651,7 +11657,39 @@
       <c r="N135" s="43"/>
       <c r="O135" s="43"/>
       <c r="P135" s="53">
-        <v>133</v>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="136" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A136" s="42" t="s">
+        <v>168</v>
+      </c>
+      <c r="B136" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C136" s="42" t="s">
+        <v>226</v>
+      </c>
+      <c r="D136" s="58" t="s">
+        <v>171</v>
+      </c>
+      <c r="E136" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="F136" s="43"/>
+      <c r="G136" s="43"/>
+      <c r="H136" s="43"/>
+      <c r="I136" s="43"/>
+      <c r="J136" s="43"/>
+      <c r="K136" s="43"/>
+      <c r="L136" s="43"/>
+      <c r="M136" s="43">
+        <v>1</v>
+      </c>
+      <c r="N136" s="43"/>
+      <c r="O136" s="43"/>
+      <c r="P136" s="53">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -11665,10 +11703,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:M55"/>
+  <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11685,9 +11723,10 @@
     <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="38" t="s">
         <v>18</v>
       </c>
@@ -11725,10 +11764,13 @@
         <v>45</v>
       </c>
       <c r="M1" s="38" t="s">
+        <v>662</v>
+      </c>
+      <c r="N1" s="38" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="83">
         <v>1</v>
       </c>
@@ -11760,8 +11802,11 @@
       <c r="M2" s="83">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2" s="83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>11</v>
       </c>
@@ -11787,10 +11832,13 @@
         <v>164</v>
       </c>
       <c r="M3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>12</v>
       </c>
@@ -11816,10 +11864,13 @@
         <v>164</v>
       </c>
       <c r="M4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>13</v>
       </c>
@@ -11845,10 +11896,13 @@
         <v>164</v>
       </c>
       <c r="M5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>14</v>
       </c>
@@ -11874,10 +11928,13 @@
         <v>164</v>
       </c>
       <c r="M6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>15</v>
       </c>
@@ -11903,10 +11960,13 @@
         <v>164</v>
       </c>
       <c r="M7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="118">
         <v>111</v>
       </c>
@@ -11935,11 +11995,14 @@
       <c r="L8" t="s">
         <v>164</v>
       </c>
-      <c r="M8" s="118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M8">
+        <v>7</v>
+      </c>
+      <c r="N8" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="118">
         <v>112</v>
       </c>
@@ -11968,11 +12031,14 @@
       <c r="L9" t="s">
         <v>164</v>
       </c>
-      <c r="M9" s="118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M9">
+        <v>8</v>
+      </c>
+      <c r="N9" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="118">
         <v>114</v>
       </c>
@@ -12001,11 +12067,14 @@
       <c r="L10" t="s">
         <v>164</v>
       </c>
-      <c r="M10" s="118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M10">
+        <v>9</v>
+      </c>
+      <c r="N10" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="118">
         <v>115</v>
       </c>
@@ -12034,11 +12103,14 @@
       <c r="L11" t="s">
         <v>164</v>
       </c>
-      <c r="M11" s="118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M11">
+        <v>10</v>
+      </c>
+      <c r="N11" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="118">
         <v>116</v>
       </c>
@@ -12067,11 +12139,14 @@
       <c r="L12" t="s">
         <v>164</v>
       </c>
-      <c r="M12" s="118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M12">
+        <v>11</v>
+      </c>
+      <c r="N12" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="83">
         <v>2</v>
       </c>
@@ -12101,10 +12176,13 @@
         <v>164</v>
       </c>
       <c r="M13" s="83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="N13" s="83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>21</v>
       </c>
@@ -12130,10 +12208,13 @@
         <v>164</v>
       </c>
       <c r="M14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>22</v>
       </c>
@@ -12159,10 +12240,13 @@
         <v>164</v>
       </c>
       <c r="M15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="83">
         <v>3</v>
       </c>
@@ -12192,10 +12276,13 @@
         <v>164</v>
       </c>
       <c r="M16" s="83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="N16" s="83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>31</v>
       </c>
@@ -12221,10 +12308,13 @@
         <v>164</v>
       </c>
       <c r="M17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>32</v>
       </c>
@@ -12250,10 +12340,13 @@
         <v>164</v>
       </c>
       <c r="M18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>33</v>
       </c>
@@ -12279,10 +12372,13 @@
         <v>164</v>
       </c>
       <c r="M19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>34</v>
       </c>
@@ -12308,10 +12404,13 @@
         <v>164</v>
       </c>
       <c r="M20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>35</v>
       </c>
@@ -12337,10 +12436,13 @@
         <v>164</v>
       </c>
       <c r="M21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>36</v>
       </c>
@@ -12366,10 +12468,13 @@
         <v>164</v>
       </c>
       <c r="M22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="83">
         <v>4</v>
       </c>
@@ -12399,10 +12504,13 @@
         <v>164</v>
       </c>
       <c r="M23" s="83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="N23" s="83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>41</v>
       </c>
@@ -12428,10 +12536,13 @@
         <v>164</v>
       </c>
       <c r="M24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>42</v>
       </c>
@@ -12457,10 +12568,13 @@
         <v>164</v>
       </c>
       <c r="M25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>43</v>
       </c>
@@ -12486,10 +12600,13 @@
         <v>164</v>
       </c>
       <c r="M26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="N26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>44</v>
       </c>
@@ -12515,10 +12632,13 @@
         <v>164</v>
       </c>
       <c r="M27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="83">
         <v>5</v>
       </c>
@@ -12548,10 +12668,13 @@
         <v>164</v>
       </c>
       <c r="M28" s="83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="N28" s="83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>51</v>
       </c>
@@ -12577,10 +12700,13 @@
         <v>164</v>
       </c>
       <c r="M29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="N29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>52</v>
       </c>
@@ -12606,10 +12732,13 @@
         <v>164</v>
       </c>
       <c r="M30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="N30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>53</v>
       </c>
@@ -12635,10 +12764,13 @@
         <v>164</v>
       </c>
       <c r="M31" s="88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="N31" s="88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>54</v>
       </c>
@@ -12664,10 +12796,13 @@
         <v>164</v>
       </c>
       <c r="M32" s="88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="N32" s="88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>55</v>
       </c>
@@ -12693,10 +12828,13 @@
         <v>164</v>
       </c>
       <c r="M33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="N33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>56</v>
       </c>
@@ -12722,10 +12860,13 @@
         <v>164</v>
       </c>
       <c r="M34" s="88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="N34" s="88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="83">
         <v>6</v>
       </c>
@@ -12755,10 +12896,13 @@
         <v>164</v>
       </c>
       <c r="M35" s="83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="N35" s="83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>61</v>
       </c>
@@ -12784,10 +12928,13 @@
         <v>164</v>
       </c>
       <c r="M36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="N36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>62</v>
       </c>
@@ -12813,10 +12960,13 @@
         <v>164</v>
       </c>
       <c r="M37" s="88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="N37" s="88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>64</v>
       </c>
@@ -12842,10 +12992,13 @@
         <v>164</v>
       </c>
       <c r="M38" s="88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="N38" s="88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>65</v>
       </c>
@@ -12871,10 +13024,13 @@
         <v>164</v>
       </c>
       <c r="M39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="N39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>66</v>
       </c>
@@ -12900,10 +13056,13 @@
         <v>164</v>
       </c>
       <c r="M40" s="88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="N40" s="88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="83">
         <v>7</v>
       </c>
@@ -12933,10 +13092,13 @@
         <v>164</v>
       </c>
       <c r="M41" s="83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="N41" s="83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>71</v>
       </c>
@@ -12962,10 +13124,13 @@
         <v>164</v>
       </c>
       <c r="M42" s="88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="N42" s="88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>72</v>
       </c>
@@ -12991,10 +13156,13 @@
         <v>164</v>
       </c>
       <c r="M43" s="88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="N43" s="88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>73</v>
       </c>
@@ -13020,10 +13188,13 @@
         <v>164</v>
       </c>
       <c r="M44" s="88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="N44" s="88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>74</v>
       </c>
@@ -13049,10 +13220,13 @@
         <v>164</v>
       </c>
       <c r="M45" s="88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="N45" s="88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="83">
         <v>8</v>
       </c>
@@ -13082,10 +13256,13 @@
         <v>164</v>
       </c>
       <c r="M46" s="83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+      <c r="N46" s="83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="18">
         <v>81</v>
       </c>
@@ -13113,10 +13290,13 @@
         <v>164</v>
       </c>
       <c r="M47" s="129">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="N47" s="129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="18">
         <v>82</v>
       </c>
@@ -13144,10 +13324,13 @@
         <v>164</v>
       </c>
       <c r="M48" s="129">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="N48" s="129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="18">
         <v>83</v>
       </c>
@@ -13175,10 +13358,13 @@
         <v>164</v>
       </c>
       <c r="M49" s="129">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+      <c r="N49" s="129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="18">
         <v>84</v>
       </c>
@@ -13206,10 +13392,13 @@
         <v>164</v>
       </c>
       <c r="M50" s="129">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="N50" s="129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="83">
         <v>9</v>
       </c>
@@ -13239,10 +13428,13 @@
         <v>164</v>
       </c>
       <c r="M51" s="83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="N51" s="83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="18">
         <v>90</v>
       </c>
@@ -13274,10 +13466,13 @@
         <v>164</v>
       </c>
       <c r="M52" s="129">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="N52" s="129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="18">
         <v>91</v>
       </c>
@@ -13309,10 +13504,13 @@
         <v>164</v>
       </c>
       <c r="M53" s="129">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+      <c r="N53" s="129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="18">
         <v>92</v>
       </c>
@@ -13344,10 +13542,13 @@
         <v>164</v>
       </c>
       <c r="M54" s="129">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+      <c r="N54" s="129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="18">
         <v>93</v>
       </c>
@@ -13379,6 +13580,9 @@
         <v>164</v>
       </c>
       <c r="M55" s="129">
+        <v>54</v>
+      </c>
+      <c r="N55" s="129">
         <v>1</v>
       </c>
     </row>

</xml_diff>